<commit_message>
Add last_update and pso_name columns to project export
</commit_message>
<xml_diff>
--- a/lib/fcerm1_template.xlsx
+++ b/lib/fcerm1_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthall/Work/pafs/pafs_core/lib/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\x959510\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16230ADF-9386-8C4D-81CA-AC41D44E0D83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED8BA3D2-F58C-4C09-9C50-FA848AD2D1BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="68800" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master local choices" sheetId="2" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="348">
   <si>
     <t>FCRM1 - National Capital Programme</t>
   </si>
@@ -1190,17 +1190,23 @@
   <si>
     <t>Lifecycle Carbon</t>
   </si>
+  <si>
+    <t>Last Updated</t>
+  </si>
+  <si>
+    <t>PSO Name</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="#,##0.0"/>
-    <numFmt numFmtId="167" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
-    <numFmt numFmtId="168" formatCode="#,##0.0_ ;[Red]\-#,##0.0\ "/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0"/>
+    <numFmt numFmtId="166" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
+    <numFmt numFmtId="167" formatCode="#,##0.0_ ;[Red]\-#,##0.0\ "/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -1471,7 +1477,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1569,10 +1575,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
@@ -1580,9 +1599,9 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -1647,7 +1666,7 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1669,7 +1688,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1678,10 +1697,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1738,106 +1757,25 @@
     <xf numFmtId="9" fontId="16" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="167" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="11" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="25" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1845,11 +1783,104 @@
     <xf numFmtId="0" fontId="12" fillId="25" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="25" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="11" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -1861,7 +1892,7 @@
     <cellStyle name="Normal 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Normal 2 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Normal_RCP" xfId="5" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Per cent" xfId="2" builtinId="5"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
     <cellStyle name="Percent 11" xfId="7" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
   </cellStyles>
   <dxfs count="1">
@@ -2155,20 +2186,20 @@
     <tabColor rgb="FF92D050"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:KM32"/>
+  <dimension ref="A1:KO32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="KD7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="KL7" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
       <selection pane="topRight" activeCell="C7" sqref="C7"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="KJ29" sqref="KJ29"/>
+      <selection pane="bottomRight" activeCell="KM12" sqref="KM12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="98.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="98.6640625" style="1" customWidth="1"/>
     <col min="3" max="4" width="21" style="3" customWidth="1"/>
     <col min="5" max="6" width="21" style="1" customWidth="1"/>
     <col min="7" max="7" width="21" style="2" customWidth="1"/>
@@ -2185,18 +2216,20 @@
     <col min="45" max="278" width="21" style="1" customWidth="1"/>
     <col min="279" max="285" width="21" style="28" customWidth="1"/>
     <col min="286" max="293" width="21" style="6" customWidth="1"/>
-    <col min="294" max="296" width="22.28515625" style="7" customWidth="1"/>
-    <col min="297" max="297" width="17.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="298" max="298" width="19.7109375" style="7" customWidth="1"/>
-    <col min="299" max="299" width="21.5703125" style="7" customWidth="1"/>
-    <col min="300" max="16384" width="8.7109375" style="7"/>
+    <col min="294" max="296" width="22.33203125" style="7" customWidth="1"/>
+    <col min="297" max="297" width="17.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="298" max="298" width="19.6640625" style="7" customWidth="1"/>
+    <col min="299" max="299" width="21.5546875" style="7" customWidth="1"/>
+    <col min="300" max="300" width="19.6640625" style="7" customWidth="1"/>
+    <col min="301" max="301" width="21.5546875" style="7" customWidth="1"/>
+    <col min="302" max="16384" width="8.6640625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:299" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="80" t="s">
+    <row r="1" spans="1:301" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="80"/>
+      <c r="B1" s="68"/>
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
       <c r="E1" s="23"/>
@@ -2494,12 +2527,14 @@
       <c r="KK1" s="47"/>
       <c r="KL1" s="47"/>
       <c r="KM1" s="47"/>
+      <c r="KN1" s="47"/>
+      <c r="KO1" s="47"/>
     </row>
-    <row r="2" spans="1:299" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="81" t="s">
+    <row r="2" spans="1:301" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="69" t="s">
         <v>337</v>
       </c>
-      <c r="B2" s="81"/>
+      <c r="B2" s="69"/>
       <c r="C2" s="36"/>
       <c r="D2" s="36"/>
       <c r="E2" s="23"/>
@@ -2797,8 +2832,10 @@
       <c r="KK2" s="47"/>
       <c r="KL2" s="47"/>
       <c r="KM2" s="47"/>
+      <c r="KN2" s="47"/>
+      <c r="KO2" s="47"/>
     </row>
-    <row r="3" spans="1:299" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:301" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="39"/>
       <c r="B3" s="40"/>
       <c r="C3" s="39"/>
@@ -3098,427 +3135,431 @@
       <c r="KK3" s="47"/>
       <c r="KL3" s="47"/>
       <c r="KM3" s="47"/>
+      <c r="KN3" s="47"/>
+      <c r="KO3" s="47"/>
     </row>
-    <row r="4" spans="1:299" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="82" t="s">
+    <row r="4" spans="1:301" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="82"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="82"/>
-      <c r="E4" s="83" t="s">
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="83"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="83"/>
-      <c r="J4" s="83"/>
-      <c r="K4" s="84" t="s">
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
+      <c r="I4" s="71"/>
+      <c r="J4" s="71"/>
+      <c r="K4" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="84"/>
-      <c r="M4" s="84"/>
-      <c r="N4" s="84"/>
-      <c r="O4" s="84"/>
-      <c r="P4" s="85" t="s">
+      <c r="L4" s="72"/>
+      <c r="M4" s="72"/>
+      <c r="N4" s="72"/>
+      <c r="O4" s="72"/>
+      <c r="P4" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="Q4" s="85"/>
-      <c r="R4" s="85"/>
-      <c r="S4" s="85"/>
-      <c r="T4" s="85"/>
-      <c r="U4" s="86" t="s">
+      <c r="Q4" s="73"/>
+      <c r="R4" s="73"/>
+      <c r="S4" s="73"/>
+      <c r="T4" s="73"/>
+      <c r="U4" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="V4" s="86"/>
-      <c r="W4" s="86"/>
-      <c r="X4" s="86"/>
-      <c r="Y4" s="86"/>
-      <c r="Z4" s="86"/>
-      <c r="AA4" s="86"/>
-      <c r="AB4" s="86"/>
-      <c r="AC4" s="87" t="s">
+      <c r="V4" s="74"/>
+      <c r="W4" s="74"/>
+      <c r="X4" s="74"/>
+      <c r="Y4" s="74"/>
+      <c r="Z4" s="74"/>
+      <c r="AA4" s="74"/>
+      <c r="AB4" s="74"/>
+      <c r="AC4" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="AD4" s="87"/>
-      <c r="AE4" s="87"/>
-      <c r="AF4" s="87"/>
-      <c r="AG4" s="87"/>
-      <c r="AH4" s="87"/>
-      <c r="AI4" s="87"/>
-      <c r="AJ4" s="88" t="s">
+      <c r="AD4" s="75"/>
+      <c r="AE4" s="75"/>
+      <c r="AF4" s="75"/>
+      <c r="AG4" s="75"/>
+      <c r="AH4" s="75"/>
+      <c r="AI4" s="75"/>
+      <c r="AJ4" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="AK4" s="88"/>
-      <c r="AL4" s="88"/>
-      <c r="AM4" s="79" t="s">
+      <c r="AK4" s="76"/>
+      <c r="AL4" s="76"/>
+      <c r="AM4" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="AN4" s="79"/>
-      <c r="AO4" s="69"/>
-      <c r="AP4" s="69"/>
-      <c r="AQ4" s="69"/>
-      <c r="AR4" s="69"/>
-      <c r="AS4" s="70" t="s">
+      <c r="AN4" s="67"/>
+      <c r="AO4" s="78"/>
+      <c r="AP4" s="78"/>
+      <c r="AQ4" s="78"/>
+      <c r="AR4" s="78"/>
+      <c r="AS4" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="AT4" s="70"/>
-      <c r="AU4" s="70"/>
-      <c r="AV4" s="70"/>
-      <c r="AW4" s="70"/>
-      <c r="AX4" s="70"/>
-      <c r="AY4" s="70"/>
-      <c r="AZ4" s="70"/>
-      <c r="BA4" s="70"/>
-      <c r="BB4" s="70"/>
-      <c r="BC4" s="70"/>
-      <c r="BD4" s="70"/>
-      <c r="BE4" s="70"/>
-      <c r="BF4" s="70"/>
-      <c r="BG4" s="70"/>
-      <c r="BH4" s="70"/>
-      <c r="BI4" s="70"/>
-      <c r="BJ4" s="70"/>
-      <c r="BK4" s="66" t="s">
+      <c r="AT4" s="79"/>
+      <c r="AU4" s="79"/>
+      <c r="AV4" s="79"/>
+      <c r="AW4" s="79"/>
+      <c r="AX4" s="79"/>
+      <c r="AY4" s="79"/>
+      <c r="AZ4" s="79"/>
+      <c r="BA4" s="79"/>
+      <c r="BB4" s="79"/>
+      <c r="BC4" s="79"/>
+      <c r="BD4" s="79"/>
+      <c r="BE4" s="79"/>
+      <c r="BF4" s="79"/>
+      <c r="BG4" s="79"/>
+      <c r="BH4" s="79"/>
+      <c r="BI4" s="79"/>
+      <c r="BJ4" s="79"/>
+      <c r="BK4" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="BL4" s="66"/>
-      <c r="BM4" s="66"/>
-      <c r="BN4" s="66"/>
-      <c r="BO4" s="66"/>
-      <c r="BP4" s="66"/>
-      <c r="BQ4" s="66"/>
-      <c r="BR4" s="66"/>
-      <c r="BS4" s="66"/>
-      <c r="BT4" s="66"/>
-      <c r="BU4" s="66"/>
-      <c r="BV4" s="66"/>
-      <c r="BW4" s="66"/>
-      <c r="BX4" s="66"/>
-      <c r="BY4" s="71" t="s">
+      <c r="BL4" s="77"/>
+      <c r="BM4" s="77"/>
+      <c r="BN4" s="77"/>
+      <c r="BO4" s="77"/>
+      <c r="BP4" s="77"/>
+      <c r="BQ4" s="77"/>
+      <c r="BR4" s="77"/>
+      <c r="BS4" s="77"/>
+      <c r="BT4" s="77"/>
+      <c r="BU4" s="77"/>
+      <c r="BV4" s="77"/>
+      <c r="BW4" s="77"/>
+      <c r="BX4" s="77"/>
+      <c r="BY4" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="BZ4" s="71"/>
-      <c r="CA4" s="71"/>
-      <c r="CB4" s="71"/>
-      <c r="CC4" s="71"/>
-      <c r="CD4" s="71"/>
-      <c r="CE4" s="71"/>
-      <c r="CF4" s="71"/>
-      <c r="CG4" s="71"/>
-      <c r="CH4" s="71"/>
-      <c r="CI4" s="71"/>
-      <c r="CJ4" s="71"/>
-      <c r="CK4" s="71"/>
-      <c r="CL4" s="71"/>
-      <c r="CM4" s="72" t="s">
+      <c r="BZ4" s="80"/>
+      <c r="CA4" s="80"/>
+      <c r="CB4" s="80"/>
+      <c r="CC4" s="80"/>
+      <c r="CD4" s="80"/>
+      <c r="CE4" s="80"/>
+      <c r="CF4" s="80"/>
+      <c r="CG4" s="80"/>
+      <c r="CH4" s="80"/>
+      <c r="CI4" s="80"/>
+      <c r="CJ4" s="80"/>
+      <c r="CK4" s="80"/>
+      <c r="CL4" s="80"/>
+      <c r="CM4" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="CN4" s="72"/>
-      <c r="CO4" s="72"/>
-      <c r="CP4" s="72"/>
-      <c r="CQ4" s="72"/>
-      <c r="CR4" s="72"/>
-      <c r="CS4" s="72"/>
-      <c r="CT4" s="72"/>
-      <c r="CU4" s="72"/>
-      <c r="CV4" s="72"/>
-      <c r="CW4" s="72"/>
-      <c r="CX4" s="72"/>
-      <c r="CY4" s="72"/>
-      <c r="CZ4" s="72"/>
-      <c r="DA4" s="73" t="s">
+      <c r="CN4" s="81"/>
+      <c r="CO4" s="81"/>
+      <c r="CP4" s="81"/>
+      <c r="CQ4" s="81"/>
+      <c r="CR4" s="81"/>
+      <c r="CS4" s="81"/>
+      <c r="CT4" s="81"/>
+      <c r="CU4" s="81"/>
+      <c r="CV4" s="81"/>
+      <c r="CW4" s="81"/>
+      <c r="CX4" s="81"/>
+      <c r="CY4" s="81"/>
+      <c r="CZ4" s="81"/>
+      <c r="DA4" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="DB4" s="73"/>
-      <c r="DC4" s="73"/>
-      <c r="DD4" s="73"/>
-      <c r="DE4" s="73"/>
-      <c r="DF4" s="73"/>
-      <c r="DG4" s="73"/>
-      <c r="DH4" s="73"/>
-      <c r="DI4" s="73"/>
-      <c r="DJ4" s="73"/>
-      <c r="DK4" s="73"/>
-      <c r="DL4" s="73"/>
-      <c r="DM4" s="73"/>
-      <c r="DN4" s="73"/>
-      <c r="DO4" s="74" t="s">
+      <c r="DB4" s="82"/>
+      <c r="DC4" s="82"/>
+      <c r="DD4" s="82"/>
+      <c r="DE4" s="82"/>
+      <c r="DF4" s="82"/>
+      <c r="DG4" s="82"/>
+      <c r="DH4" s="82"/>
+      <c r="DI4" s="82"/>
+      <c r="DJ4" s="82"/>
+      <c r="DK4" s="82"/>
+      <c r="DL4" s="82"/>
+      <c r="DM4" s="82"/>
+      <c r="DN4" s="82"/>
+      <c r="DO4" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="DP4" s="74"/>
-      <c r="DQ4" s="74"/>
-      <c r="DR4" s="74"/>
-      <c r="DS4" s="74"/>
-      <c r="DT4" s="74"/>
-      <c r="DU4" s="74"/>
-      <c r="DV4" s="74"/>
-      <c r="DW4" s="74"/>
-      <c r="DX4" s="74"/>
-      <c r="DY4" s="74"/>
-      <c r="DZ4" s="74"/>
-      <c r="EA4" s="74"/>
-      <c r="EB4" s="74"/>
-      <c r="EC4" s="75" t="s">
+      <c r="DP4" s="83"/>
+      <c r="DQ4" s="83"/>
+      <c r="DR4" s="83"/>
+      <c r="DS4" s="83"/>
+      <c r="DT4" s="83"/>
+      <c r="DU4" s="83"/>
+      <c r="DV4" s="83"/>
+      <c r="DW4" s="83"/>
+      <c r="DX4" s="83"/>
+      <c r="DY4" s="83"/>
+      <c r="DZ4" s="83"/>
+      <c r="EA4" s="83"/>
+      <c r="EB4" s="83"/>
+      <c r="EC4" s="84" t="s">
         <v>15</v>
       </c>
-      <c r="ED4" s="75"/>
-      <c r="EE4" s="75"/>
-      <c r="EF4" s="75"/>
-      <c r="EG4" s="75"/>
-      <c r="EH4" s="75"/>
-      <c r="EI4" s="75"/>
-      <c r="EJ4" s="75"/>
-      <c r="EK4" s="75"/>
-      <c r="EL4" s="75"/>
-      <c r="EM4" s="75"/>
-      <c r="EN4" s="75"/>
-      <c r="EO4" s="75"/>
-      <c r="EP4" s="75"/>
-      <c r="EQ4" s="76" t="s">
+      <c r="ED4" s="84"/>
+      <c r="EE4" s="84"/>
+      <c r="EF4" s="84"/>
+      <c r="EG4" s="84"/>
+      <c r="EH4" s="84"/>
+      <c r="EI4" s="84"/>
+      <c r="EJ4" s="84"/>
+      <c r="EK4" s="84"/>
+      <c r="EL4" s="84"/>
+      <c r="EM4" s="84"/>
+      <c r="EN4" s="84"/>
+      <c r="EO4" s="84"/>
+      <c r="EP4" s="84"/>
+      <c r="EQ4" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="ER4" s="76"/>
-      <c r="ES4" s="76"/>
-      <c r="ET4" s="76"/>
-      <c r="EU4" s="76"/>
-      <c r="EV4" s="76"/>
-      <c r="EW4" s="76"/>
-      <c r="EX4" s="76"/>
-      <c r="EY4" s="76"/>
-      <c r="EZ4" s="76"/>
-      <c r="FA4" s="76"/>
-      <c r="FB4" s="76"/>
-      <c r="FC4" s="76"/>
-      <c r="FD4" s="76"/>
-      <c r="FE4" s="77" t="s">
+      <c r="ER4" s="85"/>
+      <c r="ES4" s="85"/>
+      <c r="ET4" s="85"/>
+      <c r="EU4" s="85"/>
+      <c r="EV4" s="85"/>
+      <c r="EW4" s="85"/>
+      <c r="EX4" s="85"/>
+      <c r="EY4" s="85"/>
+      <c r="EZ4" s="85"/>
+      <c r="FA4" s="85"/>
+      <c r="FB4" s="85"/>
+      <c r="FC4" s="85"/>
+      <c r="FD4" s="85"/>
+      <c r="FE4" s="86" t="s">
         <v>17</v>
       </c>
-      <c r="FF4" s="77"/>
-      <c r="FG4" s="77"/>
-      <c r="FH4" s="77"/>
-      <c r="FI4" s="77"/>
-      <c r="FJ4" s="77"/>
-      <c r="FK4" s="77"/>
-      <c r="FL4" s="77"/>
-      <c r="FM4" s="77"/>
-      <c r="FN4" s="77"/>
-      <c r="FO4" s="77"/>
-      <c r="FP4" s="77"/>
-      <c r="FQ4" s="77"/>
-      <c r="FR4" s="77"/>
-      <c r="FS4" s="78" t="s">
+      <c r="FF4" s="86"/>
+      <c r="FG4" s="86"/>
+      <c r="FH4" s="86"/>
+      <c r="FI4" s="86"/>
+      <c r="FJ4" s="86"/>
+      <c r="FK4" s="86"/>
+      <c r="FL4" s="86"/>
+      <c r="FM4" s="86"/>
+      <c r="FN4" s="86"/>
+      <c r="FO4" s="86"/>
+      <c r="FP4" s="86"/>
+      <c r="FQ4" s="86"/>
+      <c r="FR4" s="86"/>
+      <c r="FS4" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="FT4" s="78"/>
-      <c r="FU4" s="78"/>
-      <c r="FV4" s="78"/>
-      <c r="FW4" s="78"/>
-      <c r="FX4" s="78"/>
-      <c r="FY4" s="78"/>
-      <c r="FZ4" s="78"/>
-      <c r="GA4" s="78"/>
-      <c r="GB4" s="78"/>
-      <c r="GC4" s="78"/>
-      <c r="GD4" s="78"/>
-      <c r="GE4" s="78"/>
-      <c r="GF4" s="78"/>
-      <c r="GG4" s="66" t="s">
+      <c r="FT4" s="87"/>
+      <c r="FU4" s="87"/>
+      <c r="FV4" s="87"/>
+      <c r="FW4" s="87"/>
+      <c r="FX4" s="87"/>
+      <c r="FY4" s="87"/>
+      <c r="FZ4" s="87"/>
+      <c r="GA4" s="87"/>
+      <c r="GB4" s="87"/>
+      <c r="GC4" s="87"/>
+      <c r="GD4" s="87"/>
+      <c r="GE4" s="87"/>
+      <c r="GF4" s="87"/>
+      <c r="GG4" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="GH4" s="66"/>
-      <c r="GI4" s="66"/>
-      <c r="GJ4" s="66"/>
-      <c r="GK4" s="66"/>
-      <c r="GL4" s="66"/>
-      <c r="GM4" s="66"/>
-      <c r="GN4" s="66"/>
-      <c r="GO4" s="66"/>
-      <c r="GP4" s="66"/>
-      <c r="GQ4" s="66"/>
-      <c r="GR4" s="66"/>
-      <c r="GS4" s="66"/>
-      <c r="GT4" s="66"/>
-      <c r="GU4" s="66" t="s">
+      <c r="GH4" s="77"/>
+      <c r="GI4" s="77"/>
+      <c r="GJ4" s="77"/>
+      <c r="GK4" s="77"/>
+      <c r="GL4" s="77"/>
+      <c r="GM4" s="77"/>
+      <c r="GN4" s="77"/>
+      <c r="GO4" s="77"/>
+      <c r="GP4" s="77"/>
+      <c r="GQ4" s="77"/>
+      <c r="GR4" s="77"/>
+      <c r="GS4" s="77"/>
+      <c r="GT4" s="77"/>
+      <c r="GU4" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="GV4" s="66"/>
-      <c r="GW4" s="66"/>
-      <c r="GX4" s="66"/>
-      <c r="GY4" s="66"/>
-      <c r="GZ4" s="66"/>
-      <c r="HA4" s="66"/>
-      <c r="HB4" s="66"/>
-      <c r="HC4" s="66"/>
-      <c r="HD4" s="66"/>
-      <c r="HE4" s="66"/>
-      <c r="HF4" s="66"/>
-      <c r="HG4" s="66"/>
-      <c r="HH4" s="66"/>
-      <c r="HI4" s="66" t="s">
+      <c r="GV4" s="77"/>
+      <c r="GW4" s="77"/>
+      <c r="GX4" s="77"/>
+      <c r="GY4" s="77"/>
+      <c r="GZ4" s="77"/>
+      <c r="HA4" s="77"/>
+      <c r="HB4" s="77"/>
+      <c r="HC4" s="77"/>
+      <c r="HD4" s="77"/>
+      <c r="HE4" s="77"/>
+      <c r="HF4" s="77"/>
+      <c r="HG4" s="77"/>
+      <c r="HH4" s="77"/>
+      <c r="HI4" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="HJ4" s="66"/>
-      <c r="HK4" s="66"/>
-      <c r="HL4" s="66"/>
-      <c r="HM4" s="66"/>
-      <c r="HN4" s="66"/>
-      <c r="HO4" s="66"/>
-      <c r="HP4" s="66"/>
-      <c r="HQ4" s="66"/>
-      <c r="HR4" s="66"/>
-      <c r="HS4" s="66"/>
-      <c r="HT4" s="66"/>
-      <c r="HU4" s="66"/>
-      <c r="HV4" s="66"/>
-      <c r="HW4" s="67" t="s">
+      <c r="HJ4" s="77"/>
+      <c r="HK4" s="77"/>
+      <c r="HL4" s="77"/>
+      <c r="HM4" s="77"/>
+      <c r="HN4" s="77"/>
+      <c r="HO4" s="77"/>
+      <c r="HP4" s="77"/>
+      <c r="HQ4" s="77"/>
+      <c r="HR4" s="77"/>
+      <c r="HS4" s="77"/>
+      <c r="HT4" s="77"/>
+      <c r="HU4" s="77"/>
+      <c r="HV4" s="77"/>
+      <c r="HW4" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="HX4" s="67"/>
-      <c r="HY4" s="67"/>
-      <c r="HZ4" s="67"/>
-      <c r="IA4" s="67"/>
-      <c r="IB4" s="67"/>
-      <c r="IC4" s="67"/>
-      <c r="ID4" s="67"/>
-      <c r="IE4" s="67"/>
-      <c r="IF4" s="67"/>
-      <c r="IG4" s="67"/>
-      <c r="IH4" s="67"/>
-      <c r="II4" s="67"/>
-      <c r="IJ4" s="67"/>
-      <c r="IK4" s="67" t="s">
+      <c r="HX4" s="92"/>
+      <c r="HY4" s="92"/>
+      <c r="HZ4" s="92"/>
+      <c r="IA4" s="92"/>
+      <c r="IB4" s="92"/>
+      <c r="IC4" s="92"/>
+      <c r="ID4" s="92"/>
+      <c r="IE4" s="92"/>
+      <c r="IF4" s="92"/>
+      <c r="IG4" s="92"/>
+      <c r="IH4" s="92"/>
+      <c r="II4" s="92"/>
+      <c r="IJ4" s="92"/>
+      <c r="IK4" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="IL4" s="67"/>
-      <c r="IM4" s="67"/>
-      <c r="IN4" s="67"/>
-      <c r="IO4" s="67"/>
-      <c r="IP4" s="67"/>
-      <c r="IQ4" s="67"/>
-      <c r="IR4" s="67"/>
-      <c r="IS4" s="67"/>
-      <c r="IT4" s="67"/>
-      <c r="IU4" s="67"/>
-      <c r="IV4" s="67"/>
-      <c r="IW4" s="67"/>
-      <c r="IX4" s="67"/>
-      <c r="IY4" s="67" t="s">
+      <c r="IL4" s="92"/>
+      <c r="IM4" s="92"/>
+      <c r="IN4" s="92"/>
+      <c r="IO4" s="92"/>
+      <c r="IP4" s="92"/>
+      <c r="IQ4" s="92"/>
+      <c r="IR4" s="92"/>
+      <c r="IS4" s="92"/>
+      <c r="IT4" s="92"/>
+      <c r="IU4" s="92"/>
+      <c r="IV4" s="92"/>
+      <c r="IW4" s="92"/>
+      <c r="IX4" s="92"/>
+      <c r="IY4" s="92" t="s">
         <v>24</v>
       </c>
-      <c r="IZ4" s="67"/>
-      <c r="JA4" s="67"/>
-      <c r="JB4" s="67"/>
-      <c r="JC4" s="67"/>
-      <c r="JD4" s="67"/>
-      <c r="JE4" s="67"/>
-      <c r="JF4" s="67"/>
-      <c r="JG4" s="67"/>
-      <c r="JH4" s="67"/>
-      <c r="JI4" s="67"/>
-      <c r="JJ4" s="67"/>
-      <c r="JK4" s="67"/>
-      <c r="JL4" s="67"/>
-      <c r="JM4" s="68" t="s">
+      <c r="IZ4" s="92"/>
+      <c r="JA4" s="92"/>
+      <c r="JB4" s="92"/>
+      <c r="JC4" s="92"/>
+      <c r="JD4" s="92"/>
+      <c r="JE4" s="92"/>
+      <c r="JF4" s="92"/>
+      <c r="JG4" s="92"/>
+      <c r="JH4" s="92"/>
+      <c r="JI4" s="92"/>
+      <c r="JJ4" s="92"/>
+      <c r="JK4" s="92"/>
+      <c r="JL4" s="92"/>
+      <c r="JM4" s="93" t="s">
         <v>25</v>
       </c>
-      <c r="JN4" s="68"/>
-      <c r="JO4" s="68"/>
-      <c r="JP4" s="68"/>
-      <c r="JQ4" s="68"/>
-      <c r="JR4" s="68"/>
-      <c r="JS4" s="68"/>
-      <c r="JT4" s="68"/>
-      <c r="JU4" s="68"/>
-      <c r="JV4" s="68"/>
-      <c r="JW4" s="68"/>
-      <c r="JX4" s="68"/>
-      <c r="JY4" s="68"/>
-      <c r="JZ4" s="64" t="s">
+      <c r="JN4" s="93"/>
+      <c r="JO4" s="93"/>
+      <c r="JP4" s="93"/>
+      <c r="JQ4" s="93"/>
+      <c r="JR4" s="93"/>
+      <c r="JS4" s="93"/>
+      <c r="JT4" s="93"/>
+      <c r="JU4" s="93"/>
+      <c r="JV4" s="93"/>
+      <c r="JW4" s="93"/>
+      <c r="JX4" s="93"/>
+      <c r="JY4" s="93"/>
+      <c r="JZ4" s="90" t="s">
         <v>26</v>
       </c>
-      <c r="KA4" s="65"/>
-      <c r="KB4" s="65"/>
-      <c r="KC4" s="65"/>
-      <c r="KD4" s="65"/>
-      <c r="KE4" s="65"/>
-      <c r="KF4" s="65"/>
-      <c r="KG4" s="65"/>
-      <c r="KH4" s="90" t="s">
+      <c r="KA4" s="91"/>
+      <c r="KB4" s="91"/>
+      <c r="KC4" s="91"/>
+      <c r="KD4" s="91"/>
+      <c r="KE4" s="91"/>
+      <c r="KF4" s="91"/>
+      <c r="KG4" s="91"/>
+      <c r="KH4" s="63" t="s">
         <v>316</v>
       </c>
-      <c r="KI4" s="93"/>
-      <c r="KJ4" s="91"/>
+      <c r="KI4" s="88"/>
+      <c r="KJ4" s="64"/>
       <c r="KK4" s="46"/>
-      <c r="KL4" s="90" t="s">
+      <c r="KL4" s="63" t="s">
         <v>343</v>
       </c>
-      <c r="KM4" s="91"/>
+      <c r="KM4" s="64"/>
+      <c r="KN4" s="96"/>
+      <c r="KO4" s="94"/>
     </row>
-    <row r="5" spans="1:299" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="82"/>
-      <c r="B5" s="82"/>
-      <c r="C5" s="82"/>
-      <c r="D5" s="82"/>
-      <c r="E5" s="83"/>
-      <c r="F5" s="83"/>
-      <c r="G5" s="83"/>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="84"/>
-      <c r="L5" s="84"/>
-      <c r="M5" s="84"/>
-      <c r="N5" s="84"/>
-      <c r="O5" s="84"/>
-      <c r="P5" s="85"/>
-      <c r="Q5" s="85"/>
-      <c r="R5" s="85"/>
-      <c r="S5" s="85"/>
-      <c r="T5" s="85"/>
-      <c r="U5" s="86"/>
-      <c r="V5" s="86"/>
-      <c r="W5" s="86"/>
-      <c r="X5" s="86"/>
-      <c r="Y5" s="86"/>
-      <c r="Z5" s="86"/>
-      <c r="AA5" s="86"/>
-      <c r="AB5" s="86"/>
-      <c r="AC5" s="87"/>
-      <c r="AD5" s="87"/>
-      <c r="AE5" s="87"/>
-      <c r="AF5" s="87"/>
-      <c r="AG5" s="87"/>
-      <c r="AH5" s="87"/>
-      <c r="AI5" s="87"/>
-      <c r="AJ5" s="88"/>
-      <c r="AK5" s="88"/>
-      <c r="AL5" s="88"/>
-      <c r="AM5" s="79"/>
-      <c r="AN5" s="79"/>
-      <c r="AO5" s="69"/>
-      <c r="AP5" s="69"/>
-      <c r="AQ5" s="69"/>
-      <c r="AR5" s="69"/>
-      <c r="AS5" s="70"/>
-      <c r="AT5" s="70"/>
-      <c r="AU5" s="70"/>
-      <c r="AV5" s="70"/>
-      <c r="AW5" s="70"/>
-      <c r="AX5" s="70"/>
-      <c r="AY5" s="70"/>
-      <c r="AZ5" s="70"/>
-      <c r="BA5" s="70"/>
-      <c r="BB5" s="70"/>
-      <c r="BC5" s="70"/>
-      <c r="BD5" s="70"/>
-      <c r="BE5" s="70"/>
-      <c r="BF5" s="70"/>
-      <c r="BG5" s="70"/>
-      <c r="BH5" s="70"/>
-      <c r="BI5" s="70"/>
-      <c r="BJ5" s="70"/>
+    <row r="5" spans="1:301" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="70"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
+      <c r="I5" s="71"/>
+      <c r="J5" s="71"/>
+      <c r="K5" s="72"/>
+      <c r="L5" s="72"/>
+      <c r="M5" s="72"/>
+      <c r="N5" s="72"/>
+      <c r="O5" s="72"/>
+      <c r="P5" s="73"/>
+      <c r="Q5" s="73"/>
+      <c r="R5" s="73"/>
+      <c r="S5" s="73"/>
+      <c r="T5" s="73"/>
+      <c r="U5" s="74"/>
+      <c r="V5" s="74"/>
+      <c r="W5" s="74"/>
+      <c r="X5" s="74"/>
+      <c r="Y5" s="74"/>
+      <c r="Z5" s="74"/>
+      <c r="AA5" s="74"/>
+      <c r="AB5" s="74"/>
+      <c r="AC5" s="75"/>
+      <c r="AD5" s="75"/>
+      <c r="AE5" s="75"/>
+      <c r="AF5" s="75"/>
+      <c r="AG5" s="75"/>
+      <c r="AH5" s="75"/>
+      <c r="AI5" s="75"/>
+      <c r="AJ5" s="76"/>
+      <c r="AK5" s="76"/>
+      <c r="AL5" s="76"/>
+      <c r="AM5" s="67"/>
+      <c r="AN5" s="67"/>
+      <c r="AO5" s="78"/>
+      <c r="AP5" s="78"/>
+      <c r="AQ5" s="78"/>
+      <c r="AR5" s="78"/>
+      <c r="AS5" s="79"/>
+      <c r="AT5" s="79"/>
+      <c r="AU5" s="79"/>
+      <c r="AV5" s="79"/>
+      <c r="AW5" s="79"/>
+      <c r="AX5" s="79"/>
+      <c r="AY5" s="79"/>
+      <c r="AZ5" s="79"/>
+      <c r="BA5" s="79"/>
+      <c r="BB5" s="79"/>
+      <c r="BC5" s="79"/>
+      <c r="BD5" s="79"/>
+      <c r="BE5" s="79"/>
+      <c r="BF5" s="79"/>
+      <c r="BG5" s="79"/>
+      <c r="BH5" s="79"/>
+      <c r="BI5" s="79"/>
+      <c r="BJ5" s="79"/>
       <c r="BK5" s="8" t="s">
         <v>27</v>
       </c>
@@ -4149,39 +4190,41 @@
       <c r="JL5" s="11" t="s">
         <v>315</v>
       </c>
-      <c r="JM5" s="68"/>
-      <c r="JN5" s="68"/>
-      <c r="JO5" s="68"/>
-      <c r="JP5" s="68"/>
-      <c r="JQ5" s="68"/>
-      <c r="JR5" s="68"/>
-      <c r="JS5" s="68"/>
-      <c r="JT5" s="68"/>
-      <c r="JU5" s="68"/>
-      <c r="JV5" s="68"/>
-      <c r="JW5" s="68"/>
-      <c r="JX5" s="68"/>
-      <c r="JY5" s="68"/>
-      <c r="JZ5" s="65" t="s">
+      <c r="JM5" s="93"/>
+      <c r="JN5" s="93"/>
+      <c r="JO5" s="93"/>
+      <c r="JP5" s="93"/>
+      <c r="JQ5" s="93"/>
+      <c r="JR5" s="93"/>
+      <c r="JS5" s="93"/>
+      <c r="JT5" s="93"/>
+      <c r="JU5" s="93"/>
+      <c r="JV5" s="93"/>
+      <c r="JW5" s="93"/>
+      <c r="JX5" s="93"/>
+      <c r="JY5" s="93"/>
+      <c r="JZ5" s="91" t="s">
         <v>342</v>
       </c>
-      <c r="KA5" s="65"/>
-      <c r="KB5" s="65"/>
-      <c r="KC5" s="65"/>
-      <c r="KD5" s="65" t="s">
+      <c r="KA5" s="91"/>
+      <c r="KB5" s="91"/>
+      <c r="KC5" s="91"/>
+      <c r="KD5" s="91" t="s">
         <v>38</v>
       </c>
-      <c r="KE5" s="65"/>
-      <c r="KF5" s="65"/>
-      <c r="KG5" s="65"/>
-      <c r="KH5" s="62"/>
-      <c r="KI5" s="63"/>
-      <c r="KJ5" s="92"/>
+      <c r="KE5" s="91"/>
+      <c r="KF5" s="91"/>
+      <c r="KG5" s="91"/>
+      <c r="KH5" s="65"/>
+      <c r="KI5" s="89"/>
+      <c r="KJ5" s="66"/>
       <c r="KK5" s="46"/>
-      <c r="KL5" s="62"/>
-      <c r="KM5" s="92"/>
+      <c r="KL5" s="65"/>
+      <c r="KM5" s="66"/>
+      <c r="KN5" s="97"/>
+      <c r="KO5" s="95"/>
     </row>
-    <row r="6" spans="1:299" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:301" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>39</v>
       </c>
@@ -5079,8 +5122,14 @@
       <c r="KM6" s="22" t="s">
         <v>345</v>
       </c>
+      <c r="KN6" s="22" t="s">
+        <v>346</v>
+      </c>
+      <c r="KO6" s="22" t="s">
+        <v>347</v>
+      </c>
     </row>
-    <row r="7" spans="1:299" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:301" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="49"/>
       <c r="B7" s="49"/>
       <c r="C7" s="49"/>
@@ -5514,8 +5563,10 @@
       <c r="KI7" s="47"/>
       <c r="KJ7" s="47"/>
       <c r="KK7" s="47"/>
-      <c r="KL7" s="89"/>
-      <c r="KM7" s="89"/>
+      <c r="KL7" s="62"/>
+      <c r="KM7" s="62"/>
+      <c r="KN7" s="62"/>
+      <c r="KO7" s="62"/>
     </row>
     <row r="32" spans="297:297" x14ac:dyDescent="0.2">
       <c r="KK32" s="48"/>
@@ -5523,6 +5574,23 @@
   </sheetData>
   <autoFilter ref="A6:KK6" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="33">
+    <mergeCell ref="FE4:FR4"/>
+    <mergeCell ref="FS4:GF4"/>
+    <mergeCell ref="KH4:KJ5"/>
+    <mergeCell ref="JZ4:KG4"/>
+    <mergeCell ref="JZ5:KC5"/>
+    <mergeCell ref="KD5:KG5"/>
+    <mergeCell ref="GU4:HH4"/>
+    <mergeCell ref="HI4:HV4"/>
+    <mergeCell ref="HW4:IJ4"/>
+    <mergeCell ref="IK4:IX4"/>
+    <mergeCell ref="IY4:JL4"/>
+    <mergeCell ref="JM4:JY5"/>
+    <mergeCell ref="CM4:CZ4"/>
+    <mergeCell ref="DA4:DN4"/>
+    <mergeCell ref="DO4:EB4"/>
+    <mergeCell ref="EC4:EP4"/>
+    <mergeCell ref="EQ4:FD4"/>
     <mergeCell ref="KL4:KM5"/>
     <mergeCell ref="AM4:AN5"/>
     <mergeCell ref="A1:B1"/>
@@ -5539,23 +5607,6 @@
     <mergeCell ref="AS4:BJ5"/>
     <mergeCell ref="BK4:BX4"/>
     <mergeCell ref="BY4:CL4"/>
-    <mergeCell ref="CM4:CZ4"/>
-    <mergeCell ref="DA4:DN4"/>
-    <mergeCell ref="DO4:EB4"/>
-    <mergeCell ref="EC4:EP4"/>
-    <mergeCell ref="EQ4:FD4"/>
-    <mergeCell ref="FE4:FR4"/>
-    <mergeCell ref="FS4:GF4"/>
-    <mergeCell ref="KH4:KJ5"/>
-    <mergeCell ref="JZ4:KG4"/>
-    <mergeCell ref="JZ5:KC5"/>
-    <mergeCell ref="KD5:KG5"/>
-    <mergeCell ref="GU4:HH4"/>
-    <mergeCell ref="HI4:HV4"/>
-    <mergeCell ref="HW4:IJ4"/>
-    <mergeCell ref="IK4:IX4"/>
-    <mergeCell ref="IY4:JL4"/>
-    <mergeCell ref="JM4:JY5"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A6">
     <cfRule type="duplicateValues" dxfId="0" priority="92"/>

</xml_diff>

<commit_message>
Add last_update and pso_name columns to project export (#563)
https://eaflood.atlassian.net/browse/RUBY-2394
https://eaflood.atlassian.net/browse/RUBY-2159
</commit_message>
<xml_diff>
--- a/lib/fcerm1_template.xlsx
+++ b/lib/fcerm1_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthall/Work/pafs/pafs_core/lib/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\x959510\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16230ADF-9386-8C4D-81CA-AC41D44E0D83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED8BA3D2-F58C-4C09-9C50-FA848AD2D1BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="68800" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master local choices" sheetId="2" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="348">
   <si>
     <t>FCRM1 - National Capital Programme</t>
   </si>
@@ -1190,17 +1190,23 @@
   <si>
     <t>Lifecycle Carbon</t>
   </si>
+  <si>
+    <t>Last Updated</t>
+  </si>
+  <si>
+    <t>PSO Name</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="#,##0.0"/>
-    <numFmt numFmtId="167" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
-    <numFmt numFmtId="168" formatCode="#,##0.0_ ;[Red]\-#,##0.0\ "/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0"/>
+    <numFmt numFmtId="166" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
+    <numFmt numFmtId="167" formatCode="#,##0.0_ ;[Red]\-#,##0.0\ "/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -1471,7 +1477,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1569,10 +1575,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
@@ -1580,9 +1599,9 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -1647,7 +1666,7 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1669,7 +1688,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1678,10 +1697,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1738,106 +1757,25 @@
     <xf numFmtId="9" fontId="16" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="167" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="11" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="25" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1845,11 +1783,104 @@
     <xf numFmtId="0" fontId="12" fillId="25" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="25" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="11" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -1861,7 +1892,7 @@
     <cellStyle name="Normal 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Normal 2 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Normal_RCP" xfId="5" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Per cent" xfId="2" builtinId="5"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
     <cellStyle name="Percent 11" xfId="7" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
   </cellStyles>
   <dxfs count="1">
@@ -2155,20 +2186,20 @@
     <tabColor rgb="FF92D050"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:KM32"/>
+  <dimension ref="A1:KO32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="KD7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="KL7" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
       <selection pane="topRight" activeCell="C7" sqref="C7"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="KJ29" sqref="KJ29"/>
+      <selection pane="bottomRight" activeCell="KM12" sqref="KM12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="98.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="98.6640625" style="1" customWidth="1"/>
     <col min="3" max="4" width="21" style="3" customWidth="1"/>
     <col min="5" max="6" width="21" style="1" customWidth="1"/>
     <col min="7" max="7" width="21" style="2" customWidth="1"/>
@@ -2185,18 +2216,20 @@
     <col min="45" max="278" width="21" style="1" customWidth="1"/>
     <col min="279" max="285" width="21" style="28" customWidth="1"/>
     <col min="286" max="293" width="21" style="6" customWidth="1"/>
-    <col min="294" max="296" width="22.28515625" style="7" customWidth="1"/>
-    <col min="297" max="297" width="17.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="298" max="298" width="19.7109375" style="7" customWidth="1"/>
-    <col min="299" max="299" width="21.5703125" style="7" customWidth="1"/>
-    <col min="300" max="16384" width="8.7109375" style="7"/>
+    <col min="294" max="296" width="22.33203125" style="7" customWidth="1"/>
+    <col min="297" max="297" width="17.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="298" max="298" width="19.6640625" style="7" customWidth="1"/>
+    <col min="299" max="299" width="21.5546875" style="7" customWidth="1"/>
+    <col min="300" max="300" width="19.6640625" style="7" customWidth="1"/>
+    <col min="301" max="301" width="21.5546875" style="7" customWidth="1"/>
+    <col min="302" max="16384" width="8.6640625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:299" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="80" t="s">
+    <row r="1" spans="1:301" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="80"/>
+      <c r="B1" s="68"/>
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
       <c r="E1" s="23"/>
@@ -2494,12 +2527,14 @@
       <c r="KK1" s="47"/>
       <c r="KL1" s="47"/>
       <c r="KM1" s="47"/>
+      <c r="KN1" s="47"/>
+      <c r="KO1" s="47"/>
     </row>
-    <row r="2" spans="1:299" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="81" t="s">
+    <row r="2" spans="1:301" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="69" t="s">
         <v>337</v>
       </c>
-      <c r="B2" s="81"/>
+      <c r="B2" s="69"/>
       <c r="C2" s="36"/>
       <c r="D2" s="36"/>
       <c r="E2" s="23"/>
@@ -2797,8 +2832,10 @@
       <c r="KK2" s="47"/>
       <c r="KL2" s="47"/>
       <c r="KM2" s="47"/>
+      <c r="KN2" s="47"/>
+      <c r="KO2" s="47"/>
     </row>
-    <row r="3" spans="1:299" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:301" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="39"/>
       <c r="B3" s="40"/>
       <c r="C3" s="39"/>
@@ -3098,427 +3135,431 @@
       <c r="KK3" s="47"/>
       <c r="KL3" s="47"/>
       <c r="KM3" s="47"/>
+      <c r="KN3" s="47"/>
+      <c r="KO3" s="47"/>
     </row>
-    <row r="4" spans="1:299" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="82" t="s">
+    <row r="4" spans="1:301" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="82"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="82"/>
-      <c r="E4" s="83" t="s">
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="83"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="83"/>
-      <c r="J4" s="83"/>
-      <c r="K4" s="84" t="s">
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
+      <c r="I4" s="71"/>
+      <c r="J4" s="71"/>
+      <c r="K4" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="84"/>
-      <c r="M4" s="84"/>
-      <c r="N4" s="84"/>
-      <c r="O4" s="84"/>
-      <c r="P4" s="85" t="s">
+      <c r="L4" s="72"/>
+      <c r="M4" s="72"/>
+      <c r="N4" s="72"/>
+      <c r="O4" s="72"/>
+      <c r="P4" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="Q4" s="85"/>
-      <c r="R4" s="85"/>
-      <c r="S4" s="85"/>
-      <c r="T4" s="85"/>
-      <c r="U4" s="86" t="s">
+      <c r="Q4" s="73"/>
+      <c r="R4" s="73"/>
+      <c r="S4" s="73"/>
+      <c r="T4" s="73"/>
+      <c r="U4" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="V4" s="86"/>
-      <c r="W4" s="86"/>
-      <c r="X4" s="86"/>
-      <c r="Y4" s="86"/>
-      <c r="Z4" s="86"/>
-      <c r="AA4" s="86"/>
-      <c r="AB4" s="86"/>
-      <c r="AC4" s="87" t="s">
+      <c r="V4" s="74"/>
+      <c r="W4" s="74"/>
+      <c r="X4" s="74"/>
+      <c r="Y4" s="74"/>
+      <c r="Z4" s="74"/>
+      <c r="AA4" s="74"/>
+      <c r="AB4" s="74"/>
+      <c r="AC4" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="AD4" s="87"/>
-      <c r="AE4" s="87"/>
-      <c r="AF4" s="87"/>
-      <c r="AG4" s="87"/>
-      <c r="AH4" s="87"/>
-      <c r="AI4" s="87"/>
-      <c r="AJ4" s="88" t="s">
+      <c r="AD4" s="75"/>
+      <c r="AE4" s="75"/>
+      <c r="AF4" s="75"/>
+      <c r="AG4" s="75"/>
+      <c r="AH4" s="75"/>
+      <c r="AI4" s="75"/>
+      <c r="AJ4" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="AK4" s="88"/>
-      <c r="AL4" s="88"/>
-      <c r="AM4" s="79" t="s">
+      <c r="AK4" s="76"/>
+      <c r="AL4" s="76"/>
+      <c r="AM4" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="AN4" s="79"/>
-      <c r="AO4" s="69"/>
-      <c r="AP4" s="69"/>
-      <c r="AQ4" s="69"/>
-      <c r="AR4" s="69"/>
-      <c r="AS4" s="70" t="s">
+      <c r="AN4" s="67"/>
+      <c r="AO4" s="78"/>
+      <c r="AP4" s="78"/>
+      <c r="AQ4" s="78"/>
+      <c r="AR4" s="78"/>
+      <c r="AS4" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="AT4" s="70"/>
-      <c r="AU4" s="70"/>
-      <c r="AV4" s="70"/>
-      <c r="AW4" s="70"/>
-      <c r="AX4" s="70"/>
-      <c r="AY4" s="70"/>
-      <c r="AZ4" s="70"/>
-      <c r="BA4" s="70"/>
-      <c r="BB4" s="70"/>
-      <c r="BC4" s="70"/>
-      <c r="BD4" s="70"/>
-      <c r="BE4" s="70"/>
-      <c r="BF4" s="70"/>
-      <c r="BG4" s="70"/>
-      <c r="BH4" s="70"/>
-      <c r="BI4" s="70"/>
-      <c r="BJ4" s="70"/>
-      <c r="BK4" s="66" t="s">
+      <c r="AT4" s="79"/>
+      <c r="AU4" s="79"/>
+      <c r="AV4" s="79"/>
+      <c r="AW4" s="79"/>
+      <c r="AX4" s="79"/>
+      <c r="AY4" s="79"/>
+      <c r="AZ4" s="79"/>
+      <c r="BA4" s="79"/>
+      <c r="BB4" s="79"/>
+      <c r="BC4" s="79"/>
+      <c r="BD4" s="79"/>
+      <c r="BE4" s="79"/>
+      <c r="BF4" s="79"/>
+      <c r="BG4" s="79"/>
+      <c r="BH4" s="79"/>
+      <c r="BI4" s="79"/>
+      <c r="BJ4" s="79"/>
+      <c r="BK4" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="BL4" s="66"/>
-      <c r="BM4" s="66"/>
-      <c r="BN4" s="66"/>
-      <c r="BO4" s="66"/>
-      <c r="BP4" s="66"/>
-      <c r="BQ4" s="66"/>
-      <c r="BR4" s="66"/>
-      <c r="BS4" s="66"/>
-      <c r="BT4" s="66"/>
-      <c r="BU4" s="66"/>
-      <c r="BV4" s="66"/>
-      <c r="BW4" s="66"/>
-      <c r="BX4" s="66"/>
-      <c r="BY4" s="71" t="s">
+      <c r="BL4" s="77"/>
+      <c r="BM4" s="77"/>
+      <c r="BN4" s="77"/>
+      <c r="BO4" s="77"/>
+      <c r="BP4" s="77"/>
+      <c r="BQ4" s="77"/>
+      <c r="BR4" s="77"/>
+      <c r="BS4" s="77"/>
+      <c r="BT4" s="77"/>
+      <c r="BU4" s="77"/>
+      <c r="BV4" s="77"/>
+      <c r="BW4" s="77"/>
+      <c r="BX4" s="77"/>
+      <c r="BY4" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="BZ4" s="71"/>
-      <c r="CA4" s="71"/>
-      <c r="CB4" s="71"/>
-      <c r="CC4" s="71"/>
-      <c r="CD4" s="71"/>
-      <c r="CE4" s="71"/>
-      <c r="CF4" s="71"/>
-      <c r="CG4" s="71"/>
-      <c r="CH4" s="71"/>
-      <c r="CI4" s="71"/>
-      <c r="CJ4" s="71"/>
-      <c r="CK4" s="71"/>
-      <c r="CL4" s="71"/>
-      <c r="CM4" s="72" t="s">
+      <c r="BZ4" s="80"/>
+      <c r="CA4" s="80"/>
+      <c r="CB4" s="80"/>
+      <c r="CC4" s="80"/>
+      <c r="CD4" s="80"/>
+      <c r="CE4" s="80"/>
+      <c r="CF4" s="80"/>
+      <c r="CG4" s="80"/>
+      <c r="CH4" s="80"/>
+      <c r="CI4" s="80"/>
+      <c r="CJ4" s="80"/>
+      <c r="CK4" s="80"/>
+      <c r="CL4" s="80"/>
+      <c r="CM4" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="CN4" s="72"/>
-      <c r="CO4" s="72"/>
-      <c r="CP4" s="72"/>
-      <c r="CQ4" s="72"/>
-      <c r="CR4" s="72"/>
-      <c r="CS4" s="72"/>
-      <c r="CT4" s="72"/>
-      <c r="CU4" s="72"/>
-      <c r="CV4" s="72"/>
-      <c r="CW4" s="72"/>
-      <c r="CX4" s="72"/>
-      <c r="CY4" s="72"/>
-      <c r="CZ4" s="72"/>
-      <c r="DA4" s="73" t="s">
+      <c r="CN4" s="81"/>
+      <c r="CO4" s="81"/>
+      <c r="CP4" s="81"/>
+      <c r="CQ4" s="81"/>
+      <c r="CR4" s="81"/>
+      <c r="CS4" s="81"/>
+      <c r="CT4" s="81"/>
+      <c r="CU4" s="81"/>
+      <c r="CV4" s="81"/>
+      <c r="CW4" s="81"/>
+      <c r="CX4" s="81"/>
+      <c r="CY4" s="81"/>
+      <c r="CZ4" s="81"/>
+      <c r="DA4" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="DB4" s="73"/>
-      <c r="DC4" s="73"/>
-      <c r="DD4" s="73"/>
-      <c r="DE4" s="73"/>
-      <c r="DF4" s="73"/>
-      <c r="DG4" s="73"/>
-      <c r="DH4" s="73"/>
-      <c r="DI4" s="73"/>
-      <c r="DJ4" s="73"/>
-      <c r="DK4" s="73"/>
-      <c r="DL4" s="73"/>
-      <c r="DM4" s="73"/>
-      <c r="DN4" s="73"/>
-      <c r="DO4" s="74" t="s">
+      <c r="DB4" s="82"/>
+      <c r="DC4" s="82"/>
+      <c r="DD4" s="82"/>
+      <c r="DE4" s="82"/>
+      <c r="DF4" s="82"/>
+      <c r="DG4" s="82"/>
+      <c r="DH4" s="82"/>
+      <c r="DI4" s="82"/>
+      <c r="DJ4" s="82"/>
+      <c r="DK4" s="82"/>
+      <c r="DL4" s="82"/>
+      <c r="DM4" s="82"/>
+      <c r="DN4" s="82"/>
+      <c r="DO4" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="DP4" s="74"/>
-      <c r="DQ4" s="74"/>
-      <c r="DR4" s="74"/>
-      <c r="DS4" s="74"/>
-      <c r="DT4" s="74"/>
-      <c r="DU4" s="74"/>
-      <c r="DV4" s="74"/>
-      <c r="DW4" s="74"/>
-      <c r="DX4" s="74"/>
-      <c r="DY4" s="74"/>
-      <c r="DZ4" s="74"/>
-      <c r="EA4" s="74"/>
-      <c r="EB4" s="74"/>
-      <c r="EC4" s="75" t="s">
+      <c r="DP4" s="83"/>
+      <c r="DQ4" s="83"/>
+      <c r="DR4" s="83"/>
+      <c r="DS4" s="83"/>
+      <c r="DT4" s="83"/>
+      <c r="DU4" s="83"/>
+      <c r="DV4" s="83"/>
+      <c r="DW4" s="83"/>
+      <c r="DX4" s="83"/>
+      <c r="DY4" s="83"/>
+      <c r="DZ4" s="83"/>
+      <c r="EA4" s="83"/>
+      <c r="EB4" s="83"/>
+      <c r="EC4" s="84" t="s">
         <v>15</v>
       </c>
-      <c r="ED4" s="75"/>
-      <c r="EE4" s="75"/>
-      <c r="EF4" s="75"/>
-      <c r="EG4" s="75"/>
-      <c r="EH4" s="75"/>
-      <c r="EI4" s="75"/>
-      <c r="EJ4" s="75"/>
-      <c r="EK4" s="75"/>
-      <c r="EL4" s="75"/>
-      <c r="EM4" s="75"/>
-      <c r="EN4" s="75"/>
-      <c r="EO4" s="75"/>
-      <c r="EP4" s="75"/>
-      <c r="EQ4" s="76" t="s">
+      <c r="ED4" s="84"/>
+      <c r="EE4" s="84"/>
+      <c r="EF4" s="84"/>
+      <c r="EG4" s="84"/>
+      <c r="EH4" s="84"/>
+      <c r="EI4" s="84"/>
+      <c r="EJ4" s="84"/>
+      <c r="EK4" s="84"/>
+      <c r="EL4" s="84"/>
+      <c r="EM4" s="84"/>
+      <c r="EN4" s="84"/>
+      <c r="EO4" s="84"/>
+      <c r="EP4" s="84"/>
+      <c r="EQ4" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="ER4" s="76"/>
-      <c r="ES4" s="76"/>
-      <c r="ET4" s="76"/>
-      <c r="EU4" s="76"/>
-      <c r="EV4" s="76"/>
-      <c r="EW4" s="76"/>
-      <c r="EX4" s="76"/>
-      <c r="EY4" s="76"/>
-      <c r="EZ4" s="76"/>
-      <c r="FA4" s="76"/>
-      <c r="FB4" s="76"/>
-      <c r="FC4" s="76"/>
-      <c r="FD4" s="76"/>
-      <c r="FE4" s="77" t="s">
+      <c r="ER4" s="85"/>
+      <c r="ES4" s="85"/>
+      <c r="ET4" s="85"/>
+      <c r="EU4" s="85"/>
+      <c r="EV4" s="85"/>
+      <c r="EW4" s="85"/>
+      <c r="EX4" s="85"/>
+      <c r="EY4" s="85"/>
+      <c r="EZ4" s="85"/>
+      <c r="FA4" s="85"/>
+      <c r="FB4" s="85"/>
+      <c r="FC4" s="85"/>
+      <c r="FD4" s="85"/>
+      <c r="FE4" s="86" t="s">
         <v>17</v>
       </c>
-      <c r="FF4" s="77"/>
-      <c r="FG4" s="77"/>
-      <c r="FH4" s="77"/>
-      <c r="FI4" s="77"/>
-      <c r="FJ4" s="77"/>
-      <c r="FK4" s="77"/>
-      <c r="FL4" s="77"/>
-      <c r="FM4" s="77"/>
-      <c r="FN4" s="77"/>
-      <c r="FO4" s="77"/>
-      <c r="FP4" s="77"/>
-      <c r="FQ4" s="77"/>
-      <c r="FR4" s="77"/>
-      <c r="FS4" s="78" t="s">
+      <c r="FF4" s="86"/>
+      <c r="FG4" s="86"/>
+      <c r="FH4" s="86"/>
+      <c r="FI4" s="86"/>
+      <c r="FJ4" s="86"/>
+      <c r="FK4" s="86"/>
+      <c r="FL4" s="86"/>
+      <c r="FM4" s="86"/>
+      <c r="FN4" s="86"/>
+      <c r="FO4" s="86"/>
+      <c r="FP4" s="86"/>
+      <c r="FQ4" s="86"/>
+      <c r="FR4" s="86"/>
+      <c r="FS4" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="FT4" s="78"/>
-      <c r="FU4" s="78"/>
-      <c r="FV4" s="78"/>
-      <c r="FW4" s="78"/>
-      <c r="FX4" s="78"/>
-      <c r="FY4" s="78"/>
-      <c r="FZ4" s="78"/>
-      <c r="GA4" s="78"/>
-      <c r="GB4" s="78"/>
-      <c r="GC4" s="78"/>
-      <c r="GD4" s="78"/>
-      <c r="GE4" s="78"/>
-      <c r="GF4" s="78"/>
-      <c r="GG4" s="66" t="s">
+      <c r="FT4" s="87"/>
+      <c r="FU4" s="87"/>
+      <c r="FV4" s="87"/>
+      <c r="FW4" s="87"/>
+      <c r="FX4" s="87"/>
+      <c r="FY4" s="87"/>
+      <c r="FZ4" s="87"/>
+      <c r="GA4" s="87"/>
+      <c r="GB4" s="87"/>
+      <c r="GC4" s="87"/>
+      <c r="GD4" s="87"/>
+      <c r="GE4" s="87"/>
+      <c r="GF4" s="87"/>
+      <c r="GG4" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="GH4" s="66"/>
-      <c r="GI4" s="66"/>
-      <c r="GJ4" s="66"/>
-      <c r="GK4" s="66"/>
-      <c r="GL4" s="66"/>
-      <c r="GM4" s="66"/>
-      <c r="GN4" s="66"/>
-      <c r="GO4" s="66"/>
-      <c r="GP4" s="66"/>
-      <c r="GQ4" s="66"/>
-      <c r="GR4" s="66"/>
-      <c r="GS4" s="66"/>
-      <c r="GT4" s="66"/>
-      <c r="GU4" s="66" t="s">
+      <c r="GH4" s="77"/>
+      <c r="GI4" s="77"/>
+      <c r="GJ4" s="77"/>
+      <c r="GK4" s="77"/>
+      <c r="GL4" s="77"/>
+      <c r="GM4" s="77"/>
+      <c r="GN4" s="77"/>
+      <c r="GO4" s="77"/>
+      <c r="GP4" s="77"/>
+      <c r="GQ4" s="77"/>
+      <c r="GR4" s="77"/>
+      <c r="GS4" s="77"/>
+      <c r="GT4" s="77"/>
+      <c r="GU4" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="GV4" s="66"/>
-      <c r="GW4" s="66"/>
-      <c r="GX4" s="66"/>
-      <c r="GY4" s="66"/>
-      <c r="GZ4" s="66"/>
-      <c r="HA4" s="66"/>
-      <c r="HB4" s="66"/>
-      <c r="HC4" s="66"/>
-      <c r="HD4" s="66"/>
-      <c r="HE4" s="66"/>
-      <c r="HF4" s="66"/>
-      <c r="HG4" s="66"/>
-      <c r="HH4" s="66"/>
-      <c r="HI4" s="66" t="s">
+      <c r="GV4" s="77"/>
+      <c r="GW4" s="77"/>
+      <c r="GX4" s="77"/>
+      <c r="GY4" s="77"/>
+      <c r="GZ4" s="77"/>
+      <c r="HA4" s="77"/>
+      <c r="HB4" s="77"/>
+      <c r="HC4" s="77"/>
+      <c r="HD4" s="77"/>
+      <c r="HE4" s="77"/>
+      <c r="HF4" s="77"/>
+      <c r="HG4" s="77"/>
+      <c r="HH4" s="77"/>
+      <c r="HI4" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="HJ4" s="66"/>
-      <c r="HK4" s="66"/>
-      <c r="HL4" s="66"/>
-      <c r="HM4" s="66"/>
-      <c r="HN4" s="66"/>
-      <c r="HO4" s="66"/>
-      <c r="HP4" s="66"/>
-      <c r="HQ4" s="66"/>
-      <c r="HR4" s="66"/>
-      <c r="HS4" s="66"/>
-      <c r="HT4" s="66"/>
-      <c r="HU4" s="66"/>
-      <c r="HV4" s="66"/>
-      <c r="HW4" s="67" t="s">
+      <c r="HJ4" s="77"/>
+      <c r="HK4" s="77"/>
+      <c r="HL4" s="77"/>
+      <c r="HM4" s="77"/>
+      <c r="HN4" s="77"/>
+      <c r="HO4" s="77"/>
+      <c r="HP4" s="77"/>
+      <c r="HQ4" s="77"/>
+      <c r="HR4" s="77"/>
+      <c r="HS4" s="77"/>
+      <c r="HT4" s="77"/>
+      <c r="HU4" s="77"/>
+      <c r="HV4" s="77"/>
+      <c r="HW4" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="HX4" s="67"/>
-      <c r="HY4" s="67"/>
-      <c r="HZ4" s="67"/>
-      <c r="IA4" s="67"/>
-      <c r="IB4" s="67"/>
-      <c r="IC4" s="67"/>
-      <c r="ID4" s="67"/>
-      <c r="IE4" s="67"/>
-      <c r="IF4" s="67"/>
-      <c r="IG4" s="67"/>
-      <c r="IH4" s="67"/>
-      <c r="II4" s="67"/>
-      <c r="IJ4" s="67"/>
-      <c r="IK4" s="67" t="s">
+      <c r="HX4" s="92"/>
+      <c r="HY4" s="92"/>
+      <c r="HZ4" s="92"/>
+      <c r="IA4" s="92"/>
+      <c r="IB4" s="92"/>
+      <c r="IC4" s="92"/>
+      <c r="ID4" s="92"/>
+      <c r="IE4" s="92"/>
+      <c r="IF4" s="92"/>
+      <c r="IG4" s="92"/>
+      <c r="IH4" s="92"/>
+      <c r="II4" s="92"/>
+      <c r="IJ4" s="92"/>
+      <c r="IK4" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="IL4" s="67"/>
-      <c r="IM4" s="67"/>
-      <c r="IN4" s="67"/>
-      <c r="IO4" s="67"/>
-      <c r="IP4" s="67"/>
-      <c r="IQ4" s="67"/>
-      <c r="IR4" s="67"/>
-      <c r="IS4" s="67"/>
-      <c r="IT4" s="67"/>
-      <c r="IU4" s="67"/>
-      <c r="IV4" s="67"/>
-      <c r="IW4" s="67"/>
-      <c r="IX4" s="67"/>
-      <c r="IY4" s="67" t="s">
+      <c r="IL4" s="92"/>
+      <c r="IM4" s="92"/>
+      <c r="IN4" s="92"/>
+      <c r="IO4" s="92"/>
+      <c r="IP4" s="92"/>
+      <c r="IQ4" s="92"/>
+      <c r="IR4" s="92"/>
+      <c r="IS4" s="92"/>
+      <c r="IT4" s="92"/>
+      <c r="IU4" s="92"/>
+      <c r="IV4" s="92"/>
+      <c r="IW4" s="92"/>
+      <c r="IX4" s="92"/>
+      <c r="IY4" s="92" t="s">
         <v>24</v>
       </c>
-      <c r="IZ4" s="67"/>
-      <c r="JA4" s="67"/>
-      <c r="JB4" s="67"/>
-      <c r="JC4" s="67"/>
-      <c r="JD4" s="67"/>
-      <c r="JE4" s="67"/>
-      <c r="JF4" s="67"/>
-      <c r="JG4" s="67"/>
-      <c r="JH4" s="67"/>
-      <c r="JI4" s="67"/>
-      <c r="JJ4" s="67"/>
-      <c r="JK4" s="67"/>
-      <c r="JL4" s="67"/>
-      <c r="JM4" s="68" t="s">
+      <c r="IZ4" s="92"/>
+      <c r="JA4" s="92"/>
+      <c r="JB4" s="92"/>
+      <c r="JC4" s="92"/>
+      <c r="JD4" s="92"/>
+      <c r="JE4" s="92"/>
+      <c r="JF4" s="92"/>
+      <c r="JG4" s="92"/>
+      <c r="JH4" s="92"/>
+      <c r="JI4" s="92"/>
+      <c r="JJ4" s="92"/>
+      <c r="JK4" s="92"/>
+      <c r="JL4" s="92"/>
+      <c r="JM4" s="93" t="s">
         <v>25</v>
       </c>
-      <c r="JN4" s="68"/>
-      <c r="JO4" s="68"/>
-      <c r="JP4" s="68"/>
-      <c r="JQ4" s="68"/>
-      <c r="JR4" s="68"/>
-      <c r="JS4" s="68"/>
-      <c r="JT4" s="68"/>
-      <c r="JU4" s="68"/>
-      <c r="JV4" s="68"/>
-      <c r="JW4" s="68"/>
-      <c r="JX4" s="68"/>
-      <c r="JY4" s="68"/>
-      <c r="JZ4" s="64" t="s">
+      <c r="JN4" s="93"/>
+      <c r="JO4" s="93"/>
+      <c r="JP4" s="93"/>
+      <c r="JQ4" s="93"/>
+      <c r="JR4" s="93"/>
+      <c r="JS4" s="93"/>
+      <c r="JT4" s="93"/>
+      <c r="JU4" s="93"/>
+      <c r="JV4" s="93"/>
+      <c r="JW4" s="93"/>
+      <c r="JX4" s="93"/>
+      <c r="JY4" s="93"/>
+      <c r="JZ4" s="90" t="s">
         <v>26</v>
       </c>
-      <c r="KA4" s="65"/>
-      <c r="KB4" s="65"/>
-      <c r="KC4" s="65"/>
-      <c r="KD4" s="65"/>
-      <c r="KE4" s="65"/>
-      <c r="KF4" s="65"/>
-      <c r="KG4" s="65"/>
-      <c r="KH4" s="90" t="s">
+      <c r="KA4" s="91"/>
+      <c r="KB4" s="91"/>
+      <c r="KC4" s="91"/>
+      <c r="KD4" s="91"/>
+      <c r="KE4" s="91"/>
+      <c r="KF4" s="91"/>
+      <c r="KG4" s="91"/>
+      <c r="KH4" s="63" t="s">
         <v>316</v>
       </c>
-      <c r="KI4" s="93"/>
-      <c r="KJ4" s="91"/>
+      <c r="KI4" s="88"/>
+      <c r="KJ4" s="64"/>
       <c r="KK4" s="46"/>
-      <c r="KL4" s="90" t="s">
+      <c r="KL4" s="63" t="s">
         <v>343</v>
       </c>
-      <c r="KM4" s="91"/>
+      <c r="KM4" s="64"/>
+      <c r="KN4" s="96"/>
+      <c r="KO4" s="94"/>
     </row>
-    <row r="5" spans="1:299" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="82"/>
-      <c r="B5" s="82"/>
-      <c r="C5" s="82"/>
-      <c r="D5" s="82"/>
-      <c r="E5" s="83"/>
-      <c r="F5" s="83"/>
-      <c r="G5" s="83"/>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="84"/>
-      <c r="L5" s="84"/>
-      <c r="M5" s="84"/>
-      <c r="N5" s="84"/>
-      <c r="O5" s="84"/>
-      <c r="P5" s="85"/>
-      <c r="Q5" s="85"/>
-      <c r="R5" s="85"/>
-      <c r="S5" s="85"/>
-      <c r="T5" s="85"/>
-      <c r="U5" s="86"/>
-      <c r="V5" s="86"/>
-      <c r="W5" s="86"/>
-      <c r="X5" s="86"/>
-      <c r="Y5" s="86"/>
-      <c r="Z5" s="86"/>
-      <c r="AA5" s="86"/>
-      <c r="AB5" s="86"/>
-      <c r="AC5" s="87"/>
-      <c r="AD5" s="87"/>
-      <c r="AE5" s="87"/>
-      <c r="AF5" s="87"/>
-      <c r="AG5" s="87"/>
-      <c r="AH5" s="87"/>
-      <c r="AI5" s="87"/>
-      <c r="AJ5" s="88"/>
-      <c r="AK5" s="88"/>
-      <c r="AL5" s="88"/>
-      <c r="AM5" s="79"/>
-      <c r="AN5" s="79"/>
-      <c r="AO5" s="69"/>
-      <c r="AP5" s="69"/>
-      <c r="AQ5" s="69"/>
-      <c r="AR5" s="69"/>
-      <c r="AS5" s="70"/>
-      <c r="AT5" s="70"/>
-      <c r="AU5" s="70"/>
-      <c r="AV5" s="70"/>
-      <c r="AW5" s="70"/>
-      <c r="AX5" s="70"/>
-      <c r="AY5" s="70"/>
-      <c r="AZ5" s="70"/>
-      <c r="BA5" s="70"/>
-      <c r="BB5" s="70"/>
-      <c r="BC5" s="70"/>
-      <c r="BD5" s="70"/>
-      <c r="BE5" s="70"/>
-      <c r="BF5" s="70"/>
-      <c r="BG5" s="70"/>
-      <c r="BH5" s="70"/>
-      <c r="BI5" s="70"/>
-      <c r="BJ5" s="70"/>
+    <row r="5" spans="1:301" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="70"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
+      <c r="I5" s="71"/>
+      <c r="J5" s="71"/>
+      <c r="K5" s="72"/>
+      <c r="L5" s="72"/>
+      <c r="M5" s="72"/>
+      <c r="N5" s="72"/>
+      <c r="O5" s="72"/>
+      <c r="P5" s="73"/>
+      <c r="Q5" s="73"/>
+      <c r="R5" s="73"/>
+      <c r="S5" s="73"/>
+      <c r="T5" s="73"/>
+      <c r="U5" s="74"/>
+      <c r="V5" s="74"/>
+      <c r="W5" s="74"/>
+      <c r="X5" s="74"/>
+      <c r="Y5" s="74"/>
+      <c r="Z5" s="74"/>
+      <c r="AA5" s="74"/>
+      <c r="AB5" s="74"/>
+      <c r="AC5" s="75"/>
+      <c r="AD5" s="75"/>
+      <c r="AE5" s="75"/>
+      <c r="AF5" s="75"/>
+      <c r="AG5" s="75"/>
+      <c r="AH5" s="75"/>
+      <c r="AI5" s="75"/>
+      <c r="AJ5" s="76"/>
+      <c r="AK5" s="76"/>
+      <c r="AL5" s="76"/>
+      <c r="AM5" s="67"/>
+      <c r="AN5" s="67"/>
+      <c r="AO5" s="78"/>
+      <c r="AP5" s="78"/>
+      <c r="AQ5" s="78"/>
+      <c r="AR5" s="78"/>
+      <c r="AS5" s="79"/>
+      <c r="AT5" s="79"/>
+      <c r="AU5" s="79"/>
+      <c r="AV5" s="79"/>
+      <c r="AW5" s="79"/>
+      <c r="AX5" s="79"/>
+      <c r="AY5" s="79"/>
+      <c r="AZ5" s="79"/>
+      <c r="BA5" s="79"/>
+      <c r="BB5" s="79"/>
+      <c r="BC5" s="79"/>
+      <c r="BD5" s="79"/>
+      <c r="BE5" s="79"/>
+      <c r="BF5" s="79"/>
+      <c r="BG5" s="79"/>
+      <c r="BH5" s="79"/>
+      <c r="BI5" s="79"/>
+      <c r="BJ5" s="79"/>
       <c r="BK5" s="8" t="s">
         <v>27</v>
       </c>
@@ -4149,39 +4190,41 @@
       <c r="JL5" s="11" t="s">
         <v>315</v>
       </c>
-      <c r="JM5" s="68"/>
-      <c r="JN5" s="68"/>
-      <c r="JO5" s="68"/>
-      <c r="JP5" s="68"/>
-      <c r="JQ5" s="68"/>
-      <c r="JR5" s="68"/>
-      <c r="JS5" s="68"/>
-      <c r="JT5" s="68"/>
-      <c r="JU5" s="68"/>
-      <c r="JV5" s="68"/>
-      <c r="JW5" s="68"/>
-      <c r="JX5" s="68"/>
-      <c r="JY5" s="68"/>
-      <c r="JZ5" s="65" t="s">
+      <c r="JM5" s="93"/>
+      <c r="JN5" s="93"/>
+      <c r="JO5" s="93"/>
+      <c r="JP5" s="93"/>
+      <c r="JQ5" s="93"/>
+      <c r="JR5" s="93"/>
+      <c r="JS5" s="93"/>
+      <c r="JT5" s="93"/>
+      <c r="JU5" s="93"/>
+      <c r="JV5" s="93"/>
+      <c r="JW5" s="93"/>
+      <c r="JX5" s="93"/>
+      <c r="JY5" s="93"/>
+      <c r="JZ5" s="91" t="s">
         <v>342</v>
       </c>
-      <c r="KA5" s="65"/>
-      <c r="KB5" s="65"/>
-      <c r="KC5" s="65"/>
-      <c r="KD5" s="65" t="s">
+      <c r="KA5" s="91"/>
+      <c r="KB5" s="91"/>
+      <c r="KC5" s="91"/>
+      <c r="KD5" s="91" t="s">
         <v>38</v>
       </c>
-      <c r="KE5" s="65"/>
-      <c r="KF5" s="65"/>
-      <c r="KG5" s="65"/>
-      <c r="KH5" s="62"/>
-      <c r="KI5" s="63"/>
-      <c r="KJ5" s="92"/>
+      <c r="KE5" s="91"/>
+      <c r="KF5" s="91"/>
+      <c r="KG5" s="91"/>
+      <c r="KH5" s="65"/>
+      <c r="KI5" s="89"/>
+      <c r="KJ5" s="66"/>
       <c r="KK5" s="46"/>
-      <c r="KL5" s="62"/>
-      <c r="KM5" s="92"/>
+      <c r="KL5" s="65"/>
+      <c r="KM5" s="66"/>
+      <c r="KN5" s="97"/>
+      <c r="KO5" s="95"/>
     </row>
-    <row r="6" spans="1:299" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:301" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>39</v>
       </c>
@@ -5079,8 +5122,14 @@
       <c r="KM6" s="22" t="s">
         <v>345</v>
       </c>
+      <c r="KN6" s="22" t="s">
+        <v>346</v>
+      </c>
+      <c r="KO6" s="22" t="s">
+        <v>347</v>
+      </c>
     </row>
-    <row r="7" spans="1:299" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:301" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="49"/>
       <c r="B7" s="49"/>
       <c r="C7" s="49"/>
@@ -5514,8 +5563,10 @@
       <c r="KI7" s="47"/>
       <c r="KJ7" s="47"/>
       <c r="KK7" s="47"/>
-      <c r="KL7" s="89"/>
-      <c r="KM7" s="89"/>
+      <c r="KL7" s="62"/>
+      <c r="KM7" s="62"/>
+      <c r="KN7" s="62"/>
+      <c r="KO7" s="62"/>
     </row>
     <row r="32" spans="297:297" x14ac:dyDescent="0.2">
       <c r="KK32" s="48"/>
@@ -5523,6 +5574,23 @@
   </sheetData>
   <autoFilter ref="A6:KK6" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="33">
+    <mergeCell ref="FE4:FR4"/>
+    <mergeCell ref="FS4:GF4"/>
+    <mergeCell ref="KH4:KJ5"/>
+    <mergeCell ref="JZ4:KG4"/>
+    <mergeCell ref="JZ5:KC5"/>
+    <mergeCell ref="KD5:KG5"/>
+    <mergeCell ref="GU4:HH4"/>
+    <mergeCell ref="HI4:HV4"/>
+    <mergeCell ref="HW4:IJ4"/>
+    <mergeCell ref="IK4:IX4"/>
+    <mergeCell ref="IY4:JL4"/>
+    <mergeCell ref="JM4:JY5"/>
+    <mergeCell ref="CM4:CZ4"/>
+    <mergeCell ref="DA4:DN4"/>
+    <mergeCell ref="DO4:EB4"/>
+    <mergeCell ref="EC4:EP4"/>
+    <mergeCell ref="EQ4:FD4"/>
     <mergeCell ref="KL4:KM5"/>
     <mergeCell ref="AM4:AN5"/>
     <mergeCell ref="A1:B1"/>
@@ -5539,23 +5607,6 @@
     <mergeCell ref="AS4:BJ5"/>
     <mergeCell ref="BK4:BX4"/>
     <mergeCell ref="BY4:CL4"/>
-    <mergeCell ref="CM4:CZ4"/>
-    <mergeCell ref="DA4:DN4"/>
-    <mergeCell ref="DO4:EB4"/>
-    <mergeCell ref="EC4:EP4"/>
-    <mergeCell ref="EQ4:FD4"/>
-    <mergeCell ref="FE4:FR4"/>
-    <mergeCell ref="FS4:GF4"/>
-    <mergeCell ref="KH4:KJ5"/>
-    <mergeCell ref="JZ4:KG4"/>
-    <mergeCell ref="JZ5:KC5"/>
-    <mergeCell ref="KD5:KG5"/>
-    <mergeCell ref="GU4:HH4"/>
-    <mergeCell ref="HI4:HV4"/>
-    <mergeCell ref="HW4:IJ4"/>
-    <mergeCell ref="IK4:IX4"/>
-    <mergeCell ref="IY4:JL4"/>
-    <mergeCell ref="JM4:JY5"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A6">
     <cfRule type="duplicateValues" dxfId="0" priority="92"/>

</xml_diff>

<commit_message>
RUBY-2440: FCRM report template adjusted - homes replaced with properties
</commit_message>
<xml_diff>
--- a/lib/fcerm1_template.xlsx
+++ b/lib/fcerm1_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\x959510\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\x964158\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED8BA3D2-F58C-4C09-9C50-FA848AD2D1BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3544E9C-F322-4329-9923-458155D8A7E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1131,12 +1131,6 @@
     <t>PAFS Status</t>
   </si>
   <si>
-    <t>Confidence in 'Number' of homes (all scheme including post 2021)</t>
-  </si>
-  <si>
-    <t>Confidence in Homes being delivered (by specified gateway 4 date)</t>
-  </si>
-  <si>
     <t>Confidence in Securing Partnership Funding (all schemes including post-2021)</t>
   </si>
   <si>
@@ -1195,6 +1189,12 @@
   </si>
   <si>
     <t>PSO Name</t>
+  </si>
+  <si>
+    <t>Confidence in 'Number' of properties (all scheme including post 2021)</t>
+  </si>
+  <si>
+    <t>Confidence in Properties being delivered (by specified gateway 4 date)</t>
   </si>
 </sst>
 </file>
@@ -1777,18 +1777,72 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="25" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="25" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="25" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1819,9 +1873,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="5" fillId="11" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1830,57 +1881,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -2189,11 +2189,11 @@
   <dimension ref="A1:KO32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="KL7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="KG7" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
       <selection pane="topRight" activeCell="C7" sqref="C7"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="KM12" sqref="KM12"/>
+      <selection pane="bottomRight" activeCell="KI6" sqref="KI6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2226,10 +2226,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:301" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="68"/>
+      <c r="B1" s="86"/>
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
       <c r="E1" s="23"/>
@@ -2531,10 +2531,10 @@
       <c r="KO1" s="47"/>
     </row>
     <row r="2" spans="1:301" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="69" t="s">
-        <v>337</v>
-      </c>
-      <c r="B2" s="69"/>
+      <c r="A2" s="87" t="s">
+        <v>335</v>
+      </c>
+      <c r="B2" s="87"/>
       <c r="C2" s="36"/>
       <c r="D2" s="36"/>
       <c r="E2" s="23"/>
@@ -3139,86 +3139,86 @@
       <c r="KO3" s="47"/>
     </row>
     <row r="4" spans="1:301" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="70" t="s">
+      <c r="A4" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="70"/>
-      <c r="C4" s="70"/>
-      <c r="D4" s="70"/>
-      <c r="E4" s="71" t="s">
+      <c r="B4" s="88"/>
+      <c r="C4" s="88"/>
+      <c r="D4" s="88"/>
+      <c r="E4" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="72" t="s">
+      <c r="F4" s="89"/>
+      <c r="G4" s="89"/>
+      <c r="H4" s="89"/>
+      <c r="I4" s="89"/>
+      <c r="J4" s="89"/>
+      <c r="K4" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="72"/>
-      <c r="M4" s="72"/>
-      <c r="N4" s="72"/>
-      <c r="O4" s="72"/>
-      <c r="P4" s="73" t="s">
+      <c r="L4" s="90"/>
+      <c r="M4" s="90"/>
+      <c r="N4" s="90"/>
+      <c r="O4" s="90"/>
+      <c r="P4" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="Q4" s="73"/>
-      <c r="R4" s="73"/>
-      <c r="S4" s="73"/>
-      <c r="T4" s="73"/>
-      <c r="U4" s="74" t="s">
+      <c r="Q4" s="91"/>
+      <c r="R4" s="91"/>
+      <c r="S4" s="91"/>
+      <c r="T4" s="91"/>
+      <c r="U4" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="V4" s="74"/>
-      <c r="W4" s="74"/>
-      <c r="X4" s="74"/>
-      <c r="Y4" s="74"/>
-      <c r="Z4" s="74"/>
-      <c r="AA4" s="74"/>
-      <c r="AB4" s="74"/>
-      <c r="AC4" s="75" t="s">
+      <c r="V4" s="92"/>
+      <c r="W4" s="92"/>
+      <c r="X4" s="92"/>
+      <c r="Y4" s="92"/>
+      <c r="Z4" s="92"/>
+      <c r="AA4" s="92"/>
+      <c r="AB4" s="92"/>
+      <c r="AC4" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="AD4" s="75"/>
-      <c r="AE4" s="75"/>
-      <c r="AF4" s="75"/>
-      <c r="AG4" s="75"/>
-      <c r="AH4" s="75"/>
-      <c r="AI4" s="75"/>
-      <c r="AJ4" s="76" t="s">
+      <c r="AD4" s="93"/>
+      <c r="AE4" s="93"/>
+      <c r="AF4" s="93"/>
+      <c r="AG4" s="93"/>
+      <c r="AH4" s="93"/>
+      <c r="AI4" s="93"/>
+      <c r="AJ4" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="AK4" s="76"/>
-      <c r="AL4" s="76"/>
-      <c r="AM4" s="67" t="s">
+      <c r="AK4" s="94"/>
+      <c r="AL4" s="94"/>
+      <c r="AM4" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="AN4" s="67"/>
-      <c r="AO4" s="78"/>
-      <c r="AP4" s="78"/>
-      <c r="AQ4" s="78"/>
-      <c r="AR4" s="78"/>
-      <c r="AS4" s="79" t="s">
+      <c r="AN4" s="85"/>
+      <c r="AO4" s="95"/>
+      <c r="AP4" s="95"/>
+      <c r="AQ4" s="95"/>
+      <c r="AR4" s="95"/>
+      <c r="AS4" s="96" t="s">
         <v>9</v>
       </c>
-      <c r="AT4" s="79"/>
-      <c r="AU4" s="79"/>
-      <c r="AV4" s="79"/>
-      <c r="AW4" s="79"/>
-      <c r="AX4" s="79"/>
-      <c r="AY4" s="79"/>
-      <c r="AZ4" s="79"/>
-      <c r="BA4" s="79"/>
-      <c r="BB4" s="79"/>
-      <c r="BC4" s="79"/>
-      <c r="BD4" s="79"/>
-      <c r="BE4" s="79"/>
-      <c r="BF4" s="79"/>
-      <c r="BG4" s="79"/>
-      <c r="BH4" s="79"/>
-      <c r="BI4" s="79"/>
-      <c r="BJ4" s="79"/>
+      <c r="AT4" s="96"/>
+      <c r="AU4" s="96"/>
+      <c r="AV4" s="96"/>
+      <c r="AW4" s="96"/>
+      <c r="AX4" s="96"/>
+      <c r="AY4" s="96"/>
+      <c r="AZ4" s="96"/>
+      <c r="BA4" s="96"/>
+      <c r="BB4" s="96"/>
+      <c r="BC4" s="96"/>
+      <c r="BD4" s="96"/>
+      <c r="BE4" s="96"/>
+      <c r="BF4" s="96"/>
+      <c r="BG4" s="96"/>
+      <c r="BH4" s="96"/>
+      <c r="BI4" s="96"/>
+      <c r="BJ4" s="96"/>
       <c r="BK4" s="77" t="s">
         <v>10</v>
       </c>
@@ -3235,134 +3235,134 @@
       <c r="BV4" s="77"/>
       <c r="BW4" s="77"/>
       <c r="BX4" s="77"/>
-      <c r="BY4" s="80" t="s">
+      <c r="BY4" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="BZ4" s="80"/>
-      <c r="CA4" s="80"/>
-      <c r="CB4" s="80"/>
-      <c r="CC4" s="80"/>
-      <c r="CD4" s="80"/>
-      <c r="CE4" s="80"/>
-      <c r="CF4" s="80"/>
-      <c r="CG4" s="80"/>
-      <c r="CH4" s="80"/>
-      <c r="CI4" s="80"/>
-      <c r="CJ4" s="80"/>
-      <c r="CK4" s="80"/>
-      <c r="CL4" s="80"/>
-      <c r="CM4" s="81" t="s">
+      <c r="BZ4" s="97"/>
+      <c r="CA4" s="97"/>
+      <c r="CB4" s="97"/>
+      <c r="CC4" s="97"/>
+      <c r="CD4" s="97"/>
+      <c r="CE4" s="97"/>
+      <c r="CF4" s="97"/>
+      <c r="CG4" s="97"/>
+      <c r="CH4" s="97"/>
+      <c r="CI4" s="97"/>
+      <c r="CJ4" s="97"/>
+      <c r="CK4" s="97"/>
+      <c r="CL4" s="97"/>
+      <c r="CM4" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="CN4" s="81"/>
-      <c r="CO4" s="81"/>
-      <c r="CP4" s="81"/>
-      <c r="CQ4" s="81"/>
-      <c r="CR4" s="81"/>
-      <c r="CS4" s="81"/>
-      <c r="CT4" s="81"/>
-      <c r="CU4" s="81"/>
-      <c r="CV4" s="81"/>
-      <c r="CW4" s="81"/>
-      <c r="CX4" s="81"/>
-      <c r="CY4" s="81"/>
-      <c r="CZ4" s="81"/>
-      <c r="DA4" s="82" t="s">
+      <c r="CN4" s="80"/>
+      <c r="CO4" s="80"/>
+      <c r="CP4" s="80"/>
+      <c r="CQ4" s="80"/>
+      <c r="CR4" s="80"/>
+      <c r="CS4" s="80"/>
+      <c r="CT4" s="80"/>
+      <c r="CU4" s="80"/>
+      <c r="CV4" s="80"/>
+      <c r="CW4" s="80"/>
+      <c r="CX4" s="80"/>
+      <c r="CY4" s="80"/>
+      <c r="CZ4" s="80"/>
+      <c r="DA4" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="DB4" s="82"/>
-      <c r="DC4" s="82"/>
-      <c r="DD4" s="82"/>
-      <c r="DE4" s="82"/>
-      <c r="DF4" s="82"/>
-      <c r="DG4" s="82"/>
-      <c r="DH4" s="82"/>
-      <c r="DI4" s="82"/>
-      <c r="DJ4" s="82"/>
-      <c r="DK4" s="82"/>
-      <c r="DL4" s="82"/>
-      <c r="DM4" s="82"/>
-      <c r="DN4" s="82"/>
-      <c r="DO4" s="83" t="s">
+      <c r="DB4" s="81"/>
+      <c r="DC4" s="81"/>
+      <c r="DD4" s="81"/>
+      <c r="DE4" s="81"/>
+      <c r="DF4" s="81"/>
+      <c r="DG4" s="81"/>
+      <c r="DH4" s="81"/>
+      <c r="DI4" s="81"/>
+      <c r="DJ4" s="81"/>
+      <c r="DK4" s="81"/>
+      <c r="DL4" s="81"/>
+      <c r="DM4" s="81"/>
+      <c r="DN4" s="81"/>
+      <c r="DO4" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="DP4" s="83"/>
-      <c r="DQ4" s="83"/>
-      <c r="DR4" s="83"/>
-      <c r="DS4" s="83"/>
-      <c r="DT4" s="83"/>
-      <c r="DU4" s="83"/>
-      <c r="DV4" s="83"/>
-      <c r="DW4" s="83"/>
-      <c r="DX4" s="83"/>
-      <c r="DY4" s="83"/>
-      <c r="DZ4" s="83"/>
-      <c r="EA4" s="83"/>
-      <c r="EB4" s="83"/>
-      <c r="EC4" s="84" t="s">
+      <c r="DP4" s="82"/>
+      <c r="DQ4" s="82"/>
+      <c r="DR4" s="82"/>
+      <c r="DS4" s="82"/>
+      <c r="DT4" s="82"/>
+      <c r="DU4" s="82"/>
+      <c r="DV4" s="82"/>
+      <c r="DW4" s="82"/>
+      <c r="DX4" s="82"/>
+      <c r="DY4" s="82"/>
+      <c r="DZ4" s="82"/>
+      <c r="EA4" s="82"/>
+      <c r="EB4" s="82"/>
+      <c r="EC4" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="ED4" s="84"/>
-      <c r="EE4" s="84"/>
-      <c r="EF4" s="84"/>
-      <c r="EG4" s="84"/>
-      <c r="EH4" s="84"/>
-      <c r="EI4" s="84"/>
-      <c r="EJ4" s="84"/>
-      <c r="EK4" s="84"/>
-      <c r="EL4" s="84"/>
-      <c r="EM4" s="84"/>
-      <c r="EN4" s="84"/>
-      <c r="EO4" s="84"/>
-      <c r="EP4" s="84"/>
-      <c r="EQ4" s="85" t="s">
+      <c r="ED4" s="83"/>
+      <c r="EE4" s="83"/>
+      <c r="EF4" s="83"/>
+      <c r="EG4" s="83"/>
+      <c r="EH4" s="83"/>
+      <c r="EI4" s="83"/>
+      <c r="EJ4" s="83"/>
+      <c r="EK4" s="83"/>
+      <c r="EL4" s="83"/>
+      <c r="EM4" s="83"/>
+      <c r="EN4" s="83"/>
+      <c r="EO4" s="83"/>
+      <c r="EP4" s="83"/>
+      <c r="EQ4" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="ER4" s="85"/>
-      <c r="ES4" s="85"/>
-      <c r="ET4" s="85"/>
-      <c r="EU4" s="85"/>
-      <c r="EV4" s="85"/>
-      <c r="EW4" s="85"/>
-      <c r="EX4" s="85"/>
-      <c r="EY4" s="85"/>
-      <c r="EZ4" s="85"/>
-      <c r="FA4" s="85"/>
-      <c r="FB4" s="85"/>
-      <c r="FC4" s="85"/>
-      <c r="FD4" s="85"/>
-      <c r="FE4" s="86" t="s">
+      <c r="ER4" s="84"/>
+      <c r="ES4" s="84"/>
+      <c r="ET4" s="84"/>
+      <c r="EU4" s="84"/>
+      <c r="EV4" s="84"/>
+      <c r="EW4" s="84"/>
+      <c r="EX4" s="84"/>
+      <c r="EY4" s="84"/>
+      <c r="EZ4" s="84"/>
+      <c r="FA4" s="84"/>
+      <c r="FB4" s="84"/>
+      <c r="FC4" s="84"/>
+      <c r="FD4" s="84"/>
+      <c r="FE4" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="FF4" s="86"/>
-      <c r="FG4" s="86"/>
-      <c r="FH4" s="86"/>
-      <c r="FI4" s="86"/>
-      <c r="FJ4" s="86"/>
-      <c r="FK4" s="86"/>
-      <c r="FL4" s="86"/>
-      <c r="FM4" s="86"/>
-      <c r="FN4" s="86"/>
-      <c r="FO4" s="86"/>
-      <c r="FP4" s="86"/>
-      <c r="FQ4" s="86"/>
-      <c r="FR4" s="86"/>
-      <c r="FS4" s="87" t="s">
+      <c r="FF4" s="67"/>
+      <c r="FG4" s="67"/>
+      <c r="FH4" s="67"/>
+      <c r="FI4" s="67"/>
+      <c r="FJ4" s="67"/>
+      <c r="FK4" s="67"/>
+      <c r="FL4" s="67"/>
+      <c r="FM4" s="67"/>
+      <c r="FN4" s="67"/>
+      <c r="FO4" s="67"/>
+      <c r="FP4" s="67"/>
+      <c r="FQ4" s="67"/>
+      <c r="FR4" s="67"/>
+      <c r="FS4" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="FT4" s="87"/>
-      <c r="FU4" s="87"/>
-      <c r="FV4" s="87"/>
-      <c r="FW4" s="87"/>
-      <c r="FX4" s="87"/>
-      <c r="FY4" s="87"/>
-      <c r="FZ4" s="87"/>
-      <c r="GA4" s="87"/>
-      <c r="GB4" s="87"/>
-      <c r="GC4" s="87"/>
-      <c r="GD4" s="87"/>
-      <c r="GE4" s="87"/>
-      <c r="GF4" s="87"/>
+      <c r="FT4" s="68"/>
+      <c r="FU4" s="68"/>
+      <c r="FV4" s="68"/>
+      <c r="FW4" s="68"/>
+      <c r="FX4" s="68"/>
+      <c r="FY4" s="68"/>
+      <c r="FZ4" s="68"/>
+      <c r="GA4" s="68"/>
+      <c r="GB4" s="68"/>
+      <c r="GC4" s="68"/>
+      <c r="GD4" s="68"/>
+      <c r="GE4" s="68"/>
+      <c r="GF4" s="68"/>
       <c r="GG4" s="77" t="s">
         <v>19</v>
       </c>
@@ -3411,155 +3411,155 @@
       <c r="HT4" s="77"/>
       <c r="HU4" s="77"/>
       <c r="HV4" s="77"/>
-      <c r="HW4" s="92" t="s">
+      <c r="HW4" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="HX4" s="92"/>
-      <c r="HY4" s="92"/>
-      <c r="HZ4" s="92"/>
-      <c r="IA4" s="92"/>
-      <c r="IB4" s="92"/>
-      <c r="IC4" s="92"/>
-      <c r="ID4" s="92"/>
-      <c r="IE4" s="92"/>
-      <c r="IF4" s="92"/>
-      <c r="IG4" s="92"/>
-      <c r="IH4" s="92"/>
-      <c r="II4" s="92"/>
-      <c r="IJ4" s="92"/>
-      <c r="IK4" s="92" t="s">
+      <c r="HX4" s="78"/>
+      <c r="HY4" s="78"/>
+      <c r="HZ4" s="78"/>
+      <c r="IA4" s="78"/>
+      <c r="IB4" s="78"/>
+      <c r="IC4" s="78"/>
+      <c r="ID4" s="78"/>
+      <c r="IE4" s="78"/>
+      <c r="IF4" s="78"/>
+      <c r="IG4" s="78"/>
+      <c r="IH4" s="78"/>
+      <c r="II4" s="78"/>
+      <c r="IJ4" s="78"/>
+      <c r="IK4" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="IL4" s="92"/>
-      <c r="IM4" s="92"/>
-      <c r="IN4" s="92"/>
-      <c r="IO4" s="92"/>
-      <c r="IP4" s="92"/>
-      <c r="IQ4" s="92"/>
-      <c r="IR4" s="92"/>
-      <c r="IS4" s="92"/>
-      <c r="IT4" s="92"/>
-      <c r="IU4" s="92"/>
-      <c r="IV4" s="92"/>
-      <c r="IW4" s="92"/>
-      <c r="IX4" s="92"/>
-      <c r="IY4" s="92" t="s">
+      <c r="IL4" s="78"/>
+      <c r="IM4" s="78"/>
+      <c r="IN4" s="78"/>
+      <c r="IO4" s="78"/>
+      <c r="IP4" s="78"/>
+      <c r="IQ4" s="78"/>
+      <c r="IR4" s="78"/>
+      <c r="IS4" s="78"/>
+      <c r="IT4" s="78"/>
+      <c r="IU4" s="78"/>
+      <c r="IV4" s="78"/>
+      <c r="IW4" s="78"/>
+      <c r="IX4" s="78"/>
+      <c r="IY4" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="IZ4" s="92"/>
-      <c r="JA4" s="92"/>
-      <c r="JB4" s="92"/>
-      <c r="JC4" s="92"/>
-      <c r="JD4" s="92"/>
-      <c r="JE4" s="92"/>
-      <c r="JF4" s="92"/>
-      <c r="JG4" s="92"/>
-      <c r="JH4" s="92"/>
-      <c r="JI4" s="92"/>
-      <c r="JJ4" s="92"/>
-      <c r="JK4" s="92"/>
-      <c r="JL4" s="92"/>
-      <c r="JM4" s="93" t="s">
+      <c r="IZ4" s="78"/>
+      <c r="JA4" s="78"/>
+      <c r="JB4" s="78"/>
+      <c r="JC4" s="78"/>
+      <c r="JD4" s="78"/>
+      <c r="JE4" s="78"/>
+      <c r="JF4" s="78"/>
+      <c r="JG4" s="78"/>
+      <c r="JH4" s="78"/>
+      <c r="JI4" s="78"/>
+      <c r="JJ4" s="78"/>
+      <c r="JK4" s="78"/>
+      <c r="JL4" s="78"/>
+      <c r="JM4" s="79" t="s">
         <v>25</v>
       </c>
-      <c r="JN4" s="93"/>
-      <c r="JO4" s="93"/>
-      <c r="JP4" s="93"/>
-      <c r="JQ4" s="93"/>
-      <c r="JR4" s="93"/>
-      <c r="JS4" s="93"/>
-      <c r="JT4" s="93"/>
-      <c r="JU4" s="93"/>
-      <c r="JV4" s="93"/>
-      <c r="JW4" s="93"/>
-      <c r="JX4" s="93"/>
-      <c r="JY4" s="93"/>
-      <c r="JZ4" s="90" t="s">
+      <c r="JN4" s="79"/>
+      <c r="JO4" s="79"/>
+      <c r="JP4" s="79"/>
+      <c r="JQ4" s="79"/>
+      <c r="JR4" s="79"/>
+      <c r="JS4" s="79"/>
+      <c r="JT4" s="79"/>
+      <c r="JU4" s="79"/>
+      <c r="JV4" s="79"/>
+      <c r="JW4" s="79"/>
+      <c r="JX4" s="79"/>
+      <c r="JY4" s="79"/>
+      <c r="JZ4" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="KA4" s="91"/>
-      <c r="KB4" s="91"/>
-      <c r="KC4" s="91"/>
-      <c r="KD4" s="91"/>
-      <c r="KE4" s="91"/>
-      <c r="KF4" s="91"/>
-      <c r="KG4" s="91"/>
-      <c r="KH4" s="63" t="s">
+      <c r="KA4" s="76"/>
+      <c r="KB4" s="76"/>
+      <c r="KC4" s="76"/>
+      <c r="KD4" s="76"/>
+      <c r="KE4" s="76"/>
+      <c r="KF4" s="76"/>
+      <c r="KG4" s="76"/>
+      <c r="KH4" s="69" t="s">
         <v>316</v>
       </c>
-      <c r="KI4" s="88"/>
-      <c r="KJ4" s="64"/>
+      <c r="KI4" s="70"/>
+      <c r="KJ4" s="71"/>
       <c r="KK4" s="46"/>
-      <c r="KL4" s="63" t="s">
-        <v>343</v>
-      </c>
-      <c r="KM4" s="64"/>
-      <c r="KN4" s="96"/>
-      <c r="KO4" s="94"/>
+      <c r="KL4" s="69" t="s">
+        <v>341</v>
+      </c>
+      <c r="KM4" s="71"/>
+      <c r="KN4" s="65"/>
+      <c r="KO4" s="63"/>
     </row>
     <row r="5" spans="1:301" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="70"/>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="71"/>
-      <c r="K5" s="72"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="72"/>
-      <c r="N5" s="72"/>
-      <c r="O5" s="72"/>
-      <c r="P5" s="73"/>
-      <c r="Q5" s="73"/>
-      <c r="R5" s="73"/>
-      <c r="S5" s="73"/>
-      <c r="T5" s="73"/>
-      <c r="U5" s="74"/>
-      <c r="V5" s="74"/>
-      <c r="W5" s="74"/>
-      <c r="X5" s="74"/>
-      <c r="Y5" s="74"/>
-      <c r="Z5" s="74"/>
-      <c r="AA5" s="74"/>
-      <c r="AB5" s="74"/>
-      <c r="AC5" s="75"/>
-      <c r="AD5" s="75"/>
-      <c r="AE5" s="75"/>
-      <c r="AF5" s="75"/>
-      <c r="AG5" s="75"/>
-      <c r="AH5" s="75"/>
-      <c r="AI5" s="75"/>
-      <c r="AJ5" s="76"/>
-      <c r="AK5" s="76"/>
-      <c r="AL5" s="76"/>
-      <c r="AM5" s="67"/>
-      <c r="AN5" s="67"/>
-      <c r="AO5" s="78"/>
-      <c r="AP5" s="78"/>
-      <c r="AQ5" s="78"/>
-      <c r="AR5" s="78"/>
-      <c r="AS5" s="79"/>
-      <c r="AT5" s="79"/>
-      <c r="AU5" s="79"/>
-      <c r="AV5" s="79"/>
-      <c r="AW5" s="79"/>
-      <c r="AX5" s="79"/>
-      <c r="AY5" s="79"/>
-      <c r="AZ5" s="79"/>
-      <c r="BA5" s="79"/>
-      <c r="BB5" s="79"/>
-      <c r="BC5" s="79"/>
-      <c r="BD5" s="79"/>
-      <c r="BE5" s="79"/>
-      <c r="BF5" s="79"/>
-      <c r="BG5" s="79"/>
-      <c r="BH5" s="79"/>
-      <c r="BI5" s="79"/>
-      <c r="BJ5" s="79"/>
+      <c r="A5" s="88"/>
+      <c r="B5" s="88"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="89"/>
+      <c r="F5" s="89"/>
+      <c r="G5" s="89"/>
+      <c r="H5" s="89"/>
+      <c r="I5" s="89"/>
+      <c r="J5" s="89"/>
+      <c r="K5" s="90"/>
+      <c r="L5" s="90"/>
+      <c r="M5" s="90"/>
+      <c r="N5" s="90"/>
+      <c r="O5" s="90"/>
+      <c r="P5" s="91"/>
+      <c r="Q5" s="91"/>
+      <c r="R5" s="91"/>
+      <c r="S5" s="91"/>
+      <c r="T5" s="91"/>
+      <c r="U5" s="92"/>
+      <c r="V5" s="92"/>
+      <c r="W5" s="92"/>
+      <c r="X5" s="92"/>
+      <c r="Y5" s="92"/>
+      <c r="Z5" s="92"/>
+      <c r="AA5" s="92"/>
+      <c r="AB5" s="92"/>
+      <c r="AC5" s="93"/>
+      <c r="AD5" s="93"/>
+      <c r="AE5" s="93"/>
+      <c r="AF5" s="93"/>
+      <c r="AG5" s="93"/>
+      <c r="AH5" s="93"/>
+      <c r="AI5" s="93"/>
+      <c r="AJ5" s="94"/>
+      <c r="AK5" s="94"/>
+      <c r="AL5" s="94"/>
+      <c r="AM5" s="85"/>
+      <c r="AN5" s="85"/>
+      <c r="AO5" s="95"/>
+      <c r="AP5" s="95"/>
+      <c r="AQ5" s="95"/>
+      <c r="AR5" s="95"/>
+      <c r="AS5" s="96"/>
+      <c r="AT5" s="96"/>
+      <c r="AU5" s="96"/>
+      <c r="AV5" s="96"/>
+      <c r="AW5" s="96"/>
+      <c r="AX5" s="96"/>
+      <c r="AY5" s="96"/>
+      <c r="AZ5" s="96"/>
+      <c r="BA5" s="96"/>
+      <c r="BB5" s="96"/>
+      <c r="BC5" s="96"/>
+      <c r="BD5" s="96"/>
+      <c r="BE5" s="96"/>
+      <c r="BF5" s="96"/>
+      <c r="BG5" s="96"/>
+      <c r="BH5" s="96"/>
+      <c r="BI5" s="96"/>
+      <c r="BJ5" s="96"/>
       <c r="BK5" s="8" t="s">
         <v>27</v>
       </c>
@@ -4190,39 +4190,39 @@
       <c r="JL5" s="11" t="s">
         <v>315</v>
       </c>
-      <c r="JM5" s="93"/>
-      <c r="JN5" s="93"/>
-      <c r="JO5" s="93"/>
-      <c r="JP5" s="93"/>
-      <c r="JQ5" s="93"/>
-      <c r="JR5" s="93"/>
-      <c r="JS5" s="93"/>
-      <c r="JT5" s="93"/>
-      <c r="JU5" s="93"/>
-      <c r="JV5" s="93"/>
-      <c r="JW5" s="93"/>
-      <c r="JX5" s="93"/>
-      <c r="JY5" s="93"/>
-      <c r="JZ5" s="91" t="s">
-        <v>342</v>
-      </c>
-      <c r="KA5" s="91"/>
-      <c r="KB5" s="91"/>
-      <c r="KC5" s="91"/>
-      <c r="KD5" s="91" t="s">
+      <c r="JM5" s="79"/>
+      <c r="JN5" s="79"/>
+      <c r="JO5" s="79"/>
+      <c r="JP5" s="79"/>
+      <c r="JQ5" s="79"/>
+      <c r="JR5" s="79"/>
+      <c r="JS5" s="79"/>
+      <c r="JT5" s="79"/>
+      <c r="JU5" s="79"/>
+      <c r="JV5" s="79"/>
+      <c r="JW5" s="79"/>
+      <c r="JX5" s="79"/>
+      <c r="JY5" s="79"/>
+      <c r="JZ5" s="76" t="s">
+        <v>340</v>
+      </c>
+      <c r="KA5" s="76"/>
+      <c r="KB5" s="76"/>
+      <c r="KC5" s="76"/>
+      <c r="KD5" s="76" t="s">
         <v>38</v>
       </c>
-      <c r="KE5" s="91"/>
-      <c r="KF5" s="91"/>
-      <c r="KG5" s="91"/>
-      <c r="KH5" s="65"/>
-      <c r="KI5" s="89"/>
-      <c r="KJ5" s="66"/>
+      <c r="KE5" s="76"/>
+      <c r="KF5" s="76"/>
+      <c r="KG5" s="76"/>
+      <c r="KH5" s="72"/>
+      <c r="KI5" s="73"/>
+      <c r="KJ5" s="74"/>
       <c r="KK5" s="46"/>
-      <c r="KL5" s="65"/>
-      <c r="KM5" s="66"/>
-      <c r="KN5" s="97"/>
-      <c r="KO5" s="95"/>
+      <c r="KL5" s="72"/>
+      <c r="KM5" s="74"/>
+      <c r="KN5" s="66"/>
+      <c r="KO5" s="64"/>
     </row>
     <row r="6" spans="1:301" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
@@ -5081,16 +5081,16 @@
         <v>308</v>
       </c>
       <c r="JZ6" s="22" t="s">
+        <v>337</v>
+      </c>
+      <c r="KA6" s="29" t="s">
+        <v>336</v>
+      </c>
+      <c r="KB6" s="22" t="s">
+        <v>338</v>
+      </c>
+      <c r="KC6" s="22" t="s">
         <v>339</v>
-      </c>
-      <c r="KA6" s="29" t="s">
-        <v>338</v>
-      </c>
-      <c r="KB6" s="22" t="s">
-        <v>340</v>
-      </c>
-      <c r="KC6" s="22" t="s">
-        <v>341</v>
       </c>
       <c r="KD6" s="22" t="s">
         <v>309</v>
@@ -5105,28 +5105,28 @@
         <v>311</v>
       </c>
       <c r="KH6" s="22" t="s">
+        <v>346</v>
+      </c>
+      <c r="KI6" s="22" t="s">
+        <v>347</v>
+      </c>
+      <c r="KJ6" s="22" t="s">
         <v>333</v>
-      </c>
-      <c r="KI6" s="22" t="s">
-        <v>334</v>
-      </c>
-      <c r="KJ6" s="22" t="s">
-        <v>335</v>
       </c>
       <c r="KK6" s="22" t="s">
         <v>332</v>
       </c>
       <c r="KL6" s="22" t="s">
+        <v>342</v>
+      </c>
+      <c r="KM6" s="22" t="s">
+        <v>343</v>
+      </c>
+      <c r="KN6" s="22" t="s">
         <v>344</v>
       </c>
-      <c r="KM6" s="22" t="s">
+      <c r="KO6" s="22" t="s">
         <v>345</v>
-      </c>
-      <c r="KN6" s="22" t="s">
-        <v>346</v>
-      </c>
-      <c r="KO6" s="22" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="7" spans="1:301" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5135,7 +5135,7 @@
       <c r="C7" s="49"/>
       <c r="D7" s="49"/>
       <c r="E7" s="49" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F7" s="49"/>
       <c r="G7" s="49"/>
@@ -5150,20 +5150,20 @@
       <c r="P7" s="51"/>
       <c r="Q7" s="51"/>
       <c r="R7" s="51" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="S7" s="51" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="T7" s="51"/>
       <c r="U7" s="51"/>
       <c r="V7" s="51"/>
       <c r="W7" s="51"/>
       <c r="X7" s="52" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="Y7" s="52" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="Z7" s="51"/>
       <c r="AA7" s="51"/>
@@ -5176,13 +5176,13 @@
       <c r="AH7" s="56"/>
       <c r="AI7" s="55"/>
       <c r="AJ7" s="50" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="AK7" s="50" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="AL7" s="50" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="AM7" s="51"/>
       <c r="AN7" s="57"/>
@@ -5574,23 +5574,6 @@
   </sheetData>
   <autoFilter ref="A6:KK6" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="33">
-    <mergeCell ref="FE4:FR4"/>
-    <mergeCell ref="FS4:GF4"/>
-    <mergeCell ref="KH4:KJ5"/>
-    <mergeCell ref="JZ4:KG4"/>
-    <mergeCell ref="JZ5:KC5"/>
-    <mergeCell ref="KD5:KG5"/>
-    <mergeCell ref="GU4:HH4"/>
-    <mergeCell ref="HI4:HV4"/>
-    <mergeCell ref="HW4:IJ4"/>
-    <mergeCell ref="IK4:IX4"/>
-    <mergeCell ref="IY4:JL4"/>
-    <mergeCell ref="JM4:JY5"/>
-    <mergeCell ref="CM4:CZ4"/>
-    <mergeCell ref="DA4:DN4"/>
-    <mergeCell ref="DO4:EB4"/>
-    <mergeCell ref="EC4:EP4"/>
-    <mergeCell ref="EQ4:FD4"/>
     <mergeCell ref="KL4:KM5"/>
     <mergeCell ref="AM4:AN5"/>
     <mergeCell ref="A1:B1"/>
@@ -5607,15 +5590,38 @@
     <mergeCell ref="AS4:BJ5"/>
     <mergeCell ref="BK4:BX4"/>
     <mergeCell ref="BY4:CL4"/>
+    <mergeCell ref="CM4:CZ4"/>
+    <mergeCell ref="DA4:DN4"/>
+    <mergeCell ref="DO4:EB4"/>
+    <mergeCell ref="EC4:EP4"/>
+    <mergeCell ref="EQ4:FD4"/>
+    <mergeCell ref="FE4:FR4"/>
+    <mergeCell ref="FS4:GF4"/>
+    <mergeCell ref="KH4:KJ5"/>
+    <mergeCell ref="JZ4:KG4"/>
+    <mergeCell ref="JZ5:KC5"/>
+    <mergeCell ref="KD5:KG5"/>
+    <mergeCell ref="GU4:HH4"/>
+    <mergeCell ref="HI4:HV4"/>
+    <mergeCell ref="HW4:IJ4"/>
+    <mergeCell ref="IK4:IX4"/>
+    <mergeCell ref="IY4:JL4"/>
+    <mergeCell ref="JM4:JY5"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A6">
     <cfRule type="duplicateValues" dxfId="0" priority="92"/>
   </conditionalFormatting>
-  <dataValidations count="2">
+  <dataValidations count="4">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP1:AR3 AO1:AO4 AO7:AR7" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>36526</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KH6:KJ999996" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KH7:KH999996 KJ6:KJ999996 KI7:KI999996" xr:uid="{00000000-0002-0000-0000-000001000000}">
+      <formula1>"4. High, 3. Medium High, 2. Medium Low, 1. Low, N/A"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KH6" xr:uid="{AE8924C3-193D-4315-9473-E5B199D2EA5A}">
+      <formula1>"4. High, 3. Medium High, 2. Medium Low, 1. Low, N/A"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KI6" xr:uid="{88DBC02B-9C99-479C-9C30-897AB3F898A4}">
       <formula1>"4. High, 3. Medium High, 2. Medium Low, 1. Low, N/A"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[RUBY-2579] Alter FCRM report: add Additional GiA for each FY
</commit_message>
<xml_diff>
--- a/lib/fcerm1_template.xlsx
+++ b/lib/fcerm1_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lb000070\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3861FEFA-904D-4589-8E55-E12BB9A2682F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A3B3BD-977F-460D-B4D1-61F23CCD872C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Master local choices" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Master local choices'!$A$6:$KC$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Master local choices'!$A$6:$MU$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="411">
   <si>
     <t>FCRM1 - National Capital Programme</t>
   </si>
@@ -1066,6 +1066,237 @@
   </si>
   <si>
     <t>DESCRIPTIVE DETAILS</t>
+  </si>
+  <si>
+    <t>Additional FCRM GiA (Asset replacement allowance)</t>
+  </si>
+  <si>
+    <t>Additional FCRM GiA (Environment statutory funding)</t>
+  </si>
+  <si>
+    <t>Additional FCRM GiA (Frequently flooded communities)</t>
+  </si>
+  <si>
+    <t>Additional FCRM GiA (Other additional grant in aid)</t>
+  </si>
+  <si>
+    <t>ARA GiA - 2023/24</t>
+  </si>
+  <si>
+    <t>ARA GiA - 2024/25</t>
+  </si>
+  <si>
+    <t>ARA GiA - 2025/26</t>
+  </si>
+  <si>
+    <t>ARA GiA - 2026/27</t>
+  </si>
+  <si>
+    <t>ARA GiA - 2027/28</t>
+  </si>
+  <si>
+    <t>ARA GiA - 2028/29</t>
+  </si>
+  <si>
+    <t>ARA GiA - 2029/30</t>
+  </si>
+  <si>
+    <t>ARA GiA - 2030/31</t>
+  </si>
+  <si>
+    <t>ARA GiA - 2031/32</t>
+  </si>
+  <si>
+    <t>ARA GiA - 2032/33</t>
+  </si>
+  <si>
+    <t>ESF GiA - 2023/24</t>
+  </si>
+  <si>
+    <t>ESF GiA - 2024/25</t>
+  </si>
+  <si>
+    <t>ESF GiA - 2025/26</t>
+  </si>
+  <si>
+    <t>ESF GiA - 2026/27</t>
+  </si>
+  <si>
+    <t>ESF GiA- 2027/28</t>
+  </si>
+  <si>
+    <t>ESF GiA - 2028/29</t>
+  </si>
+  <si>
+    <t>ESF GiA - 2029/30</t>
+  </si>
+  <si>
+    <t>ESF GiA - 2030/31</t>
+  </si>
+  <si>
+    <t>ESF GiA - 2031/32</t>
+  </si>
+  <si>
+    <t>ESF GiA - 2032/33</t>
+  </si>
+  <si>
+    <t>FFC GiA - 2023/24</t>
+  </si>
+  <si>
+    <t>FFC GiA - 2024/25</t>
+  </si>
+  <si>
+    <t>FFC GiA - 2025/26</t>
+  </si>
+  <si>
+    <t>FFC GiA - 2026/27</t>
+  </si>
+  <si>
+    <t>FFC GiA - 2027/28</t>
+  </si>
+  <si>
+    <t>FFC GiA - 2028/29</t>
+  </si>
+  <si>
+    <t>FFC GiA - 2029/30</t>
+  </si>
+  <si>
+    <t>FFC GiA - 2030/31</t>
+  </si>
+  <si>
+    <t>FFC GiA - 2031/32</t>
+  </si>
+  <si>
+    <t>FFC GiA - 2032/33</t>
+  </si>
+  <si>
+    <t>OTHER GiA - 2023/24</t>
+  </si>
+  <si>
+    <t>OTHER GiA - 2024/25</t>
+  </si>
+  <si>
+    <t>OTHER GiA - 2025/26</t>
+  </si>
+  <si>
+    <t>OTHER GiA - 2026/27</t>
+  </si>
+  <si>
+    <t>OTHER GiA - 2027/28</t>
+  </si>
+  <si>
+    <t>OTHER GiA - 2028/29</t>
+  </si>
+  <si>
+    <t>OTHER GiA - 2029/30</t>
+  </si>
+  <si>
+    <t>OTHER GiA - 2030/31</t>
+  </si>
+  <si>
+    <t>OTHER GiA - 2031/32</t>
+  </si>
+  <si>
+    <t>OTHER GiA - 2032/33</t>
+  </si>
+  <si>
+    <t>Additional FCRM GiA (Other Government department)</t>
+  </si>
+  <si>
+    <t>OGD GiA - 2023/24</t>
+  </si>
+  <si>
+    <t>OGD GiA - 2024/25</t>
+  </si>
+  <si>
+    <t>OGD GiA - 2025/26</t>
+  </si>
+  <si>
+    <t>OGD GiA - 2026/27</t>
+  </si>
+  <si>
+    <t>OGD GiA - 2027/28</t>
+  </si>
+  <si>
+    <t>OGD GiA - 2028/29</t>
+  </si>
+  <si>
+    <t>OGD GiA - 2029/30</t>
+  </si>
+  <si>
+    <t>OGD GiA - 2030/31</t>
+  </si>
+  <si>
+    <t>OGD GiA - 2031/32</t>
+  </si>
+  <si>
+    <t>OGD GiA - 2032/33</t>
+  </si>
+  <si>
+    <t>Additional FCRM GiA (Recovery)</t>
+  </si>
+  <si>
+    <t>REC GiA - 2023/24</t>
+  </si>
+  <si>
+    <t>REC GiA - 2024/25</t>
+  </si>
+  <si>
+    <t>REC GiA - 2025/26</t>
+  </si>
+  <si>
+    <t>REC GiA - 2026/27</t>
+  </si>
+  <si>
+    <t>REC GiA - 2027/28</t>
+  </si>
+  <si>
+    <t>REC GiA - 2028/29</t>
+  </si>
+  <si>
+    <t>REC GiA - 2029/30</t>
+  </si>
+  <si>
+    <t>REC GiA - 2030/31</t>
+  </si>
+  <si>
+    <t>REC GiA - 2031/32</t>
+  </si>
+  <si>
+    <t>REC GiA - 2032/33</t>
+  </si>
+  <si>
+    <t>Additional FCRM GiA (Summer economic fund)</t>
+  </si>
+  <si>
+    <t>SEF GiA - 2023/24</t>
+  </si>
+  <si>
+    <t>SEF GiA - 2024/25</t>
+  </si>
+  <si>
+    <t>SEF GiA - 2025/26</t>
+  </si>
+  <si>
+    <t>SEF GiA - 2026/27</t>
+  </si>
+  <si>
+    <t>SEF GiA - 2027/28</t>
+  </si>
+  <si>
+    <t>SEF GiA - 2028/29</t>
+  </si>
+  <si>
+    <t>SEF GiA - 2029/30</t>
+  </si>
+  <si>
+    <t>SEF GiA - 2030/31</t>
+  </si>
+  <si>
+    <t>SEF GiA - 2031/32</t>
+  </si>
+  <si>
+    <t>SEF GiA - 2032/33</t>
   </si>
 </sst>
 </file>
@@ -1251,12 +1482,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="47"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor indexed="43"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1306,6 +1531,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1471,7 +1702,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1489,7 +1720,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1583,7 +1814,7 @@
     <xf numFmtId="3" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1623,41 +1854,92 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="11" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1668,64 +1950,25 @@
     <xf numFmtId="0" fontId="5" fillId="13" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="11" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2032,14 +2275,14 @@
     <tabColor rgb="FF92D050"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:KG7"/>
+  <dimension ref="A1:MY7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="BQ7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="Z7" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
       <selection pane="topRight" activeCell="C7" sqref="C7"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="BT7" sqref="BT7"/>
+      <selection pane="bottomRight" activeCell="BT8" sqref="BT8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2056,22 +2299,22 @@
     <col min="22" max="23" width="21" style="4" customWidth="1"/>
     <col min="24" max="31" width="21" style="1" customWidth="1"/>
     <col min="32" max="37" width="21" style="5" customWidth="1"/>
-    <col min="38" max="278" width="21" style="1" customWidth="1"/>
-    <col min="279" max="285" width="21" style="6" customWidth="1"/>
-    <col min="286" max="288" width="22.33203125" style="6" customWidth="1"/>
-    <col min="289" max="289" width="17.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="290" max="290" width="19.6640625" style="6" customWidth="1"/>
-    <col min="291" max="291" width="21.5546875" style="6" customWidth="1"/>
-    <col min="292" max="292" width="19.6640625" style="6" customWidth="1"/>
-    <col min="293" max="293" width="21.5546875" style="6" customWidth="1"/>
-    <col min="294" max="16384" width="8.6640625" style="6"/>
+    <col min="38" max="348" width="21" style="1" customWidth="1"/>
+    <col min="349" max="355" width="21" style="6" customWidth="1"/>
+    <col min="356" max="358" width="22.33203125" style="6" customWidth="1"/>
+    <col min="359" max="359" width="17.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="360" max="360" width="19.6640625" style="6" customWidth="1"/>
+    <col min="361" max="361" width="21.5546875" style="6" customWidth="1"/>
+    <col min="362" max="362" width="19.6640625" style="6" customWidth="1"/>
+    <col min="363" max="363" width="21.5546875" style="6" customWidth="1"/>
+    <col min="364" max="16384" width="8.6640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:293" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="77" t="s">
+    <row r="1" spans="1:363" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="77"/>
+      <c r="B1" s="63"/>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
       <c r="E1" s="20"/>
@@ -2155,70 +2398,70 @@
       <c r="CE1" s="19"/>
       <c r="CF1" s="19"/>
       <c r="CG1" s="19"/>
-      <c r="CH1" s="19"/>
-      <c r="CI1" s="19"/>
-      <c r="CJ1" s="19"/>
-      <c r="CK1" s="19"/>
+      <c r="CH1" s="26"/>
+      <c r="CI1" s="23"/>
+      <c r="CJ1" s="23"/>
+      <c r="CK1" s="23"/>
       <c r="CL1" s="19"/>
       <c r="CM1" s="19"/>
       <c r="CN1" s="19"/>
       <c r="CO1" s="19"/>
       <c r="CP1" s="19"/>
       <c r="CQ1" s="19"/>
-      <c r="CR1" s="19"/>
-      <c r="CS1" s="19"/>
-      <c r="CT1" s="19"/>
-      <c r="CU1" s="19"/>
+      <c r="CR1" s="26"/>
+      <c r="CS1" s="23"/>
+      <c r="CT1" s="23"/>
+      <c r="CU1" s="23"/>
       <c r="CV1" s="19"/>
       <c r="CW1" s="19"/>
       <c r="CX1" s="19"/>
       <c r="CY1" s="19"/>
       <c r="CZ1" s="19"/>
       <c r="DA1" s="19"/>
-      <c r="DB1" s="19"/>
-      <c r="DC1" s="19"/>
-      <c r="DD1" s="19"/>
-      <c r="DE1" s="19"/>
+      <c r="DB1" s="26"/>
+      <c r="DC1" s="23"/>
+      <c r="DD1" s="23"/>
+      <c r="DE1" s="23"/>
       <c r="DF1" s="19"/>
       <c r="DG1" s="19"/>
       <c r="DH1" s="19"/>
       <c r="DI1" s="19"/>
       <c r="DJ1" s="19"/>
       <c r="DK1" s="19"/>
-      <c r="DL1" s="19"/>
-      <c r="DM1" s="19"/>
-      <c r="DN1" s="19"/>
-      <c r="DO1" s="19"/>
+      <c r="DL1" s="26"/>
+      <c r="DM1" s="23"/>
+      <c r="DN1" s="23"/>
+      <c r="DO1" s="23"/>
       <c r="DP1" s="19"/>
       <c r="DQ1" s="19"/>
       <c r="DR1" s="19"/>
       <c r="DS1" s="19"/>
       <c r="DT1" s="19"/>
       <c r="DU1" s="19"/>
-      <c r="DV1" s="19"/>
-      <c r="DW1" s="19"/>
-      <c r="DX1" s="19"/>
-      <c r="DY1" s="19"/>
+      <c r="DV1" s="26"/>
+      <c r="DW1" s="23"/>
+      <c r="DX1" s="23"/>
+      <c r="DY1" s="23"/>
       <c r="DZ1" s="19"/>
       <c r="EA1" s="19"/>
       <c r="EB1" s="19"/>
       <c r="EC1" s="19"/>
       <c r="ED1" s="19"/>
       <c r="EE1" s="19"/>
-      <c r="EF1" s="19"/>
-      <c r="EG1" s="19"/>
-      <c r="EH1" s="19"/>
-      <c r="EI1" s="19"/>
+      <c r="EF1" s="26"/>
+      <c r="EG1" s="23"/>
+      <c r="EH1" s="23"/>
+      <c r="EI1" s="23"/>
       <c r="EJ1" s="19"/>
       <c r="EK1" s="19"/>
       <c r="EL1" s="19"/>
       <c r="EM1" s="19"/>
       <c r="EN1" s="19"/>
       <c r="EO1" s="19"/>
-      <c r="EP1" s="19"/>
-      <c r="EQ1" s="19"/>
-      <c r="ER1" s="19"/>
-      <c r="ES1" s="19"/>
+      <c r="EP1" s="26"/>
+      <c r="EQ1" s="23"/>
+      <c r="ER1" s="23"/>
+      <c r="ES1" s="23"/>
       <c r="ET1" s="19"/>
       <c r="EU1" s="19"/>
       <c r="EV1" s="19"/>
@@ -2348,27 +2591,97 @@
       <c r="JP1" s="19"/>
       <c r="JQ1" s="19"/>
       <c r="JR1" s="19"/>
-      <c r="JS1" s="28"/>
-      <c r="JT1" s="28"/>
-      <c r="JU1" s="28"/>
-      <c r="JV1" s="28"/>
-      <c r="JW1" s="28"/>
-      <c r="JX1" s="28"/>
-      <c r="JY1" s="28"/>
-      <c r="JZ1" s="39"/>
-      <c r="KA1" s="39"/>
-      <c r="KB1" s="39"/>
-      <c r="KC1" s="39"/>
-      <c r="KD1" s="39"/>
-      <c r="KE1" s="39"/>
-      <c r="KF1" s="39"/>
-      <c r="KG1" s="39"/>
+      <c r="JS1" s="19"/>
+      <c r="JT1" s="19"/>
+      <c r="JU1" s="19"/>
+      <c r="JV1" s="19"/>
+      <c r="JW1" s="19"/>
+      <c r="JX1" s="19"/>
+      <c r="JY1" s="19"/>
+      <c r="JZ1" s="19"/>
+      <c r="KA1" s="19"/>
+      <c r="KB1" s="19"/>
+      <c r="KC1" s="19"/>
+      <c r="KD1" s="19"/>
+      <c r="KE1" s="19"/>
+      <c r="KF1" s="19"/>
+      <c r="KG1" s="19"/>
+      <c r="KH1" s="19"/>
+      <c r="KI1" s="19"/>
+      <c r="KJ1" s="19"/>
+      <c r="KK1" s="19"/>
+      <c r="KL1" s="19"/>
+      <c r="KM1" s="19"/>
+      <c r="KN1" s="19"/>
+      <c r="KO1" s="19"/>
+      <c r="KP1" s="19"/>
+      <c r="KQ1" s="19"/>
+      <c r="KR1" s="19"/>
+      <c r="KS1" s="19"/>
+      <c r="KT1" s="19"/>
+      <c r="KU1" s="19"/>
+      <c r="KV1" s="19"/>
+      <c r="KW1" s="19"/>
+      <c r="KX1" s="19"/>
+      <c r="KY1" s="19"/>
+      <c r="KZ1" s="19"/>
+      <c r="LA1" s="19"/>
+      <c r="LB1" s="19"/>
+      <c r="LC1" s="19"/>
+      <c r="LD1" s="19"/>
+      <c r="LE1" s="19"/>
+      <c r="LF1" s="19"/>
+      <c r="LG1" s="19"/>
+      <c r="LH1" s="19"/>
+      <c r="LI1" s="19"/>
+      <c r="LJ1" s="19"/>
+      <c r="LK1" s="19"/>
+      <c r="LL1" s="19"/>
+      <c r="LM1" s="19"/>
+      <c r="LN1" s="19"/>
+      <c r="LO1" s="19"/>
+      <c r="LP1" s="19"/>
+      <c r="LQ1" s="19"/>
+      <c r="LR1" s="19"/>
+      <c r="LS1" s="19"/>
+      <c r="LT1" s="19"/>
+      <c r="LU1" s="19"/>
+      <c r="LV1" s="19"/>
+      <c r="LW1" s="19"/>
+      <c r="LX1" s="19"/>
+      <c r="LY1" s="19"/>
+      <c r="LZ1" s="19"/>
+      <c r="MA1" s="19"/>
+      <c r="MB1" s="19"/>
+      <c r="MC1" s="19"/>
+      <c r="MD1" s="19"/>
+      <c r="ME1" s="19"/>
+      <c r="MF1" s="19"/>
+      <c r="MG1" s="19"/>
+      <c r="MH1" s="19"/>
+      <c r="MI1" s="19"/>
+      <c r="MJ1" s="19"/>
+      <c r="MK1" s="28"/>
+      <c r="ML1" s="28"/>
+      <c r="MM1" s="28"/>
+      <c r="MN1" s="28"/>
+      <c r="MO1" s="28"/>
+      <c r="MP1" s="28"/>
+      <c r="MQ1" s="28"/>
+      <c r="MR1" s="39"/>
+      <c r="MS1" s="39"/>
+      <c r="MT1" s="39"/>
+      <c r="MU1" s="39"/>
+      <c r="MV1" s="39"/>
+      <c r="MW1" s="39"/>
+      <c r="MX1" s="39"/>
+      <c r="MY1" s="39"/>
     </row>
-    <row r="2" spans="1:293" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="78" t="s">
+    <row r="2" spans="1:363" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="64" t="s">
         <v>175</v>
       </c>
-      <c r="B2" s="78"/>
+      <c r="B2" s="64"/>
       <c r="C2" s="19"/>
       <c r="D2" s="29"/>
       <c r="E2" s="20"/>
@@ -2450,75 +2763,75 @@
       <c r="CC2" s="27"/>
       <c r="CD2" s="27"/>
       <c r="CE2" s="19"/>
-      <c r="CF2" s="19"/>
-      <c r="CG2" s="19"/>
-      <c r="CH2" s="19"/>
-      <c r="CI2" s="19"/>
-      <c r="CJ2" s="19"/>
-      <c r="CK2" s="19"/>
+      <c r="CF2" s="30"/>
+      <c r="CG2" s="30"/>
+      <c r="CH2" s="23"/>
+      <c r="CI2" s="23"/>
+      <c r="CJ2" s="23"/>
+      <c r="CK2" s="23"/>
       <c r="CL2" s="19"/>
-      <c r="CM2" s="19"/>
-      <c r="CN2" s="19"/>
+      <c r="CM2" s="27"/>
+      <c r="CN2" s="27"/>
       <c r="CO2" s="19"/>
-      <c r="CP2" s="19"/>
-      <c r="CQ2" s="19"/>
-      <c r="CR2" s="19"/>
-      <c r="CS2" s="19"/>
-      <c r="CT2" s="19"/>
-      <c r="CU2" s="19"/>
+      <c r="CP2" s="30"/>
+      <c r="CQ2" s="30"/>
+      <c r="CR2" s="23"/>
+      <c r="CS2" s="23"/>
+      <c r="CT2" s="23"/>
+      <c r="CU2" s="23"/>
       <c r="CV2" s="19"/>
-      <c r="CW2" s="19"/>
-      <c r="CX2" s="19"/>
+      <c r="CW2" s="27"/>
+      <c r="CX2" s="27"/>
       <c r="CY2" s="19"/>
-      <c r="CZ2" s="19"/>
-      <c r="DA2" s="19"/>
-      <c r="DB2" s="19"/>
-      <c r="DC2" s="19"/>
-      <c r="DD2" s="19"/>
-      <c r="DE2" s="19"/>
+      <c r="CZ2" s="30"/>
+      <c r="DA2" s="30"/>
+      <c r="DB2" s="23"/>
+      <c r="DC2" s="23"/>
+      <c r="DD2" s="23"/>
+      <c r="DE2" s="23"/>
       <c r="DF2" s="19"/>
-      <c r="DG2" s="19"/>
-      <c r="DH2" s="19"/>
+      <c r="DG2" s="27"/>
+      <c r="DH2" s="27"/>
       <c r="DI2" s="19"/>
-      <c r="DJ2" s="19"/>
-      <c r="DK2" s="19"/>
-      <c r="DL2" s="19"/>
-      <c r="DM2" s="19"/>
-      <c r="DN2" s="19"/>
-      <c r="DO2" s="19"/>
+      <c r="DJ2" s="30"/>
+      <c r="DK2" s="30"/>
+      <c r="DL2" s="23"/>
+      <c r="DM2" s="23"/>
+      <c r="DN2" s="23"/>
+      <c r="DO2" s="23"/>
       <c r="DP2" s="19"/>
-      <c r="DQ2" s="19"/>
-      <c r="DR2" s="19"/>
+      <c r="DQ2" s="27"/>
+      <c r="DR2" s="27"/>
       <c r="DS2" s="19"/>
-      <c r="DT2" s="19"/>
-      <c r="DU2" s="19"/>
-      <c r="DV2" s="19"/>
-      <c r="DW2" s="19"/>
-      <c r="DX2" s="19"/>
-      <c r="DY2" s="19"/>
+      <c r="DT2" s="30"/>
+      <c r="DU2" s="30"/>
+      <c r="DV2" s="23"/>
+      <c r="DW2" s="23"/>
+      <c r="DX2" s="23"/>
+      <c r="DY2" s="23"/>
       <c r="DZ2" s="19"/>
-      <c r="EA2" s="19"/>
-      <c r="EB2" s="19"/>
+      <c r="EA2" s="27"/>
+      <c r="EB2" s="27"/>
       <c r="EC2" s="19"/>
-      <c r="ED2" s="19"/>
-      <c r="EE2" s="19"/>
-      <c r="EF2" s="19"/>
-      <c r="EG2" s="19"/>
-      <c r="EH2" s="19"/>
-      <c r="EI2" s="19"/>
+      <c r="ED2" s="30"/>
+      <c r="EE2" s="30"/>
+      <c r="EF2" s="23"/>
+      <c r="EG2" s="23"/>
+      <c r="EH2" s="23"/>
+      <c r="EI2" s="23"/>
       <c r="EJ2" s="19"/>
-      <c r="EK2" s="19"/>
-      <c r="EL2" s="19"/>
+      <c r="EK2" s="27"/>
+      <c r="EL2" s="27"/>
       <c r="EM2" s="19"/>
-      <c r="EN2" s="19"/>
-      <c r="EO2" s="19"/>
-      <c r="EP2" s="19"/>
-      <c r="EQ2" s="19"/>
-      <c r="ER2" s="19"/>
-      <c r="ES2" s="19"/>
+      <c r="EN2" s="30"/>
+      <c r="EO2" s="30"/>
+      <c r="EP2" s="23"/>
+      <c r="EQ2" s="23"/>
+      <c r="ER2" s="23"/>
+      <c r="ES2" s="23"/>
       <c r="ET2" s="19"/>
-      <c r="EU2" s="19"/>
-      <c r="EV2" s="19"/>
+      <c r="EU2" s="27"/>
+      <c r="EV2" s="27"/>
       <c r="EW2" s="19"/>
       <c r="EX2" s="19"/>
       <c r="EY2" s="19"/>
@@ -2645,23 +2958,93 @@
       <c r="JP2" s="19"/>
       <c r="JQ2" s="19"/>
       <c r="JR2" s="19"/>
-      <c r="JS2" s="29"/>
-      <c r="JT2" s="29"/>
-      <c r="JU2" s="29"/>
-      <c r="JV2" s="29"/>
-      <c r="JW2" s="29"/>
-      <c r="JX2" s="29"/>
-      <c r="JY2" s="29"/>
-      <c r="JZ2" s="39"/>
-      <c r="KA2" s="39"/>
-      <c r="KB2" s="39"/>
-      <c r="KC2" s="39"/>
-      <c r="KD2" s="39"/>
-      <c r="KE2" s="39"/>
-      <c r="KF2" s="39"/>
-      <c r="KG2" s="39"/>
+      <c r="JS2" s="19"/>
+      <c r="JT2" s="19"/>
+      <c r="JU2" s="19"/>
+      <c r="JV2" s="19"/>
+      <c r="JW2" s="19"/>
+      <c r="JX2" s="19"/>
+      <c r="JY2" s="19"/>
+      <c r="JZ2" s="19"/>
+      <c r="KA2" s="19"/>
+      <c r="KB2" s="19"/>
+      <c r="KC2" s="19"/>
+      <c r="KD2" s="19"/>
+      <c r="KE2" s="19"/>
+      <c r="KF2" s="19"/>
+      <c r="KG2" s="19"/>
+      <c r="KH2" s="19"/>
+      <c r="KI2" s="19"/>
+      <c r="KJ2" s="19"/>
+      <c r="KK2" s="19"/>
+      <c r="KL2" s="19"/>
+      <c r="KM2" s="19"/>
+      <c r="KN2" s="19"/>
+      <c r="KO2" s="19"/>
+      <c r="KP2" s="19"/>
+      <c r="KQ2" s="19"/>
+      <c r="KR2" s="19"/>
+      <c r="KS2" s="19"/>
+      <c r="KT2" s="19"/>
+      <c r="KU2" s="19"/>
+      <c r="KV2" s="19"/>
+      <c r="KW2" s="19"/>
+      <c r="KX2" s="19"/>
+      <c r="KY2" s="19"/>
+      <c r="KZ2" s="19"/>
+      <c r="LA2" s="19"/>
+      <c r="LB2" s="19"/>
+      <c r="LC2" s="19"/>
+      <c r="LD2" s="19"/>
+      <c r="LE2" s="19"/>
+      <c r="LF2" s="19"/>
+      <c r="LG2" s="19"/>
+      <c r="LH2" s="19"/>
+      <c r="LI2" s="19"/>
+      <c r="LJ2" s="19"/>
+      <c r="LK2" s="19"/>
+      <c r="LL2" s="19"/>
+      <c r="LM2" s="19"/>
+      <c r="LN2" s="19"/>
+      <c r="LO2" s="19"/>
+      <c r="LP2" s="19"/>
+      <c r="LQ2" s="19"/>
+      <c r="LR2" s="19"/>
+      <c r="LS2" s="19"/>
+      <c r="LT2" s="19"/>
+      <c r="LU2" s="19"/>
+      <c r="LV2" s="19"/>
+      <c r="LW2" s="19"/>
+      <c r="LX2" s="19"/>
+      <c r="LY2" s="19"/>
+      <c r="LZ2" s="19"/>
+      <c r="MA2" s="19"/>
+      <c r="MB2" s="19"/>
+      <c r="MC2" s="19"/>
+      <c r="MD2" s="19"/>
+      <c r="ME2" s="19"/>
+      <c r="MF2" s="19"/>
+      <c r="MG2" s="19"/>
+      <c r="MH2" s="19"/>
+      <c r="MI2" s="19"/>
+      <c r="MJ2" s="19"/>
+      <c r="MK2" s="29"/>
+      <c r="ML2" s="29"/>
+      <c r="MM2" s="29"/>
+      <c r="MN2" s="29"/>
+      <c r="MO2" s="29"/>
+      <c r="MP2" s="29"/>
+      <c r="MQ2" s="29"/>
+      <c r="MR2" s="39"/>
+      <c r="MS2" s="39"/>
+      <c r="MT2" s="39"/>
+      <c r="MU2" s="39"/>
+      <c r="MV2" s="39"/>
+      <c r="MW2" s="39"/>
+      <c r="MX2" s="39"/>
+      <c r="MY2" s="39"/>
     </row>
-    <row r="3" spans="1:293" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:363" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="31"/>
       <c r="B3" s="32"/>
       <c r="C3" s="32"/>
@@ -2947,108 +3330,178 @@
       <c r="JW3" s="37"/>
       <c r="JX3" s="37"/>
       <c r="JY3" s="37"/>
-      <c r="JZ3" s="39"/>
-      <c r="KA3" s="39"/>
-      <c r="KB3" s="39"/>
-      <c r="KC3" s="39"/>
-      <c r="KD3" s="39"/>
-      <c r="KE3" s="39"/>
-      <c r="KF3" s="39"/>
-      <c r="KG3" s="39"/>
+      <c r="JZ3" s="37"/>
+      <c r="KA3" s="37"/>
+      <c r="KB3" s="37"/>
+      <c r="KC3" s="37"/>
+      <c r="KD3" s="37"/>
+      <c r="KE3" s="37"/>
+      <c r="KF3" s="37"/>
+      <c r="KG3" s="37"/>
+      <c r="KH3" s="37"/>
+      <c r="KI3" s="37"/>
+      <c r="KJ3" s="37"/>
+      <c r="KK3" s="37"/>
+      <c r="KL3" s="37"/>
+      <c r="KM3" s="37"/>
+      <c r="KN3" s="37"/>
+      <c r="KO3" s="37"/>
+      <c r="KP3" s="37"/>
+      <c r="KQ3" s="37"/>
+      <c r="KR3" s="37"/>
+      <c r="KS3" s="37"/>
+      <c r="KT3" s="37"/>
+      <c r="KU3" s="37"/>
+      <c r="KV3" s="37"/>
+      <c r="KW3" s="37"/>
+      <c r="KX3" s="37"/>
+      <c r="KY3" s="37"/>
+      <c r="KZ3" s="37"/>
+      <c r="LA3" s="37"/>
+      <c r="LB3" s="37"/>
+      <c r="LC3" s="37"/>
+      <c r="LD3" s="37"/>
+      <c r="LE3" s="37"/>
+      <c r="LF3" s="37"/>
+      <c r="LG3" s="37"/>
+      <c r="LH3" s="37"/>
+      <c r="LI3" s="37"/>
+      <c r="LJ3" s="37"/>
+      <c r="LK3" s="37"/>
+      <c r="LL3" s="37"/>
+      <c r="LM3" s="37"/>
+      <c r="LN3" s="37"/>
+      <c r="LO3" s="37"/>
+      <c r="LP3" s="37"/>
+      <c r="LQ3" s="37"/>
+      <c r="LR3" s="37"/>
+      <c r="LS3" s="37"/>
+      <c r="LT3" s="37"/>
+      <c r="LU3" s="37"/>
+      <c r="LV3" s="37"/>
+      <c r="LW3" s="37"/>
+      <c r="LX3" s="37"/>
+      <c r="LY3" s="37"/>
+      <c r="LZ3" s="37"/>
+      <c r="MA3" s="37"/>
+      <c r="MB3" s="37"/>
+      <c r="MC3" s="37"/>
+      <c r="MD3" s="37"/>
+      <c r="ME3" s="37"/>
+      <c r="MF3" s="37"/>
+      <c r="MG3" s="37"/>
+      <c r="MH3" s="37"/>
+      <c r="MI3" s="37"/>
+      <c r="MJ3" s="37"/>
+      <c r="MK3" s="37"/>
+      <c r="ML3" s="37"/>
+      <c r="MM3" s="37"/>
+      <c r="MN3" s="37"/>
+      <c r="MO3" s="37"/>
+      <c r="MP3" s="37"/>
+      <c r="MQ3" s="37"/>
+      <c r="MR3" s="39"/>
+      <c r="MS3" s="39"/>
+      <c r="MT3" s="39"/>
+      <c r="MU3" s="39"/>
+      <c r="MV3" s="39"/>
+      <c r="MW3" s="39"/>
+      <c r="MX3" s="39"/>
+      <c r="MY3" s="39"/>
     </row>
-    <row r="4" spans="1:293" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="79" t="s">
+    <row r="4" spans="1:363" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="79"/>
-      <c r="C4" s="80" t="s">
+      <c r="B4" s="65"/>
+      <c r="C4" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
-      <c r="F4" s="80"/>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80"/>
-      <c r="I4" s="81" t="s">
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="81"/>
-      <c r="K4" s="81"/>
-      <c r="L4" s="81"/>
-      <c r="M4" s="82" t="s">
+      <c r="J4" s="67"/>
+      <c r="K4" s="67"/>
+      <c r="L4" s="67"/>
+      <c r="M4" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="N4" s="82"/>
-      <c r="O4" s="82"/>
-      <c r="P4" s="83" t="s">
+      <c r="N4" s="68"/>
+      <c r="O4" s="68"/>
+      <c r="P4" s="69" t="s">
         <v>333</v>
       </c>
-      <c r="Q4" s="83"/>
-      <c r="R4" s="83"/>
-      <c r="S4" s="83"/>
-      <c r="T4" s="83"/>
-      <c r="U4" s="84" t="s">
+      <c r="Q4" s="69"/>
+      <c r="R4" s="69"/>
+      <c r="S4" s="69"/>
+      <c r="T4" s="69"/>
+      <c r="U4" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="V4" s="84"/>
-      <c r="W4" s="84"/>
-      <c r="X4" s="84"/>
-      <c r="Y4" s="84"/>
-      <c r="Z4" s="84"/>
-      <c r="AA4" s="84"/>
-      <c r="AB4" s="85" t="s">
+      <c r="V4" s="70"/>
+      <c r="W4" s="70"/>
+      <c r="X4" s="70"/>
+      <c r="Y4" s="70"/>
+      <c r="Z4" s="70"/>
+      <c r="AA4" s="70"/>
+      <c r="AB4" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="AC4" s="85"/>
-      <c r="AD4" s="85"/>
-      <c r="AE4" s="76" t="s">
+      <c r="AC4" s="71"/>
+      <c r="AD4" s="71"/>
+      <c r="AE4" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="AF4" s="76"/>
-      <c r="AG4" s="86"/>
-      <c r="AH4" s="86"/>
-      <c r="AI4" s="86"/>
-      <c r="AJ4" s="86"/>
-      <c r="AK4" s="86"/>
-      <c r="AL4" s="87" t="s">
+      <c r="AF4" s="62"/>
+      <c r="AG4" s="73"/>
+      <c r="AH4" s="73"/>
+      <c r="AI4" s="73"/>
+      <c r="AJ4" s="73"/>
+      <c r="AK4" s="73"/>
+      <c r="AL4" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="AM4" s="87"/>
-      <c r="AN4" s="87"/>
-      <c r="AO4" s="87"/>
-      <c r="AP4" s="87"/>
-      <c r="AQ4" s="87"/>
-      <c r="AR4" s="87"/>
-      <c r="AS4" s="87"/>
-      <c r="AT4" s="87"/>
-      <c r="AU4" s="87"/>
-      <c r="AV4" s="87"/>
-      <c r="AW4" s="87"/>
-      <c r="AX4" s="87"/>
-      <c r="AY4" s="87"/>
-      <c r="AZ4" s="87"/>
-      <c r="BA4" s="87"/>
-      <c r="BB4" s="87"/>
-      <c r="BC4" s="87"/>
-      <c r="BD4" s="87"/>
-      <c r="BE4" s="87"/>
-      <c r="BF4" s="87"/>
-      <c r="BG4" s="87"/>
-      <c r="BH4" s="87"/>
-      <c r="BI4" s="87"/>
-      <c r="BJ4" s="87"/>
-      <c r="BK4" s="65" t="s">
+      <c r="AM4" s="74"/>
+      <c r="AN4" s="74"/>
+      <c r="AO4" s="74"/>
+      <c r="AP4" s="74"/>
+      <c r="AQ4" s="74"/>
+      <c r="AR4" s="74"/>
+      <c r="AS4" s="74"/>
+      <c r="AT4" s="74"/>
+      <c r="AU4" s="74"/>
+      <c r="AV4" s="74"/>
+      <c r="AW4" s="74"/>
+      <c r="AX4" s="74"/>
+      <c r="AY4" s="74"/>
+      <c r="AZ4" s="74"/>
+      <c r="BA4" s="74"/>
+      <c r="BB4" s="74"/>
+      <c r="BC4" s="74"/>
+      <c r="BD4" s="74"/>
+      <c r="BE4" s="74"/>
+      <c r="BF4" s="74"/>
+      <c r="BG4" s="74"/>
+      <c r="BH4" s="74"/>
+      <c r="BI4" s="74"/>
+      <c r="BJ4" s="74"/>
+      <c r="BK4" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="BL4" s="65"/>
-      <c r="BM4" s="65"/>
-      <c r="BN4" s="65"/>
-      <c r="BO4" s="65"/>
-      <c r="BP4" s="65"/>
-      <c r="BQ4" s="65"/>
-      <c r="BR4" s="65"/>
-      <c r="BS4" s="65"/>
-      <c r="BT4" s="65"/>
+      <c r="BL4" s="72"/>
+      <c r="BM4" s="72"/>
+      <c r="BN4" s="72"/>
+      <c r="BO4" s="72"/>
+      <c r="BP4" s="72"/>
+      <c r="BQ4" s="72"/>
+      <c r="BR4" s="72"/>
+      <c r="BS4" s="72"/>
+      <c r="BT4" s="72"/>
       <c r="BU4" s="88" t="s">
         <v>10</v>
       </c>
@@ -3061,325 +3514,409 @@
       <c r="CB4" s="88"/>
       <c r="CC4" s="88"/>
       <c r="CD4" s="88"/>
-      <c r="CE4" s="71" t="s">
+      <c r="CE4" s="89" t="s">
+        <v>334</v>
+      </c>
+      <c r="CF4" s="89"/>
+      <c r="CG4" s="89"/>
+      <c r="CH4" s="89"/>
+      <c r="CI4" s="89"/>
+      <c r="CJ4" s="89"/>
+      <c r="CK4" s="89"/>
+      <c r="CL4" s="89"/>
+      <c r="CM4" s="89"/>
+      <c r="CN4" s="89"/>
+      <c r="CO4" s="88" t="s">
+        <v>335</v>
+      </c>
+      <c r="CP4" s="88"/>
+      <c r="CQ4" s="88"/>
+      <c r="CR4" s="88"/>
+      <c r="CS4" s="88"/>
+      <c r="CT4" s="88"/>
+      <c r="CU4" s="88"/>
+      <c r="CV4" s="88"/>
+      <c r="CW4" s="88"/>
+      <c r="CX4" s="88"/>
+      <c r="CY4" s="89" t="s">
+        <v>336</v>
+      </c>
+      <c r="CZ4" s="89"/>
+      <c r="DA4" s="89"/>
+      <c r="DB4" s="89"/>
+      <c r="DC4" s="89"/>
+      <c r="DD4" s="89"/>
+      <c r="DE4" s="89"/>
+      <c r="DF4" s="89"/>
+      <c r="DG4" s="89"/>
+      <c r="DH4" s="89"/>
+      <c r="DI4" s="88" t="s">
+        <v>337</v>
+      </c>
+      <c r="DJ4" s="88"/>
+      <c r="DK4" s="88"/>
+      <c r="DL4" s="88"/>
+      <c r="DM4" s="88"/>
+      <c r="DN4" s="88"/>
+      <c r="DO4" s="88"/>
+      <c r="DP4" s="88"/>
+      <c r="DQ4" s="88"/>
+      <c r="DR4" s="88"/>
+      <c r="DS4" s="90" t="s">
+        <v>378</v>
+      </c>
+      <c r="DT4" s="91"/>
+      <c r="DU4" s="91"/>
+      <c r="DV4" s="91"/>
+      <c r="DW4" s="91"/>
+      <c r="DX4" s="91"/>
+      <c r="DY4" s="91"/>
+      <c r="DZ4" s="91"/>
+      <c r="EA4" s="91"/>
+      <c r="EB4" s="92"/>
+      <c r="EC4" s="88" t="s">
+        <v>389</v>
+      </c>
+      <c r="ED4" s="88"/>
+      <c r="EE4" s="88"/>
+      <c r="EF4" s="88"/>
+      <c r="EG4" s="88"/>
+      <c r="EH4" s="88"/>
+      <c r="EI4" s="88"/>
+      <c r="EJ4" s="88"/>
+      <c r="EK4" s="88"/>
+      <c r="EL4" s="88"/>
+      <c r="EM4" s="90" t="s">
+        <v>400</v>
+      </c>
+      <c r="EN4" s="91"/>
+      <c r="EO4" s="91"/>
+      <c r="EP4" s="91"/>
+      <c r="EQ4" s="91"/>
+      <c r="ER4" s="91"/>
+      <c r="ES4" s="91"/>
+      <c r="ET4" s="91"/>
+      <c r="EU4" s="91"/>
+      <c r="EV4" s="92"/>
+      <c r="EW4" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="CF4" s="71"/>
-      <c r="CG4" s="71"/>
-      <c r="CH4" s="71"/>
-      <c r="CI4" s="71"/>
-      <c r="CJ4" s="71"/>
-      <c r="CK4" s="71"/>
-      <c r="CL4" s="71"/>
-      <c r="CM4" s="71"/>
-      <c r="CN4" s="71"/>
-      <c r="CO4" s="72" t="s">
+      <c r="EX4" s="75"/>
+      <c r="EY4" s="75"/>
+      <c r="EZ4" s="75"/>
+      <c r="FA4" s="75"/>
+      <c r="FB4" s="75"/>
+      <c r="FC4" s="75"/>
+      <c r="FD4" s="75"/>
+      <c r="FE4" s="75"/>
+      <c r="FF4" s="75"/>
+      <c r="FG4" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="CP4" s="72"/>
-      <c r="CQ4" s="72"/>
-      <c r="CR4" s="72"/>
-      <c r="CS4" s="72"/>
-      <c r="CT4" s="72"/>
-      <c r="CU4" s="72"/>
-      <c r="CV4" s="72"/>
-      <c r="CW4" s="72"/>
-      <c r="CX4" s="72"/>
-      <c r="CY4" s="73" t="s">
+      <c r="FH4" s="76"/>
+      <c r="FI4" s="76"/>
+      <c r="FJ4" s="76"/>
+      <c r="FK4" s="76"/>
+      <c r="FL4" s="76"/>
+      <c r="FM4" s="76"/>
+      <c r="FN4" s="76"/>
+      <c r="FO4" s="76"/>
+      <c r="FP4" s="76"/>
+      <c r="FQ4" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="CZ4" s="73"/>
-      <c r="DA4" s="73"/>
-      <c r="DB4" s="73"/>
-      <c r="DC4" s="73"/>
-      <c r="DD4" s="73"/>
-      <c r="DE4" s="73"/>
-      <c r="DF4" s="73"/>
-      <c r="DG4" s="73"/>
-      <c r="DH4" s="73"/>
-      <c r="DI4" s="74" t="s">
+      <c r="FR4" s="77"/>
+      <c r="FS4" s="77"/>
+      <c r="FT4" s="77"/>
+      <c r="FU4" s="77"/>
+      <c r="FV4" s="77"/>
+      <c r="FW4" s="77"/>
+      <c r="FX4" s="77"/>
+      <c r="FY4" s="77"/>
+      <c r="FZ4" s="77"/>
+      <c r="GA4" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="DJ4" s="74"/>
-      <c r="DK4" s="74"/>
-      <c r="DL4" s="74"/>
-      <c r="DM4" s="74"/>
-      <c r="DN4" s="74"/>
-      <c r="DO4" s="74"/>
-      <c r="DP4" s="74"/>
-      <c r="DQ4" s="74"/>
-      <c r="DR4" s="74"/>
-      <c r="DS4" s="75" t="s">
+      <c r="GB4" s="78"/>
+      <c r="GC4" s="78"/>
+      <c r="GD4" s="78"/>
+      <c r="GE4" s="78"/>
+      <c r="GF4" s="78"/>
+      <c r="GG4" s="78"/>
+      <c r="GH4" s="78"/>
+      <c r="GI4" s="78"/>
+      <c r="GJ4" s="78"/>
+      <c r="GK4" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="DT4" s="75"/>
-      <c r="DU4" s="75"/>
-      <c r="DV4" s="75"/>
-      <c r="DW4" s="75"/>
-      <c r="DX4" s="75"/>
-      <c r="DY4" s="75"/>
-      <c r="DZ4" s="75"/>
-      <c r="EA4" s="75"/>
-      <c r="EB4" s="75"/>
-      <c r="EC4" s="58" t="s">
+      <c r="GL4" s="79"/>
+      <c r="GM4" s="79"/>
+      <c r="GN4" s="79"/>
+      <c r="GO4" s="79"/>
+      <c r="GP4" s="79"/>
+      <c r="GQ4" s="79"/>
+      <c r="GR4" s="79"/>
+      <c r="GS4" s="79"/>
+      <c r="GT4" s="79"/>
+      <c r="GU4" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="ED4" s="58"/>
-      <c r="EE4" s="58"/>
-      <c r="EF4" s="58"/>
-      <c r="EG4" s="58"/>
-      <c r="EH4" s="58"/>
-      <c r="EI4" s="58"/>
-      <c r="EJ4" s="58"/>
-      <c r="EK4" s="58"/>
-      <c r="EL4" s="58"/>
-      <c r="EM4" s="65" t="s">
+      <c r="GV4" s="80"/>
+      <c r="GW4" s="80"/>
+      <c r="GX4" s="80"/>
+      <c r="GY4" s="80"/>
+      <c r="GZ4" s="80"/>
+      <c r="HA4" s="80"/>
+      <c r="HB4" s="80"/>
+      <c r="HC4" s="80"/>
+      <c r="HD4" s="80"/>
+      <c r="HE4" s="72" t="s">
         <v>178</v>
       </c>
-      <c r="EN4" s="65"/>
-      <c r="EO4" s="65"/>
-      <c r="EP4" s="65"/>
-      <c r="EQ4" s="65"/>
-      <c r="ER4" s="65"/>
-      <c r="ES4" s="65"/>
-      <c r="ET4" s="65"/>
-      <c r="EU4" s="65"/>
-      <c r="EV4" s="65"/>
-      <c r="EW4" s="65" t="s">
+      <c r="HF4" s="72"/>
+      <c r="HG4" s="72"/>
+      <c r="HH4" s="72"/>
+      <c r="HI4" s="72"/>
+      <c r="HJ4" s="72"/>
+      <c r="HK4" s="72"/>
+      <c r="HL4" s="72"/>
+      <c r="HM4" s="72"/>
+      <c r="HN4" s="72"/>
+      <c r="HO4" s="72" t="s">
         <v>189</v>
       </c>
-      <c r="EX4" s="65"/>
-      <c r="EY4" s="65"/>
-      <c r="EZ4" s="65"/>
-      <c r="FA4" s="65"/>
-      <c r="FB4" s="65"/>
-      <c r="FC4" s="65"/>
-      <c r="FD4" s="65"/>
-      <c r="FE4" s="65"/>
-      <c r="FF4" s="65"/>
-      <c r="FG4" s="65" t="s">
+      <c r="HP4" s="72"/>
+      <c r="HQ4" s="72"/>
+      <c r="HR4" s="72"/>
+      <c r="HS4" s="72"/>
+      <c r="HT4" s="72"/>
+      <c r="HU4" s="72"/>
+      <c r="HV4" s="72"/>
+      <c r="HW4" s="72"/>
+      <c r="HX4" s="72"/>
+      <c r="HY4" s="72" t="s">
         <v>200</v>
       </c>
-      <c r="FH4" s="65"/>
-      <c r="FI4" s="65"/>
-      <c r="FJ4" s="65"/>
-      <c r="FK4" s="65"/>
-      <c r="FL4" s="65"/>
-      <c r="FM4" s="65"/>
-      <c r="FN4" s="65"/>
-      <c r="FO4" s="65"/>
-      <c r="FP4" s="65"/>
-      <c r="FQ4" s="65" t="s">
+      <c r="HZ4" s="72"/>
+      <c r="IA4" s="72"/>
+      <c r="IB4" s="72"/>
+      <c r="IC4" s="72"/>
+      <c r="ID4" s="72"/>
+      <c r="IE4" s="72"/>
+      <c r="IF4" s="72"/>
+      <c r="IG4" s="72"/>
+      <c r="IH4" s="72"/>
+      <c r="II4" s="72" t="s">
         <v>211</v>
       </c>
-      <c r="FR4" s="65"/>
-      <c r="FS4" s="65"/>
-      <c r="FT4" s="65"/>
-      <c r="FU4" s="65"/>
-      <c r="FV4" s="65"/>
-      <c r="FW4" s="65"/>
-      <c r="FX4" s="65"/>
-      <c r="FY4" s="65"/>
-      <c r="FZ4" s="65"/>
-      <c r="GA4" s="66" t="s">
+      <c r="IJ4" s="72"/>
+      <c r="IK4" s="72"/>
+      <c r="IL4" s="72"/>
+      <c r="IM4" s="72"/>
+      <c r="IN4" s="72"/>
+      <c r="IO4" s="72"/>
+      <c r="IP4" s="72"/>
+      <c r="IQ4" s="72"/>
+      <c r="IR4" s="72"/>
+      <c r="IS4" s="83" t="s">
         <v>222</v>
       </c>
-      <c r="GB4" s="67"/>
-      <c r="GC4" s="67"/>
-      <c r="GD4" s="67"/>
-      <c r="GE4" s="67"/>
-      <c r="GF4" s="67"/>
-      <c r="GG4" s="67"/>
-      <c r="GH4" s="67"/>
-      <c r="GI4" s="67"/>
-      <c r="GJ4" s="68"/>
-      <c r="GK4" s="66" t="s">
+      <c r="IT4" s="84"/>
+      <c r="IU4" s="84"/>
+      <c r="IV4" s="84"/>
+      <c r="IW4" s="84"/>
+      <c r="IX4" s="84"/>
+      <c r="IY4" s="84"/>
+      <c r="IZ4" s="84"/>
+      <c r="JA4" s="84"/>
+      <c r="JB4" s="85"/>
+      <c r="JC4" s="83" t="s">
         <v>233</v>
       </c>
-      <c r="GL4" s="67"/>
-      <c r="GM4" s="67"/>
-      <c r="GN4" s="67"/>
-      <c r="GO4" s="67"/>
-      <c r="GP4" s="67"/>
-      <c r="GQ4" s="67"/>
-      <c r="GR4" s="67"/>
-      <c r="GS4" s="67"/>
-      <c r="GT4" s="68"/>
-      <c r="GU4" s="66" t="s">
+      <c r="JD4" s="84"/>
+      <c r="JE4" s="84"/>
+      <c r="JF4" s="84"/>
+      <c r="JG4" s="84"/>
+      <c r="JH4" s="84"/>
+      <c r="JI4" s="84"/>
+      <c r="JJ4" s="84"/>
+      <c r="JK4" s="84"/>
+      <c r="JL4" s="85"/>
+      <c r="JM4" s="83" t="s">
         <v>244</v>
       </c>
-      <c r="GV4" s="67"/>
-      <c r="GW4" s="67"/>
-      <c r="GX4" s="67"/>
-      <c r="GY4" s="67"/>
-      <c r="GZ4" s="67"/>
-      <c r="HA4" s="67"/>
-      <c r="HB4" s="67"/>
-      <c r="HC4" s="67"/>
-      <c r="HD4" s="68"/>
-      <c r="HE4" s="66" t="s">
+      <c r="JN4" s="84"/>
+      <c r="JO4" s="84"/>
+      <c r="JP4" s="84"/>
+      <c r="JQ4" s="84"/>
+      <c r="JR4" s="84"/>
+      <c r="JS4" s="84"/>
+      <c r="JT4" s="84"/>
+      <c r="JU4" s="84"/>
+      <c r="JV4" s="85"/>
+      <c r="JW4" s="83" t="s">
         <v>244</v>
       </c>
-      <c r="HF4" s="67"/>
-      <c r="HG4" s="67"/>
-      <c r="HH4" s="67"/>
-      <c r="HI4" s="67"/>
-      <c r="HJ4" s="67"/>
-      <c r="HK4" s="67"/>
-      <c r="HL4" s="67"/>
-      <c r="HM4" s="67"/>
-      <c r="HN4" s="68"/>
-      <c r="HO4" s="66" t="s">
+      <c r="JX4" s="84"/>
+      <c r="JY4" s="84"/>
+      <c r="JZ4" s="84"/>
+      <c r="KA4" s="84"/>
+      <c r="KB4" s="84"/>
+      <c r="KC4" s="84"/>
+      <c r="KD4" s="84"/>
+      <c r="KE4" s="84"/>
+      <c r="KF4" s="85"/>
+      <c r="KG4" s="83" t="s">
         <v>265</v>
       </c>
-      <c r="HP4" s="67"/>
-      <c r="HQ4" s="67"/>
-      <c r="HR4" s="67"/>
-      <c r="HS4" s="67"/>
-      <c r="HT4" s="67"/>
-      <c r="HU4" s="67"/>
-      <c r="HV4" s="67"/>
-      <c r="HW4" s="67"/>
-      <c r="HX4" s="68"/>
-      <c r="HY4" s="69" t="s">
+      <c r="KH4" s="84"/>
+      <c r="KI4" s="84"/>
+      <c r="KJ4" s="84"/>
+      <c r="KK4" s="84"/>
+      <c r="KL4" s="84"/>
+      <c r="KM4" s="84"/>
+      <c r="KN4" s="84"/>
+      <c r="KO4" s="84"/>
+      <c r="KP4" s="85"/>
+      <c r="KQ4" s="86" t="s">
         <v>276</v>
       </c>
-      <c r="HZ4" s="69"/>
-      <c r="IA4" s="69"/>
-      <c r="IB4" s="69"/>
-      <c r="IC4" s="69"/>
-      <c r="ID4" s="69"/>
-      <c r="IE4" s="69"/>
-      <c r="IF4" s="69"/>
-      <c r="IG4" s="69"/>
-      <c r="IH4" s="69"/>
-      <c r="II4" s="69" t="s">
+      <c r="KR4" s="86"/>
+      <c r="KS4" s="86"/>
+      <c r="KT4" s="86"/>
+      <c r="KU4" s="86"/>
+      <c r="KV4" s="86"/>
+      <c r="KW4" s="86"/>
+      <c r="KX4" s="86"/>
+      <c r="KY4" s="86"/>
+      <c r="KZ4" s="86"/>
+      <c r="LA4" s="86" t="s">
         <v>287</v>
       </c>
-      <c r="IJ4" s="69"/>
-      <c r="IK4" s="69"/>
-      <c r="IL4" s="69"/>
-      <c r="IM4" s="69"/>
-      <c r="IN4" s="69"/>
-      <c r="IO4" s="69"/>
-      <c r="IP4" s="69"/>
-      <c r="IQ4" s="69"/>
-      <c r="IR4" s="69"/>
-      <c r="IS4" s="69" t="s">
+      <c r="LB4" s="86"/>
+      <c r="LC4" s="86"/>
+      <c r="LD4" s="86"/>
+      <c r="LE4" s="86"/>
+      <c r="LF4" s="86"/>
+      <c r="LG4" s="86"/>
+      <c r="LH4" s="86"/>
+      <c r="LI4" s="86"/>
+      <c r="LJ4" s="86"/>
+      <c r="LK4" s="86" t="s">
         <v>293</v>
       </c>
-      <c r="IT4" s="69"/>
-      <c r="IU4" s="69"/>
-      <c r="IV4" s="69"/>
-      <c r="IW4" s="69"/>
-      <c r="IX4" s="69"/>
-      <c r="IY4" s="69"/>
-      <c r="IZ4" s="69"/>
-      <c r="JA4" s="69"/>
-      <c r="JB4" s="69"/>
-      <c r="JC4" s="69" t="s">
+      <c r="LL4" s="86"/>
+      <c r="LM4" s="86"/>
+      <c r="LN4" s="86"/>
+      <c r="LO4" s="86"/>
+      <c r="LP4" s="86"/>
+      <c r="LQ4" s="86"/>
+      <c r="LR4" s="86"/>
+      <c r="LS4" s="86"/>
+      <c r="LT4" s="86"/>
+      <c r="LU4" s="86" t="s">
         <v>304</v>
       </c>
-      <c r="JD4" s="69"/>
-      <c r="JE4" s="69"/>
-      <c r="JF4" s="69"/>
-      <c r="JG4" s="69"/>
-      <c r="JH4" s="69"/>
-      <c r="JI4" s="69"/>
-      <c r="JJ4" s="69"/>
-      <c r="JK4" s="69"/>
-      <c r="JL4" s="69"/>
-      <c r="JM4" s="70" t="s">
+      <c r="LV4" s="86"/>
+      <c r="LW4" s="86"/>
+      <c r="LX4" s="86"/>
+      <c r="LY4" s="86"/>
+      <c r="LZ4" s="86"/>
+      <c r="MA4" s="86"/>
+      <c r="MB4" s="86"/>
+      <c r="MC4" s="86"/>
+      <c r="MD4" s="86"/>
+      <c r="ME4" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="JN4" s="70"/>
-      <c r="JO4" s="70"/>
-      <c r="JP4" s="70"/>
-      <c r="JQ4" s="70"/>
-      <c r="JR4" s="70"/>
-      <c r="JS4" s="70"/>
-      <c r="JT4" s="70"/>
-      <c r="JU4" s="70"/>
-      <c r="JV4" s="70"/>
-      <c r="JW4" s="70"/>
-      <c r="JX4" s="70"/>
-      <c r="JY4" s="70"/>
-      <c r="JZ4" s="59" t="s">
+      <c r="MF4" s="87"/>
+      <c r="MG4" s="87"/>
+      <c r="MH4" s="87"/>
+      <c r="MI4" s="87"/>
+      <c r="MJ4" s="87"/>
+      <c r="MK4" s="87"/>
+      <c r="ML4" s="87"/>
+      <c r="MM4" s="87"/>
+      <c r="MN4" s="87"/>
+      <c r="MO4" s="87"/>
+      <c r="MP4" s="87"/>
+      <c r="MQ4" s="87"/>
+      <c r="MR4" s="58" t="s">
         <v>116</v>
       </c>
-      <c r="KA4" s="60"/>
-      <c r="KB4" s="61"/>
-      <c r="KC4" s="38"/>
-      <c r="KD4" s="59" t="s">
+      <c r="MS4" s="81"/>
+      <c r="MT4" s="59"/>
+      <c r="MU4" s="38"/>
+      <c r="MV4" s="58" t="s">
         <v>120</v>
       </c>
-      <c r="KE4" s="61"/>
-      <c r="KF4" s="56"/>
-      <c r="KG4" s="54"/>
+      <c r="MW4" s="59"/>
+      <c r="MX4" s="56"/>
+      <c r="MY4" s="54"/>
     </row>
-    <row r="5" spans="1:293" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="79"/>
-      <c r="B5" s="79"/>
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="80"/>
-      <c r="F5" s="80"/>
-      <c r="G5" s="80"/>
-      <c r="H5" s="80"/>
-      <c r="I5" s="81"/>
-      <c r="J5" s="81"/>
-      <c r="K5" s="81"/>
-      <c r="L5" s="81"/>
-      <c r="M5" s="82"/>
-      <c r="N5" s="82"/>
-      <c r="O5" s="82"/>
-      <c r="P5" s="83"/>
-      <c r="Q5" s="83"/>
-      <c r="R5" s="83"/>
-      <c r="S5" s="83"/>
-      <c r="T5" s="83"/>
-      <c r="U5" s="84"/>
-      <c r="V5" s="84"/>
-      <c r="W5" s="84"/>
-      <c r="X5" s="84"/>
-      <c r="Y5" s="84"/>
-      <c r="Z5" s="84"/>
-      <c r="AA5" s="84"/>
-      <c r="AB5" s="85"/>
-      <c r="AC5" s="85"/>
-      <c r="AD5" s="85"/>
-      <c r="AE5" s="76"/>
-      <c r="AF5" s="76"/>
-      <c r="AG5" s="86"/>
-      <c r="AH5" s="86"/>
-      <c r="AI5" s="86"/>
-      <c r="AJ5" s="86"/>
-      <c r="AK5" s="86"/>
-      <c r="AL5" s="87"/>
-      <c r="AM5" s="87"/>
-      <c r="AN5" s="87"/>
-      <c r="AO5" s="87"/>
-      <c r="AP5" s="87"/>
-      <c r="AQ5" s="87"/>
-      <c r="AR5" s="87"/>
-      <c r="AS5" s="87"/>
-      <c r="AT5" s="87"/>
-      <c r="AU5" s="87"/>
-      <c r="AV5" s="87"/>
-      <c r="AW5" s="87"/>
-      <c r="AX5" s="87"/>
-      <c r="AY5" s="87"/>
-      <c r="AZ5" s="87"/>
-      <c r="BA5" s="87"/>
-      <c r="BB5" s="87"/>
-      <c r="BC5" s="87"/>
-      <c r="BD5" s="87"/>
-      <c r="BE5" s="87"/>
-      <c r="BF5" s="87"/>
-      <c r="BG5" s="87"/>
-      <c r="BH5" s="87"/>
-      <c r="BI5" s="87"/>
-      <c r="BJ5" s="87"/>
+    <row r="5" spans="1:363" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="65"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="67"/>
+      <c r="K5" s="67"/>
+      <c r="L5" s="67"/>
+      <c r="M5" s="68"/>
+      <c r="N5" s="68"/>
+      <c r="O5" s="68"/>
+      <c r="P5" s="69"/>
+      <c r="Q5" s="69"/>
+      <c r="R5" s="69"/>
+      <c r="S5" s="69"/>
+      <c r="T5" s="69"/>
+      <c r="U5" s="70"/>
+      <c r="V5" s="70"/>
+      <c r="W5" s="70"/>
+      <c r="X5" s="70"/>
+      <c r="Y5" s="70"/>
+      <c r="Z5" s="70"/>
+      <c r="AA5" s="70"/>
+      <c r="AB5" s="71"/>
+      <c r="AC5" s="71"/>
+      <c r="AD5" s="71"/>
+      <c r="AE5" s="62"/>
+      <c r="AF5" s="62"/>
+      <c r="AG5" s="73"/>
+      <c r="AH5" s="73"/>
+      <c r="AI5" s="73"/>
+      <c r="AJ5" s="73"/>
+      <c r="AK5" s="73"/>
+      <c r="AL5" s="74"/>
+      <c r="AM5" s="74"/>
+      <c r="AN5" s="74"/>
+      <c r="AO5" s="74"/>
+      <c r="AP5" s="74"/>
+      <c r="AQ5" s="74"/>
+      <c r="AR5" s="74"/>
+      <c r="AS5" s="74"/>
+      <c r="AT5" s="74"/>
+      <c r="AU5" s="74"/>
+      <c r="AV5" s="74"/>
+      <c r="AW5" s="74"/>
+      <c r="AX5" s="74"/>
+      <c r="AY5" s="74"/>
+      <c r="AZ5" s="74"/>
+      <c r="BA5" s="74"/>
+      <c r="BB5" s="74"/>
+      <c r="BC5" s="74"/>
+      <c r="BD5" s="74"/>
+      <c r="BE5" s="74"/>
+      <c r="BF5" s="74"/>
+      <c r="BG5" s="74"/>
+      <c r="BH5" s="74"/>
+      <c r="BI5" s="74"/>
+      <c r="BJ5" s="74"/>
       <c r="BK5" s="7" t="s">
         <v>20</v>
       </c>
@@ -4010,29 +4547,239 @@
       <c r="JL5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="JM5" s="70"/>
-      <c r="JN5" s="70"/>
-      <c r="JO5" s="70"/>
-      <c r="JP5" s="70"/>
-      <c r="JQ5" s="70"/>
-      <c r="JR5" s="70"/>
-      <c r="JS5" s="70"/>
-      <c r="JT5" s="70"/>
-      <c r="JU5" s="70"/>
-      <c r="JV5" s="70"/>
-      <c r="JW5" s="70"/>
-      <c r="JX5" s="70"/>
-      <c r="JY5" s="70"/>
-      <c r="JZ5" s="62"/>
-      <c r="KA5" s="63"/>
-      <c r="KB5" s="64"/>
-      <c r="KC5" s="38"/>
-      <c r="KD5" s="62"/>
-      <c r="KE5" s="64"/>
-      <c r="KF5" s="57"/>
-      <c r="KG5" s="55"/>
+      <c r="JM5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="JN5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="JO5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="JP5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="JQ5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="JR5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="JS5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="JT5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="JU5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="JV5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="JW5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="JX5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="JY5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="JZ5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="KA5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="KB5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="KC5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="KD5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="KE5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="KF5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="KG5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="KH5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="KI5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="KJ5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="KK5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="KL5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="KM5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="KN5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="KO5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="KP5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="KQ5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="KR5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="KS5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="KT5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="KU5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="KV5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="KW5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="KX5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="KY5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="KZ5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="LA5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="LB5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="LC5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="LD5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="LE5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="LF5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="LG5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="LH5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="LI5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="LJ5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="LK5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="LL5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="LM5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="LN5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="LO5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="LP5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="LQ5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="LR5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="LS5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="LT5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="LU5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="LV5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="LW5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="LX5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="LY5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="LZ5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="MA5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="MB5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="MC5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="MD5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="ME5" s="87"/>
+      <c r="MF5" s="87"/>
+      <c r="MG5" s="87"/>
+      <c r="MH5" s="87"/>
+      <c r="MI5" s="87"/>
+      <c r="MJ5" s="87"/>
+      <c r="MK5" s="87"/>
+      <c r="ML5" s="87"/>
+      <c r="MM5" s="87"/>
+      <c r="MN5" s="87"/>
+      <c r="MO5" s="87"/>
+      <c r="MP5" s="87"/>
+      <c r="MQ5" s="87"/>
+      <c r="MR5" s="60"/>
+      <c r="MS5" s="82"/>
+      <c r="MT5" s="61"/>
+      <c r="MU5" s="38"/>
+      <c r="MV5" s="60"/>
+      <c r="MW5" s="61"/>
+      <c r="MX5" s="57"/>
+      <c r="MY5" s="55"/>
     </row>
-    <row r="6" spans="1:293" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:363" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>24</v>
       </c>
@@ -4280,640 +5027,850 @@
         <v>138</v>
       </c>
       <c r="CE6" s="18" t="s">
+        <v>338</v>
+      </c>
+      <c r="CF6" s="18" t="s">
+        <v>339</v>
+      </c>
+      <c r="CG6" s="18" t="s">
+        <v>340</v>
+      </c>
+      <c r="CH6" s="18" t="s">
+        <v>341</v>
+      </c>
+      <c r="CI6" s="18" t="s">
+        <v>342</v>
+      </c>
+      <c r="CJ6" s="18" t="s">
+        <v>343</v>
+      </c>
+      <c r="CK6" s="18" t="s">
+        <v>344</v>
+      </c>
+      <c r="CL6" s="18" t="s">
+        <v>345</v>
+      </c>
+      <c r="CM6" s="18" t="s">
+        <v>346</v>
+      </c>
+      <c r="CN6" s="18" t="s">
+        <v>347</v>
+      </c>
+      <c r="CO6" s="18" t="s">
+        <v>348</v>
+      </c>
+      <c r="CP6" s="18" t="s">
+        <v>349</v>
+      </c>
+      <c r="CQ6" s="18" t="s">
+        <v>350</v>
+      </c>
+      <c r="CR6" s="18" t="s">
+        <v>351</v>
+      </c>
+      <c r="CS6" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="CT6" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="CU6" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="CV6" s="18" t="s">
+        <v>355</v>
+      </c>
+      <c r="CW6" s="18" t="s">
+        <v>356</v>
+      </c>
+      <c r="CX6" s="18" t="s">
+        <v>357</v>
+      </c>
+      <c r="CY6" s="18" t="s">
+        <v>358</v>
+      </c>
+      <c r="CZ6" s="18" t="s">
+        <v>359</v>
+      </c>
+      <c r="DA6" s="18" t="s">
+        <v>360</v>
+      </c>
+      <c r="DB6" s="18" t="s">
+        <v>361</v>
+      </c>
+      <c r="DC6" s="18" t="s">
+        <v>362</v>
+      </c>
+      <c r="DD6" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="DE6" s="18" t="s">
+        <v>364</v>
+      </c>
+      <c r="DF6" s="18" t="s">
+        <v>365</v>
+      </c>
+      <c r="DG6" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="DH6" s="18" t="s">
+        <v>367</v>
+      </c>
+      <c r="DI6" s="18" t="s">
+        <v>368</v>
+      </c>
+      <c r="DJ6" s="18" t="s">
+        <v>369</v>
+      </c>
+      <c r="DK6" s="18" t="s">
+        <v>370</v>
+      </c>
+      <c r="DL6" s="18" t="s">
+        <v>371</v>
+      </c>
+      <c r="DM6" s="18" t="s">
+        <v>372</v>
+      </c>
+      <c r="DN6" s="18" t="s">
+        <v>373</v>
+      </c>
+      <c r="DO6" s="18" t="s">
+        <v>374</v>
+      </c>
+      <c r="DP6" s="18" t="s">
+        <v>375</v>
+      </c>
+      <c r="DQ6" s="18" t="s">
+        <v>376</v>
+      </c>
+      <c r="DR6" s="18" t="s">
+        <v>377</v>
+      </c>
+      <c r="DS6" s="18" t="s">
+        <v>379</v>
+      </c>
+      <c r="DT6" s="18" t="s">
+        <v>380</v>
+      </c>
+      <c r="DU6" s="18" t="s">
+        <v>381</v>
+      </c>
+      <c r="DV6" s="18" t="s">
+        <v>382</v>
+      </c>
+      <c r="DW6" s="18" t="s">
+        <v>383</v>
+      </c>
+      <c r="DX6" s="18" t="s">
+        <v>384</v>
+      </c>
+      <c r="DY6" s="18" t="s">
+        <v>385</v>
+      </c>
+      <c r="DZ6" s="18" t="s">
+        <v>386</v>
+      </c>
+      <c r="EA6" s="18" t="s">
+        <v>387</v>
+      </c>
+      <c r="EB6" s="18" t="s">
+        <v>388</v>
+      </c>
+      <c r="EC6" s="18" t="s">
+        <v>390</v>
+      </c>
+      <c r="ED6" s="18" t="s">
+        <v>391</v>
+      </c>
+      <c r="EE6" s="18" t="s">
+        <v>392</v>
+      </c>
+      <c r="EF6" s="18" t="s">
+        <v>393</v>
+      </c>
+      <c r="EG6" s="18" t="s">
+        <v>394</v>
+      </c>
+      <c r="EH6" s="18" t="s">
+        <v>395</v>
+      </c>
+      <c r="EI6" s="18" t="s">
+        <v>396</v>
+      </c>
+      <c r="EJ6" s="18" t="s">
+        <v>397</v>
+      </c>
+      <c r="EK6" s="18" t="s">
+        <v>398</v>
+      </c>
+      <c r="EL6" s="18" t="s">
+        <v>399</v>
+      </c>
+      <c r="EM6" s="18" t="s">
+        <v>401</v>
+      </c>
+      <c r="EN6" s="18" t="s">
+        <v>402</v>
+      </c>
+      <c r="EO6" s="18" t="s">
+        <v>403</v>
+      </c>
+      <c r="EP6" s="18" t="s">
+        <v>404</v>
+      </c>
+      <c r="EQ6" s="18" t="s">
+        <v>405</v>
+      </c>
+      <c r="ER6" s="18" t="s">
+        <v>406</v>
+      </c>
+      <c r="ES6" s="18" t="s">
+        <v>407</v>
+      </c>
+      <c r="ET6" s="18" t="s">
+        <v>408</v>
+      </c>
+      <c r="EU6" s="18" t="s">
+        <v>409</v>
+      </c>
+      <c r="EV6" s="18" t="s">
+        <v>410</v>
+      </c>
+      <c r="EW6" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="CF6" s="18" t="s">
+      <c r="EX6" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="CG6" s="18" t="s">
+      <c r="EY6" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="CH6" s="18" t="s">
+      <c r="EZ6" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="CI6" s="18" t="s">
+      <c r="FA6" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="CJ6" s="18" t="s">
+      <c r="FB6" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="CK6" s="18" t="s">
+      <c r="FC6" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="CL6" s="18" t="s">
+      <c r="FD6" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="CM6" s="18" t="s">
+      <c r="FE6" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="CN6" s="18" t="s">
+      <c r="FF6" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="CO6" s="18" t="s">
+      <c r="FG6" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="CP6" s="18" t="s">
+      <c r="FH6" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="CQ6" s="18" t="s">
+      <c r="FI6" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="CR6" s="18" t="s">
+      <c r="FJ6" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="CS6" s="18" t="s">
+      <c r="FK6" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="CT6" s="18" t="s">
+      <c r="FL6" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="CU6" s="18" t="s">
+      <c r="FM6" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="CV6" s="18" t="s">
+      <c r="FN6" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="CW6" s="18" t="s">
+      <c r="FO6" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="CX6" s="18" t="s">
+      <c r="FP6" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="CY6" s="9" t="s">
+      <c r="FQ6" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="CZ6" s="9" t="s">
+      <c r="FR6" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="DA6" s="9" t="s">
+      <c r="FS6" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="DB6" s="9" t="s">
+      <c r="FT6" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="DC6" s="9" t="s">
+      <c r="FU6" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="DD6" s="9" t="s">
+      <c r="FV6" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="DE6" s="9" t="s">
+      <c r="FW6" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="DF6" s="9" t="s">
+      <c r="FX6" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="DG6" s="9" t="s">
+      <c r="FY6" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="DH6" s="9" t="s">
+      <c r="FZ6" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="DI6" s="9" t="s">
+      <c r="GA6" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="DJ6" s="9" t="s">
+      <c r="GB6" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="DK6" s="9" t="s">
+      <c r="GC6" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="DL6" s="9" t="s">
+      <c r="GD6" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="DM6" s="9" t="s">
+      <c r="GE6" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="DN6" s="9" t="s">
+      <c r="GF6" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="DO6" s="9" t="s">
+      <c r="GG6" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="DP6" s="9" t="s">
+      <c r="GH6" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="DQ6" s="9" t="s">
+      <c r="GI6" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="DR6" s="9" t="s">
+      <c r="GJ6" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="DS6" s="9" t="s">
+      <c r="GK6" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="DT6" s="9" t="s">
+      <c r="GL6" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="DU6" s="9" t="s">
+      <c r="GM6" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="DV6" s="9" t="s">
+      <c r="GN6" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="DW6" s="9" t="s">
+      <c r="GO6" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="DX6" s="9" t="s">
+      <c r="GP6" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="DY6" s="9" t="s">
+      <c r="GQ6" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="DZ6" s="9" t="s">
+      <c r="GR6" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="EA6" s="9" t="s">
+      <c r="GS6" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="EB6" s="9" t="s">
+      <c r="GT6" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="EC6" s="18" t="s">
+      <c r="GU6" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="ED6" s="18" t="s">
+      <c r="GV6" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="EE6" s="18" t="s">
+      <c r="GW6" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="EF6" s="18" t="s">
+      <c r="GX6" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="EG6" s="18" t="s">
+      <c r="GY6" s="18" t="s">
         <v>169</v>
       </c>
-      <c r="EH6" s="18" t="s">
+      <c r="GZ6" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="EI6" s="18" t="s">
+      <c r="HA6" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="EJ6" s="18" t="s">
+      <c r="HB6" s="18" t="s">
         <v>172</v>
       </c>
-      <c r="EK6" s="18" t="s">
+      <c r="HC6" s="18" t="s">
         <v>173</v>
       </c>
-      <c r="EL6" s="18" t="s">
+      <c r="HD6" s="18" t="s">
         <v>174</v>
       </c>
-      <c r="EM6" s="18" t="s">
+      <c r="HE6" s="18" t="s">
         <v>179</v>
       </c>
-      <c r="EN6" s="18" t="s">
+      <c r="HF6" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="EO6" s="18" t="s">
+      <c r="HG6" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="EP6" s="18" t="s">
+      <c r="HH6" s="18" t="s">
         <v>182</v>
       </c>
-      <c r="EQ6" s="18" t="s">
+      <c r="HI6" s="18" t="s">
         <v>183</v>
       </c>
-      <c r="ER6" s="18" t="s">
+      <c r="HJ6" s="18" t="s">
         <v>184</v>
       </c>
-      <c r="ES6" s="18" t="s">
+      <c r="HK6" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="ET6" s="18" t="s">
+      <c r="HL6" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="EU6" s="18" t="s">
+      <c r="HM6" s="18" t="s">
         <v>187</v>
       </c>
-      <c r="EV6" s="18" t="s">
+      <c r="HN6" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="EW6" s="18" t="s">
+      <c r="HO6" s="18" t="s">
         <v>190</v>
       </c>
-      <c r="EX6" s="18" t="s">
+      <c r="HP6" s="18" t="s">
         <v>191</v>
       </c>
-      <c r="EY6" s="18" t="s">
+      <c r="HQ6" s="18" t="s">
         <v>192</v>
       </c>
-      <c r="EZ6" s="18" t="s">
+      <c r="HR6" s="18" t="s">
         <v>193</v>
       </c>
-      <c r="FA6" s="18" t="s">
+      <c r="HS6" s="18" t="s">
         <v>194</v>
       </c>
-      <c r="FB6" s="18" t="s">
+      <c r="HT6" s="18" t="s">
         <v>195</v>
       </c>
-      <c r="FC6" s="18" t="s">
+      <c r="HU6" s="18" t="s">
         <v>196</v>
       </c>
-      <c r="FD6" s="18" t="s">
+      <c r="HV6" s="18" t="s">
         <v>197</v>
       </c>
-      <c r="FE6" s="18" t="s">
+      <c r="HW6" s="18" t="s">
         <v>198</v>
       </c>
-      <c r="FF6" s="18" t="s">
+      <c r="HX6" s="18" t="s">
         <v>199</v>
       </c>
-      <c r="FG6" s="18" t="s">
+      <c r="HY6" s="18" t="s">
         <v>201</v>
       </c>
-      <c r="FH6" s="18" t="s">
+      <c r="HZ6" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="FI6" s="18" t="s">
+      <c r="IA6" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="FJ6" s="18" t="s">
+      <c r="IB6" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="FK6" s="18" t="s">
+      <c r="IC6" s="18" t="s">
         <v>205</v>
       </c>
-      <c r="FL6" s="18" t="s">
+      <c r="ID6" s="18" t="s">
         <v>206</v>
       </c>
-      <c r="FM6" s="18" t="s">
+      <c r="IE6" s="18" t="s">
         <v>207</v>
       </c>
-      <c r="FN6" s="18" t="s">
+      <c r="IF6" s="18" t="s">
         <v>208</v>
       </c>
-      <c r="FO6" s="18" t="s">
+      <c r="IG6" s="18" t="s">
         <v>209</v>
       </c>
-      <c r="FP6" s="18" t="s">
+      <c r="IH6" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="FQ6" s="18" t="s">
+      <c r="II6" s="18" t="s">
         <v>212</v>
       </c>
-      <c r="FR6" s="18" t="s">
+      <c r="IJ6" s="18" t="s">
         <v>213</v>
       </c>
-      <c r="FS6" s="18" t="s">
+      <c r="IK6" s="18" t="s">
         <v>214</v>
       </c>
-      <c r="FT6" s="18" t="s">
+      <c r="IL6" s="18" t="s">
         <v>215</v>
       </c>
-      <c r="FU6" s="18" t="s">
+      <c r="IM6" s="18" t="s">
         <v>216</v>
       </c>
-      <c r="FV6" s="18" t="s">
+      <c r="IN6" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="FW6" s="18" t="s">
+      <c r="IO6" s="18" t="s">
         <v>218</v>
       </c>
-      <c r="FX6" s="18" t="s">
+      <c r="IP6" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="FY6" s="18" t="s">
+      <c r="IQ6" s="18" t="s">
         <v>220</v>
       </c>
-      <c r="FZ6" s="18" t="s">
+      <c r="IR6" s="18" t="s">
         <v>221</v>
       </c>
-      <c r="GA6" s="18" t="s">
+      <c r="IS6" s="18" t="s">
         <v>223</v>
       </c>
-      <c r="GB6" s="18" t="s">
+      <c r="IT6" s="18" t="s">
         <v>224</v>
       </c>
-      <c r="GC6" s="18" t="s">
+      <c r="IU6" s="18" t="s">
         <v>225</v>
       </c>
-      <c r="GD6" s="18" t="s">
+      <c r="IV6" s="18" t="s">
         <v>226</v>
       </c>
-      <c r="GE6" s="18" t="s">
+      <c r="IW6" s="18" t="s">
         <v>227</v>
       </c>
-      <c r="GF6" s="18" t="s">
+      <c r="IX6" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="GG6" s="18" t="s">
+      <c r="IY6" s="18" t="s">
         <v>229</v>
       </c>
-      <c r="GH6" s="18" t="s">
+      <c r="IZ6" s="18" t="s">
         <v>230</v>
       </c>
-      <c r="GI6" s="18" t="s">
+      <c r="JA6" s="18" t="s">
         <v>231</v>
       </c>
-      <c r="GJ6" s="18" t="s">
+      <c r="JB6" s="18" t="s">
         <v>232</v>
       </c>
-      <c r="GK6" s="18" t="s">
+      <c r="JC6" s="18" t="s">
         <v>234</v>
       </c>
-      <c r="GL6" s="18" t="s">
+      <c r="JD6" s="18" t="s">
         <v>235</v>
       </c>
-      <c r="GM6" s="18" t="s">
+      <c r="JE6" s="18" t="s">
         <v>236</v>
       </c>
-      <c r="GN6" s="18" t="s">
+      <c r="JF6" s="18" t="s">
         <v>237</v>
       </c>
-      <c r="GO6" s="18" t="s">
+      <c r="JG6" s="18" t="s">
         <v>238</v>
       </c>
-      <c r="GP6" s="18" t="s">
+      <c r="JH6" s="18" t="s">
         <v>239</v>
       </c>
-      <c r="GQ6" s="18" t="s">
+      <c r="JI6" s="18" t="s">
         <v>240</v>
       </c>
-      <c r="GR6" s="18" t="s">
+      <c r="JJ6" s="18" t="s">
         <v>241</v>
       </c>
-      <c r="GS6" s="18" t="s">
+      <c r="JK6" s="18" t="s">
         <v>242</v>
       </c>
-      <c r="GT6" s="18" t="s">
+      <c r="JL6" s="18" t="s">
         <v>243</v>
       </c>
-      <c r="GU6" s="18" t="s">
+      <c r="JM6" s="18" t="s">
         <v>246</v>
       </c>
-      <c r="GV6" s="18" t="s">
+      <c r="JN6" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="GW6" s="18" t="s">
+      <c r="JO6" s="18" t="s">
         <v>247</v>
       </c>
-      <c r="GX6" s="18" t="s">
+      <c r="JP6" s="18" t="s">
         <v>248</v>
       </c>
-      <c r="GY6" s="18" t="s">
+      <c r="JQ6" s="18" t="s">
         <v>249</v>
       </c>
-      <c r="GZ6" s="18" t="s">
+      <c r="JR6" s="18" t="s">
         <v>250</v>
       </c>
-      <c r="HA6" s="18" t="s">
+      <c r="JS6" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="HB6" s="18" t="s">
+      <c r="JT6" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="HC6" s="18" t="s">
+      <c r="JU6" s="18" t="s">
         <v>253</v>
       </c>
-      <c r="HD6" s="18" t="s">
+      <c r="JV6" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="HE6" s="18" t="s">
+      <c r="JW6" s="18" t="s">
         <v>255</v>
       </c>
-      <c r="HF6" s="18" t="s">
+      <c r="JX6" s="18" t="s">
         <v>256</v>
       </c>
-      <c r="HG6" s="18" t="s">
+      <c r="JY6" s="18" t="s">
         <v>257</v>
       </c>
-      <c r="HH6" s="18" t="s">
+      <c r="JZ6" s="18" t="s">
         <v>258</v>
       </c>
-      <c r="HI6" s="18" t="s">
+      <c r="KA6" s="18" t="s">
         <v>259</v>
       </c>
-      <c r="HJ6" s="18" t="s">
+      <c r="KB6" s="18" t="s">
         <v>260</v>
       </c>
-      <c r="HK6" s="18" t="s">
+      <c r="KC6" s="18" t="s">
         <v>261</v>
       </c>
-      <c r="HL6" s="18" t="s">
+      <c r="KD6" s="18" t="s">
         <v>262</v>
       </c>
-      <c r="HM6" s="18" t="s">
+      <c r="KE6" s="18" t="s">
         <v>263</v>
       </c>
-      <c r="HN6" s="18" t="s">
+      <c r="KF6" s="18" t="s">
         <v>264</v>
       </c>
-      <c r="HO6" s="18" t="s">
+      <c r="KG6" s="18" t="s">
         <v>266</v>
       </c>
-      <c r="HP6" s="18" t="s">
+      <c r="KH6" s="18" t="s">
         <v>267</v>
       </c>
-      <c r="HQ6" s="18" t="s">
+      <c r="KI6" s="18" t="s">
         <v>268</v>
       </c>
-      <c r="HR6" s="18" t="s">
+      <c r="KJ6" s="18" t="s">
         <v>269</v>
       </c>
-      <c r="HS6" s="18" t="s">
+      <c r="KK6" s="18" t="s">
         <v>270</v>
       </c>
-      <c r="HT6" s="18" t="s">
+      <c r="KL6" s="18" t="s">
         <v>271</v>
       </c>
-      <c r="HU6" s="18" t="s">
+      <c r="KM6" s="18" t="s">
         <v>272</v>
       </c>
-      <c r="HV6" s="18" t="s">
+      <c r="KN6" s="18" t="s">
         <v>273</v>
       </c>
-      <c r="HW6" s="18" t="s">
+      <c r="KO6" s="18" t="s">
         <v>274</v>
       </c>
-      <c r="HX6" s="18" t="s">
+      <c r="KP6" s="18" t="s">
         <v>275</v>
       </c>
-      <c r="HY6" s="18" t="s">
+      <c r="KQ6" s="18" t="s">
         <v>277</v>
       </c>
-      <c r="HZ6" s="18" t="s">
+      <c r="KR6" s="18" t="s">
         <v>278</v>
       </c>
-      <c r="IA6" s="18" t="s">
+      <c r="KS6" s="18" t="s">
         <v>279</v>
       </c>
-      <c r="IB6" s="18" t="s">
+      <c r="KT6" s="18" t="s">
         <v>280</v>
       </c>
-      <c r="IC6" s="18" t="s">
+      <c r="KU6" s="18" t="s">
         <v>281</v>
       </c>
-      <c r="ID6" s="18" t="s">
+      <c r="KV6" s="18" t="s">
         <v>282</v>
       </c>
-      <c r="IE6" s="18" t="s">
+      <c r="KW6" s="18" t="s">
         <v>283</v>
       </c>
-      <c r="IF6" s="18" t="s">
+      <c r="KX6" s="18" t="s">
         <v>284</v>
       </c>
-      <c r="IG6" s="18" t="s">
+      <c r="KY6" s="18" t="s">
         <v>285</v>
       </c>
-      <c r="IH6" s="18" t="s">
+      <c r="KZ6" s="18" t="s">
         <v>286</v>
       </c>
-      <c r="II6" s="18" t="s">
+      <c r="LA6" s="18" t="s">
         <v>288</v>
       </c>
-      <c r="IJ6" s="18" t="s">
+      <c r="LB6" s="18" t="s">
         <v>289</v>
       </c>
-      <c r="IK6" s="18" t="s">
+      <c r="LC6" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="IL6" s="18" t="s">
+      <c r="LD6" s="18" t="s">
         <v>291</v>
       </c>
-      <c r="IM6" s="18" t="s">
+      <c r="LE6" s="18" t="s">
         <v>292</v>
       </c>
-      <c r="IN6" s="18" t="s">
+      <c r="LF6" s="18" t="s">
         <v>315</v>
       </c>
-      <c r="IO6" s="18" t="s">
+      <c r="LG6" s="18" t="s">
         <v>316</v>
       </c>
-      <c r="IP6" s="18" t="s">
+      <c r="LH6" s="18" t="s">
         <v>317</v>
       </c>
-      <c r="IQ6" s="18" t="s">
+      <c r="LI6" s="18" t="s">
         <v>318</v>
       </c>
-      <c r="IR6" s="18" t="s">
+      <c r="LJ6" s="18" t="s">
         <v>319</v>
       </c>
-      <c r="IS6" s="18" t="s">
+      <c r="LK6" s="18" t="s">
         <v>294</v>
       </c>
-      <c r="IT6" s="18" t="s">
+      <c r="LL6" s="18" t="s">
         <v>295</v>
       </c>
-      <c r="IU6" s="18" t="s">
+      <c r="LM6" s="18" t="s">
         <v>296</v>
       </c>
-      <c r="IV6" s="18" t="s">
+      <c r="LN6" s="18" t="s">
         <v>297</v>
       </c>
-      <c r="IW6" s="18" t="s">
+      <c r="LO6" s="18" t="s">
         <v>298</v>
       </c>
-      <c r="IX6" s="18" t="s">
+      <c r="LP6" s="18" t="s">
         <v>299</v>
       </c>
-      <c r="IY6" s="18" t="s">
+      <c r="LQ6" s="18" t="s">
         <v>300</v>
       </c>
-      <c r="IZ6" s="18" t="s">
+      <c r="LR6" s="18" t="s">
         <v>301</v>
       </c>
-      <c r="JA6" s="18" t="s">
+      <c r="LS6" s="18" t="s">
         <v>302</v>
       </c>
-      <c r="JB6" s="18" t="s">
+      <c r="LT6" s="18" t="s">
         <v>303</v>
       </c>
-      <c r="JC6" s="18" t="s">
+      <c r="LU6" s="18" t="s">
         <v>305</v>
       </c>
-      <c r="JD6" s="18" t="s">
+      <c r="LV6" s="18" t="s">
         <v>306</v>
       </c>
-      <c r="JE6" s="18" t="s">
+      <c r="LW6" s="18" t="s">
         <v>307</v>
       </c>
-      <c r="JF6" s="18" t="s">
+      <c r="LX6" s="18" t="s">
         <v>308</v>
       </c>
-      <c r="JG6" s="18" t="s">
+      <c r="LY6" s="18" t="s">
         <v>309</v>
       </c>
-      <c r="JH6" s="18" t="s">
+      <c r="LZ6" s="18" t="s">
         <v>310</v>
       </c>
-      <c r="JI6" s="18" t="s">
+      <c r="MA6" s="18" t="s">
         <v>311</v>
       </c>
-      <c r="JJ6" s="18" t="s">
+      <c r="MB6" s="18" t="s">
         <v>312</v>
       </c>
-      <c r="JK6" s="18" t="s">
+      <c r="MC6" s="18" t="s">
         <v>313</v>
       </c>
-      <c r="JL6" s="18" t="s">
+      <c r="MD6" s="18" t="s">
         <v>314</v>
       </c>
-      <c r="JM6" s="18" t="s">
+      <c r="ME6" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="JN6" s="18" t="s">
+      <c r="MF6" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="JO6" s="18" t="s">
+      <c r="MG6" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="JP6" s="18" t="s">
+      <c r="MH6" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="JQ6" s="18" t="s">
+      <c r="MI6" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="JR6" s="18" t="s">
+      <c r="MJ6" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="JS6" s="18" t="s">
+      <c r="MK6" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="JT6" s="18" t="s">
+      <c r="ML6" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="JU6" s="18" t="s">
+      <c r="MM6" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="JV6" s="18" t="s">
+      <c r="MN6" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="JW6" s="18" t="s">
+      <c r="MO6" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="JX6" s="18" t="s">
+      <c r="MP6" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="JY6" s="18" t="s">
+      <c r="MQ6" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="JZ6" s="18" t="s">
+      <c r="MR6" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="KA6" s="18" t="s">
+      <c r="MS6" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="KB6" s="18" t="s">
+      <c r="MT6" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="KC6" s="18" t="s">
+      <c r="MU6" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="KD6" s="18" t="s">
+      <c r="MV6" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="KE6" s="18" t="s">
+      <c r="MW6" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="KF6" s="18" t="s">
+      <c r="MX6" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="KG6" s="18" t="s">
+      <c r="MY6" s="18" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:293" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:363" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="40"/>
       <c r="B7" s="40"/>
       <c r="C7" s="40" t="s">
@@ -4972,7 +5929,7 @@
         <v>0</v>
       </c>
       <c r="AM7" s="51">
-        <f>SUM(BU7:CD7)</f>
+        <f>SUM(CE7:CN7)</f>
         <v>0</v>
       </c>
       <c r="AN7" s="51" t="e">
@@ -4980,131 +5937,131 @@
         <v>#REF!</v>
       </c>
       <c r="AO7" s="51">
-        <f>SUM(CE7:CN7)</f>
-        <v>0</v>
-      </c>
-      <c r="AP7" s="51">
-        <f>SUM(CO7:CX7)</f>
-        <v>0</v>
-      </c>
-      <c r="AQ7" s="51">
-        <f>SUM(CY7:DH7)</f>
-        <v>0</v>
-      </c>
-      <c r="AR7" s="51">
-        <f>SUM(DI7:DR7)</f>
-        <v>0</v>
-      </c>
-      <c r="AS7" s="51">
-        <f>SUM(DS7:EB7)</f>
-        <v>0</v>
-      </c>
-      <c r="AT7" s="51">
-        <f>SUM(EC7:EL7)</f>
-        <v>0</v>
-      </c>
-      <c r="AU7" s="51">
-        <f>SUM(EM7:EV7)</f>
-        <v>0</v>
-      </c>
-      <c r="AV7" s="51">
         <f>SUM(EW7:FF7)</f>
         <v>0</v>
       </c>
-      <c r="AW7" s="51">
+      <c r="AP7" s="51">
         <f>SUM(FG7:FP7)</f>
         <v>0</v>
       </c>
-      <c r="AX7" s="51">
+      <c r="AQ7" s="51">
         <f>SUM(FQ7:FZ7)</f>
         <v>0</v>
       </c>
-      <c r="AY7" s="51">
+      <c r="AR7" s="51">
         <f>SUM(GA7:GJ7)</f>
         <v>0</v>
       </c>
-      <c r="AZ7" s="51">
+      <c r="AS7" s="51">
         <f>SUM(GK7:GT7)</f>
         <v>0</v>
       </c>
-      <c r="BA7" s="51">
+      <c r="AT7" s="51">
         <f>SUM(GU7:HD7)</f>
         <v>0</v>
       </c>
-      <c r="BB7" s="51">
+      <c r="AU7" s="51">
         <f>SUM(HE7:HN7)</f>
         <v>0</v>
       </c>
-      <c r="BC7" s="51">
+      <c r="AV7" s="51">
         <f>SUM(HO7:HX7)</f>
         <v>0</v>
       </c>
-      <c r="BD7" s="51">
+      <c r="AW7" s="51">
         <f>SUM(HY7:IH7)</f>
         <v>0</v>
       </c>
-      <c r="BE7" s="51">
+      <c r="AX7" s="51">
         <f>SUM(II7:IR7)</f>
         <v>0</v>
       </c>
-      <c r="BF7" s="51">
+      <c r="AY7" s="51">
         <f>SUM(IS7:JB7)</f>
         <v>0</v>
       </c>
-      <c r="BG7" s="51">
+      <c r="AZ7" s="51">
         <f>SUM(JC7:JL7)</f>
         <v>0</v>
       </c>
+      <c r="BA7" s="51">
+        <f>SUM(JM7:JV7)</f>
+        <v>0</v>
+      </c>
+      <c r="BB7" s="51">
+        <f>SUM(JW7:KF7)</f>
+        <v>0</v>
+      </c>
+      <c r="BC7" s="51">
+        <f>SUM(KG7:KP7)</f>
+        <v>0</v>
+      </c>
+      <c r="BD7" s="51">
+        <f>SUM(KQ7:KZ7)</f>
+        <v>0</v>
+      </c>
+      <c r="BE7" s="51">
+        <f>SUM(LA7:LJ7)</f>
+        <v>0</v>
+      </c>
+      <c r="BF7" s="51">
+        <f>SUM(LK7:LT7)</f>
+        <v>0</v>
+      </c>
+      <c r="BG7" s="51">
+        <f>SUM(LU7:MD7)</f>
+        <v>0</v>
+      </c>
       <c r="BH7" s="51">
-        <f t="shared" ref="BH7" si="0">JM7</f>
+        <f t="shared" ref="BH7" si="0">ME7</f>
         <v>0</v>
       </c>
       <c r="BI7" s="51">
-        <f>JN7</f>
+        <f>MF7</f>
         <v>0</v>
       </c>
       <c r="BJ7" s="51">
-        <f>JO7</f>
+        <f>MG7</f>
         <v>0</v>
       </c>
       <c r="BK7" s="51">
-        <f t="shared" ref="BK7:BT7" si="1">BU7+CE7+CO7+CY7+DI7+DS7+EC7</f>
+        <f>BU7+CE7+CO7+CY7+DI7+DS7+EC7+EM7+EW7+FG7+FQ7+GA7+GK7+GU7</f>
         <v>0</v>
       </c>
       <c r="BL7" s="51">
-        <f t="shared" si="1"/>
+        <f>BV7+CF7+CP7+CZ7+DJ7+DT7+ED7+EN7+EX7+FH7+FR7+GB7+GL7+GV7</f>
         <v>0</v>
       </c>
       <c r="BM7" s="51">
-        <f t="shared" si="1"/>
+        <f>BW7+CG7+CQ7+DA7+DK7+DU7+EE7+EO7+EY7+FI7+FS7+GC7+GM7+GW7</f>
         <v>0</v>
       </c>
       <c r="BN7" s="51">
-        <f t="shared" si="1"/>
+        <f>BX7+CH7+CR7+DB7+DL7+DV7+EF7+EP7+EZ7+FJ7+FT7+GD7+GN7+GX7</f>
         <v>0</v>
       </c>
       <c r="BO7" s="51">
-        <f t="shared" si="1"/>
+        <f>BY7+CI7+CS7+DC7+DM7+DW7+EG7+EQ7+FA7+FK7+FU7+GE7+GO7+GY7</f>
         <v>0</v>
       </c>
       <c r="BP7" s="51">
-        <f t="shared" si="1"/>
+        <f>BZ7+CJ7+CT7+DD7+DN7+DX7+EH7+ER7+FB7+FL7+FV7+GF7+GP7+GZ7</f>
         <v>0</v>
       </c>
       <c r="BQ7" s="51">
-        <f t="shared" si="1"/>
+        <f>CA7+CK7+CU7+DE7+DO7+DY7+EI7+ES7+FC7+FM7+FW7+GG7+GQ7+HA7</f>
         <v>0</v>
       </c>
       <c r="BR7" s="51">
-        <f t="shared" si="1"/>
+        <f>CB7+CL7+CV7+DF7+DP7+DZ7+EJ7+ET7+FD7+FN7+FX7+GH7+GR7+HB7</f>
         <v>0</v>
       </c>
       <c r="BS7" s="51">
-        <f t="shared" si="1"/>
+        <f>CC7+CM7+CW7+DG7+DQ7+EA7+EK7+EU7+FE7+FO7+FY7+GI7+GS7+HC7</f>
         <v>0</v>
       </c>
       <c r="BT7" s="51">
-        <f t="shared" si="1"/>
+        <f>CD7+CN7+CX7+DH7+DR7+EB7+EL7+EV7+FF7+FP7+FZ7+GJ7+GT7+HD7</f>
         <v>0</v>
       </c>
       <c r="BU7" s="46"/>
@@ -5310,29 +6267,126 @@
       <c r="JM7" s="46"/>
       <c r="JN7" s="46"/>
       <c r="JO7" s="46"/>
-      <c r="JP7" s="41"/>
-      <c r="JQ7" s="41"/>
-      <c r="JR7" s="41"/>
-      <c r="JS7" s="52"/>
-      <c r="JT7" s="52"/>
-      <c r="JU7" s="52"/>
-      <c r="JV7" s="52"/>
-      <c r="JW7" s="52"/>
-      <c r="JX7" s="52"/>
-      <c r="JY7" s="52"/>
-      <c r="JZ7" s="39"/>
-      <c r="KA7" s="39"/>
-      <c r="KB7" s="39"/>
-      <c r="KC7" s="39"/>
-      <c r="KD7" s="53"/>
-      <c r="KE7" s="53"/>
-      <c r="KF7" s="53"/>
-      <c r="KG7" s="53"/>
+      <c r="JP7" s="46"/>
+      <c r="JQ7" s="46"/>
+      <c r="JR7" s="46"/>
+      <c r="JS7" s="46"/>
+      <c r="JT7" s="46"/>
+      <c r="JU7" s="46"/>
+      <c r="JV7" s="46"/>
+      <c r="JW7" s="46"/>
+      <c r="JX7" s="46"/>
+      <c r="JY7" s="46"/>
+      <c r="JZ7" s="46"/>
+      <c r="KA7" s="46"/>
+      <c r="KB7" s="46"/>
+      <c r="KC7" s="46"/>
+      <c r="KD7" s="46"/>
+      <c r="KE7" s="46"/>
+      <c r="KF7" s="46"/>
+      <c r="KG7" s="46"/>
+      <c r="KH7" s="46"/>
+      <c r="KI7" s="46"/>
+      <c r="KJ7" s="46"/>
+      <c r="KK7" s="46"/>
+      <c r="KL7" s="46"/>
+      <c r="KM7" s="46"/>
+      <c r="KN7" s="46"/>
+      <c r="KO7" s="46"/>
+      <c r="KP7" s="46"/>
+      <c r="KQ7" s="46"/>
+      <c r="KR7" s="46"/>
+      <c r="KS7" s="46"/>
+      <c r="KT7" s="46"/>
+      <c r="KU7" s="46"/>
+      <c r="KV7" s="46"/>
+      <c r="KW7" s="46"/>
+      <c r="KX7" s="46"/>
+      <c r="KY7" s="46"/>
+      <c r="KZ7" s="46"/>
+      <c r="LA7" s="46"/>
+      <c r="LB7" s="46"/>
+      <c r="LC7" s="46"/>
+      <c r="LD7" s="46"/>
+      <c r="LE7" s="46"/>
+      <c r="LF7" s="46"/>
+      <c r="LG7" s="46"/>
+      <c r="LH7" s="46"/>
+      <c r="LI7" s="46"/>
+      <c r="LJ7" s="46"/>
+      <c r="LK7" s="46"/>
+      <c r="LL7" s="46"/>
+      <c r="LM7" s="46"/>
+      <c r="LN7" s="46"/>
+      <c r="LO7" s="46"/>
+      <c r="LP7" s="46"/>
+      <c r="LQ7" s="46"/>
+      <c r="LR7" s="46"/>
+      <c r="LS7" s="46"/>
+      <c r="LT7" s="46"/>
+      <c r="LU7" s="46"/>
+      <c r="LV7" s="46"/>
+      <c r="LW7" s="46"/>
+      <c r="LX7" s="46"/>
+      <c r="LY7" s="46"/>
+      <c r="LZ7" s="46"/>
+      <c r="MA7" s="46"/>
+      <c r="MB7" s="46"/>
+      <c r="MC7" s="46"/>
+      <c r="MD7" s="46"/>
+      <c r="ME7" s="46"/>
+      <c r="MF7" s="46"/>
+      <c r="MG7" s="46"/>
+      <c r="MH7" s="41"/>
+      <c r="MI7" s="41"/>
+      <c r="MJ7" s="41"/>
+      <c r="MK7" s="52"/>
+      <c r="ML7" s="52"/>
+      <c r="MM7" s="52"/>
+      <c r="MN7" s="52"/>
+      <c r="MO7" s="52"/>
+      <c r="MP7" s="52"/>
+      <c r="MQ7" s="52"/>
+      <c r="MR7" s="39"/>
+      <c r="MS7" s="39"/>
+      <c r="MT7" s="39"/>
+      <c r="MU7" s="39"/>
+      <c r="MV7" s="53"/>
+      <c r="MW7" s="53"/>
+      <c r="MX7" s="53"/>
+      <c r="MY7" s="53"/>
     </row>
   </sheetData>
-  <autoFilter ref="A6:KC6" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <mergeCells count="36">
-    <mergeCell ref="KD4:KE5"/>
+  <autoFilter ref="A6:MU6" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <mergeCells count="43">
+    <mergeCell ref="EC4:EL4"/>
+    <mergeCell ref="EM4:EV4"/>
+    <mergeCell ref="BU4:CD4"/>
+    <mergeCell ref="CO4:CX4"/>
+    <mergeCell ref="CY4:DH4"/>
+    <mergeCell ref="DI4:DR4"/>
+    <mergeCell ref="DS4:EB4"/>
+    <mergeCell ref="GU4:HD4"/>
+    <mergeCell ref="MR4:MT5"/>
+    <mergeCell ref="HO4:HX4"/>
+    <mergeCell ref="KG4:KP4"/>
+    <mergeCell ref="KQ4:KZ4"/>
+    <mergeCell ref="LA4:LJ4"/>
+    <mergeCell ref="LU4:MD4"/>
+    <mergeCell ref="ME4:MQ5"/>
+    <mergeCell ref="HY4:IH4"/>
+    <mergeCell ref="II4:IR4"/>
+    <mergeCell ref="IS4:JB4"/>
+    <mergeCell ref="JC4:JL4"/>
+    <mergeCell ref="JM4:JV4"/>
+    <mergeCell ref="JW4:KF4"/>
+    <mergeCell ref="LK4:LT4"/>
+    <mergeCell ref="EW4:FF4"/>
+    <mergeCell ref="FG4:FP4"/>
+    <mergeCell ref="FQ4:FZ4"/>
+    <mergeCell ref="GA4:GJ4"/>
+    <mergeCell ref="GK4:GT4"/>
+    <mergeCell ref="MV4:MW5"/>
     <mergeCell ref="AE4:AF5"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
@@ -5343,31 +6397,11 @@
     <mergeCell ref="P4:T5"/>
     <mergeCell ref="U4:AA5"/>
     <mergeCell ref="AB4:AD5"/>
-    <mergeCell ref="EM4:EV4"/>
+    <mergeCell ref="HE4:HN4"/>
     <mergeCell ref="AG4:AK5"/>
     <mergeCell ref="AL4:BJ5"/>
     <mergeCell ref="BK4:BT4"/>
-    <mergeCell ref="BU4:CD4"/>
     <mergeCell ref="CE4:CN4"/>
-    <mergeCell ref="CO4:CX4"/>
-    <mergeCell ref="CY4:DH4"/>
-    <mergeCell ref="DI4:DR4"/>
-    <mergeCell ref="DS4:EB4"/>
-    <mergeCell ref="EC4:EL4"/>
-    <mergeCell ref="JZ4:KB5"/>
-    <mergeCell ref="EW4:FF4"/>
-    <mergeCell ref="HO4:HX4"/>
-    <mergeCell ref="HY4:IH4"/>
-    <mergeCell ref="II4:IR4"/>
-    <mergeCell ref="JC4:JL4"/>
-    <mergeCell ref="JM4:JY5"/>
-    <mergeCell ref="FG4:FP4"/>
-    <mergeCell ref="FQ4:FZ4"/>
-    <mergeCell ref="GA4:GJ4"/>
-    <mergeCell ref="GK4:GT4"/>
-    <mergeCell ref="GU4:HD4"/>
-    <mergeCell ref="HE4:HN4"/>
-    <mergeCell ref="IS4:JB4"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A6">
     <cfRule type="duplicateValues" dxfId="0" priority="92"/>
@@ -5376,7 +6410,7 @@
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI1:AK3 AG1:AH4 AG7:AK7" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>36526</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="JZ6:KB999996" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="MR6:MT999996" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"4. High, 3. Medium High, 2. Medium Low, 1. Low, N/A"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[RUBY-2579] RUBY-2573: alter FCRM report - replace Growth with Additional FCRM GiA
</commit_message>
<xml_diff>
--- a/lib/fcerm1_template.xlsx
+++ b/lib/fcerm1_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lb000070\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A3B3BD-977F-460D-B4D1-61F23CCD872C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC3CA89-D856-4B66-BCD6-966DBA67D01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Master local choices" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Master local choices'!$A$6:$MU$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Master local choices'!$A$6:$NA$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="417">
   <si>
     <t>FCRM1 - National Capital Programme</t>
   </si>
@@ -237,9 +237,6 @@
     <t>Grant in Aid - PROJECT TOTAL</t>
   </si>
   <si>
-    <t>Growth - PROJECT TOTAL</t>
-  </si>
-  <si>
     <t>Local Levy - PROJECT TOTAL</t>
   </si>
   <si>
@@ -1297,6 +1294,27 @@
   </si>
   <si>
     <t>SEF GiA - 2032/33</t>
+  </si>
+  <si>
+    <t>Additional FCRM GiA (Asset replacement allowance) - PROJECT TOTAL</t>
+  </si>
+  <si>
+    <t>Additional FCRM GiA (Environment statutory funding) - PROJECT TOTAL</t>
+  </si>
+  <si>
+    <t>Additional FCRM GiA (Frequently flooded communities) - PROJECT TOTAL</t>
+  </si>
+  <si>
+    <t>Additional FCRM GiA (Other additional grant in aid) - PROJECT TOTAL</t>
+  </si>
+  <si>
+    <t>Additional FCRM GiA (Other Government department) - PROJECT TOTAL</t>
+  </si>
+  <si>
+    <t>Additional FCRM GiA (Recovery) - PROJECT TOTAL</t>
+  </si>
+  <si>
+    <t>Additional FCRM GiA (Summer economic fund) - PROJECT TOTAL</t>
   </si>
 </sst>
 </file>
@@ -2275,14 +2293,14 @@
     <tabColor rgb="FF92D050"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:MY7"/>
+  <dimension ref="A1:NE7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="Z7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="AE7" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
       <selection pane="topRight" activeCell="C7" sqref="C7"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="BT8" sqref="BT8"/>
+      <selection pane="bottomRight" activeCell="AT8" sqref="AT8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2299,18 +2317,18 @@
     <col min="22" max="23" width="21" style="4" customWidth="1"/>
     <col min="24" max="31" width="21" style="1" customWidth="1"/>
     <col min="32" max="37" width="21" style="5" customWidth="1"/>
-    <col min="38" max="348" width="21" style="1" customWidth="1"/>
-    <col min="349" max="355" width="21" style="6" customWidth="1"/>
-    <col min="356" max="358" width="22.33203125" style="6" customWidth="1"/>
-    <col min="359" max="359" width="17.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="360" max="360" width="19.6640625" style="6" customWidth="1"/>
-    <col min="361" max="361" width="21.5546875" style="6" customWidth="1"/>
-    <col min="362" max="362" width="19.6640625" style="6" customWidth="1"/>
-    <col min="363" max="363" width="21.5546875" style="6" customWidth="1"/>
-    <col min="364" max="16384" width="8.6640625" style="6"/>
+    <col min="38" max="354" width="21" style="1" customWidth="1"/>
+    <col min="355" max="361" width="21" style="6" customWidth="1"/>
+    <col min="362" max="364" width="22.33203125" style="6" customWidth="1"/>
+    <col min="365" max="365" width="17.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="366" max="366" width="19.6640625" style="6" customWidth="1"/>
+    <col min="367" max="367" width="21.5546875" style="6" customWidth="1"/>
+    <col min="368" max="368" width="19.6640625" style="6" customWidth="1"/>
+    <col min="369" max="369" width="21.5546875" style="6" customWidth="1"/>
+    <col min="370" max="16384" width="8.6640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:363" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:369" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="63" t="s">
         <v>0</v>
       </c>
@@ -2388,86 +2406,86 @@
       <c r="BU1" s="19"/>
       <c r="BV1" s="19"/>
       <c r="BW1" s="19"/>
-      <c r="BX1" s="26"/>
-      <c r="BY1" s="23"/>
-      <c r="BZ1" s="23"/>
-      <c r="CA1" s="23"/>
+      <c r="BX1" s="19"/>
+      <c r="BY1" s="19"/>
+      <c r="BZ1" s="19"/>
+      <c r="CA1" s="19"/>
       <c r="CB1" s="19"/>
       <c r="CC1" s="19"/>
-      <c r="CD1" s="19"/>
-      <c r="CE1" s="19"/>
-      <c r="CF1" s="19"/>
-      <c r="CG1" s="19"/>
-      <c r="CH1" s="26"/>
-      <c r="CI1" s="23"/>
-      <c r="CJ1" s="23"/>
-      <c r="CK1" s="23"/>
+      <c r="CD1" s="26"/>
+      <c r="CE1" s="23"/>
+      <c r="CF1" s="23"/>
+      <c r="CG1" s="23"/>
+      <c r="CH1" s="19"/>
+      <c r="CI1" s="19"/>
+      <c r="CJ1" s="19"/>
+      <c r="CK1" s="19"/>
       <c r="CL1" s="19"/>
       <c r="CM1" s="19"/>
-      <c r="CN1" s="19"/>
-      <c r="CO1" s="19"/>
-      <c r="CP1" s="19"/>
-      <c r="CQ1" s="19"/>
-      <c r="CR1" s="26"/>
-      <c r="CS1" s="23"/>
-      <c r="CT1" s="23"/>
-      <c r="CU1" s="23"/>
+      <c r="CN1" s="26"/>
+      <c r="CO1" s="23"/>
+      <c r="CP1" s="23"/>
+      <c r="CQ1" s="23"/>
+      <c r="CR1" s="19"/>
+      <c r="CS1" s="19"/>
+      <c r="CT1" s="19"/>
+      <c r="CU1" s="19"/>
       <c r="CV1" s="19"/>
       <c r="CW1" s="19"/>
-      <c r="CX1" s="19"/>
-      <c r="CY1" s="19"/>
-      <c r="CZ1" s="19"/>
-      <c r="DA1" s="19"/>
-      <c r="DB1" s="26"/>
-      <c r="DC1" s="23"/>
-      <c r="DD1" s="23"/>
-      <c r="DE1" s="23"/>
+      <c r="CX1" s="26"/>
+      <c r="CY1" s="23"/>
+      <c r="CZ1" s="23"/>
+      <c r="DA1" s="23"/>
+      <c r="DB1" s="19"/>
+      <c r="DC1" s="19"/>
+      <c r="DD1" s="19"/>
+      <c r="DE1" s="19"/>
       <c r="DF1" s="19"/>
       <c r="DG1" s="19"/>
-      <c r="DH1" s="19"/>
-      <c r="DI1" s="19"/>
-      <c r="DJ1" s="19"/>
-      <c r="DK1" s="19"/>
-      <c r="DL1" s="26"/>
-      <c r="DM1" s="23"/>
-      <c r="DN1" s="23"/>
-      <c r="DO1" s="23"/>
+      <c r="DH1" s="26"/>
+      <c r="DI1" s="23"/>
+      <c r="DJ1" s="23"/>
+      <c r="DK1" s="23"/>
+      <c r="DL1" s="19"/>
+      <c r="DM1" s="19"/>
+      <c r="DN1" s="19"/>
+      <c r="DO1" s="19"/>
       <c r="DP1" s="19"/>
       <c r="DQ1" s="19"/>
-      <c r="DR1" s="19"/>
-      <c r="DS1" s="19"/>
-      <c r="DT1" s="19"/>
-      <c r="DU1" s="19"/>
-      <c r="DV1" s="26"/>
-      <c r="DW1" s="23"/>
-      <c r="DX1" s="23"/>
-      <c r="DY1" s="23"/>
+      <c r="DR1" s="26"/>
+      <c r="DS1" s="23"/>
+      <c r="DT1" s="23"/>
+      <c r="DU1" s="23"/>
+      <c r="DV1" s="19"/>
+      <c r="DW1" s="19"/>
+      <c r="DX1" s="19"/>
+      <c r="DY1" s="19"/>
       <c r="DZ1" s="19"/>
       <c r="EA1" s="19"/>
-      <c r="EB1" s="19"/>
-      <c r="EC1" s="19"/>
-      <c r="ED1" s="19"/>
-      <c r="EE1" s="19"/>
-      <c r="EF1" s="26"/>
-      <c r="EG1" s="23"/>
-      <c r="EH1" s="23"/>
-      <c r="EI1" s="23"/>
+      <c r="EB1" s="26"/>
+      <c r="EC1" s="23"/>
+      <c r="ED1" s="23"/>
+      <c r="EE1" s="23"/>
+      <c r="EF1" s="19"/>
+      <c r="EG1" s="19"/>
+      <c r="EH1" s="19"/>
+      <c r="EI1" s="19"/>
       <c r="EJ1" s="19"/>
       <c r="EK1" s="19"/>
-      <c r="EL1" s="19"/>
-      <c r="EM1" s="19"/>
-      <c r="EN1" s="19"/>
-      <c r="EO1" s="19"/>
-      <c r="EP1" s="26"/>
-      <c r="EQ1" s="23"/>
-      <c r="ER1" s="23"/>
-      <c r="ES1" s="23"/>
+      <c r="EL1" s="26"/>
+      <c r="EM1" s="23"/>
+      <c r="EN1" s="23"/>
+      <c r="EO1" s="23"/>
+      <c r="EP1" s="19"/>
+      <c r="EQ1" s="19"/>
+      <c r="ER1" s="19"/>
+      <c r="ES1" s="19"/>
       <c r="ET1" s="19"/>
       <c r="EU1" s="19"/>
-      <c r="EV1" s="19"/>
-      <c r="EW1" s="19"/>
-      <c r="EX1" s="19"/>
-      <c r="EY1" s="19"/>
+      <c r="EV1" s="26"/>
+      <c r="EW1" s="23"/>
+      <c r="EX1" s="23"/>
+      <c r="EY1" s="23"/>
       <c r="EZ1" s="19"/>
       <c r="FA1" s="19"/>
       <c r="FB1" s="19"/>
@@ -2661,25 +2679,31 @@
       <c r="MH1" s="19"/>
       <c r="MI1" s="19"/>
       <c r="MJ1" s="19"/>
-      <c r="MK1" s="28"/>
-      <c r="ML1" s="28"/>
-      <c r="MM1" s="28"/>
-      <c r="MN1" s="28"/>
-      <c r="MO1" s="28"/>
-      <c r="MP1" s="28"/>
+      <c r="MK1" s="19"/>
+      <c r="ML1" s="19"/>
+      <c r="MM1" s="19"/>
+      <c r="MN1" s="19"/>
+      <c r="MO1" s="19"/>
+      <c r="MP1" s="19"/>
       <c r="MQ1" s="28"/>
-      <c r="MR1" s="39"/>
-      <c r="MS1" s="39"/>
-      <c r="MT1" s="39"/>
-      <c r="MU1" s="39"/>
-      <c r="MV1" s="39"/>
-      <c r="MW1" s="39"/>
+      <c r="MR1" s="28"/>
+      <c r="MS1" s="28"/>
+      <c r="MT1" s="28"/>
+      <c r="MU1" s="28"/>
+      <c r="MV1" s="28"/>
+      <c r="MW1" s="28"/>
       <c r="MX1" s="39"/>
       <c r="MY1" s="39"/>
+      <c r="MZ1" s="39"/>
+      <c r="NA1" s="39"/>
+      <c r="NB1" s="39"/>
+      <c r="NC1" s="39"/>
+      <c r="ND1" s="39"/>
+      <c r="NE1" s="39"/>
     </row>
-    <row r="2" spans="1:363" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:369" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="64" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B2" s="64"/>
       <c r="C2" s="19"/>
@@ -2753,91 +2777,91 @@
       <c r="BS2" s="19"/>
       <c r="BT2" s="19"/>
       <c r="BU2" s="19"/>
-      <c r="BV2" s="30"/>
-      <c r="BW2" s="30"/>
-      <c r="BX2" s="23"/>
-      <c r="BY2" s="23"/>
-      <c r="BZ2" s="23"/>
-      <c r="CA2" s="23"/>
-      <c r="CB2" s="19"/>
-      <c r="CC2" s="27"/>
-      <c r="CD2" s="27"/>
-      <c r="CE2" s="19"/>
-      <c r="CF2" s="30"/>
-      <c r="CG2" s="30"/>
-      <c r="CH2" s="23"/>
-      <c r="CI2" s="23"/>
-      <c r="CJ2" s="23"/>
-      <c r="CK2" s="23"/>
-      <c r="CL2" s="19"/>
-      <c r="CM2" s="27"/>
-      <c r="CN2" s="27"/>
-      <c r="CO2" s="19"/>
-      <c r="CP2" s="30"/>
-      <c r="CQ2" s="30"/>
-      <c r="CR2" s="23"/>
-      <c r="CS2" s="23"/>
-      <c r="CT2" s="23"/>
-      <c r="CU2" s="23"/>
-      <c r="CV2" s="19"/>
-      <c r="CW2" s="27"/>
-      <c r="CX2" s="27"/>
-      <c r="CY2" s="19"/>
-      <c r="CZ2" s="30"/>
-      <c r="DA2" s="30"/>
-      <c r="DB2" s="23"/>
-      <c r="DC2" s="23"/>
-      <c r="DD2" s="23"/>
-      <c r="DE2" s="23"/>
-      <c r="DF2" s="19"/>
-      <c r="DG2" s="27"/>
-      <c r="DH2" s="27"/>
-      <c r="DI2" s="19"/>
-      <c r="DJ2" s="30"/>
-      <c r="DK2" s="30"/>
-      <c r="DL2" s="23"/>
-      <c r="DM2" s="23"/>
-      <c r="DN2" s="23"/>
-      <c r="DO2" s="23"/>
-      <c r="DP2" s="19"/>
-      <c r="DQ2" s="27"/>
-      <c r="DR2" s="27"/>
-      <c r="DS2" s="19"/>
-      <c r="DT2" s="30"/>
-      <c r="DU2" s="30"/>
-      <c r="DV2" s="23"/>
-      <c r="DW2" s="23"/>
-      <c r="DX2" s="23"/>
-      <c r="DY2" s="23"/>
-      <c r="DZ2" s="19"/>
-      <c r="EA2" s="27"/>
-      <c r="EB2" s="27"/>
-      <c r="EC2" s="19"/>
-      <c r="ED2" s="30"/>
-      <c r="EE2" s="30"/>
-      <c r="EF2" s="23"/>
-      <c r="EG2" s="23"/>
-      <c r="EH2" s="23"/>
-      <c r="EI2" s="23"/>
-      <c r="EJ2" s="19"/>
-      <c r="EK2" s="27"/>
-      <c r="EL2" s="27"/>
-      <c r="EM2" s="19"/>
-      <c r="EN2" s="30"/>
-      <c r="EO2" s="30"/>
-      <c r="EP2" s="23"/>
-      <c r="EQ2" s="23"/>
-      <c r="ER2" s="23"/>
-      <c r="ES2" s="23"/>
-      <c r="ET2" s="19"/>
-      <c r="EU2" s="27"/>
-      <c r="EV2" s="27"/>
-      <c r="EW2" s="19"/>
-      <c r="EX2" s="19"/>
-      <c r="EY2" s="19"/>
+      <c r="BV2" s="19"/>
+      <c r="BW2" s="19"/>
+      <c r="BX2" s="19"/>
+      <c r="BY2" s="19"/>
+      <c r="BZ2" s="19"/>
+      <c r="CA2" s="19"/>
+      <c r="CB2" s="30"/>
+      <c r="CC2" s="30"/>
+      <c r="CD2" s="23"/>
+      <c r="CE2" s="23"/>
+      <c r="CF2" s="23"/>
+      <c r="CG2" s="23"/>
+      <c r="CH2" s="19"/>
+      <c r="CI2" s="27"/>
+      <c r="CJ2" s="27"/>
+      <c r="CK2" s="19"/>
+      <c r="CL2" s="30"/>
+      <c r="CM2" s="30"/>
+      <c r="CN2" s="23"/>
+      <c r="CO2" s="23"/>
+      <c r="CP2" s="23"/>
+      <c r="CQ2" s="23"/>
+      <c r="CR2" s="19"/>
+      <c r="CS2" s="27"/>
+      <c r="CT2" s="27"/>
+      <c r="CU2" s="19"/>
+      <c r="CV2" s="30"/>
+      <c r="CW2" s="30"/>
+      <c r="CX2" s="23"/>
+      <c r="CY2" s="23"/>
+      <c r="CZ2" s="23"/>
+      <c r="DA2" s="23"/>
+      <c r="DB2" s="19"/>
+      <c r="DC2" s="27"/>
+      <c r="DD2" s="27"/>
+      <c r="DE2" s="19"/>
+      <c r="DF2" s="30"/>
+      <c r="DG2" s="30"/>
+      <c r="DH2" s="23"/>
+      <c r="DI2" s="23"/>
+      <c r="DJ2" s="23"/>
+      <c r="DK2" s="23"/>
+      <c r="DL2" s="19"/>
+      <c r="DM2" s="27"/>
+      <c r="DN2" s="27"/>
+      <c r="DO2" s="19"/>
+      <c r="DP2" s="30"/>
+      <c r="DQ2" s="30"/>
+      <c r="DR2" s="23"/>
+      <c r="DS2" s="23"/>
+      <c r="DT2" s="23"/>
+      <c r="DU2" s="23"/>
+      <c r="DV2" s="19"/>
+      <c r="DW2" s="27"/>
+      <c r="DX2" s="27"/>
+      <c r="DY2" s="19"/>
+      <c r="DZ2" s="30"/>
+      <c r="EA2" s="30"/>
+      <c r="EB2" s="23"/>
+      <c r="EC2" s="23"/>
+      <c r="ED2" s="23"/>
+      <c r="EE2" s="23"/>
+      <c r="EF2" s="19"/>
+      <c r="EG2" s="27"/>
+      <c r="EH2" s="27"/>
+      <c r="EI2" s="19"/>
+      <c r="EJ2" s="30"/>
+      <c r="EK2" s="30"/>
+      <c r="EL2" s="23"/>
+      <c r="EM2" s="23"/>
+      <c r="EN2" s="23"/>
+      <c r="EO2" s="23"/>
+      <c r="EP2" s="19"/>
+      <c r="EQ2" s="27"/>
+      <c r="ER2" s="27"/>
+      <c r="ES2" s="19"/>
+      <c r="ET2" s="30"/>
+      <c r="EU2" s="30"/>
+      <c r="EV2" s="23"/>
+      <c r="EW2" s="23"/>
+      <c r="EX2" s="23"/>
+      <c r="EY2" s="23"/>
       <c r="EZ2" s="19"/>
-      <c r="FA2" s="19"/>
-      <c r="FB2" s="19"/>
+      <c r="FA2" s="27"/>
+      <c r="FB2" s="27"/>
       <c r="FC2" s="19"/>
       <c r="FD2" s="19"/>
       <c r="FE2" s="19"/>
@@ -3028,23 +3052,29 @@
       <c r="MH2" s="19"/>
       <c r="MI2" s="19"/>
       <c r="MJ2" s="19"/>
-      <c r="MK2" s="29"/>
-      <c r="ML2" s="29"/>
-      <c r="MM2" s="29"/>
-      <c r="MN2" s="29"/>
-      <c r="MO2" s="29"/>
-      <c r="MP2" s="29"/>
+      <c r="MK2" s="19"/>
+      <c r="ML2" s="19"/>
+      <c r="MM2" s="19"/>
+      <c r="MN2" s="19"/>
+      <c r="MO2" s="19"/>
+      <c r="MP2" s="19"/>
       <c r="MQ2" s="29"/>
-      <c r="MR2" s="39"/>
-      <c r="MS2" s="39"/>
-      <c r="MT2" s="39"/>
-      <c r="MU2" s="39"/>
-      <c r="MV2" s="39"/>
-      <c r="MW2" s="39"/>
+      <c r="MR2" s="29"/>
+      <c r="MS2" s="29"/>
+      <c r="MT2" s="29"/>
+      <c r="MU2" s="29"/>
+      <c r="MV2" s="29"/>
+      <c r="MW2" s="29"/>
       <c r="MX2" s="39"/>
       <c r="MY2" s="39"/>
+      <c r="MZ2" s="39"/>
+      <c r="NA2" s="39"/>
+      <c r="NB2" s="39"/>
+      <c r="NC2" s="39"/>
+      <c r="ND2" s="39"/>
+      <c r="NE2" s="39"/>
     </row>
-    <row r="3" spans="1:363" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:369" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="31"/>
       <c r="B3" s="32"/>
       <c r="C3" s="32"/>
@@ -3110,12 +3140,12 @@
       <c r="BK3" s="36"/>
       <c r="BL3" s="36"/>
       <c r="BM3" s="36"/>
-      <c r="BN3" s="37"/>
-      <c r="BO3" s="37"/>
-      <c r="BP3" s="37"/>
-      <c r="BQ3" s="37"/>
-      <c r="BR3" s="37"/>
-      <c r="BS3" s="37"/>
+      <c r="BN3" s="36"/>
+      <c r="BO3" s="36"/>
+      <c r="BP3" s="36"/>
+      <c r="BQ3" s="36"/>
+      <c r="BR3" s="36"/>
+      <c r="BS3" s="36"/>
       <c r="BT3" s="37"/>
       <c r="BU3" s="37"/>
       <c r="BV3" s="37"/>
@@ -3400,16 +3430,22 @@
       <c r="MO3" s="37"/>
       <c r="MP3" s="37"/>
       <c r="MQ3" s="37"/>
-      <c r="MR3" s="39"/>
-      <c r="MS3" s="39"/>
-      <c r="MT3" s="39"/>
-      <c r="MU3" s="39"/>
-      <c r="MV3" s="39"/>
-      <c r="MW3" s="39"/>
+      <c r="MR3" s="37"/>
+      <c r="MS3" s="37"/>
+      <c r="MT3" s="37"/>
+      <c r="MU3" s="37"/>
+      <c r="MV3" s="37"/>
+      <c r="MW3" s="37"/>
       <c r="MX3" s="39"/>
       <c r="MY3" s="39"/>
+      <c r="MZ3" s="39"/>
+      <c r="NA3" s="39"/>
+      <c r="NB3" s="39"/>
+      <c r="NC3" s="39"/>
+      <c r="ND3" s="39"/>
+      <c r="NE3" s="39"/>
     </row>
-    <row r="4" spans="1:363" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:369" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="65" t="s">
         <v>1</v>
       </c>
@@ -3434,7 +3470,7 @@
       <c r="N4" s="68"/>
       <c r="O4" s="68"/>
       <c r="P4" s="69" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="Q4" s="69"/>
       <c r="R4" s="69"/>
@@ -3490,371 +3526,377 @@
       <c r="BH4" s="74"/>
       <c r="BI4" s="74"/>
       <c r="BJ4" s="74"/>
-      <c r="BK4" s="72" t="s">
+      <c r="BK4" s="74"/>
+      <c r="BL4" s="74"/>
+      <c r="BM4" s="74"/>
+      <c r="BN4" s="74"/>
+      <c r="BO4" s="74"/>
+      <c r="BP4" s="74"/>
+      <c r="BQ4" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="BL4" s="72"/>
-      <c r="BM4" s="72"/>
-      <c r="BN4" s="72"/>
-      <c r="BO4" s="72"/>
-      <c r="BP4" s="72"/>
-      <c r="BQ4" s="72"/>
       <c r="BR4" s="72"/>
       <c r="BS4" s="72"/>
       <c r="BT4" s="72"/>
-      <c r="BU4" s="88" t="s">
+      <c r="BU4" s="72"/>
+      <c r="BV4" s="72"/>
+      <c r="BW4" s="72"/>
+      <c r="BX4" s="72"/>
+      <c r="BY4" s="72"/>
+      <c r="BZ4" s="72"/>
+      <c r="CA4" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="BV4" s="88"/>
-      <c r="BW4" s="88"/>
-      <c r="BX4" s="88"/>
-      <c r="BY4" s="88"/>
-      <c r="BZ4" s="88"/>
-      <c r="CA4" s="88"/>
       <c r="CB4" s="88"/>
       <c r="CC4" s="88"/>
       <c r="CD4" s="88"/>
-      <c r="CE4" s="89" t="s">
-        <v>334</v>
-      </c>
-      <c r="CF4" s="89"/>
-      <c r="CG4" s="89"/>
-      <c r="CH4" s="89"/>
-      <c r="CI4" s="89"/>
-      <c r="CJ4" s="89"/>
-      <c r="CK4" s="89"/>
+      <c r="CE4" s="88"/>
+      <c r="CF4" s="88"/>
+      <c r="CG4" s="88"/>
+      <c r="CH4" s="88"/>
+      <c r="CI4" s="88"/>
+      <c r="CJ4" s="88"/>
+      <c r="CK4" s="89" t="s">
+        <v>333</v>
+      </c>
       <c r="CL4" s="89"/>
       <c r="CM4" s="89"/>
       <c r="CN4" s="89"/>
-      <c r="CO4" s="88" t="s">
-        <v>335</v>
-      </c>
-      <c r="CP4" s="88"/>
-      <c r="CQ4" s="88"/>
-      <c r="CR4" s="88"/>
-      <c r="CS4" s="88"/>
-      <c r="CT4" s="88"/>
-      <c r="CU4" s="88"/>
+      <c r="CO4" s="89"/>
+      <c r="CP4" s="89"/>
+      <c r="CQ4" s="89"/>
+      <c r="CR4" s="89"/>
+      <c r="CS4" s="89"/>
+      <c r="CT4" s="89"/>
+      <c r="CU4" s="88" t="s">
+        <v>334</v>
+      </c>
       <c r="CV4" s="88"/>
       <c r="CW4" s="88"/>
       <c r="CX4" s="88"/>
-      <c r="CY4" s="89" t="s">
-        <v>336</v>
-      </c>
-      <c r="CZ4" s="89"/>
-      <c r="DA4" s="89"/>
-      <c r="DB4" s="89"/>
-      <c r="DC4" s="89"/>
-      <c r="DD4" s="89"/>
-      <c r="DE4" s="89"/>
+      <c r="CY4" s="88"/>
+      <c r="CZ4" s="88"/>
+      <c r="DA4" s="88"/>
+      <c r="DB4" s="88"/>
+      <c r="DC4" s="88"/>
+      <c r="DD4" s="88"/>
+      <c r="DE4" s="89" t="s">
+        <v>335</v>
+      </c>
       <c r="DF4" s="89"/>
       <c r="DG4" s="89"/>
       <c r="DH4" s="89"/>
-      <c r="DI4" s="88" t="s">
-        <v>337</v>
-      </c>
-      <c r="DJ4" s="88"/>
-      <c r="DK4" s="88"/>
-      <c r="DL4" s="88"/>
-      <c r="DM4" s="88"/>
-      <c r="DN4" s="88"/>
-      <c r="DO4" s="88"/>
+      <c r="DI4" s="89"/>
+      <c r="DJ4" s="89"/>
+      <c r="DK4" s="89"/>
+      <c r="DL4" s="89"/>
+      <c r="DM4" s="89"/>
+      <c r="DN4" s="89"/>
+      <c r="DO4" s="88" t="s">
+        <v>336</v>
+      </c>
       <c r="DP4" s="88"/>
       <c r="DQ4" s="88"/>
       <c r="DR4" s="88"/>
-      <c r="DS4" s="90" t="s">
-        <v>378</v>
-      </c>
-      <c r="DT4" s="91"/>
-      <c r="DU4" s="91"/>
-      <c r="DV4" s="91"/>
-      <c r="DW4" s="91"/>
-      <c r="DX4" s="91"/>
-      <c r="DY4" s="91"/>
+      <c r="DS4" s="88"/>
+      <c r="DT4" s="88"/>
+      <c r="DU4" s="88"/>
+      <c r="DV4" s="88"/>
+      <c r="DW4" s="88"/>
+      <c r="DX4" s="88"/>
+      <c r="DY4" s="90" t="s">
+        <v>377</v>
+      </c>
       <c r="DZ4" s="91"/>
       <c r="EA4" s="91"/>
-      <c r="EB4" s="92"/>
-      <c r="EC4" s="88" t="s">
-        <v>389</v>
-      </c>
-      <c r="ED4" s="88"/>
-      <c r="EE4" s="88"/>
-      <c r="EF4" s="88"/>
-      <c r="EG4" s="88"/>
-      <c r="EH4" s="88"/>
-      <c r="EI4" s="88"/>
+      <c r="EB4" s="91"/>
+      <c r="EC4" s="91"/>
+      <c r="ED4" s="91"/>
+      <c r="EE4" s="91"/>
+      <c r="EF4" s="91"/>
+      <c r="EG4" s="91"/>
+      <c r="EH4" s="92"/>
+      <c r="EI4" s="88" t="s">
+        <v>388</v>
+      </c>
       <c r="EJ4" s="88"/>
       <c r="EK4" s="88"/>
       <c r="EL4" s="88"/>
-      <c r="EM4" s="90" t="s">
-        <v>400</v>
-      </c>
-      <c r="EN4" s="91"/>
-      <c r="EO4" s="91"/>
-      <c r="EP4" s="91"/>
-      <c r="EQ4" s="91"/>
-      <c r="ER4" s="91"/>
-      <c r="ES4" s="91"/>
+      <c r="EM4" s="88"/>
+      <c r="EN4" s="88"/>
+      <c r="EO4" s="88"/>
+      <c r="EP4" s="88"/>
+      <c r="EQ4" s="88"/>
+      <c r="ER4" s="88"/>
+      <c r="ES4" s="90" t="s">
+        <v>399</v>
+      </c>
       <c r="ET4" s="91"/>
       <c r="EU4" s="91"/>
-      <c r="EV4" s="92"/>
-      <c r="EW4" s="75" t="s">
+      <c r="EV4" s="91"/>
+      <c r="EW4" s="91"/>
+      <c r="EX4" s="91"/>
+      <c r="EY4" s="91"/>
+      <c r="EZ4" s="91"/>
+      <c r="FA4" s="91"/>
+      <c r="FB4" s="92"/>
+      <c r="FC4" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="EX4" s="75"/>
-      <c r="EY4" s="75"/>
-      <c r="EZ4" s="75"/>
-      <c r="FA4" s="75"/>
-      <c r="FB4" s="75"/>
-      <c r="FC4" s="75"/>
       <c r="FD4" s="75"/>
       <c r="FE4" s="75"/>
       <c r="FF4" s="75"/>
-      <c r="FG4" s="76" t="s">
+      <c r="FG4" s="75"/>
+      <c r="FH4" s="75"/>
+      <c r="FI4" s="75"/>
+      <c r="FJ4" s="75"/>
+      <c r="FK4" s="75"/>
+      <c r="FL4" s="75"/>
+      <c r="FM4" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="FH4" s="76"/>
-      <c r="FI4" s="76"/>
-      <c r="FJ4" s="76"/>
-      <c r="FK4" s="76"/>
-      <c r="FL4" s="76"/>
-      <c r="FM4" s="76"/>
       <c r="FN4" s="76"/>
       <c r="FO4" s="76"/>
       <c r="FP4" s="76"/>
-      <c r="FQ4" s="77" t="s">
+      <c r="FQ4" s="76"/>
+      <c r="FR4" s="76"/>
+      <c r="FS4" s="76"/>
+      <c r="FT4" s="76"/>
+      <c r="FU4" s="76"/>
+      <c r="FV4" s="76"/>
+      <c r="FW4" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="FR4" s="77"/>
-      <c r="FS4" s="77"/>
-      <c r="FT4" s="77"/>
-      <c r="FU4" s="77"/>
-      <c r="FV4" s="77"/>
-      <c r="FW4" s="77"/>
       <c r="FX4" s="77"/>
       <c r="FY4" s="77"/>
       <c r="FZ4" s="77"/>
-      <c r="GA4" s="78" t="s">
+      <c r="GA4" s="77"/>
+      <c r="GB4" s="77"/>
+      <c r="GC4" s="77"/>
+      <c r="GD4" s="77"/>
+      <c r="GE4" s="77"/>
+      <c r="GF4" s="77"/>
+      <c r="GG4" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="GB4" s="78"/>
-      <c r="GC4" s="78"/>
-      <c r="GD4" s="78"/>
-      <c r="GE4" s="78"/>
-      <c r="GF4" s="78"/>
-      <c r="GG4" s="78"/>
       <c r="GH4" s="78"/>
       <c r="GI4" s="78"/>
       <c r="GJ4" s="78"/>
-      <c r="GK4" s="79" t="s">
+      <c r="GK4" s="78"/>
+      <c r="GL4" s="78"/>
+      <c r="GM4" s="78"/>
+      <c r="GN4" s="78"/>
+      <c r="GO4" s="78"/>
+      <c r="GP4" s="78"/>
+      <c r="GQ4" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="GL4" s="79"/>
-      <c r="GM4" s="79"/>
-      <c r="GN4" s="79"/>
-      <c r="GO4" s="79"/>
-      <c r="GP4" s="79"/>
-      <c r="GQ4" s="79"/>
       <c r="GR4" s="79"/>
       <c r="GS4" s="79"/>
       <c r="GT4" s="79"/>
-      <c r="GU4" s="80" t="s">
+      <c r="GU4" s="79"/>
+      <c r="GV4" s="79"/>
+      <c r="GW4" s="79"/>
+      <c r="GX4" s="79"/>
+      <c r="GY4" s="79"/>
+      <c r="GZ4" s="79"/>
+      <c r="HA4" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="GV4" s="80"/>
-      <c r="GW4" s="80"/>
-      <c r="GX4" s="80"/>
-      <c r="GY4" s="80"/>
-      <c r="GZ4" s="80"/>
-      <c r="HA4" s="80"/>
       <c r="HB4" s="80"/>
       <c r="HC4" s="80"/>
       <c r="HD4" s="80"/>
-      <c r="HE4" s="72" t="s">
-        <v>178</v>
-      </c>
-      <c r="HF4" s="72"/>
-      <c r="HG4" s="72"/>
-      <c r="HH4" s="72"/>
-      <c r="HI4" s="72"/>
-      <c r="HJ4" s="72"/>
-      <c r="HK4" s="72"/>
+      <c r="HE4" s="80"/>
+      <c r="HF4" s="80"/>
+      <c r="HG4" s="80"/>
+      <c r="HH4" s="80"/>
+      <c r="HI4" s="80"/>
+      <c r="HJ4" s="80"/>
+      <c r="HK4" s="72" t="s">
+        <v>177</v>
+      </c>
       <c r="HL4" s="72"/>
       <c r="HM4" s="72"/>
       <c r="HN4" s="72"/>
-      <c r="HO4" s="72" t="s">
-        <v>189</v>
-      </c>
+      <c r="HO4" s="72"/>
       <c r="HP4" s="72"/>
       <c r="HQ4" s="72"/>
       <c r="HR4" s="72"/>
       <c r="HS4" s="72"/>
       <c r="HT4" s="72"/>
-      <c r="HU4" s="72"/>
+      <c r="HU4" s="72" t="s">
+        <v>188</v>
+      </c>
       <c r="HV4" s="72"/>
       <c r="HW4" s="72"/>
       <c r="HX4" s="72"/>
-      <c r="HY4" s="72" t="s">
-        <v>200</v>
-      </c>
+      <c r="HY4" s="72"/>
       <c r="HZ4" s="72"/>
       <c r="IA4" s="72"/>
       <c r="IB4" s="72"/>
       <c r="IC4" s="72"/>
       <c r="ID4" s="72"/>
-      <c r="IE4" s="72"/>
+      <c r="IE4" s="72" t="s">
+        <v>199</v>
+      </c>
       <c r="IF4" s="72"/>
       <c r="IG4" s="72"/>
       <c r="IH4" s="72"/>
-      <c r="II4" s="72" t="s">
-        <v>211</v>
-      </c>
+      <c r="II4" s="72"/>
       <c r="IJ4" s="72"/>
       <c r="IK4" s="72"/>
       <c r="IL4" s="72"/>
       <c r="IM4" s="72"/>
       <c r="IN4" s="72"/>
-      <c r="IO4" s="72"/>
+      <c r="IO4" s="72" t="s">
+        <v>210</v>
+      </c>
       <c r="IP4" s="72"/>
       <c r="IQ4" s="72"/>
       <c r="IR4" s="72"/>
-      <c r="IS4" s="83" t="s">
-        <v>222</v>
-      </c>
-      <c r="IT4" s="84"/>
-      <c r="IU4" s="84"/>
-      <c r="IV4" s="84"/>
-      <c r="IW4" s="84"/>
-      <c r="IX4" s="84"/>
-      <c r="IY4" s="84"/>
+      <c r="IS4" s="72"/>
+      <c r="IT4" s="72"/>
+      <c r="IU4" s="72"/>
+      <c r="IV4" s="72"/>
+      <c r="IW4" s="72"/>
+      <c r="IX4" s="72"/>
+      <c r="IY4" s="83" t="s">
+        <v>221</v>
+      </c>
       <c r="IZ4" s="84"/>
       <c r="JA4" s="84"/>
-      <c r="JB4" s="85"/>
-      <c r="JC4" s="83" t="s">
-        <v>233</v>
-      </c>
+      <c r="JB4" s="84"/>
+      <c r="JC4" s="84"/>
       <c r="JD4" s="84"/>
       <c r="JE4" s="84"/>
       <c r="JF4" s="84"/>
       <c r="JG4" s="84"/>
-      <c r="JH4" s="84"/>
-      <c r="JI4" s="84"/>
+      <c r="JH4" s="85"/>
+      <c r="JI4" s="83" t="s">
+        <v>232</v>
+      </c>
       <c r="JJ4" s="84"/>
       <c r="JK4" s="84"/>
-      <c r="JL4" s="85"/>
-      <c r="JM4" s="83" t="s">
-        <v>244</v>
-      </c>
+      <c r="JL4" s="84"/>
+      <c r="JM4" s="84"/>
       <c r="JN4" s="84"/>
       <c r="JO4" s="84"/>
       <c r="JP4" s="84"/>
       <c r="JQ4" s="84"/>
-      <c r="JR4" s="84"/>
-      <c r="JS4" s="84"/>
+      <c r="JR4" s="85"/>
+      <c r="JS4" s="83" t="s">
+        <v>243</v>
+      </c>
       <c r="JT4" s="84"/>
       <c r="JU4" s="84"/>
-      <c r="JV4" s="85"/>
-      <c r="JW4" s="83" t="s">
-        <v>244</v>
-      </c>
+      <c r="JV4" s="84"/>
+      <c r="JW4" s="84"/>
       <c r="JX4" s="84"/>
       <c r="JY4" s="84"/>
       <c r="JZ4" s="84"/>
       <c r="KA4" s="84"/>
-      <c r="KB4" s="84"/>
-      <c r="KC4" s="84"/>
+      <c r="KB4" s="85"/>
+      <c r="KC4" s="83" t="s">
+        <v>243</v>
+      </c>
       <c r="KD4" s="84"/>
       <c r="KE4" s="84"/>
-      <c r="KF4" s="85"/>
-      <c r="KG4" s="83" t="s">
-        <v>265</v>
-      </c>
+      <c r="KF4" s="84"/>
+      <c r="KG4" s="84"/>
       <c r="KH4" s="84"/>
       <c r="KI4" s="84"/>
       <c r="KJ4" s="84"/>
       <c r="KK4" s="84"/>
-      <c r="KL4" s="84"/>
-      <c r="KM4" s="84"/>
+      <c r="KL4" s="85"/>
+      <c r="KM4" s="83" t="s">
+        <v>264</v>
+      </c>
       <c r="KN4" s="84"/>
       <c r="KO4" s="84"/>
-      <c r="KP4" s="85"/>
-      <c r="KQ4" s="86" t="s">
-        <v>276</v>
-      </c>
-      <c r="KR4" s="86"/>
-      <c r="KS4" s="86"/>
-      <c r="KT4" s="86"/>
-      <c r="KU4" s="86"/>
-      <c r="KV4" s="86"/>
-      <c r="KW4" s="86"/>
+      <c r="KP4" s="84"/>
+      <c r="KQ4" s="84"/>
+      <c r="KR4" s="84"/>
+      <c r="KS4" s="84"/>
+      <c r="KT4" s="84"/>
+      <c r="KU4" s="84"/>
+      <c r="KV4" s="85"/>
+      <c r="KW4" s="86" t="s">
+        <v>275</v>
+      </c>
       <c r="KX4" s="86"/>
       <c r="KY4" s="86"/>
       <c r="KZ4" s="86"/>
-      <c r="LA4" s="86" t="s">
-        <v>287</v>
-      </c>
+      <c r="LA4" s="86"/>
       <c r="LB4" s="86"/>
       <c r="LC4" s="86"/>
       <c r="LD4" s="86"/>
       <c r="LE4" s="86"/>
       <c r="LF4" s="86"/>
-      <c r="LG4" s="86"/>
+      <c r="LG4" s="86" t="s">
+        <v>286</v>
+      </c>
       <c r="LH4" s="86"/>
       <c r="LI4" s="86"/>
       <c r="LJ4" s="86"/>
-      <c r="LK4" s="86" t="s">
-        <v>293</v>
-      </c>
+      <c r="LK4" s="86"/>
       <c r="LL4" s="86"/>
       <c r="LM4" s="86"/>
       <c r="LN4" s="86"/>
       <c r="LO4" s="86"/>
       <c r="LP4" s="86"/>
-      <c r="LQ4" s="86"/>
+      <c r="LQ4" s="86" t="s">
+        <v>292</v>
+      </c>
       <c r="LR4" s="86"/>
       <c r="LS4" s="86"/>
       <c r="LT4" s="86"/>
-      <c r="LU4" s="86" t="s">
-        <v>304</v>
-      </c>
+      <c r="LU4" s="86"/>
       <c r="LV4" s="86"/>
       <c r="LW4" s="86"/>
       <c r="LX4" s="86"/>
       <c r="LY4" s="86"/>
       <c r="LZ4" s="86"/>
-      <c r="MA4" s="86"/>
+      <c r="MA4" s="86" t="s">
+        <v>303</v>
+      </c>
       <c r="MB4" s="86"/>
       <c r="MC4" s="86"/>
       <c r="MD4" s="86"/>
-      <c r="ME4" s="87" t="s">
+      <c r="ME4" s="86"/>
+      <c r="MF4" s="86"/>
+      <c r="MG4" s="86"/>
+      <c r="MH4" s="86"/>
+      <c r="MI4" s="86"/>
+      <c r="MJ4" s="86"/>
+      <c r="MK4" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="MF4" s="87"/>
-      <c r="MG4" s="87"/>
-      <c r="MH4" s="87"/>
-      <c r="MI4" s="87"/>
-      <c r="MJ4" s="87"/>
-      <c r="MK4" s="87"/>
       <c r="ML4" s="87"/>
       <c r="MM4" s="87"/>
       <c r="MN4" s="87"/>
       <c r="MO4" s="87"/>
       <c r="MP4" s="87"/>
       <c r="MQ4" s="87"/>
-      <c r="MR4" s="58" t="s">
-        <v>116</v>
-      </c>
-      <c r="MS4" s="81"/>
-      <c r="MT4" s="59"/>
-      <c r="MU4" s="38"/>
-      <c r="MV4" s="58" t="s">
-        <v>120</v>
-      </c>
-      <c r="MW4" s="59"/>
-      <c r="MX4" s="56"/>
-      <c r="MY4" s="54"/>
+      <c r="MR4" s="87"/>
+      <c r="MS4" s="87"/>
+      <c r="MT4" s="87"/>
+      <c r="MU4" s="87"/>
+      <c r="MV4" s="87"/>
+      <c r="MW4" s="87"/>
+      <c r="MX4" s="58" t="s">
+        <v>115</v>
+      </c>
+      <c r="MY4" s="81"/>
+      <c r="MZ4" s="59"/>
+      <c r="NA4" s="38"/>
+      <c r="NB4" s="58" t="s">
+        <v>119</v>
+      </c>
+      <c r="NC4" s="59"/>
+      <c r="ND4" s="56"/>
+      <c r="NE4" s="54"/>
     </row>
-    <row r="5" spans="1:363" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:369" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="65"/>
       <c r="B5" s="65"/>
       <c r="C5" s="66"/>
@@ -3917,852 +3959,852 @@
       <c r="BH5" s="74"/>
       <c r="BI5" s="74"/>
       <c r="BJ5" s="74"/>
-      <c r="BK5" s="7" t="s">
+      <c r="BK5" s="74"/>
+      <c r="BL5" s="74"/>
+      <c r="BM5" s="74"/>
+      <c r="BN5" s="74"/>
+      <c r="BO5" s="74"/>
+      <c r="BP5" s="74"/>
+      <c r="BQ5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="BL5" s="7" t="s">
+      <c r="BR5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="BM5" s="7" t="s">
+      <c r="BS5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="BN5" s="7" t="s">
+      <c r="BT5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="BO5" s="8" t="s">
+      <c r="BU5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="BP5" s="8" t="s">
+      <c r="BV5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="BQ5" s="8" t="s">
+      <c r="BW5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="BR5" s="8" t="s">
+      <c r="BX5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="BS5" s="8" t="s">
+      <c r="BY5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="BT5" s="8" t="s">
+      <c r="BZ5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="BU5" s="7" t="s">
+      <c r="CA5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="BV5" s="7" t="s">
+      <c r="CB5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="BW5" s="7" t="s">
+      <c r="CC5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="BX5" s="7" t="s">
+      <c r="CD5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="BY5" s="8" t="s">
+      <c r="CE5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="BZ5" s="8" t="s">
+      <c r="CF5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="CA5" s="8" t="s">
+      <c r="CG5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="CB5" s="8" t="s">
+      <c r="CH5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="CC5" s="8" t="s">
+      <c r="CI5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="CD5" s="8" t="s">
+      <c r="CJ5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="CE5" s="7" t="s">
+      <c r="CK5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="CF5" s="7" t="s">
+      <c r="CL5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="CG5" s="7" t="s">
+      <c r="CM5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="CH5" s="7" t="s">
+      <c r="CN5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="CI5" s="8" t="s">
+      <c r="CO5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="CJ5" s="8" t="s">
+      <c r="CP5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="CK5" s="8" t="s">
+      <c r="CQ5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="CL5" s="8" t="s">
+      <c r="CR5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="CM5" s="8" t="s">
+      <c r="CS5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="CN5" s="8" t="s">
+      <c r="CT5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="CO5" s="7" t="s">
+      <c r="CU5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="CP5" s="7" t="s">
+      <c r="CV5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="CQ5" s="7" t="s">
+      <c r="CW5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="CR5" s="7" t="s">
+      <c r="CX5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="CS5" s="8" t="s">
+      <c r="CY5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="CT5" s="8" t="s">
+      <c r="CZ5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="CU5" s="8" t="s">
+      <c r="DA5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="CV5" s="8" t="s">
+      <c r="DB5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="CW5" s="8" t="s">
+      <c r="DC5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="CX5" s="8" t="s">
+      <c r="DD5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="CY5" s="7" t="s">
+      <c r="DE5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="CZ5" s="7" t="s">
+      <c r="DF5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="DA5" s="7" t="s">
+      <c r="DG5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="DB5" s="7" t="s">
+      <c r="DH5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="DC5" s="8" t="s">
+      <c r="DI5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="DD5" s="8" t="s">
+      <c r="DJ5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="DE5" s="8" t="s">
+      <c r="DK5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="DF5" s="8" t="s">
+      <c r="DL5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="DG5" s="8" t="s">
+      <c r="DM5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="DH5" s="8" t="s">
+      <c r="DN5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="DI5" s="7" t="s">
+      <c r="DO5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="DJ5" s="7" t="s">
+      <c r="DP5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="DK5" s="7" t="s">
+      <c r="DQ5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="DL5" s="7" t="s">
+      <c r="DR5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="DM5" s="8" t="s">
+      <c r="DS5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="DN5" s="8" t="s">
+      <c r="DT5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="DO5" s="8" t="s">
+      <c r="DU5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="DP5" s="8" t="s">
+      <c r="DV5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="DQ5" s="8" t="s">
+      <c r="DW5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="DR5" s="8" t="s">
+      <c r="DX5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="DS5" s="7" t="s">
+      <c r="DY5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="DT5" s="7" t="s">
+      <c r="DZ5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="DU5" s="7" t="s">
+      <c r="EA5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="DV5" s="7" t="s">
+      <c r="EB5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="DW5" s="8" t="s">
+      <c r="EC5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="DX5" s="8" t="s">
+      <c r="ED5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="DY5" s="8" t="s">
+      <c r="EE5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="DZ5" s="8" t="s">
+      <c r="EF5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="EA5" s="8" t="s">
+      <c r="EG5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="EB5" s="8" t="s">
+      <c r="EH5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="EC5" s="7" t="s">
+      <c r="EI5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="ED5" s="7" t="s">
+      <c r="EJ5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="EE5" s="7" t="s">
+      <c r="EK5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="EF5" s="7" t="s">
+      <c r="EL5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="EG5" s="8" t="s">
+      <c r="EM5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="EH5" s="8" t="s">
+      <c r="EN5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="EI5" s="8" t="s">
+      <c r="EO5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="EJ5" s="8" t="s">
+      <c r="EP5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="EK5" s="8" t="s">
+      <c r="EQ5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="EL5" s="8" t="s">
+      <c r="ER5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="EM5" s="7" t="s">
+      <c r="ES5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="EN5" s="7" t="s">
+      <c r="ET5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="EO5" s="7" t="s">
+      <c r="EU5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="EP5" s="7" t="s">
+      <c r="EV5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="EQ5" s="8" t="s">
+      <c r="EW5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="ER5" s="8" t="s">
+      <c r="EX5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="ES5" s="8" t="s">
+      <c r="EY5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="ET5" s="8" t="s">
+      <c r="EZ5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="EU5" s="8" t="s">
+      <c r="FA5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="EV5" s="8" t="s">
+      <c r="FB5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="EW5" s="7" t="s">
+      <c r="FC5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="EX5" s="7" t="s">
+      <c r="FD5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="EY5" s="7" t="s">
+      <c r="FE5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="EZ5" s="7" t="s">
+      <c r="FF5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="FA5" s="8" t="s">
+      <c r="FG5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="FB5" s="8" t="s">
+      <c r="FH5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="FC5" s="8" t="s">
+      <c r="FI5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="FD5" s="8" t="s">
+      <c r="FJ5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="FE5" s="8" t="s">
+      <c r="FK5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="FF5" s="8" t="s">
+      <c r="FL5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="FG5" s="7" t="s">
+      <c r="FM5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="FH5" s="7" t="s">
+      <c r="FN5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="FI5" s="7" t="s">
+      <c r="FO5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="FJ5" s="7" t="s">
+      <c r="FP5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="FK5" s="8" t="s">
+      <c r="FQ5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="FL5" s="8" t="s">
+      <c r="FR5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="FM5" s="8" t="s">
+      <c r="FS5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="FN5" s="8" t="s">
+      <c r="FT5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="FO5" s="8" t="s">
+      <c r="FU5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="FP5" s="8" t="s">
+      <c r="FV5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="FQ5" s="7" t="s">
+      <c r="FW5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="FR5" s="7" t="s">
+      <c r="FX5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="FS5" s="7" t="s">
+      <c r="FY5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="FT5" s="7" t="s">
+      <c r="FZ5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="FU5" s="8" t="s">
+      <c r="GA5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="FV5" s="8" t="s">
+      <c r="GB5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="FW5" s="8" t="s">
+      <c r="GC5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="FX5" s="8" t="s">
+      <c r="GD5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="FY5" s="8" t="s">
+      <c r="GE5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="FZ5" s="8" t="s">
+      <c r="GF5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="GA5" s="7" t="s">
+      <c r="GG5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="GB5" s="7" t="s">
+      <c r="GH5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="GC5" s="7" t="s">
+      <c r="GI5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="GD5" s="7" t="s">
+      <c r="GJ5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="GE5" s="8" t="s">
+      <c r="GK5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="GF5" s="8" t="s">
+      <c r="GL5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="GG5" s="8" t="s">
+      <c r="GM5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="GH5" s="8" t="s">
+      <c r="GN5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="GI5" s="8" t="s">
+      <c r="GO5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="GJ5" s="8" t="s">
+      <c r="GP5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="GK5" s="7" t="s">
+      <c r="GQ5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="GL5" s="7" t="s">
+      <c r="GR5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="GM5" s="7" t="s">
+      <c r="GS5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="GN5" s="7" t="s">
+      <c r="GT5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="GO5" s="8" t="s">
+      <c r="GU5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="GP5" s="8" t="s">
+      <c r="GV5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="GQ5" s="8" t="s">
+      <c r="GW5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="GR5" s="8" t="s">
+      <c r="GX5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="GS5" s="8" t="s">
+      <c r="GY5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="GT5" s="8" t="s">
+      <c r="GZ5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="GU5" s="7" t="s">
+      <c r="HA5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="GV5" s="7" t="s">
+      <c r="HB5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="GW5" s="7" t="s">
+      <c r="HC5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="GX5" s="7" t="s">
+      <c r="HD5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="GY5" s="8" t="s">
+      <c r="HE5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="GZ5" s="8" t="s">
+      <c r="HF5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="HA5" s="8" t="s">
+      <c r="HG5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="HB5" s="8" t="s">
+      <c r="HH5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="HC5" s="8" t="s">
+      <c r="HI5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="HD5" s="8" t="s">
+      <c r="HJ5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="HE5" s="7" t="s">
+      <c r="HK5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="HF5" s="7" t="s">
+      <c r="HL5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="HG5" s="7" t="s">
+      <c r="HM5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="HH5" s="7" t="s">
+      <c r="HN5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="HI5" s="8" t="s">
+      <c r="HO5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="HJ5" s="8" t="s">
+      <c r="HP5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="HK5" s="8" t="s">
+      <c r="HQ5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="HL5" s="8" t="s">
+      <c r="HR5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="HM5" s="8" t="s">
+      <c r="HS5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="HN5" s="8" t="s">
+      <c r="HT5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="HO5" s="7" t="s">
+      <c r="HU5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="HP5" s="7" t="s">
+      <c r="HV5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="HQ5" s="7" t="s">
+      <c r="HW5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="HR5" s="7" t="s">
+      <c r="HX5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="HS5" s="8" t="s">
+      <c r="HY5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="HT5" s="8" t="s">
+      <c r="HZ5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="HU5" s="8" t="s">
+      <c r="IA5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="HV5" s="8" t="s">
+      <c r="IB5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="HW5" s="8" t="s">
+      <c r="IC5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="HX5" s="8" t="s">
+      <c r="ID5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="HY5" s="7" t="s">
+      <c r="IE5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="HZ5" s="7" t="s">
+      <c r="IF5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="IA5" s="7" t="s">
+      <c r="IG5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="IB5" s="7" t="s">
+      <c r="IH5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="IC5" s="8" t="s">
+      <c r="II5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="ID5" s="8" t="s">
+      <c r="IJ5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="IE5" s="8" t="s">
+      <c r="IK5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="IF5" s="8" t="s">
+      <c r="IL5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="IG5" s="8" t="s">
+      <c r="IM5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="IH5" s="8" t="s">
+      <c r="IN5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="II5" s="7" t="s">
+      <c r="IO5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="IJ5" s="7" t="s">
+      <c r="IP5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="IK5" s="7" t="s">
+      <c r="IQ5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="IL5" s="7" t="s">
+      <c r="IR5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="IM5" s="8" t="s">
+      <c r="IS5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="IN5" s="8" t="s">
+      <c r="IT5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="IO5" s="8" t="s">
+      <c r="IU5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="IP5" s="8" t="s">
+      <c r="IV5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="IQ5" s="8" t="s">
+      <c r="IW5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="IR5" s="8" t="s">
+      <c r="IX5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="IS5" s="7" t="s">
+      <c r="IY5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="IT5" s="7" t="s">
+      <c r="IZ5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="IU5" s="7" t="s">
+      <c r="JA5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="IV5" s="7" t="s">
+      <c r="JB5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="IW5" s="8" t="s">
+      <c r="JC5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="IX5" s="8" t="s">
+      <c r="JD5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="IY5" s="8" t="s">
+      <c r="JE5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="IZ5" s="8" t="s">
+      <c r="JF5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="JA5" s="8" t="s">
+      <c r="JG5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="JB5" s="8" t="s">
+      <c r="JH5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="JC5" s="7" t="s">
+      <c r="JI5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="JD5" s="7" t="s">
+      <c r="JJ5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="JE5" s="7" t="s">
+      <c r="JK5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="JF5" s="7" t="s">
+      <c r="JL5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="JG5" s="8" t="s">
+      <c r="JM5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="JH5" s="8" t="s">
+      <c r="JN5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="JI5" s="8" t="s">
+      <c r="JO5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="JJ5" s="8" t="s">
+      <c r="JP5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="JK5" s="8" t="s">
+      <c r="JQ5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="JL5" s="8" t="s">
+      <c r="JR5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="JM5" s="7" t="s">
+      <c r="JS5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="JN5" s="7" t="s">
+      <c r="JT5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="JO5" s="7" t="s">
+      <c r="JU5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="JP5" s="7" t="s">
+      <c r="JV5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="JQ5" s="8" t="s">
+      <c r="JW5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="JR5" s="8" t="s">
+      <c r="JX5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="JS5" s="8" t="s">
+      <c r="JY5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="JT5" s="8" t="s">
+      <c r="JZ5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="JU5" s="8" t="s">
+      <c r="KA5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="JV5" s="8" t="s">
+      <c r="KB5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="JW5" s="7" t="s">
+      <c r="KC5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="JX5" s="7" t="s">
+      <c r="KD5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="JY5" s="7" t="s">
+      <c r="KE5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="JZ5" s="7" t="s">
+      <c r="KF5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="KA5" s="8" t="s">
+      <c r="KG5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="KB5" s="8" t="s">
+      <c r="KH5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="KC5" s="8" t="s">
+      <c r="KI5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="KD5" s="8" t="s">
+      <c r="KJ5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="KE5" s="8" t="s">
+      <c r="KK5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="KF5" s="8" t="s">
+      <c r="KL5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="KG5" s="7" t="s">
+      <c r="KM5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="KH5" s="7" t="s">
+      <c r="KN5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="KI5" s="7" t="s">
+      <c r="KO5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="KJ5" s="7" t="s">
+      <c r="KP5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="KK5" s="8" t="s">
+      <c r="KQ5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="KL5" s="8" t="s">
+      <c r="KR5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="KM5" s="8" t="s">
+      <c r="KS5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="KN5" s="8" t="s">
+      <c r="KT5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="KO5" s="8" t="s">
+      <c r="KU5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="KP5" s="8" t="s">
+      <c r="KV5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="KQ5" s="7" t="s">
+      <c r="KW5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="KR5" s="7" t="s">
+      <c r="KX5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="KS5" s="7" t="s">
+      <c r="KY5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="KT5" s="7" t="s">
+      <c r="KZ5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="KU5" s="8" t="s">
+      <c r="LA5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="KV5" s="8" t="s">
+      <c r="LB5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="KW5" s="8" t="s">
+      <c r="LC5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="KX5" s="8" t="s">
+      <c r="LD5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="KY5" s="8" t="s">
+      <c r="LE5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="KZ5" s="8" t="s">
+      <c r="LF5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="LA5" s="7" t="s">
+      <c r="LG5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="LB5" s="7" t="s">
+      <c r="LH5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="LC5" s="7" t="s">
+      <c r="LI5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="LD5" s="7" t="s">
+      <c r="LJ5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="LE5" s="8" t="s">
+      <c r="LK5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="LF5" s="8" t="s">
+      <c r="LL5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="LG5" s="8" t="s">
+      <c r="LM5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="LH5" s="8" t="s">
+      <c r="LN5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="LI5" s="8" t="s">
+      <c r="LO5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="LJ5" s="8" t="s">
+      <c r="LP5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="LK5" s="7" t="s">
+      <c r="LQ5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="LL5" s="7" t="s">
+      <c r="LR5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="LM5" s="7" t="s">
+      <c r="LS5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="LN5" s="7" t="s">
+      <c r="LT5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="LO5" s="8" t="s">
+      <c r="LU5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="LP5" s="8" t="s">
+      <c r="LV5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="LQ5" s="8" t="s">
+      <c r="LW5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="LR5" s="8" t="s">
+      <c r="LX5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="LS5" s="8" t="s">
+      <c r="LY5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="LT5" s="8" t="s">
+      <c r="LZ5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="LU5" s="7" t="s">
+      <c r="MA5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="LV5" s="7" t="s">
+      <c r="MB5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="LW5" s="7" t="s">
+      <c r="MC5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="LX5" s="7" t="s">
+      <c r="MD5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="LY5" s="8" t="s">
+      <c r="ME5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="LZ5" s="8" t="s">
+      <c r="MF5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="MA5" s="8" t="s">
+      <c r="MG5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="MB5" s="8" t="s">
+      <c r="MH5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="MC5" s="8" t="s">
+      <c r="MI5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="MD5" s="8" t="s">
+      <c r="MJ5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="ME5" s="87"/>
-      <c r="MF5" s="87"/>
-      <c r="MG5" s="87"/>
-      <c r="MH5" s="87"/>
-      <c r="MI5" s="87"/>
-      <c r="MJ5" s="87"/>
       <c r="MK5" s="87"/>
       <c r="ML5" s="87"/>
       <c r="MM5" s="87"/>
@@ -4770,16 +4812,22 @@
       <c r="MO5" s="87"/>
       <c r="MP5" s="87"/>
       <c r="MQ5" s="87"/>
-      <c r="MR5" s="60"/>
-      <c r="MS5" s="82"/>
-      <c r="MT5" s="61"/>
-      <c r="MU5" s="38"/>
-      <c r="MV5" s="60"/>
-      <c r="MW5" s="61"/>
-      <c r="MX5" s="57"/>
-      <c r="MY5" s="55"/>
+      <c r="MR5" s="87"/>
+      <c r="MS5" s="87"/>
+      <c r="MT5" s="87"/>
+      <c r="MU5" s="87"/>
+      <c r="MV5" s="87"/>
+      <c r="MW5" s="87"/>
+      <c r="MX5" s="60"/>
+      <c r="MY5" s="82"/>
+      <c r="MZ5" s="61"/>
+      <c r="NA5" s="38"/>
+      <c r="NB5" s="60"/>
+      <c r="NC5" s="61"/>
+      <c r="ND5" s="57"/>
+      <c r="NE5" s="55"/>
     </row>
-    <row r="6" spans="1:363" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:369" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>24</v>
       </c>
@@ -4871,7 +4919,7 @@
         <v>53</v>
       </c>
       <c r="AE6" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AF6" s="16" t="s">
         <v>54</v>
@@ -4880,7 +4928,7 @@
         <v>55</v>
       </c>
       <c r="AH6" s="17" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AI6" s="17" t="s">
         <v>56</v>
@@ -4898,983 +4946,1001 @@
         <v>60</v>
       </c>
       <c r="AN6" s="18" t="s">
+        <v>410</v>
+      </c>
+      <c r="AO6" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="AP6" s="18" t="s">
+        <v>412</v>
+      </c>
+      <c r="AQ6" s="18" t="s">
+        <v>413</v>
+      </c>
+      <c r="AR6" s="18" t="s">
+        <v>414</v>
+      </c>
+      <c r="AS6" s="18" t="s">
+        <v>415</v>
+      </c>
+      <c r="AT6" s="18" t="s">
+        <v>416</v>
+      </c>
+      <c r="AU6" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="AO6" s="18" t="s">
+      <c r="AV6" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="AP6" s="18" t="s">
+      <c r="AW6" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="AQ6" s="18" t="s">
+      <c r="AX6" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="AR6" s="18" t="s">
+      <c r="AY6" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="AS6" s="18" t="s">
+      <c r="AZ6" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="AT6" s="18" t="s">
+      <c r="BA6" s="18" t="s">
+        <v>319</v>
+      </c>
+      <c r="BB6" s="18" t="s">
+        <v>320</v>
+      </c>
+      <c r="BC6" s="18" t="s">
+        <v>321</v>
+      </c>
+      <c r="BD6" s="18" t="s">
+        <v>322</v>
+      </c>
+      <c r="BE6" s="18" t="s">
+        <v>323</v>
+      </c>
+      <c r="BF6" s="18" t="s">
+        <v>324</v>
+      </c>
+      <c r="BG6" s="18" t="s">
+        <v>325</v>
+      </c>
+      <c r="BH6" s="18" t="s">
+        <v>326</v>
+      </c>
+      <c r="BI6" s="18" t="s">
+        <v>327</v>
+      </c>
+      <c r="BJ6" s="18" t="s">
+        <v>328</v>
+      </c>
+      <c r="BK6" s="18" t="s">
+        <v>329</v>
+      </c>
+      <c r="BL6" s="18" t="s">
+        <v>330</v>
+      </c>
+      <c r="BM6" s="18" t="s">
+        <v>331</v>
+      </c>
+      <c r="BN6" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="AU6" s="18" t="s">
-        <v>320</v>
-      </c>
-      <c r="AV6" s="18" t="s">
-        <v>321</v>
-      </c>
-      <c r="AW6" s="18" t="s">
-        <v>322</v>
-      </c>
-      <c r="AX6" s="18" t="s">
-        <v>323</v>
-      </c>
-      <c r="AY6" s="18" t="s">
-        <v>324</v>
-      </c>
-      <c r="AZ6" s="18" t="s">
-        <v>325</v>
-      </c>
-      <c r="BA6" s="18" t="s">
-        <v>326</v>
-      </c>
-      <c r="BB6" s="18" t="s">
-        <v>327</v>
-      </c>
-      <c r="BC6" s="18" t="s">
-        <v>328</v>
-      </c>
-      <c r="BD6" s="18" t="s">
-        <v>329</v>
-      </c>
-      <c r="BE6" s="18" t="s">
-        <v>330</v>
-      </c>
-      <c r="BF6" s="18" t="s">
-        <v>331</v>
-      </c>
-      <c r="BG6" s="18" t="s">
-        <v>332</v>
-      </c>
-      <c r="BH6" s="18" t="s">
+      <c r="BO6" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="BI6" s="18" t="s">
+      <c r="BP6" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="BJ6" s="18" t="s">
+      <c r="BQ6" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="BK6" s="18" t="s">
+      <c r="BR6" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="BL6" s="18" t="s">
+      <c r="BS6" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="BM6" s="18" t="s">
+      <c r="BT6" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="BN6" s="18" t="s">
+      <c r="BU6" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="BV6" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="BW6" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="BX6" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="BY6" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="BZ6" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="CA6" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="BO6" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="BP6" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="BQ6" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="BR6" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="BS6" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="BT6" s="18" t="s">
+      <c r="CB6" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="CC6" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="CD6" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="CE6" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="BU6" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="BV6" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="BW6" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="BX6" s="18" t="s">
+      <c r="CF6" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="CG6" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="CH6" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="CI6" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="CJ6" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="CK6" s="18" t="s">
+        <v>337</v>
+      </c>
+      <c r="CL6" s="18" t="s">
+        <v>338</v>
+      </c>
+      <c r="CM6" s="18" t="s">
+        <v>339</v>
+      </c>
+      <c r="CN6" s="18" t="s">
+        <v>340</v>
+      </c>
+      <c r="CO6" s="18" t="s">
+        <v>341</v>
+      </c>
+      <c r="CP6" s="18" t="s">
+        <v>342</v>
+      </c>
+      <c r="CQ6" s="18" t="s">
+        <v>343</v>
+      </c>
+      <c r="CR6" s="18" t="s">
+        <v>344</v>
+      </c>
+      <c r="CS6" s="18" t="s">
+        <v>345</v>
+      </c>
+      <c r="CT6" s="18" t="s">
+        <v>346</v>
+      </c>
+      <c r="CU6" s="18" t="s">
+        <v>347</v>
+      </c>
+      <c r="CV6" s="18" t="s">
+        <v>348</v>
+      </c>
+      <c r="CW6" s="18" t="s">
+        <v>349</v>
+      </c>
+      <c r="CX6" s="18" t="s">
+        <v>350</v>
+      </c>
+      <c r="CY6" s="18" t="s">
+        <v>351</v>
+      </c>
+      <c r="CZ6" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="DA6" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="DB6" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="DC6" s="18" t="s">
+        <v>355</v>
+      </c>
+      <c r="DD6" s="18" t="s">
+        <v>356</v>
+      </c>
+      <c r="DE6" s="18" t="s">
+        <v>357</v>
+      </c>
+      <c r="DF6" s="18" t="s">
+        <v>358</v>
+      </c>
+      <c r="DG6" s="18" t="s">
+        <v>359</v>
+      </c>
+      <c r="DH6" s="18" t="s">
+        <v>360</v>
+      </c>
+      <c r="DI6" s="18" t="s">
+        <v>361</v>
+      </c>
+      <c r="DJ6" s="18" t="s">
+        <v>362</v>
+      </c>
+      <c r="DK6" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="DL6" s="18" t="s">
+        <v>364</v>
+      </c>
+      <c r="DM6" s="18" t="s">
+        <v>365</v>
+      </c>
+      <c r="DN6" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="DO6" s="18" t="s">
+        <v>367</v>
+      </c>
+      <c r="DP6" s="18" t="s">
+        <v>368</v>
+      </c>
+      <c r="DQ6" s="18" t="s">
+        <v>369</v>
+      </c>
+      <c r="DR6" s="18" t="s">
+        <v>370</v>
+      </c>
+      <c r="DS6" s="18" t="s">
+        <v>371</v>
+      </c>
+      <c r="DT6" s="18" t="s">
+        <v>372</v>
+      </c>
+      <c r="DU6" s="18" t="s">
+        <v>373</v>
+      </c>
+      <c r="DV6" s="18" t="s">
+        <v>374</v>
+      </c>
+      <c r="DW6" s="18" t="s">
+        <v>375</v>
+      </c>
+      <c r="DX6" s="18" t="s">
+        <v>376</v>
+      </c>
+      <c r="DY6" s="18" t="s">
+        <v>378</v>
+      </c>
+      <c r="DZ6" s="18" t="s">
+        <v>379</v>
+      </c>
+      <c r="EA6" s="18" t="s">
+        <v>380</v>
+      </c>
+      <c r="EB6" s="18" t="s">
+        <v>381</v>
+      </c>
+      <c r="EC6" s="18" t="s">
+        <v>382</v>
+      </c>
+      <c r="ED6" s="18" t="s">
+        <v>383</v>
+      </c>
+      <c r="EE6" s="18" t="s">
+        <v>384</v>
+      </c>
+      <c r="EF6" s="18" t="s">
+        <v>385</v>
+      </c>
+      <c r="EG6" s="18" t="s">
+        <v>386</v>
+      </c>
+      <c r="EH6" s="18" t="s">
+        <v>387</v>
+      </c>
+      <c r="EI6" s="18" t="s">
+        <v>389</v>
+      </c>
+      <c r="EJ6" s="18" t="s">
+        <v>390</v>
+      </c>
+      <c r="EK6" s="18" t="s">
+        <v>391</v>
+      </c>
+      <c r="EL6" s="18" t="s">
+        <v>392</v>
+      </c>
+      <c r="EM6" s="18" t="s">
+        <v>393</v>
+      </c>
+      <c r="EN6" s="18" t="s">
+        <v>394</v>
+      </c>
+      <c r="EO6" s="18" t="s">
+        <v>395</v>
+      </c>
+      <c r="EP6" s="18" t="s">
+        <v>396</v>
+      </c>
+      <c r="EQ6" s="18" t="s">
+        <v>397</v>
+      </c>
+      <c r="ER6" s="18" t="s">
+        <v>398</v>
+      </c>
+      <c r="ES6" s="18" t="s">
+        <v>400</v>
+      </c>
+      <c r="ET6" s="18" t="s">
+        <v>401</v>
+      </c>
+      <c r="EU6" s="18" t="s">
+        <v>402</v>
+      </c>
+      <c r="EV6" s="18" t="s">
+        <v>403</v>
+      </c>
+      <c r="EW6" s="18" t="s">
+        <v>404</v>
+      </c>
+      <c r="EX6" s="18" t="s">
+        <v>405</v>
+      </c>
+      <c r="EY6" s="18" t="s">
+        <v>406</v>
+      </c>
+      <c r="EZ6" s="18" t="s">
+        <v>407</v>
+      </c>
+      <c r="FA6" s="18" t="s">
+        <v>408</v>
+      </c>
+      <c r="FB6" s="18" t="s">
+        <v>409</v>
+      </c>
+      <c r="FC6" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="BY6" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="BZ6" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="CA6" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="CB6" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="CC6" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="CD6" s="18" t="s">
+      <c r="FD6" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="FE6" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="FF6" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="FG6" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="CE6" s="18" t="s">
-        <v>338</v>
-      </c>
-      <c r="CF6" s="18" t="s">
-        <v>339</v>
-      </c>
-      <c r="CG6" s="18" t="s">
-        <v>340</v>
-      </c>
-      <c r="CH6" s="18" t="s">
-        <v>341</v>
-      </c>
-      <c r="CI6" s="18" t="s">
-        <v>342</v>
-      </c>
-      <c r="CJ6" s="18" t="s">
-        <v>343</v>
-      </c>
-      <c r="CK6" s="18" t="s">
-        <v>344</v>
-      </c>
-      <c r="CL6" s="18" t="s">
-        <v>345</v>
-      </c>
-      <c r="CM6" s="18" t="s">
-        <v>346</v>
-      </c>
-      <c r="CN6" s="18" t="s">
-        <v>347</v>
-      </c>
-      <c r="CO6" s="18" t="s">
-        <v>348</v>
-      </c>
-      <c r="CP6" s="18" t="s">
-        <v>349</v>
-      </c>
-      <c r="CQ6" s="18" t="s">
-        <v>350</v>
-      </c>
-      <c r="CR6" s="18" t="s">
-        <v>351</v>
-      </c>
-      <c r="CS6" s="18" t="s">
-        <v>352</v>
-      </c>
-      <c r="CT6" s="18" t="s">
-        <v>353</v>
-      </c>
-      <c r="CU6" s="18" t="s">
-        <v>354</v>
-      </c>
-      <c r="CV6" s="18" t="s">
-        <v>355</v>
-      </c>
-      <c r="CW6" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="CX6" s="18" t="s">
-        <v>357</v>
-      </c>
-      <c r="CY6" s="18" t="s">
-        <v>358</v>
-      </c>
-      <c r="CZ6" s="18" t="s">
-        <v>359</v>
-      </c>
-      <c r="DA6" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="DB6" s="18" t="s">
-        <v>361</v>
-      </c>
-      <c r="DC6" s="18" t="s">
-        <v>362</v>
-      </c>
-      <c r="DD6" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="DE6" s="18" t="s">
-        <v>364</v>
-      </c>
-      <c r="DF6" s="18" t="s">
-        <v>365</v>
-      </c>
-      <c r="DG6" s="18" t="s">
-        <v>366</v>
-      </c>
-      <c r="DH6" s="18" t="s">
-        <v>367</v>
-      </c>
-      <c r="DI6" s="18" t="s">
-        <v>368</v>
-      </c>
-      <c r="DJ6" s="18" t="s">
-        <v>369</v>
-      </c>
-      <c r="DK6" s="18" t="s">
-        <v>370</v>
-      </c>
-      <c r="DL6" s="18" t="s">
-        <v>371</v>
-      </c>
-      <c r="DM6" s="18" t="s">
-        <v>372</v>
-      </c>
-      <c r="DN6" s="18" t="s">
-        <v>373</v>
-      </c>
-      <c r="DO6" s="18" t="s">
-        <v>374</v>
-      </c>
-      <c r="DP6" s="18" t="s">
-        <v>375</v>
-      </c>
-      <c r="DQ6" s="18" t="s">
-        <v>376</v>
-      </c>
-      <c r="DR6" s="18" t="s">
-        <v>377</v>
-      </c>
-      <c r="DS6" s="18" t="s">
-        <v>379</v>
-      </c>
-      <c r="DT6" s="18" t="s">
-        <v>380</v>
-      </c>
-      <c r="DU6" s="18" t="s">
-        <v>381</v>
-      </c>
-      <c r="DV6" s="18" t="s">
-        <v>382</v>
-      </c>
-      <c r="DW6" s="18" t="s">
-        <v>383</v>
-      </c>
-      <c r="DX6" s="18" t="s">
-        <v>384</v>
-      </c>
-      <c r="DY6" s="18" t="s">
-        <v>385</v>
-      </c>
-      <c r="DZ6" s="18" t="s">
-        <v>386</v>
-      </c>
-      <c r="EA6" s="18" t="s">
-        <v>387</v>
-      </c>
-      <c r="EB6" s="18" t="s">
-        <v>388</v>
-      </c>
-      <c r="EC6" s="18" t="s">
-        <v>390</v>
-      </c>
-      <c r="ED6" s="18" t="s">
-        <v>391</v>
-      </c>
-      <c r="EE6" s="18" t="s">
-        <v>392</v>
-      </c>
-      <c r="EF6" s="18" t="s">
-        <v>393</v>
-      </c>
-      <c r="EG6" s="18" t="s">
-        <v>394</v>
-      </c>
-      <c r="EH6" s="18" t="s">
-        <v>395</v>
-      </c>
-      <c r="EI6" s="18" t="s">
-        <v>396</v>
-      </c>
-      <c r="EJ6" s="18" t="s">
-        <v>397</v>
-      </c>
-      <c r="EK6" s="18" t="s">
-        <v>398</v>
-      </c>
-      <c r="EL6" s="18" t="s">
-        <v>399</v>
-      </c>
-      <c r="EM6" s="18" t="s">
-        <v>401</v>
-      </c>
-      <c r="EN6" s="18" t="s">
-        <v>402</v>
-      </c>
-      <c r="EO6" s="18" t="s">
-        <v>403</v>
-      </c>
-      <c r="EP6" s="18" t="s">
-        <v>404</v>
-      </c>
-      <c r="EQ6" s="18" t="s">
-        <v>405</v>
-      </c>
-      <c r="ER6" s="18" t="s">
-        <v>406</v>
-      </c>
-      <c r="ES6" s="18" t="s">
-        <v>407</v>
-      </c>
-      <c r="ET6" s="18" t="s">
-        <v>408</v>
-      </c>
-      <c r="EU6" s="18" t="s">
-        <v>409</v>
-      </c>
-      <c r="EV6" s="18" t="s">
-        <v>410</v>
-      </c>
-      <c r="EW6" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="EX6" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="EY6" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="EZ6" s="18" t="s">
+      <c r="FH6" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="FI6" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="FJ6" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="FK6" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="FL6" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="FM6" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="FA6" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="FB6" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="FC6" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="FD6" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="FE6" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="FF6" s="18" t="s">
+      <c r="FN6" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="FO6" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="FP6" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="FQ6" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="FG6" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="FH6" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="FI6" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="FJ6" s="18" t="s">
+      <c r="FR6" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="FS6" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="FT6" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="FU6" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="FV6" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="FW6" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="FK6" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="FL6" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="FM6" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="FN6" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="FO6" s="18" t="s">
-        <v>149</v>
-      </c>
-      <c r="FP6" s="18" t="s">
+      <c r="FX6" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="FY6" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="FZ6" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="GA6" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="FQ6" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="FR6" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="FS6" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="FT6" s="9" t="s">
+      <c r="GB6" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="GC6" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="GD6" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="GE6" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="GF6" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="GG6" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="FU6" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="FV6" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="FW6" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="FX6" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="FY6" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="FZ6" s="9" t="s">
+      <c r="GH6" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="GI6" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="GJ6" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="GK6" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="GA6" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="GB6" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="GC6" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="GD6" s="9" t="s">
+      <c r="GL6" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="GM6" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="GN6" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="GO6" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="GP6" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="GQ6" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="GE6" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="GF6" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="GG6" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="GH6" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="GI6" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="GJ6" s="9" t="s">
+      <c r="GR6" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="GS6" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="GT6" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="GU6" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="GK6" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="GL6" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="GM6" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="GN6" s="9" t="s">
+      <c r="GV6" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="GW6" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="GX6" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="GY6" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="GZ6" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="HA6" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="GO6" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="GP6" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="GQ6" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="GR6" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="GS6" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="GT6" s="9" t="s">
+      <c r="HB6" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="HC6" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="HD6" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="HE6" s="18" t="s">
         <v>168</v>
       </c>
-      <c r="GU6" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="GV6" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="GW6" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="GX6" s="18" t="s">
+      <c r="HF6" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="HG6" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="HH6" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="HI6" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="HJ6" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="HK6" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="HL6" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="HM6" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="HN6" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="HO6" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="HP6" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="HQ6" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="HR6" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="HS6" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="HT6" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="HU6" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="HV6" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="HW6" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="HX6" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="HY6" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="HZ6" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="IA6" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="IB6" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="IC6" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="ID6" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="IE6" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="IF6" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="IG6" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="IH6" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="II6" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="IJ6" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="IK6" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="IL6" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="IM6" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="IN6" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="IO6" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="IP6" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="IQ6" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="IR6" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="IS6" s="18" t="s">
+        <v>215</v>
+      </c>
+      <c r="IT6" s="18" t="s">
+        <v>216</v>
+      </c>
+      <c r="IU6" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="IV6" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="IW6" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="IX6" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="IY6" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="IZ6" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="JA6" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="JB6" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="JC6" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="JD6" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="JE6" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="JF6" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="JG6" s="18" t="s">
+        <v>230</v>
+      </c>
+      <c r="JH6" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="JI6" s="18" t="s">
+        <v>233</v>
+      </c>
+      <c r="JJ6" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="JK6" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="JL6" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="JM6" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="JN6" s="18" t="s">
+        <v>238</v>
+      </c>
+      <c r="JO6" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="JP6" s="18" t="s">
+        <v>240</v>
+      </c>
+      <c r="JQ6" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="JR6" s="18" t="s">
+        <v>242</v>
+      </c>
+      <c r="JS6" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="JT6" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="JU6" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="JV6" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="JW6" s="18" t="s">
+        <v>248</v>
+      </c>
+      <c r="JX6" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="JY6" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="JZ6" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="KA6" s="18" t="s">
+        <v>252</v>
+      </c>
+      <c r="KB6" s="18" t="s">
+        <v>253</v>
+      </c>
+      <c r="KC6" s="18" t="s">
+        <v>254</v>
+      </c>
+      <c r="KD6" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="KE6" s="18" t="s">
+        <v>256</v>
+      </c>
+      <c r="KF6" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="KG6" s="18" t="s">
+        <v>258</v>
+      </c>
+      <c r="KH6" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="KI6" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="KJ6" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="KK6" s="18" t="s">
+        <v>262</v>
+      </c>
+      <c r="KL6" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="KM6" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="KN6" s="18" t="s">
+        <v>266</v>
+      </c>
+      <c r="KO6" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="KP6" s="18" t="s">
+        <v>268</v>
+      </c>
+      <c r="KQ6" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="KR6" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="KS6" s="18" t="s">
+        <v>271</v>
+      </c>
+      <c r="KT6" s="18" t="s">
+        <v>272</v>
+      </c>
+      <c r="KU6" s="18" t="s">
+        <v>273</v>
+      </c>
+      <c r="KV6" s="18" t="s">
+        <v>274</v>
+      </c>
+      <c r="KW6" s="18" t="s">
+        <v>276</v>
+      </c>
+      <c r="KX6" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="KY6" s="18" t="s">
+        <v>278</v>
+      </c>
+      <c r="KZ6" s="18" t="s">
+        <v>279</v>
+      </c>
+      <c r="LA6" s="18" t="s">
+        <v>280</v>
+      </c>
+      <c r="LB6" s="18" t="s">
+        <v>281</v>
+      </c>
+      <c r="LC6" s="18" t="s">
+        <v>282</v>
+      </c>
+      <c r="LD6" s="18" t="s">
+        <v>283</v>
+      </c>
+      <c r="LE6" s="18" t="s">
+        <v>284</v>
+      </c>
+      <c r="LF6" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="LG6" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="LH6" s="18" t="s">
+        <v>288</v>
+      </c>
+      <c r="LI6" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="LJ6" s="18" t="s">
+        <v>290</v>
+      </c>
+      <c r="LK6" s="18" t="s">
+        <v>291</v>
+      </c>
+      <c r="LL6" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="LM6" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="LN6" s="18" t="s">
+        <v>316</v>
+      </c>
+      <c r="LO6" s="18" t="s">
+        <v>317</v>
+      </c>
+      <c r="LP6" s="18" t="s">
+        <v>318</v>
+      </c>
+      <c r="LQ6" s="18" t="s">
+        <v>293</v>
+      </c>
+      <c r="LR6" s="18" t="s">
+        <v>294</v>
+      </c>
+      <c r="LS6" s="18" t="s">
+        <v>295</v>
+      </c>
+      <c r="LT6" s="18" t="s">
+        <v>296</v>
+      </c>
+      <c r="LU6" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="LV6" s="18" t="s">
+        <v>298</v>
+      </c>
+      <c r="LW6" s="18" t="s">
+        <v>299</v>
+      </c>
+      <c r="LX6" s="18" t="s">
+        <v>300</v>
+      </c>
+      <c r="LY6" s="18" t="s">
+        <v>301</v>
+      </c>
+      <c r="LZ6" s="18" t="s">
+        <v>302</v>
+      </c>
+      <c r="MA6" s="18" t="s">
+        <v>304</v>
+      </c>
+      <c r="MB6" s="18" t="s">
+        <v>305</v>
+      </c>
+      <c r="MC6" s="18" t="s">
+        <v>306</v>
+      </c>
+      <c r="MD6" s="18" t="s">
+        <v>307</v>
+      </c>
+      <c r="ME6" s="18" t="s">
+        <v>308</v>
+      </c>
+      <c r="MF6" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="MG6" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="MH6" s="18" t="s">
+        <v>311</v>
+      </c>
+      <c r="MI6" s="18" t="s">
+        <v>312</v>
+      </c>
+      <c r="MJ6" s="18" t="s">
+        <v>313</v>
+      </c>
+      <c r="MK6" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="GY6" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="GZ6" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="HA6" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="HB6" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="HC6" s="18" t="s">
-        <v>173</v>
-      </c>
-      <c r="HD6" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="HE6" s="18" t="s">
-        <v>179</v>
-      </c>
-      <c r="HF6" s="18" t="s">
-        <v>180</v>
-      </c>
-      <c r="HG6" s="18" t="s">
-        <v>181</v>
-      </c>
-      <c r="HH6" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="HI6" s="18" t="s">
-        <v>183</v>
-      </c>
-      <c r="HJ6" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="HK6" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="HL6" s="18" t="s">
-        <v>186</v>
-      </c>
-      <c r="HM6" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="HN6" s="18" t="s">
-        <v>188</v>
-      </c>
-      <c r="HO6" s="18" t="s">
-        <v>190</v>
-      </c>
-      <c r="HP6" s="18" t="s">
-        <v>191</v>
-      </c>
-      <c r="HQ6" s="18" t="s">
-        <v>192</v>
-      </c>
-      <c r="HR6" s="18" t="s">
-        <v>193</v>
-      </c>
-      <c r="HS6" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="HT6" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="HU6" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="HV6" s="18" t="s">
-        <v>197</v>
-      </c>
-      <c r="HW6" s="18" t="s">
-        <v>198</v>
-      </c>
-      <c r="HX6" s="18" t="s">
-        <v>199</v>
-      </c>
-      <c r="HY6" s="18" t="s">
-        <v>201</v>
-      </c>
-      <c r="HZ6" s="18" t="s">
-        <v>202</v>
-      </c>
-      <c r="IA6" s="18" t="s">
-        <v>203</v>
-      </c>
-      <c r="IB6" s="18" t="s">
-        <v>204</v>
-      </c>
-      <c r="IC6" s="18" t="s">
-        <v>205</v>
-      </c>
-      <c r="ID6" s="18" t="s">
-        <v>206</v>
-      </c>
-      <c r="IE6" s="18" t="s">
-        <v>207</v>
-      </c>
-      <c r="IF6" s="18" t="s">
-        <v>208</v>
-      </c>
-      <c r="IG6" s="18" t="s">
-        <v>209</v>
-      </c>
-      <c r="IH6" s="18" t="s">
-        <v>210</v>
-      </c>
-      <c r="II6" s="18" t="s">
-        <v>212</v>
-      </c>
-      <c r="IJ6" s="18" t="s">
-        <v>213</v>
-      </c>
-      <c r="IK6" s="18" t="s">
-        <v>214</v>
-      </c>
-      <c r="IL6" s="18" t="s">
-        <v>215</v>
-      </c>
-      <c r="IM6" s="18" t="s">
-        <v>216</v>
-      </c>
-      <c r="IN6" s="18" t="s">
-        <v>217</v>
-      </c>
-      <c r="IO6" s="18" t="s">
-        <v>218</v>
-      </c>
-      <c r="IP6" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="IQ6" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="IR6" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="IS6" s="18" t="s">
-        <v>223</v>
-      </c>
-      <c r="IT6" s="18" t="s">
-        <v>224</v>
-      </c>
-      <c r="IU6" s="18" t="s">
-        <v>225</v>
-      </c>
-      <c r="IV6" s="18" t="s">
-        <v>226</v>
-      </c>
-      <c r="IW6" s="18" t="s">
-        <v>227</v>
-      </c>
-      <c r="IX6" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="IY6" s="18" t="s">
-        <v>229</v>
-      </c>
-      <c r="IZ6" s="18" t="s">
-        <v>230</v>
-      </c>
-      <c r="JA6" s="18" t="s">
-        <v>231</v>
-      </c>
-      <c r="JB6" s="18" t="s">
-        <v>232</v>
-      </c>
-      <c r="JC6" s="18" t="s">
-        <v>234</v>
-      </c>
-      <c r="JD6" s="18" t="s">
-        <v>235</v>
-      </c>
-      <c r="JE6" s="18" t="s">
-        <v>236</v>
-      </c>
-      <c r="JF6" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="JG6" s="18" t="s">
-        <v>238</v>
-      </c>
-      <c r="JH6" s="18" t="s">
-        <v>239</v>
-      </c>
-      <c r="JI6" s="18" t="s">
-        <v>240</v>
-      </c>
-      <c r="JJ6" s="18" t="s">
-        <v>241</v>
-      </c>
-      <c r="JK6" s="18" t="s">
-        <v>242</v>
-      </c>
-      <c r="JL6" s="18" t="s">
-        <v>243</v>
-      </c>
-      <c r="JM6" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="JN6" s="18" t="s">
-        <v>245</v>
-      </c>
-      <c r="JO6" s="18" t="s">
-        <v>247</v>
-      </c>
-      <c r="JP6" s="18" t="s">
-        <v>248</v>
-      </c>
-      <c r="JQ6" s="18" t="s">
-        <v>249</v>
-      </c>
-      <c r="JR6" s="18" t="s">
-        <v>250</v>
-      </c>
-      <c r="JS6" s="18" t="s">
-        <v>251</v>
-      </c>
-      <c r="JT6" s="18" t="s">
-        <v>252</v>
-      </c>
-      <c r="JU6" s="18" t="s">
-        <v>253</v>
-      </c>
-      <c r="JV6" s="18" t="s">
-        <v>254</v>
-      </c>
-      <c r="JW6" s="18" t="s">
-        <v>255</v>
-      </c>
-      <c r="JX6" s="18" t="s">
-        <v>256</v>
-      </c>
-      <c r="JY6" s="18" t="s">
-        <v>257</v>
-      </c>
-      <c r="JZ6" s="18" t="s">
-        <v>258</v>
-      </c>
-      <c r="KA6" s="18" t="s">
-        <v>259</v>
-      </c>
-      <c r="KB6" s="18" t="s">
-        <v>260</v>
-      </c>
-      <c r="KC6" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="KD6" s="18" t="s">
-        <v>262</v>
-      </c>
-      <c r="KE6" s="18" t="s">
-        <v>263</v>
-      </c>
-      <c r="KF6" s="18" t="s">
-        <v>264</v>
-      </c>
-      <c r="KG6" s="18" t="s">
-        <v>266</v>
-      </c>
-      <c r="KH6" s="18" t="s">
-        <v>267</v>
-      </c>
-      <c r="KI6" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="KJ6" s="18" t="s">
-        <v>269</v>
-      </c>
-      <c r="KK6" s="18" t="s">
-        <v>270</v>
-      </c>
-      <c r="KL6" s="18" t="s">
-        <v>271</v>
-      </c>
-      <c r="KM6" s="18" t="s">
-        <v>272</v>
-      </c>
-      <c r="KN6" s="18" t="s">
-        <v>273</v>
-      </c>
-      <c r="KO6" s="18" t="s">
-        <v>274</v>
-      </c>
-      <c r="KP6" s="18" t="s">
-        <v>275</v>
-      </c>
-      <c r="KQ6" s="18" t="s">
-        <v>277</v>
-      </c>
-      <c r="KR6" s="18" t="s">
-        <v>278</v>
-      </c>
-      <c r="KS6" s="18" t="s">
-        <v>279</v>
-      </c>
-      <c r="KT6" s="18" t="s">
-        <v>280</v>
-      </c>
-      <c r="KU6" s="18" t="s">
-        <v>281</v>
-      </c>
-      <c r="KV6" s="18" t="s">
-        <v>282</v>
-      </c>
-      <c r="KW6" s="18" t="s">
-        <v>283</v>
-      </c>
-      <c r="KX6" s="18" t="s">
-        <v>284</v>
-      </c>
-      <c r="KY6" s="18" t="s">
-        <v>285</v>
-      </c>
-      <c r="KZ6" s="18" t="s">
-        <v>286</v>
-      </c>
-      <c r="LA6" s="18" t="s">
-        <v>288</v>
-      </c>
-      <c r="LB6" s="18" t="s">
-        <v>289</v>
-      </c>
-      <c r="LC6" s="18" t="s">
-        <v>290</v>
-      </c>
-      <c r="LD6" s="18" t="s">
-        <v>291</v>
-      </c>
-      <c r="LE6" s="18" t="s">
-        <v>292</v>
-      </c>
-      <c r="LF6" s="18" t="s">
-        <v>315</v>
-      </c>
-      <c r="LG6" s="18" t="s">
-        <v>316</v>
-      </c>
-      <c r="LH6" s="18" t="s">
-        <v>317</v>
-      </c>
-      <c r="LI6" s="18" t="s">
-        <v>318</v>
-      </c>
-      <c r="LJ6" s="18" t="s">
-        <v>319</v>
-      </c>
-      <c r="LK6" s="18" t="s">
-        <v>294</v>
-      </c>
-      <c r="LL6" s="18" t="s">
-        <v>295</v>
-      </c>
-      <c r="LM6" s="18" t="s">
-        <v>296</v>
-      </c>
-      <c r="LN6" s="18" t="s">
-        <v>297</v>
-      </c>
-      <c r="LO6" s="18" t="s">
-        <v>298</v>
-      </c>
-      <c r="LP6" s="18" t="s">
-        <v>299</v>
-      </c>
-      <c r="LQ6" s="18" t="s">
-        <v>300</v>
-      </c>
-      <c r="LR6" s="18" t="s">
-        <v>301</v>
-      </c>
-      <c r="LS6" s="18" t="s">
-        <v>302</v>
-      </c>
-      <c r="LT6" s="18" t="s">
-        <v>303</v>
-      </c>
-      <c r="LU6" s="18" t="s">
-        <v>305</v>
-      </c>
-      <c r="LV6" s="18" t="s">
-        <v>306</v>
-      </c>
-      <c r="LW6" s="18" t="s">
-        <v>307</v>
-      </c>
-      <c r="LX6" s="18" t="s">
-        <v>308</v>
-      </c>
-      <c r="LY6" s="18" t="s">
-        <v>309</v>
-      </c>
-      <c r="LZ6" s="18" t="s">
-        <v>310</v>
-      </c>
-      <c r="MA6" s="18" t="s">
-        <v>311</v>
-      </c>
-      <c r="MB6" s="18" t="s">
-        <v>312</v>
-      </c>
-      <c r="MC6" s="18" t="s">
-        <v>313</v>
-      </c>
-      <c r="MD6" s="18" t="s">
-        <v>314</v>
-      </c>
-      <c r="ME6" s="18" t="s">
+      <c r="ML6" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="MF6" s="18" t="s">
+      <c r="MM6" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="MG6" s="18" t="s">
+      <c r="MN6" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="MH6" s="18" t="s">
+      <c r="MO6" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="MI6" s="18" t="s">
+      <c r="MP6" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="MJ6" s="18" t="s">
+      <c r="MQ6" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="MK6" s="18" t="s">
+      <c r="MR6" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="ML6" s="18" t="s">
+      <c r="MS6" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="MM6" s="18" t="s">
+      <c r="MT6" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="MN6" s="18" t="s">
+      <c r="MU6" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="MO6" s="18" t="s">
+      <c r="MV6" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="MP6" s="18" t="s">
+      <c r="MW6" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="MQ6" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="MR6" s="18" t="s">
+      <c r="MX6" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="MY6" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="MS6" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="MT6" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="MU6" s="18" t="s">
+      <c r="MZ6" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="MV6" s="18" t="s">
+      <c r="NA6" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="NB6" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="NC6" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="MW6" s="18" t="s">
+      <c r="ND6" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="MX6" s="18" t="s">
+      <c r="NE6" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="MY6" s="18" t="s">
-        <v>124</v>
-      </c>
     </row>
-    <row r="7" spans="1:363" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:369" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="40"/>
       <c r="B7" s="40"/>
       <c r="C7" s="40" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D7" s="40"/>
       <c r="E7" s="40"/>
@@ -5887,17 +5953,17 @@
       <c r="L7" s="42"/>
       <c r="M7" s="42"/>
       <c r="N7" s="42" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="O7" s="42" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P7" s="42"/>
       <c r="Q7" s="43" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="R7" s="43" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="S7" s="42"/>
       <c r="T7" s="42"/>
@@ -5909,13 +5975,13 @@
       <c r="Z7" s="47"/>
       <c r="AA7" s="46"/>
       <c r="AB7" s="41" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AC7" s="41" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AD7" s="41" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AE7" s="42"/>
       <c r="AF7" s="48"/>
@@ -5925,127 +5991,127 @@
       <c r="AJ7" s="49"/>
       <c r="AK7" s="49"/>
       <c r="AL7" s="50">
-        <f>SUM(BK7:BT7)</f>
+        <f>SUM(BQ7:BZ7)</f>
         <v>0</v>
       </c>
       <c r="AM7" s="51">
-        <f>SUM(CE7:CN7)</f>
+        <f>SUM(CK7:CT7)</f>
         <v>0</v>
       </c>
-      <c r="AN7" s="51" t="e">
-        <f>SUM(#REF!)</f>
-        <v>#REF!</v>
+      <c r="AN7" s="51">
+        <f>SUM(CK7:CT7)</f>
+        <v>0</v>
       </c>
       <c r="AO7" s="51">
-        <f>SUM(EW7:FF7)</f>
+        <f>SUM(CU7:DD7)</f>
         <v>0</v>
       </c>
       <c r="AP7" s="51">
-        <f>SUM(FG7:FP7)</f>
+        <f>SUM(DE7:DN7)</f>
         <v>0</v>
       </c>
       <c r="AQ7" s="51">
-        <f>SUM(FQ7:FZ7)</f>
+        <f>SUM(DO7:DX7)</f>
         <v>0</v>
       </c>
       <c r="AR7" s="51">
-        <f>SUM(GA7:GJ7)</f>
+        <f>SUM(DY7:EH7)</f>
         <v>0</v>
       </c>
       <c r="AS7" s="51">
-        <f>SUM(GK7:GT7)</f>
+        <f>SUM(EI7:ER7)</f>
         <v>0</v>
       </c>
       <c r="AT7" s="51">
-        <f>SUM(GU7:HD7)</f>
+        <f>SUM(ES7:FB7)</f>
         <v>0</v>
       </c>
       <c r="AU7" s="51">
-        <f>SUM(HE7:HN7)</f>
+        <f>SUM(FC7:FL7)</f>
         <v>0</v>
       </c>
       <c r="AV7" s="51">
-        <f>SUM(HO7:HX7)</f>
+        <f>SUM(FM7:FV7)</f>
         <v>0</v>
       </c>
       <c r="AW7" s="51">
-        <f>SUM(HY7:IH7)</f>
+        <f>SUM(FW7:GF7)</f>
         <v>0</v>
       </c>
       <c r="AX7" s="51">
-        <f>SUM(II7:IR7)</f>
+        <f>SUM(GG7:GP7)</f>
         <v>0</v>
       </c>
       <c r="AY7" s="51">
-        <f>SUM(IS7:JB7)</f>
+        <f>SUM(GQ7:GZ7)</f>
         <v>0</v>
       </c>
       <c r="AZ7" s="51">
-        <f>SUM(JC7:JL7)</f>
+        <f>SUM(HA7:HJ7)</f>
         <v>0</v>
       </c>
       <c r="BA7" s="51">
-        <f>SUM(JM7:JV7)</f>
+        <f>SUM(HK7:HT7)</f>
         <v>0</v>
       </c>
       <c r="BB7" s="51">
-        <f>SUM(JW7:KF7)</f>
+        <f>SUM(HU7:ID7)</f>
         <v>0</v>
       </c>
       <c r="BC7" s="51">
-        <f>SUM(KG7:KP7)</f>
+        <f>SUM(IE7:IN7)</f>
         <v>0</v>
       </c>
       <c r="BD7" s="51">
-        <f>SUM(KQ7:KZ7)</f>
+        <f>SUM(IO7:IX7)</f>
         <v>0</v>
       </c>
       <c r="BE7" s="51">
-        <f>SUM(LA7:LJ7)</f>
+        <f>SUM(IY7:JH7)</f>
         <v>0</v>
       </c>
       <c r="BF7" s="51">
-        <f>SUM(LK7:LT7)</f>
+        <f>SUM(JI7:JR7)</f>
         <v>0</v>
       </c>
       <c r="BG7" s="51">
-        <f>SUM(LU7:MD7)</f>
+        <f>SUM(JS7:KB7)</f>
         <v>0</v>
       </c>
       <c r="BH7" s="51">
-        <f t="shared" ref="BH7" si="0">ME7</f>
+        <f>SUM(KC7:KL7)</f>
         <v>0</v>
       </c>
       <c r="BI7" s="51">
-        <f>MF7</f>
+        <f>SUM(KM7:KV7)</f>
         <v>0</v>
       </c>
       <c r="BJ7" s="51">
-        <f>MG7</f>
+        <f>SUM(KW7:LF7)</f>
         <v>0</v>
       </c>
       <c r="BK7" s="51">
-        <f>BU7+CE7+CO7+CY7+DI7+DS7+EC7+EM7+EW7+FG7+FQ7+GA7+GK7+GU7</f>
+        <f>SUM(LG7:LP7)</f>
         <v>0</v>
       </c>
       <c r="BL7" s="51">
-        <f>BV7+CF7+CP7+CZ7+DJ7+DT7+ED7+EN7+EX7+FH7+FR7+GB7+GL7+GV7</f>
+        <f>SUM(LQ7:LZ7)</f>
         <v>0</v>
       </c>
       <c r="BM7" s="51">
-        <f>BW7+CG7+CQ7+DA7+DK7+DU7+EE7+EO7+EY7+FI7+FS7+GC7+GM7+GW7</f>
+        <f>SUM(MA7:MJ7)</f>
         <v>0</v>
       </c>
       <c r="BN7" s="51">
-        <f>BX7+CH7+CR7+DB7+DL7+DV7+EF7+EP7+EZ7+FJ7+FT7+GD7+GN7+GX7</f>
+        <f t="shared" ref="BN7" si="0">MK7</f>
         <v>0</v>
       </c>
       <c r="BO7" s="51">
-        <f>BY7+CI7+CS7+DC7+DM7+DW7+EG7+EQ7+FA7+FK7+FU7+GE7+GO7+GY7</f>
+        <f>ML7</f>
         <v>0</v>
       </c>
       <c r="BP7" s="51">
-        <f>BZ7+CJ7+CT7+DD7+DN7+DX7+EH7+ER7+FB7+FL7+FV7+GF7+GP7+GZ7</f>
+        <f>MM7</f>
         <v>0</v>
       </c>
       <c r="BQ7" s="51">
@@ -6064,12 +6130,30 @@
         <f>CD7+CN7+CX7+DH7+DR7+EB7+EL7+EV7+FF7+FP7+FZ7+GJ7+GT7+HD7</f>
         <v>0</v>
       </c>
-      <c r="BU7" s="46"/>
-      <c r="BV7" s="46"/>
-      <c r="BW7" s="46"/>
-      <c r="BX7" s="46"/>
-      <c r="BY7" s="46"/>
-      <c r="BZ7" s="46"/>
+      <c r="BU7" s="51">
+        <f>CE7+CO7+CY7+DI7+DS7+EC7+EM7+EW7+FG7+FQ7+GA7+GK7+GU7+HE7</f>
+        <v>0</v>
+      </c>
+      <c r="BV7" s="51">
+        <f>CF7+CP7+CZ7+DJ7+DT7+ED7+EN7+EX7+FH7+FR7+GB7+GL7+GV7+HF7</f>
+        <v>0</v>
+      </c>
+      <c r="BW7" s="51">
+        <f>CG7+CQ7+DA7+DK7+DU7+EE7+EO7+EY7+FI7+FS7+GC7+GM7+GW7+HG7</f>
+        <v>0</v>
+      </c>
+      <c r="BX7" s="51">
+        <f>CH7+CR7+DB7+DL7+DV7+EF7+EP7+EZ7+FJ7+FT7+GD7+GN7+GX7+HH7</f>
+        <v>0</v>
+      </c>
+      <c r="BY7" s="51">
+        <f>CI7+CS7+DC7+DM7+DW7+EG7+EQ7+FA7+FK7+FU7+GE7+GO7+GY7+HI7</f>
+        <v>0</v>
+      </c>
+      <c r="BZ7" s="51">
+        <f>CJ7+CT7+DD7+DN7+DX7+EH7+ER7+FB7+FL7+FV7+GF7+GP7+GZ7+HJ7</f>
+        <v>0</v>
+      </c>
       <c r="CA7" s="46"/>
       <c r="CB7" s="46"/>
       <c r="CC7" s="46"/>
@@ -6337,56 +6421,62 @@
       <c r="ME7" s="46"/>
       <c r="MF7" s="46"/>
       <c r="MG7" s="46"/>
-      <c r="MH7" s="41"/>
-      <c r="MI7" s="41"/>
-      <c r="MJ7" s="41"/>
-      <c r="MK7" s="52"/>
-      <c r="ML7" s="52"/>
-      <c r="MM7" s="52"/>
-      <c r="MN7" s="52"/>
-      <c r="MO7" s="52"/>
-      <c r="MP7" s="52"/>
+      <c r="MH7" s="46"/>
+      <c r="MI7" s="46"/>
+      <c r="MJ7" s="46"/>
+      <c r="MK7" s="46"/>
+      <c r="ML7" s="46"/>
+      <c r="MM7" s="46"/>
+      <c r="MN7" s="41"/>
+      <c r="MO7" s="41"/>
+      <c r="MP7" s="41"/>
       <c r="MQ7" s="52"/>
-      <c r="MR7" s="39"/>
-      <c r="MS7" s="39"/>
-      <c r="MT7" s="39"/>
-      <c r="MU7" s="39"/>
-      <c r="MV7" s="53"/>
-      <c r="MW7" s="53"/>
-      <c r="MX7" s="53"/>
-      <c r="MY7" s="53"/>
+      <c r="MR7" s="52"/>
+      <c r="MS7" s="52"/>
+      <c r="MT7" s="52"/>
+      <c r="MU7" s="52"/>
+      <c r="MV7" s="52"/>
+      <c r="MW7" s="52"/>
+      <c r="MX7" s="39"/>
+      <c r="MY7" s="39"/>
+      <c r="MZ7" s="39"/>
+      <c r="NA7" s="39"/>
+      <c r="NB7" s="53"/>
+      <c r="NC7" s="53"/>
+      <c r="ND7" s="53"/>
+      <c r="NE7" s="53"/>
     </row>
   </sheetData>
-  <autoFilter ref="A6:MU6" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A6:NA6" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="43">
-    <mergeCell ref="EC4:EL4"/>
-    <mergeCell ref="EM4:EV4"/>
-    <mergeCell ref="BU4:CD4"/>
-    <mergeCell ref="CO4:CX4"/>
-    <mergeCell ref="CY4:DH4"/>
-    <mergeCell ref="DI4:DR4"/>
-    <mergeCell ref="DS4:EB4"/>
-    <mergeCell ref="GU4:HD4"/>
-    <mergeCell ref="MR4:MT5"/>
-    <mergeCell ref="HO4:HX4"/>
-    <mergeCell ref="KG4:KP4"/>
-    <mergeCell ref="KQ4:KZ4"/>
-    <mergeCell ref="LA4:LJ4"/>
-    <mergeCell ref="LU4:MD4"/>
-    <mergeCell ref="ME4:MQ5"/>
-    <mergeCell ref="HY4:IH4"/>
-    <mergeCell ref="II4:IR4"/>
-    <mergeCell ref="IS4:JB4"/>
-    <mergeCell ref="JC4:JL4"/>
-    <mergeCell ref="JM4:JV4"/>
-    <mergeCell ref="JW4:KF4"/>
-    <mergeCell ref="LK4:LT4"/>
-    <mergeCell ref="EW4:FF4"/>
-    <mergeCell ref="FG4:FP4"/>
-    <mergeCell ref="FQ4:FZ4"/>
-    <mergeCell ref="GA4:GJ4"/>
-    <mergeCell ref="GK4:GT4"/>
-    <mergeCell ref="MV4:MW5"/>
+    <mergeCell ref="EI4:ER4"/>
+    <mergeCell ref="ES4:FB4"/>
+    <mergeCell ref="CA4:CJ4"/>
+    <mergeCell ref="CU4:DD4"/>
+    <mergeCell ref="DE4:DN4"/>
+    <mergeCell ref="DO4:DX4"/>
+    <mergeCell ref="DY4:EH4"/>
+    <mergeCell ref="HA4:HJ4"/>
+    <mergeCell ref="MX4:MZ5"/>
+    <mergeCell ref="HU4:ID4"/>
+    <mergeCell ref="KM4:KV4"/>
+    <mergeCell ref="KW4:LF4"/>
+    <mergeCell ref="LG4:LP4"/>
+    <mergeCell ref="MA4:MJ4"/>
+    <mergeCell ref="MK4:MW5"/>
+    <mergeCell ref="IE4:IN4"/>
+    <mergeCell ref="IO4:IX4"/>
+    <mergeCell ref="IY4:JH4"/>
+    <mergeCell ref="JI4:JR4"/>
+    <mergeCell ref="JS4:KB4"/>
+    <mergeCell ref="KC4:KL4"/>
+    <mergeCell ref="LQ4:LZ4"/>
+    <mergeCell ref="FC4:FL4"/>
+    <mergeCell ref="FM4:FV4"/>
+    <mergeCell ref="FW4:GF4"/>
+    <mergeCell ref="GG4:GP4"/>
+    <mergeCell ref="GQ4:GZ4"/>
+    <mergeCell ref="NB4:NC5"/>
     <mergeCell ref="AE4:AF5"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
@@ -6397,20 +6487,20 @@
     <mergeCell ref="P4:T5"/>
     <mergeCell ref="U4:AA5"/>
     <mergeCell ref="AB4:AD5"/>
-    <mergeCell ref="HE4:HN4"/>
+    <mergeCell ref="HK4:HT4"/>
     <mergeCell ref="AG4:AK5"/>
-    <mergeCell ref="AL4:BJ5"/>
-    <mergeCell ref="BK4:BT4"/>
-    <mergeCell ref="CE4:CN4"/>
+    <mergeCell ref="AL4:BP5"/>
+    <mergeCell ref="BQ4:BZ4"/>
+    <mergeCell ref="CK4:CT4"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A6">
     <cfRule type="duplicateValues" dxfId="0" priority="92"/>
   </conditionalFormatting>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI1:AK3 AG1:AH4 AG7:AK7" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>36526</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="MR6:MT999996" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="MX6:MZ999996" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"4. High, 3. Medium High, 2. Medium Low, 1. Low, N/A"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[RUBY-2580] Adjusting FCRM report titles
</commit_message>
<xml_diff>
--- a/lib/fcerm1_template.xlsx
+++ b/lib/fcerm1_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lb000070\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC3CA89-D856-4B66-BCD6-966DBA67D01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4942BD2C-5EE9-4304-9B8A-6A3718D9F79E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -99,10 +99,6 @@
 £ CASH</t>
   </si>
   <si>
-    <t>FURTHER CONTRIBUTIONS REQUIRED
- £ CASH</t>
-  </si>
-  <si>
     <t>Environmental performance specification indicators</t>
   </si>
   <si>
@@ -348,18 +344,6 @@
     <t>Other EA - 2026/27</t>
   </si>
   <si>
-    <t>Further required - 2023/24</t>
-  </si>
-  <si>
-    <t>Further required - 2024/25</t>
-  </si>
-  <si>
-    <t>Further required - 2025/26</t>
-  </si>
-  <si>
-    <t>Further required - 2026/27</t>
-  </si>
-  <si>
     <t>OM4a Total</t>
   </si>
   <si>
@@ -556,24 +540,6 @@
   </si>
   <si>
     <t>Other EA - 2032/33</t>
-  </si>
-  <si>
-    <t>Further required - 2027/28</t>
-  </si>
-  <si>
-    <t>Further required - 2028/29</t>
-  </si>
-  <si>
-    <t>Further required - 2029/30</t>
-  </si>
-  <si>
-    <t>Further required - 2030/31</t>
-  </si>
-  <si>
-    <t>Further required - 2031/32</t>
-  </si>
-  <si>
-    <t>Further required - 2032/33</t>
   </si>
   <si>
     <t>PAFS Base 2023/24</t>
@@ -1315,6 +1281,39 @@
   </si>
   <si>
     <t>Additional FCRM GiA (Summer economic fund) - PROJECT TOTAL</t>
+  </si>
+  <si>
+    <t>Future funding not yet identified - 2023/24</t>
+  </si>
+  <si>
+    <t>Future funding not yet identified - 2024/25</t>
+  </si>
+  <si>
+    <t>Future funding not yet identified - 2025/26</t>
+  </si>
+  <si>
+    <t>Future funding not yet identified - 2026/27</t>
+  </si>
+  <si>
+    <t>Future funding not yet identified - 2027/28</t>
+  </si>
+  <si>
+    <t>Future funding not yet identified - 2028/29</t>
+  </si>
+  <si>
+    <t>Future funding not yet identified - 2029/30</t>
+  </si>
+  <si>
+    <t>Future funding not yet identified - 2030/31</t>
+  </si>
+  <si>
+    <t>Future funding not yet identified - 2031/32</t>
+  </si>
+  <si>
+    <t>Future funding not yet identified - 2032/33</t>
+  </si>
+  <si>
+    <t>OTHER FUNDING SOURCES NOT YET IDENTIFIED £</t>
   </si>
 </sst>
 </file>
@@ -2296,11 +2295,11 @@
   <dimension ref="A1:NE7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="AE7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="DH7" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
       <selection pane="topRight" activeCell="C7" sqref="C7"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="AT8" sqref="AT8"/>
+      <selection pane="bottomRight" activeCell="HB6" sqref="HB6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2703,7 +2702,7 @@
     </row>
     <row r="2" spans="1:369" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="64" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="B2" s="64"/>
       <c r="C2" s="19"/>
@@ -3470,7 +3469,7 @@
       <c r="N4" s="68"/>
       <c r="O4" s="68"/>
       <c r="P4" s="69" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
       <c r="Q4" s="69"/>
       <c r="R4" s="69"/>
@@ -3557,7 +3556,7 @@
       <c r="CI4" s="88"/>
       <c r="CJ4" s="88"/>
       <c r="CK4" s="89" t="s">
-        <v>333</v>
+        <v>322</v>
       </c>
       <c r="CL4" s="89"/>
       <c r="CM4" s="89"/>
@@ -3569,7 +3568,7 @@
       <c r="CS4" s="89"/>
       <c r="CT4" s="89"/>
       <c r="CU4" s="88" t="s">
-        <v>334</v>
+        <v>323</v>
       </c>
       <c r="CV4" s="88"/>
       <c r="CW4" s="88"/>
@@ -3581,7 +3580,7 @@
       <c r="DC4" s="88"/>
       <c r="DD4" s="88"/>
       <c r="DE4" s="89" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
       <c r="DF4" s="89"/>
       <c r="DG4" s="89"/>
@@ -3593,7 +3592,7 @@
       <c r="DM4" s="89"/>
       <c r="DN4" s="89"/>
       <c r="DO4" s="88" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
       <c r="DP4" s="88"/>
       <c r="DQ4" s="88"/>
@@ -3605,7 +3604,7 @@
       <c r="DW4" s="88"/>
       <c r="DX4" s="88"/>
       <c r="DY4" s="90" t="s">
-        <v>377</v>
+        <v>366</v>
       </c>
       <c r="DZ4" s="91"/>
       <c r="EA4" s="91"/>
@@ -3617,7 +3616,7 @@
       <c r="EG4" s="91"/>
       <c r="EH4" s="92"/>
       <c r="EI4" s="88" t="s">
-        <v>388</v>
+        <v>377</v>
       </c>
       <c r="EJ4" s="88"/>
       <c r="EK4" s="88"/>
@@ -3629,7 +3628,7 @@
       <c r="EQ4" s="88"/>
       <c r="ER4" s="88"/>
       <c r="ES4" s="90" t="s">
-        <v>399</v>
+        <v>388</v>
       </c>
       <c r="ET4" s="91"/>
       <c r="EU4" s="91"/>
@@ -3701,7 +3700,7 @@
       <c r="GY4" s="79"/>
       <c r="GZ4" s="79"/>
       <c r="HA4" s="80" t="s">
-        <v>16</v>
+        <v>416</v>
       </c>
       <c r="HB4" s="80"/>
       <c r="HC4" s="80"/>
@@ -3713,7 +3712,7 @@
       <c r="HI4" s="80"/>
       <c r="HJ4" s="80"/>
       <c r="HK4" s="72" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="HL4" s="72"/>
       <c r="HM4" s="72"/>
@@ -3725,7 +3724,7 @@
       <c r="HS4" s="72"/>
       <c r="HT4" s="72"/>
       <c r="HU4" s="72" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="HV4" s="72"/>
       <c r="HW4" s="72"/>
@@ -3737,7 +3736,7 @@
       <c r="IC4" s="72"/>
       <c r="ID4" s="72"/>
       <c r="IE4" s="72" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="IF4" s="72"/>
       <c r="IG4" s="72"/>
@@ -3749,7 +3748,7 @@
       <c r="IM4" s="72"/>
       <c r="IN4" s="72"/>
       <c r="IO4" s="72" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="IP4" s="72"/>
       <c r="IQ4" s="72"/>
@@ -3761,7 +3760,7 @@
       <c r="IW4" s="72"/>
       <c r="IX4" s="72"/>
       <c r="IY4" s="83" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="IZ4" s="84"/>
       <c r="JA4" s="84"/>
@@ -3773,7 +3772,7 @@
       <c r="JG4" s="84"/>
       <c r="JH4" s="85"/>
       <c r="JI4" s="83" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="JJ4" s="84"/>
       <c r="JK4" s="84"/>
@@ -3785,7 +3784,7 @@
       <c r="JQ4" s="84"/>
       <c r="JR4" s="85"/>
       <c r="JS4" s="83" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="JT4" s="84"/>
       <c r="JU4" s="84"/>
@@ -3797,7 +3796,7 @@
       <c r="KA4" s="84"/>
       <c r="KB4" s="85"/>
       <c r="KC4" s="83" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="KD4" s="84"/>
       <c r="KE4" s="84"/>
@@ -3809,7 +3808,7 @@
       <c r="KK4" s="84"/>
       <c r="KL4" s="85"/>
       <c r="KM4" s="83" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="KN4" s="84"/>
       <c r="KO4" s="84"/>
@@ -3821,7 +3820,7 @@
       <c r="KU4" s="84"/>
       <c r="KV4" s="85"/>
       <c r="KW4" s="86" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="KX4" s="86"/>
       <c r="KY4" s="86"/>
@@ -3833,7 +3832,7 @@
       <c r="LE4" s="86"/>
       <c r="LF4" s="86"/>
       <c r="LG4" s="86" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="LH4" s="86"/>
       <c r="LI4" s="86"/>
@@ -3845,7 +3844,7 @@
       <c r="LO4" s="86"/>
       <c r="LP4" s="86"/>
       <c r="LQ4" s="86" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="LR4" s="86"/>
       <c r="LS4" s="86"/>
@@ -3857,7 +3856,7 @@
       <c r="LY4" s="86"/>
       <c r="LZ4" s="86"/>
       <c r="MA4" s="86" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="MB4" s="86"/>
       <c r="MC4" s="86"/>
@@ -3869,7 +3868,7 @@
       <c r="MI4" s="86"/>
       <c r="MJ4" s="86"/>
       <c r="MK4" s="87" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="ML4" s="87"/>
       <c r="MM4" s="87"/>
@@ -3884,13 +3883,13 @@
       <c r="MV4" s="87"/>
       <c r="MW4" s="87"/>
       <c r="MX4" s="58" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="MY4" s="81"/>
       <c r="MZ4" s="59"/>
       <c r="NA4" s="38"/>
       <c r="NB4" s="58" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="NC4" s="59"/>
       <c r="ND4" s="56"/>
@@ -3966,844 +3965,844 @@
       <c r="BO5" s="74"/>
       <c r="BP5" s="74"/>
       <c r="BQ5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="BR5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="BR5" s="7" t="s">
+      <c r="BS5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="BS5" s="7" t="s">
+      <c r="BT5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="BT5" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="BU5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="BV5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="BV5" s="8" t="s">
+      <c r="BW5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="BW5" s="8" t="s">
+      <c r="BX5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="BX5" s="8" t="s">
+      <c r="BY5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="BY5" s="8" t="s">
+      <c r="BZ5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="BZ5" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="CA5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="CB5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="CB5" s="7" t="s">
+      <c r="CC5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="CC5" s="7" t="s">
+      <c r="CD5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="CD5" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="CE5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="CF5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="CF5" s="8" t="s">
+      <c r="CG5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="CG5" s="8" t="s">
+      <c r="CH5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="CH5" s="8" t="s">
+      <c r="CI5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="CI5" s="8" t="s">
+      <c r="CJ5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="CJ5" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="CK5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="CL5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="CL5" s="7" t="s">
+      <c r="CM5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="CM5" s="7" t="s">
+      <c r="CN5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="CN5" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="CO5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="CP5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="CP5" s="8" t="s">
+      <c r="CQ5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="CQ5" s="8" t="s">
+      <c r="CR5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="CR5" s="8" t="s">
+      <c r="CS5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="CS5" s="8" t="s">
+      <c r="CT5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="CT5" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="CU5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="CV5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="CV5" s="7" t="s">
+      <c r="CW5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="CW5" s="7" t="s">
+      <c r="CX5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="CX5" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="CY5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="CZ5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="CZ5" s="8" t="s">
+      <c r="DA5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="DA5" s="8" t="s">
+      <c r="DB5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="DB5" s="8" t="s">
+      <c r="DC5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="DC5" s="8" t="s">
+      <c r="DD5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="DD5" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="DE5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="DF5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="DF5" s="7" t="s">
+      <c r="DG5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="DG5" s="7" t="s">
+      <c r="DH5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="DH5" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="DI5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="DJ5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="DJ5" s="8" t="s">
+      <c r="DK5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="DK5" s="8" t="s">
+      <c r="DL5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="DL5" s="8" t="s">
+      <c r="DM5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="DM5" s="8" t="s">
+      <c r="DN5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="DN5" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="DO5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="DP5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="DP5" s="7" t="s">
+      <c r="DQ5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="DQ5" s="7" t="s">
+      <c r="DR5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="DR5" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="DS5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="DT5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="DT5" s="8" t="s">
+      <c r="DU5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="DU5" s="8" t="s">
+      <c r="DV5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="DV5" s="8" t="s">
+      <c r="DW5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="DW5" s="8" t="s">
+      <c r="DX5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="DX5" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="DY5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="DZ5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="DZ5" s="7" t="s">
+      <c r="EA5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="EA5" s="7" t="s">
+      <c r="EB5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="EB5" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="EC5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="ED5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="ED5" s="8" t="s">
+      <c r="EE5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="EE5" s="8" t="s">
+      <c r="EF5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="EF5" s="8" t="s">
+      <c r="EG5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="EG5" s="8" t="s">
+      <c r="EH5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="EH5" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="EI5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="EJ5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="EJ5" s="7" t="s">
+      <c r="EK5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="EK5" s="7" t="s">
+      <c r="EL5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="EL5" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="EM5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="EN5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="EN5" s="8" t="s">
+      <c r="EO5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="EO5" s="8" t="s">
+      <c r="EP5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="EP5" s="8" t="s">
+      <c r="EQ5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="EQ5" s="8" t="s">
+      <c r="ER5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="ER5" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="ES5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="ET5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="ET5" s="7" t="s">
+      <c r="EU5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="EU5" s="7" t="s">
+      <c r="EV5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="EV5" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="EW5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="EX5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="EX5" s="8" t="s">
+      <c r="EY5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="EY5" s="8" t="s">
+      <c r="EZ5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="EZ5" s="8" t="s">
+      <c r="FA5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="FA5" s="8" t="s">
+      <c r="FB5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="FB5" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="FC5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="FD5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="FD5" s="7" t="s">
+      <c r="FE5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="FE5" s="7" t="s">
+      <c r="FF5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="FF5" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="FG5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="FH5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="FH5" s="8" t="s">
+      <c r="FI5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="FI5" s="8" t="s">
+      <c r="FJ5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="FJ5" s="8" t="s">
+      <c r="FK5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="FK5" s="8" t="s">
+      <c r="FL5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="FL5" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="FM5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="FN5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="FN5" s="7" t="s">
+      <c r="FO5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="FO5" s="7" t="s">
+      <c r="FP5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="FP5" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="FQ5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="FR5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="FR5" s="8" t="s">
+      <c r="FS5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="FS5" s="8" t="s">
+      <c r="FT5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="FT5" s="8" t="s">
+      <c r="FU5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="FU5" s="8" t="s">
+      <c r="FV5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="FV5" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="FW5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="FX5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="FX5" s="7" t="s">
+      <c r="FY5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="FY5" s="7" t="s">
+      <c r="FZ5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="FZ5" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="GA5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="GB5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="GB5" s="8" t="s">
+      <c r="GC5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="GC5" s="8" t="s">
+      <c r="GD5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="GD5" s="8" t="s">
+      <c r="GE5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="GE5" s="8" t="s">
+      <c r="GF5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="GF5" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="GG5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="GH5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="GH5" s="7" t="s">
+      <c r="GI5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="GI5" s="7" t="s">
+      <c r="GJ5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="GJ5" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="GK5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="GL5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="GL5" s="8" t="s">
+      <c r="GM5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="GM5" s="8" t="s">
+      <c r="GN5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="GN5" s="8" t="s">
+      <c r="GO5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="GO5" s="8" t="s">
+      <c r="GP5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="GP5" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="GQ5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="GR5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="GR5" s="7" t="s">
+      <c r="GS5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="GS5" s="7" t="s">
+      <c r="GT5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="GT5" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="GU5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="GV5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="GV5" s="8" t="s">
+      <c r="GW5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="GW5" s="8" t="s">
+      <c r="GX5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="GX5" s="8" t="s">
+      <c r="GY5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="GY5" s="8" t="s">
+      <c r="GZ5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="GZ5" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="HA5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="HB5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="HB5" s="7" t="s">
+      <c r="HC5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="HC5" s="7" t="s">
+      <c r="HD5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="HD5" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="HE5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="HF5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="HF5" s="8" t="s">
+      <c r="HG5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="HG5" s="8" t="s">
+      <c r="HH5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="HH5" s="8" t="s">
+      <c r="HI5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="HI5" s="8" t="s">
+      <c r="HJ5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="HJ5" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="HK5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="HL5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="HL5" s="7" t="s">
+      <c r="HM5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="HM5" s="7" t="s">
+      <c r="HN5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="HN5" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="HO5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="HP5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="HP5" s="8" t="s">
+      <c r="HQ5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="HQ5" s="8" t="s">
+      <c r="HR5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="HR5" s="8" t="s">
+      <c r="HS5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="HS5" s="8" t="s">
+      <c r="HT5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="HT5" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="HU5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="HV5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="HV5" s="7" t="s">
+      <c r="HW5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="HW5" s="7" t="s">
+      <c r="HX5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="HX5" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="HY5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="HZ5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="HZ5" s="8" t="s">
+      <c r="IA5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="IA5" s="8" t="s">
+      <c r="IB5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="IB5" s="8" t="s">
+      <c r="IC5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="IC5" s="8" t="s">
+      <c r="ID5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="ID5" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="IE5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="IF5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="IF5" s="7" t="s">
+      <c r="IG5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="IG5" s="7" t="s">
+      <c r="IH5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="IH5" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="II5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="IJ5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="IJ5" s="8" t="s">
+      <c r="IK5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="IK5" s="8" t="s">
+      <c r="IL5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="IL5" s="8" t="s">
+      <c r="IM5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="IM5" s="8" t="s">
+      <c r="IN5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="IN5" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="IO5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="IP5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="IP5" s="7" t="s">
+      <c r="IQ5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="IQ5" s="7" t="s">
+      <c r="IR5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="IR5" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="IS5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="IT5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="IT5" s="8" t="s">
+      <c r="IU5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="IU5" s="8" t="s">
+      <c r="IV5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="IV5" s="8" t="s">
+      <c r="IW5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="IW5" s="8" t="s">
+      <c r="IX5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="IX5" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="IY5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="IZ5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="IZ5" s="7" t="s">
+      <c r="JA5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="JA5" s="7" t="s">
+      <c r="JB5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="JB5" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="JC5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="JD5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="JD5" s="8" t="s">
+      <c r="JE5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="JE5" s="8" t="s">
+      <c r="JF5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="JF5" s="8" t="s">
+      <c r="JG5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="JG5" s="8" t="s">
+      <c r="JH5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="JH5" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="JI5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="JJ5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="JJ5" s="7" t="s">
+      <c r="JK5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="JK5" s="7" t="s">
+      <c r="JL5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="JL5" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="JM5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="JN5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="JN5" s="8" t="s">
+      <c r="JO5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="JO5" s="8" t="s">
+      <c r="JP5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="JP5" s="8" t="s">
+      <c r="JQ5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="JQ5" s="8" t="s">
+      <c r="JR5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="JR5" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="JS5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="JT5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="JT5" s="7" t="s">
+      <c r="JU5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="JU5" s="7" t="s">
+      <c r="JV5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="JV5" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="JW5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="JX5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="JX5" s="8" t="s">
+      <c r="JY5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="JY5" s="8" t="s">
+      <c r="JZ5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="JZ5" s="8" t="s">
+      <c r="KA5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="KA5" s="8" t="s">
+      <c r="KB5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="KB5" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="KC5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="KD5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="KD5" s="7" t="s">
+      <c r="KE5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="KE5" s="7" t="s">
+      <c r="KF5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="KF5" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="KG5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="KH5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="KH5" s="8" t="s">
+      <c r="KI5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="KI5" s="8" t="s">
+      <c r="KJ5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="KJ5" s="8" t="s">
+      <c r="KK5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="KK5" s="8" t="s">
+      <c r="KL5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="KL5" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="KM5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="KN5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="KN5" s="7" t="s">
+      <c r="KO5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="KO5" s="7" t="s">
+      <c r="KP5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="KP5" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="KQ5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="KR5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="KR5" s="8" t="s">
+      <c r="KS5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="KS5" s="8" t="s">
+      <c r="KT5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="KT5" s="8" t="s">
+      <c r="KU5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="KU5" s="8" t="s">
+      <c r="KV5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="KV5" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="KW5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="KX5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="KX5" s="7" t="s">
+      <c r="KY5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="KY5" s="7" t="s">
+      <c r="KZ5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="KZ5" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="LA5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="LB5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="LB5" s="8" t="s">
+      <c r="LC5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="LC5" s="8" t="s">
+      <c r="LD5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="LD5" s="8" t="s">
+      <c r="LE5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="LE5" s="8" t="s">
+      <c r="LF5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="LF5" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="LG5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="LH5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="LH5" s="7" t="s">
+      <c r="LI5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="LI5" s="7" t="s">
+      <c r="LJ5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="LJ5" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="LK5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="LL5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="LL5" s="8" t="s">
+      <c r="LM5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="LM5" s="8" t="s">
+      <c r="LN5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="LN5" s="8" t="s">
+      <c r="LO5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="LO5" s="8" t="s">
+      <c r="LP5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="LP5" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="LQ5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="LR5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="LR5" s="7" t="s">
+      <c r="LS5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="LS5" s="7" t="s">
+      <c r="LT5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="LT5" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="LU5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="LV5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="LV5" s="8" t="s">
+      <c r="LW5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="LW5" s="8" t="s">
+      <c r="LX5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="LX5" s="8" t="s">
+      <c r="LY5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="LY5" s="8" t="s">
+      <c r="LZ5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="LZ5" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="MA5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="MB5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="MB5" s="7" t="s">
+      <c r="MC5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="MC5" s="7" t="s">
+      <c r="MD5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="MD5" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="ME5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="MF5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="MF5" s="8" t="s">
+      <c r="MG5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="MG5" s="8" t="s">
+      <c r="MH5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="MH5" s="8" t="s">
+      <c r="MI5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="MI5" s="8" t="s">
+      <c r="MJ5" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="MJ5" s="8" t="s">
-        <v>23</v>
       </c>
       <c r="MK5" s="87"/>
       <c r="ML5" s="87"/>
@@ -4829,1118 +4828,1118 @@
     </row>
     <row r="6" spans="1:369" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="D6" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="E6" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="F6" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="G6" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="H6" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="I6" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="J6" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="K6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="L6" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="L6" s="9" t="s">
+      <c r="M6" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="M6" s="12" t="s">
+      <c r="N6" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="N6" s="13" t="s">
+      <c r="O6" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="O6" s="12" t="s">
+      <c r="P6" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="P6" s="14" t="s">
+      <c r="Q6" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="Q6" s="15" t="s">
+      <c r="R6" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="R6" s="15" t="s">
+      <c r="S6" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="S6" s="9" t="s">
+      <c r="T6" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="T6" s="9" t="s">
+      <c r="U6" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="U6" s="9" t="s">
+      <c r="V6" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="V6" s="15" t="s">
+      <c r="W6" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="W6" s="15" t="s">
+      <c r="X6" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="X6" s="9" t="s">
+      <c r="Y6" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="Y6" s="9" t="s">
+      <c r="Z6" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="Z6" s="9" t="s">
+      <c r="AA6" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="AA6" s="9" t="s">
+      <c r="AB6" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="AB6" s="9" t="s">
+      <c r="AC6" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="AC6" s="9" t="s">
+      <c r="AD6" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="AD6" s="9" t="s">
+      <c r="AE6" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="AF6" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="AE6" s="9" t="s">
+      <c r="AG6" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH6" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="AI6" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ6" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK6" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL6" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM6" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN6" s="18" t="s">
+        <v>399</v>
+      </c>
+      <c r="AO6" s="18" t="s">
+        <v>400</v>
+      </c>
+      <c r="AP6" s="18" t="s">
+        <v>401</v>
+      </c>
+      <c r="AQ6" s="18" t="s">
+        <v>402</v>
+      </c>
+      <c r="AR6" s="18" t="s">
+        <v>403</v>
+      </c>
+      <c r="AS6" s="18" t="s">
+        <v>404</v>
+      </c>
+      <c r="AT6" s="18" t="s">
+        <v>405</v>
+      </c>
+      <c r="AU6" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="AV6" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="AW6" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="AX6" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="AY6" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="AZ6" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="BA6" s="18" t="s">
+        <v>308</v>
+      </c>
+      <c r="BB6" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="BC6" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="BD6" s="18" t="s">
+        <v>311</v>
+      </c>
+      <c r="BE6" s="18" t="s">
+        <v>312</v>
+      </c>
+      <c r="BF6" s="18" t="s">
+        <v>313</v>
+      </c>
+      <c r="BG6" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="BH6" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="BI6" s="18" t="s">
+        <v>316</v>
+      </c>
+      <c r="BJ6" s="18" t="s">
+        <v>317</v>
+      </c>
+      <c r="BK6" s="18" t="s">
+        <v>318</v>
+      </c>
+      <c r="BL6" s="18" t="s">
+        <v>319</v>
+      </c>
+      <c r="BM6" s="18" t="s">
+        <v>320</v>
+      </c>
+      <c r="BN6" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="BO6" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="BP6" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="BQ6" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="BR6" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="BS6" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="BT6" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="BU6" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="BV6" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="BW6" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="BX6" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="BY6" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="BZ6" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="CA6" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="CB6" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="CC6" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="CD6" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="CE6" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="CF6" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="CG6" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="CH6" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="CI6" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="CJ6" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="CK6" s="18" t="s">
+        <v>326</v>
+      </c>
+      <c r="CL6" s="18" t="s">
+        <v>327</v>
+      </c>
+      <c r="CM6" s="18" t="s">
+        <v>328</v>
+      </c>
+      <c r="CN6" s="18" t="s">
+        <v>329</v>
+      </c>
+      <c r="CO6" s="18" t="s">
+        <v>330</v>
+      </c>
+      <c r="CP6" s="18" t="s">
+        <v>331</v>
+      </c>
+      <c r="CQ6" s="18" t="s">
+        <v>332</v>
+      </c>
+      <c r="CR6" s="18" t="s">
+        <v>333</v>
+      </c>
+      <c r="CS6" s="18" t="s">
+        <v>334</v>
+      </c>
+      <c r="CT6" s="18" t="s">
+        <v>335</v>
+      </c>
+      <c r="CU6" s="18" t="s">
+        <v>336</v>
+      </c>
+      <c r="CV6" s="18" t="s">
+        <v>337</v>
+      </c>
+      <c r="CW6" s="18" t="s">
+        <v>338</v>
+      </c>
+      <c r="CX6" s="18" t="s">
+        <v>339</v>
+      </c>
+      <c r="CY6" s="18" t="s">
+        <v>340</v>
+      </c>
+      <c r="CZ6" s="18" t="s">
+        <v>341</v>
+      </c>
+      <c r="DA6" s="18" t="s">
+        <v>342</v>
+      </c>
+      <c r="DB6" s="18" t="s">
+        <v>343</v>
+      </c>
+      <c r="DC6" s="18" t="s">
+        <v>344</v>
+      </c>
+      <c r="DD6" s="18" t="s">
+        <v>345</v>
+      </c>
+      <c r="DE6" s="18" t="s">
+        <v>346</v>
+      </c>
+      <c r="DF6" s="18" t="s">
+        <v>347</v>
+      </c>
+      <c r="DG6" s="18" t="s">
+        <v>348</v>
+      </c>
+      <c r="DH6" s="18" t="s">
+        <v>349</v>
+      </c>
+      <c r="DI6" s="18" t="s">
+        <v>350</v>
+      </c>
+      <c r="DJ6" s="18" t="s">
+        <v>351</v>
+      </c>
+      <c r="DK6" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="DL6" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="DM6" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="DN6" s="18" t="s">
+        <v>355</v>
+      </c>
+      <c r="DO6" s="18" t="s">
+        <v>356</v>
+      </c>
+      <c r="DP6" s="18" t="s">
+        <v>357</v>
+      </c>
+      <c r="DQ6" s="18" t="s">
+        <v>358</v>
+      </c>
+      <c r="DR6" s="18" t="s">
+        <v>359</v>
+      </c>
+      <c r="DS6" s="18" t="s">
+        <v>360</v>
+      </c>
+      <c r="DT6" s="18" t="s">
+        <v>361</v>
+      </c>
+      <c r="DU6" s="18" t="s">
+        <v>362</v>
+      </c>
+      <c r="DV6" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="DW6" s="18" t="s">
+        <v>364</v>
+      </c>
+      <c r="DX6" s="18" t="s">
+        <v>365</v>
+      </c>
+      <c r="DY6" s="18" t="s">
+        <v>367</v>
+      </c>
+      <c r="DZ6" s="18" t="s">
+        <v>368</v>
+      </c>
+      <c r="EA6" s="18" t="s">
+        <v>369</v>
+      </c>
+      <c r="EB6" s="18" t="s">
+        <v>370</v>
+      </c>
+      <c r="EC6" s="18" t="s">
+        <v>371</v>
+      </c>
+      <c r="ED6" s="18" t="s">
+        <v>372</v>
+      </c>
+      <c r="EE6" s="18" t="s">
+        <v>373</v>
+      </c>
+      <c r="EF6" s="18" t="s">
+        <v>374</v>
+      </c>
+      <c r="EG6" s="18" t="s">
+        <v>375</v>
+      </c>
+      <c r="EH6" s="18" t="s">
+        <v>376</v>
+      </c>
+      <c r="EI6" s="18" t="s">
+        <v>378</v>
+      </c>
+      <c r="EJ6" s="18" t="s">
+        <v>379</v>
+      </c>
+      <c r="EK6" s="18" t="s">
+        <v>380</v>
+      </c>
+      <c r="EL6" s="18" t="s">
+        <v>381</v>
+      </c>
+      <c r="EM6" s="18" t="s">
+        <v>382</v>
+      </c>
+      <c r="EN6" s="18" t="s">
+        <v>383</v>
+      </c>
+      <c r="EO6" s="18" t="s">
+        <v>384</v>
+      </c>
+      <c r="EP6" s="18" t="s">
+        <v>385</v>
+      </c>
+      <c r="EQ6" s="18" t="s">
+        <v>386</v>
+      </c>
+      <c r="ER6" s="18" t="s">
+        <v>387</v>
+      </c>
+      <c r="ES6" s="18" t="s">
+        <v>389</v>
+      </c>
+      <c r="ET6" s="18" t="s">
+        <v>390</v>
+      </c>
+      <c r="EU6" s="18" t="s">
+        <v>391</v>
+      </c>
+      <c r="EV6" s="18" t="s">
+        <v>392</v>
+      </c>
+      <c r="EW6" s="18" t="s">
+        <v>393</v>
+      </c>
+      <c r="EX6" s="18" t="s">
+        <v>394</v>
+      </c>
+      <c r="EY6" s="18" t="s">
+        <v>395</v>
+      </c>
+      <c r="EZ6" s="18" t="s">
+        <v>396</v>
+      </c>
+      <c r="FA6" s="18" t="s">
+        <v>397</v>
+      </c>
+      <c r="FB6" s="18" t="s">
+        <v>398</v>
+      </c>
+      <c r="FC6" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="FD6" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="FE6" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="FF6" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="FG6" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="FH6" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="FI6" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="FJ6" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="FK6" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="FL6" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="FM6" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="FN6" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="FO6" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="FP6" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="FQ6" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="FR6" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="FS6" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="FT6" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="FU6" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="FV6" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="FW6" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="FX6" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="FY6" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="FZ6" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="GA6" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="GB6" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="GC6" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="GD6" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="GE6" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="GF6" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="GG6" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="GH6" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="GI6" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="GJ6" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="GK6" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="GL6" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="GM6" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="GN6" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="GO6" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="GP6" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="GQ6" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="GR6" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="GS6" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="GT6" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="GU6" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="GV6" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="GW6" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="GX6" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="GY6" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="GZ6" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="HA6" s="18" t="s">
+        <v>406</v>
+      </c>
+      <c r="HB6" s="18" t="s">
+        <v>407</v>
+      </c>
+      <c r="HC6" s="18" t="s">
+        <v>408</v>
+      </c>
+      <c r="HD6" s="18" t="s">
+        <v>409</v>
+      </c>
+      <c r="HE6" s="18" t="s">
+        <v>410</v>
+      </c>
+      <c r="HF6" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="HG6" s="18" t="s">
+        <v>412</v>
+      </c>
+      <c r="HH6" s="18" t="s">
+        <v>413</v>
+      </c>
+      <c r="HI6" s="18" t="s">
+        <v>414</v>
+      </c>
+      <c r="HJ6" s="18" t="s">
+        <v>415</v>
+      </c>
+      <c r="HK6" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="HL6" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="HM6" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="HN6" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="HO6" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="HP6" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="HQ6" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="HR6" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="HS6" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="AF6" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="AG6" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH6" s="17" t="s">
+      <c r="HT6" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="AI6" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="AJ6" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="AK6" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="AL6" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="AM6" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="AN6" s="18" t="s">
-        <v>410</v>
-      </c>
-      <c r="AO6" s="18" t="s">
-        <v>411</v>
-      </c>
-      <c r="AP6" s="18" t="s">
-        <v>412</v>
-      </c>
-      <c r="AQ6" s="18" t="s">
-        <v>413</v>
-      </c>
-      <c r="AR6" s="18" t="s">
-        <v>414</v>
-      </c>
-      <c r="AS6" s="18" t="s">
-        <v>415</v>
-      </c>
-      <c r="AT6" s="18" t="s">
-        <v>416</v>
-      </c>
-      <c r="AU6" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="AV6" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="AW6" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="AX6" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="AY6" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="AZ6" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="BA6" s="18" t="s">
-        <v>319</v>
-      </c>
-      <c r="BB6" s="18" t="s">
-        <v>320</v>
-      </c>
-      <c r="BC6" s="18" t="s">
-        <v>321</v>
-      </c>
-      <c r="BD6" s="18" t="s">
-        <v>322</v>
-      </c>
-      <c r="BE6" s="18" t="s">
-        <v>323</v>
-      </c>
-      <c r="BF6" s="18" t="s">
-        <v>324</v>
-      </c>
-      <c r="BG6" s="18" t="s">
-        <v>325</v>
-      </c>
-      <c r="BH6" s="18" t="s">
-        <v>326</v>
-      </c>
-      <c r="BI6" s="18" t="s">
-        <v>327</v>
-      </c>
-      <c r="BJ6" s="18" t="s">
-        <v>328</v>
-      </c>
-      <c r="BK6" s="18" t="s">
-        <v>329</v>
-      </c>
-      <c r="BL6" s="18" t="s">
-        <v>330</v>
-      </c>
-      <c r="BM6" s="18" t="s">
-        <v>331</v>
-      </c>
-      <c r="BN6" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="BO6" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="BP6" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="BQ6" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="BR6" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="BS6" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="BT6" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="BU6" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="BV6" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="BW6" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="BX6" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="BY6" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="BZ6" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="CA6" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="CB6" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="CC6" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="CD6" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="CE6" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="CF6" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="CG6" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="CH6" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="CI6" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="CJ6" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="CK6" s="18" t="s">
-        <v>337</v>
-      </c>
-      <c r="CL6" s="18" t="s">
-        <v>338</v>
-      </c>
-      <c r="CM6" s="18" t="s">
-        <v>339</v>
-      </c>
-      <c r="CN6" s="18" t="s">
-        <v>340</v>
-      </c>
-      <c r="CO6" s="18" t="s">
-        <v>341</v>
-      </c>
-      <c r="CP6" s="18" t="s">
-        <v>342</v>
-      </c>
-      <c r="CQ6" s="18" t="s">
-        <v>343</v>
-      </c>
-      <c r="CR6" s="18" t="s">
-        <v>344</v>
-      </c>
-      <c r="CS6" s="18" t="s">
-        <v>345</v>
-      </c>
-      <c r="CT6" s="18" t="s">
-        <v>346</v>
-      </c>
-      <c r="CU6" s="18" t="s">
-        <v>347</v>
-      </c>
-      <c r="CV6" s="18" t="s">
-        <v>348</v>
-      </c>
-      <c r="CW6" s="18" t="s">
-        <v>349</v>
-      </c>
-      <c r="CX6" s="18" t="s">
-        <v>350</v>
-      </c>
-      <c r="CY6" s="18" t="s">
-        <v>351</v>
-      </c>
-      <c r="CZ6" s="18" t="s">
-        <v>352</v>
-      </c>
-      <c r="DA6" s="18" t="s">
-        <v>353</v>
-      </c>
-      <c r="DB6" s="18" t="s">
-        <v>354</v>
-      </c>
-      <c r="DC6" s="18" t="s">
-        <v>355</v>
-      </c>
-      <c r="DD6" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="DE6" s="18" t="s">
-        <v>357</v>
-      </c>
-      <c r="DF6" s="18" t="s">
-        <v>358</v>
-      </c>
-      <c r="DG6" s="18" t="s">
-        <v>359</v>
-      </c>
-      <c r="DH6" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="DI6" s="18" t="s">
-        <v>361</v>
-      </c>
-      <c r="DJ6" s="18" t="s">
-        <v>362</v>
-      </c>
-      <c r="DK6" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="DL6" s="18" t="s">
-        <v>364</v>
-      </c>
-      <c r="DM6" s="18" t="s">
-        <v>365</v>
-      </c>
-      <c r="DN6" s="18" t="s">
-        <v>366</v>
-      </c>
-      <c r="DO6" s="18" t="s">
-        <v>367</v>
-      </c>
-      <c r="DP6" s="18" t="s">
-        <v>368</v>
-      </c>
-      <c r="DQ6" s="18" t="s">
-        <v>369</v>
-      </c>
-      <c r="DR6" s="18" t="s">
-        <v>370</v>
-      </c>
-      <c r="DS6" s="18" t="s">
-        <v>371</v>
-      </c>
-      <c r="DT6" s="18" t="s">
-        <v>372</v>
-      </c>
-      <c r="DU6" s="18" t="s">
-        <v>373</v>
-      </c>
-      <c r="DV6" s="18" t="s">
-        <v>374</v>
-      </c>
-      <c r="DW6" s="18" t="s">
-        <v>375</v>
-      </c>
-      <c r="DX6" s="18" t="s">
-        <v>376</v>
-      </c>
-      <c r="DY6" s="18" t="s">
-        <v>378</v>
-      </c>
-      <c r="DZ6" s="18" t="s">
-        <v>379</v>
-      </c>
-      <c r="EA6" s="18" t="s">
-        <v>380</v>
-      </c>
-      <c r="EB6" s="18" t="s">
-        <v>381</v>
-      </c>
-      <c r="EC6" s="18" t="s">
-        <v>382</v>
-      </c>
-      <c r="ED6" s="18" t="s">
-        <v>383</v>
-      </c>
-      <c r="EE6" s="18" t="s">
-        <v>384</v>
-      </c>
-      <c r="EF6" s="18" t="s">
-        <v>385</v>
-      </c>
-      <c r="EG6" s="18" t="s">
-        <v>386</v>
-      </c>
-      <c r="EH6" s="18" t="s">
-        <v>387</v>
-      </c>
-      <c r="EI6" s="18" t="s">
-        <v>389</v>
-      </c>
-      <c r="EJ6" s="18" t="s">
-        <v>390</v>
-      </c>
-      <c r="EK6" s="18" t="s">
-        <v>391</v>
-      </c>
-      <c r="EL6" s="18" t="s">
-        <v>392</v>
-      </c>
-      <c r="EM6" s="18" t="s">
-        <v>393</v>
-      </c>
-      <c r="EN6" s="18" t="s">
-        <v>394</v>
-      </c>
-      <c r="EO6" s="18" t="s">
-        <v>395</v>
-      </c>
-      <c r="EP6" s="18" t="s">
-        <v>396</v>
-      </c>
-      <c r="EQ6" s="18" t="s">
-        <v>397</v>
-      </c>
-      <c r="ER6" s="18" t="s">
-        <v>398</v>
-      </c>
-      <c r="ES6" s="18" t="s">
-        <v>400</v>
-      </c>
-      <c r="ET6" s="18" t="s">
-        <v>401</v>
-      </c>
-      <c r="EU6" s="18" t="s">
-        <v>402</v>
-      </c>
-      <c r="EV6" s="18" t="s">
-        <v>403</v>
-      </c>
-      <c r="EW6" s="18" t="s">
-        <v>404</v>
-      </c>
-      <c r="EX6" s="18" t="s">
-        <v>405</v>
-      </c>
-      <c r="EY6" s="18" t="s">
-        <v>406</v>
-      </c>
-      <c r="EZ6" s="18" t="s">
-        <v>407</v>
-      </c>
-      <c r="FA6" s="18" t="s">
-        <v>408</v>
-      </c>
-      <c r="FB6" s="18" t="s">
-        <v>409</v>
-      </c>
-      <c r="FC6" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="FD6" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="FE6" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="FF6" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="FG6" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="FH6" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="FI6" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="FJ6" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="FK6" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="FL6" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="FM6" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="FN6" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="FO6" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="FP6" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="FQ6" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="FR6" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="FS6" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="FT6" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="FU6" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="FV6" s="18" t="s">
-        <v>149</v>
-      </c>
-      <c r="FW6" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="FX6" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="FY6" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="FZ6" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="GA6" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="GB6" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="GC6" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="GD6" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="GE6" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="GF6" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="GG6" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="GH6" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="GI6" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="GJ6" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="GK6" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="GL6" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="GM6" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="GN6" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="GO6" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="GP6" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="GQ6" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="GR6" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="GS6" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="GT6" s="9" t="s">
+      <c r="HU6" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="HV6" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="HW6" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="HX6" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="HY6" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="HZ6" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="IA6" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="IB6" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="IC6" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="ID6" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="IE6" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="IF6" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="IG6" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="IH6" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="II6" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="IJ6" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="IK6" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="IL6" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="IM6" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="IN6" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="IO6" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="IP6" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="IQ6" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="IR6" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="IS6" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="IT6" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="IU6" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="IV6" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="IW6" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="IX6" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="IY6" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="IZ6" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="JA6" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="JB6" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="JC6" s="18" t="s">
+        <v>215</v>
+      </c>
+      <c r="JD6" s="18" t="s">
+        <v>216</v>
+      </c>
+      <c r="JE6" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="JF6" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="JG6" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="JH6" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="JI6" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="JJ6" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="JK6" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="JL6" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="JM6" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="JN6" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="JO6" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="JP6" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="JQ6" s="18" t="s">
+        <v>230</v>
+      </c>
+      <c r="JR6" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="JS6" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="JT6" s="18" t="s">
+        <v>233</v>
+      </c>
+      <c r="JU6" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="JV6" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="JW6" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="JX6" s="18" t="s">
+        <v>238</v>
+      </c>
+      <c r="JY6" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="JZ6" s="18" t="s">
+        <v>240</v>
+      </c>
+      <c r="KA6" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="KB6" s="18" t="s">
+        <v>242</v>
+      </c>
+      <c r="KC6" s="18" t="s">
+        <v>243</v>
+      </c>
+      <c r="KD6" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="KE6" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="KF6" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="KG6" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="KH6" s="18" t="s">
+        <v>248</v>
+      </c>
+      <c r="KI6" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="KJ6" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="KK6" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="KL6" s="18" t="s">
+        <v>252</v>
+      </c>
+      <c r="KM6" s="18" t="s">
+        <v>254</v>
+      </c>
+      <c r="KN6" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="KO6" s="18" t="s">
+        <v>256</v>
+      </c>
+      <c r="KP6" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="KQ6" s="18" t="s">
+        <v>258</v>
+      </c>
+      <c r="KR6" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="KS6" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="KT6" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="KU6" s="18" t="s">
+        <v>262</v>
+      </c>
+      <c r="KV6" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="KW6" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="KX6" s="18" t="s">
+        <v>266</v>
+      </c>
+      <c r="KY6" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="KZ6" s="18" t="s">
+        <v>268</v>
+      </c>
+      <c r="LA6" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="LB6" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="LC6" s="18" t="s">
+        <v>271</v>
+      </c>
+      <c r="LD6" s="18" t="s">
+        <v>272</v>
+      </c>
+      <c r="LE6" s="18" t="s">
+        <v>273</v>
+      </c>
+      <c r="LF6" s="18" t="s">
+        <v>274</v>
+      </c>
+      <c r="LG6" s="18" t="s">
+        <v>276</v>
+      </c>
+      <c r="LH6" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="LI6" s="18" t="s">
+        <v>278</v>
+      </c>
+      <c r="LJ6" s="18" t="s">
+        <v>279</v>
+      </c>
+      <c r="LK6" s="18" t="s">
+        <v>280</v>
+      </c>
+      <c r="LL6" s="18" t="s">
+        <v>303</v>
+      </c>
+      <c r="LM6" s="18" t="s">
+        <v>304</v>
+      </c>
+      <c r="LN6" s="18" t="s">
+        <v>305</v>
+      </c>
+      <c r="LO6" s="18" t="s">
+        <v>306</v>
+      </c>
+      <c r="LP6" s="18" t="s">
+        <v>307</v>
+      </c>
+      <c r="LQ6" s="18" t="s">
+        <v>282</v>
+      </c>
+      <c r="LR6" s="18" t="s">
+        <v>283</v>
+      </c>
+      <c r="LS6" s="18" t="s">
+        <v>284</v>
+      </c>
+      <c r="LT6" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="LU6" s="18" t="s">
+        <v>286</v>
+      </c>
+      <c r="LV6" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="LW6" s="18" t="s">
+        <v>288</v>
+      </c>
+      <c r="LX6" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="LY6" s="18" t="s">
+        <v>290</v>
+      </c>
+      <c r="LZ6" s="18" t="s">
+        <v>291</v>
+      </c>
+      <c r="MA6" s="18" t="s">
+        <v>293</v>
+      </c>
+      <c r="MB6" s="18" t="s">
+        <v>294</v>
+      </c>
+      <c r="MC6" s="18" t="s">
+        <v>295</v>
+      </c>
+      <c r="MD6" s="18" t="s">
+        <v>296</v>
+      </c>
+      <c r="ME6" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="MF6" s="18" t="s">
+        <v>298</v>
+      </c>
+      <c r="MG6" s="18" t="s">
+        <v>299</v>
+      </c>
+      <c r="MH6" s="18" t="s">
+        <v>300</v>
+      </c>
+      <c r="MI6" s="18" t="s">
+        <v>301</v>
+      </c>
+      <c r="MJ6" s="18" t="s">
+        <v>302</v>
+      </c>
+      <c r="MK6" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="GU6" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="GV6" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="GW6" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="GX6" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="GY6" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="GZ6" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="HA6" s="18" t="s">
+      <c r="ML6" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="HB6" s="18" t="s">
+      <c r="MM6" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="HC6" s="18" t="s">
+      <c r="MN6" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="HD6" s="18" t="s">
+      <c r="MO6" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="HE6" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="HF6" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="HG6" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="HH6" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="HI6" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="HJ6" s="18" t="s">
-        <v>173</v>
-      </c>
-      <c r="HK6" s="18" t="s">
-        <v>178</v>
-      </c>
-      <c r="HL6" s="18" t="s">
-        <v>179</v>
-      </c>
-      <c r="HM6" s="18" t="s">
-        <v>180</v>
-      </c>
-      <c r="HN6" s="18" t="s">
-        <v>181</v>
-      </c>
-      <c r="HO6" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="HP6" s="18" t="s">
-        <v>183</v>
-      </c>
-      <c r="HQ6" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="HR6" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="HS6" s="18" t="s">
-        <v>186</v>
-      </c>
-      <c r="HT6" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="HU6" s="18" t="s">
-        <v>189</v>
-      </c>
-      <c r="HV6" s="18" t="s">
-        <v>190</v>
-      </c>
-      <c r="HW6" s="18" t="s">
-        <v>191</v>
-      </c>
-      <c r="HX6" s="18" t="s">
-        <v>192</v>
-      </c>
-      <c r="HY6" s="18" t="s">
-        <v>193</v>
-      </c>
-      <c r="HZ6" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="IA6" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="IB6" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="IC6" s="18" t="s">
-        <v>197</v>
-      </c>
-      <c r="ID6" s="18" t="s">
-        <v>198</v>
-      </c>
-      <c r="IE6" s="18" t="s">
-        <v>200</v>
-      </c>
-      <c r="IF6" s="18" t="s">
-        <v>201</v>
-      </c>
-      <c r="IG6" s="18" t="s">
-        <v>202</v>
-      </c>
-      <c r="IH6" s="18" t="s">
-        <v>203</v>
-      </c>
-      <c r="II6" s="18" t="s">
-        <v>204</v>
-      </c>
-      <c r="IJ6" s="18" t="s">
-        <v>205</v>
-      </c>
-      <c r="IK6" s="18" t="s">
-        <v>206</v>
-      </c>
-      <c r="IL6" s="18" t="s">
-        <v>207</v>
-      </c>
-      <c r="IM6" s="18" t="s">
-        <v>208</v>
-      </c>
-      <c r="IN6" s="18" t="s">
-        <v>209</v>
-      </c>
-      <c r="IO6" s="18" t="s">
-        <v>211</v>
-      </c>
-      <c r="IP6" s="18" t="s">
-        <v>212</v>
-      </c>
-      <c r="IQ6" s="18" t="s">
-        <v>213</v>
-      </c>
-      <c r="IR6" s="18" t="s">
-        <v>214</v>
-      </c>
-      <c r="IS6" s="18" t="s">
-        <v>215</v>
-      </c>
-      <c r="IT6" s="18" t="s">
-        <v>216</v>
-      </c>
-      <c r="IU6" s="18" t="s">
-        <v>217</v>
-      </c>
-      <c r="IV6" s="18" t="s">
-        <v>218</v>
-      </c>
-      <c r="IW6" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="IX6" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="IY6" s="18" t="s">
-        <v>222</v>
-      </c>
-      <c r="IZ6" s="18" t="s">
-        <v>223</v>
-      </c>
-      <c r="JA6" s="18" t="s">
-        <v>224</v>
-      </c>
-      <c r="JB6" s="18" t="s">
-        <v>225</v>
-      </c>
-      <c r="JC6" s="18" t="s">
-        <v>226</v>
-      </c>
-      <c r="JD6" s="18" t="s">
-        <v>227</v>
-      </c>
-      <c r="JE6" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="JF6" s="18" t="s">
-        <v>229</v>
-      </c>
-      <c r="JG6" s="18" t="s">
-        <v>230</v>
-      </c>
-      <c r="JH6" s="18" t="s">
-        <v>231</v>
-      </c>
-      <c r="JI6" s="18" t="s">
-        <v>233</v>
-      </c>
-      <c r="JJ6" s="18" t="s">
-        <v>234</v>
-      </c>
-      <c r="JK6" s="18" t="s">
-        <v>235</v>
-      </c>
-      <c r="JL6" s="18" t="s">
-        <v>236</v>
-      </c>
-      <c r="JM6" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="JN6" s="18" t="s">
-        <v>238</v>
-      </c>
-      <c r="JO6" s="18" t="s">
-        <v>239</v>
-      </c>
-      <c r="JP6" s="18" t="s">
-        <v>240</v>
-      </c>
-      <c r="JQ6" s="18" t="s">
-        <v>241</v>
-      </c>
-      <c r="JR6" s="18" t="s">
-        <v>242</v>
-      </c>
-      <c r="JS6" s="18" t="s">
-        <v>245</v>
-      </c>
-      <c r="JT6" s="18" t="s">
-        <v>244</v>
-      </c>
-      <c r="JU6" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="JV6" s="18" t="s">
-        <v>247</v>
-      </c>
-      <c r="JW6" s="18" t="s">
-        <v>248</v>
-      </c>
-      <c r="JX6" s="18" t="s">
-        <v>249</v>
-      </c>
-      <c r="JY6" s="18" t="s">
-        <v>250</v>
-      </c>
-      <c r="JZ6" s="18" t="s">
-        <v>251</v>
-      </c>
-      <c r="KA6" s="18" t="s">
-        <v>252</v>
-      </c>
-      <c r="KB6" s="18" t="s">
-        <v>253</v>
-      </c>
-      <c r="KC6" s="18" t="s">
-        <v>254</v>
-      </c>
-      <c r="KD6" s="18" t="s">
-        <v>255</v>
-      </c>
-      <c r="KE6" s="18" t="s">
-        <v>256</v>
-      </c>
-      <c r="KF6" s="18" t="s">
-        <v>257</v>
-      </c>
-      <c r="KG6" s="18" t="s">
-        <v>258</v>
-      </c>
-      <c r="KH6" s="18" t="s">
-        <v>259</v>
-      </c>
-      <c r="KI6" s="18" t="s">
-        <v>260</v>
-      </c>
-      <c r="KJ6" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="KK6" s="18" t="s">
-        <v>262</v>
-      </c>
-      <c r="KL6" s="18" t="s">
-        <v>263</v>
-      </c>
-      <c r="KM6" s="18" t="s">
-        <v>265</v>
-      </c>
-      <c r="KN6" s="18" t="s">
-        <v>266</v>
-      </c>
-      <c r="KO6" s="18" t="s">
-        <v>267</v>
-      </c>
-      <c r="KP6" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="KQ6" s="18" t="s">
-        <v>269</v>
-      </c>
-      <c r="KR6" s="18" t="s">
-        <v>270</v>
-      </c>
-      <c r="KS6" s="18" t="s">
-        <v>271</v>
-      </c>
-      <c r="KT6" s="18" t="s">
-        <v>272</v>
-      </c>
-      <c r="KU6" s="18" t="s">
-        <v>273</v>
-      </c>
-      <c r="KV6" s="18" t="s">
-        <v>274</v>
-      </c>
-      <c r="KW6" s="18" t="s">
-        <v>276</v>
-      </c>
-      <c r="KX6" s="18" t="s">
-        <v>277</v>
-      </c>
-      <c r="KY6" s="18" t="s">
-        <v>278</v>
-      </c>
-      <c r="KZ6" s="18" t="s">
-        <v>279</v>
-      </c>
-      <c r="LA6" s="18" t="s">
-        <v>280</v>
-      </c>
-      <c r="LB6" s="18" t="s">
-        <v>281</v>
-      </c>
-      <c r="LC6" s="18" t="s">
-        <v>282</v>
-      </c>
-      <c r="LD6" s="18" t="s">
-        <v>283</v>
-      </c>
-      <c r="LE6" s="18" t="s">
-        <v>284</v>
-      </c>
-      <c r="LF6" s="18" t="s">
-        <v>285</v>
-      </c>
-      <c r="LG6" s="18" t="s">
-        <v>287</v>
-      </c>
-      <c r="LH6" s="18" t="s">
-        <v>288</v>
-      </c>
-      <c r="LI6" s="18" t="s">
-        <v>289</v>
-      </c>
-      <c r="LJ6" s="18" t="s">
-        <v>290</v>
-      </c>
-      <c r="LK6" s="18" t="s">
-        <v>291</v>
-      </c>
-      <c r="LL6" s="18" t="s">
-        <v>314</v>
-      </c>
-      <c r="LM6" s="18" t="s">
-        <v>315</v>
-      </c>
-      <c r="LN6" s="18" t="s">
-        <v>316</v>
-      </c>
-      <c r="LO6" s="18" t="s">
-        <v>317</v>
-      </c>
-      <c r="LP6" s="18" t="s">
-        <v>318</v>
-      </c>
-      <c r="LQ6" s="18" t="s">
-        <v>293</v>
-      </c>
-      <c r="LR6" s="18" t="s">
-        <v>294</v>
-      </c>
-      <c r="LS6" s="18" t="s">
-        <v>295</v>
-      </c>
-      <c r="LT6" s="18" t="s">
-        <v>296</v>
-      </c>
-      <c r="LU6" s="18" t="s">
-        <v>297</v>
-      </c>
-      <c r="LV6" s="18" t="s">
-        <v>298</v>
-      </c>
-      <c r="LW6" s="18" t="s">
-        <v>299</v>
-      </c>
-      <c r="LX6" s="18" t="s">
-        <v>300</v>
-      </c>
-      <c r="LY6" s="18" t="s">
-        <v>301</v>
-      </c>
-      <c r="LZ6" s="18" t="s">
-        <v>302</v>
-      </c>
-      <c r="MA6" s="18" t="s">
-        <v>304</v>
-      </c>
-      <c r="MB6" s="18" t="s">
-        <v>305</v>
-      </c>
-      <c r="MC6" s="18" t="s">
-        <v>306</v>
-      </c>
-      <c r="MD6" s="18" t="s">
-        <v>307</v>
-      </c>
-      <c r="ME6" s="18" t="s">
-        <v>308</v>
-      </c>
-      <c r="MF6" s="18" t="s">
-        <v>309</v>
-      </c>
-      <c r="MG6" s="18" t="s">
-        <v>310</v>
-      </c>
-      <c r="MH6" s="18" t="s">
-        <v>311</v>
-      </c>
-      <c r="MI6" s="18" t="s">
-        <v>312</v>
-      </c>
-      <c r="MJ6" s="18" t="s">
-        <v>313</v>
-      </c>
-      <c r="MK6" s="18" t="s">
+      <c r="MP6" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="ML6" s="18" t="s">
+      <c r="MQ6" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="MM6" s="18" t="s">
+      <c r="MR6" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="MN6" s="18" t="s">
+      <c r="MS6" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="MO6" s="18" t="s">
+      <c r="MT6" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="MP6" s="18" t="s">
+      <c r="MU6" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="MQ6" s="18" t="s">
+      <c r="MV6" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="MR6" s="18" t="s">
+      <c r="MW6" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="MS6" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="MT6" s="18" t="s">
+      <c r="MX6" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="MY6" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="MZ6" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="NA6" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="MU6" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="MV6" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="MW6" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="MX6" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="MY6" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="MZ6" s="18" t="s">
+      <c r="NB6" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="NC6" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="ND6" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="NA6" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="NB6" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="NC6" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="ND6" s="18" t="s">
-        <v>122</v>
-      </c>
       <c r="NE6" s="18" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:369" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="40"/>
       <c r="B7" s="40"/>
       <c r="C7" s="40" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D7" s="40"/>
       <c r="E7" s="40"/>
@@ -5953,17 +5952,17 @@
       <c r="L7" s="42"/>
       <c r="M7" s="42"/>
       <c r="N7" s="42" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="O7" s="42" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="P7" s="42"/>
       <c r="Q7" s="43" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="R7" s="43" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="S7" s="42"/>
       <c r="T7" s="42"/>
@@ -5975,13 +5974,13 @@
       <c r="Z7" s="47"/>
       <c r="AA7" s="46"/>
       <c r="AB7" s="41" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="AC7" s="41" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="AD7" s="41" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="AE7" s="42"/>
       <c r="AF7" s="48"/>
@@ -5995,7 +5994,7 @@
         <v>0</v>
       </c>
       <c r="AM7" s="51">
-        <f>SUM(CK7:CT7)</f>
+        <f>SUM(CA7:CJ7)</f>
         <v>0</v>
       </c>
       <c r="AN7" s="51">

</xml_diff>

<commit_message>
[RUBY-2584] FCRM1 report - Replace Main natural flood management measure
</commit_message>
<xml_diff>
--- a/lib/fcerm1_template.xlsx
+++ b/lib/fcerm1_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lb000070\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4942BD2C-5EE9-4304-9B8A-6A3718D9F79E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0924BB34-705D-4C39-9887-6F1B89CAF939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -236,9 +236,6 @@
     <t>Local Levy - PROJECT TOTAL</t>
   </si>
   <si>
-    <t>Internal Drainaged Board Precept - PROJECT TOTAL</t>
-  </si>
-  <si>
     <t>Public Contributions - PROJECT TOTAL</t>
   </si>
   <si>
@@ -246,9 +243,6 @@
   </si>
   <si>
     <t>Other EA Contributions - PROJECT TOTAL</t>
-  </si>
-  <si>
-    <t>Further Contributions Required - PROJECT TOTAL</t>
   </si>
   <si>
     <t>OM4a - PROJECT TOTAL</t>
@@ -1314,6 +1308,12 @@
   </si>
   <si>
     <t>OTHER FUNDING SOURCES NOT YET IDENTIFIED £</t>
+  </si>
+  <si>
+    <t>Internal Drainage Board Precept - PROJECT TOTAL</t>
+  </si>
+  <si>
+    <t>Future funding not yet identified - PROJECT TOTAL</t>
   </si>
 </sst>
 </file>
@@ -1883,18 +1883,75 @@
     <xf numFmtId="0" fontId="12" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="21" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1925,68 +1982,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="5" fillId="11" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -2295,11 +2295,11 @@
   <dimension ref="A1:NE7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="DH7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="AX7" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
       <selection pane="topRight" activeCell="C7" sqref="C7"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="HB6" sqref="HB6"/>
+      <selection pane="bottomRight" activeCell="AZ7" sqref="AZ7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2328,10 +2328,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:369" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="63"/>
+      <c r="B1" s="82"/>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
       <c r="E1" s="20"/>
@@ -2701,10 +2701,10 @@
       <c r="NE1" s="39"/>
     </row>
     <row r="2" spans="1:369" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="64" t="s">
-        <v>163</v>
-      </c>
-      <c r="B2" s="64"/>
+      <c r="A2" s="83" t="s">
+        <v>161</v>
+      </c>
+      <c r="B2" s="83"/>
       <c r="C2" s="19"/>
       <c r="D2" s="29"/>
       <c r="E2" s="20"/>
@@ -3445,525 +3445,525 @@
       <c r="NE3" s="39"/>
     </row>
     <row r="4" spans="1:369" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="66" t="s">
+      <c r="B4" s="84"/>
+      <c r="C4" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="67" t="s">
+      <c r="D4" s="85"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="85"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
+      <c r="I4" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="67"/>
-      <c r="K4" s="67"/>
-      <c r="L4" s="67"/>
-      <c r="M4" s="68" t="s">
+      <c r="J4" s="86"/>
+      <c r="K4" s="86"/>
+      <c r="L4" s="86"/>
+      <c r="M4" s="87" t="s">
         <v>4</v>
       </c>
-      <c r="N4" s="68"/>
-      <c r="O4" s="68"/>
-      <c r="P4" s="69" t="s">
+      <c r="N4" s="87"/>
+      <c r="O4" s="87"/>
+      <c r="P4" s="88" t="s">
+        <v>319</v>
+      </c>
+      <c r="Q4" s="88"/>
+      <c r="R4" s="88"/>
+      <c r="S4" s="88"/>
+      <c r="T4" s="88"/>
+      <c r="U4" s="89" t="s">
+        <v>5</v>
+      </c>
+      <c r="V4" s="89"/>
+      <c r="W4" s="89"/>
+      <c r="X4" s="89"/>
+      <c r="Y4" s="89"/>
+      <c r="Z4" s="89"/>
+      <c r="AA4" s="89"/>
+      <c r="AB4" s="90" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC4" s="90"/>
+      <c r="AD4" s="90"/>
+      <c r="AE4" s="81" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF4" s="81"/>
+      <c r="AG4" s="91"/>
+      <c r="AH4" s="91"/>
+      <c r="AI4" s="91"/>
+      <c r="AJ4" s="91"/>
+      <c r="AK4" s="91"/>
+      <c r="AL4" s="92" t="s">
+        <v>8</v>
+      </c>
+      <c r="AM4" s="92"/>
+      <c r="AN4" s="92"/>
+      <c r="AO4" s="92"/>
+      <c r="AP4" s="92"/>
+      <c r="AQ4" s="92"/>
+      <c r="AR4" s="92"/>
+      <c r="AS4" s="92"/>
+      <c r="AT4" s="92"/>
+      <c r="AU4" s="92"/>
+      <c r="AV4" s="92"/>
+      <c r="AW4" s="92"/>
+      <c r="AX4" s="92"/>
+      <c r="AY4" s="92"/>
+      <c r="AZ4" s="92"/>
+      <c r="BA4" s="92"/>
+      <c r="BB4" s="92"/>
+      <c r="BC4" s="92"/>
+      <c r="BD4" s="92"/>
+      <c r="BE4" s="92"/>
+      <c r="BF4" s="92"/>
+      <c r="BG4" s="92"/>
+      <c r="BH4" s="92"/>
+      <c r="BI4" s="92"/>
+      <c r="BJ4" s="92"/>
+      <c r="BK4" s="92"/>
+      <c r="BL4" s="92"/>
+      <c r="BM4" s="92"/>
+      <c r="BN4" s="92"/>
+      <c r="BO4" s="92"/>
+      <c r="BP4" s="92"/>
+      <c r="BQ4" s="70" t="s">
+        <v>9</v>
+      </c>
+      <c r="BR4" s="70"/>
+      <c r="BS4" s="70"/>
+      <c r="BT4" s="70"/>
+      <c r="BU4" s="70"/>
+      <c r="BV4" s="70"/>
+      <c r="BW4" s="70"/>
+      <c r="BX4" s="70"/>
+      <c r="BY4" s="70"/>
+      <c r="BZ4" s="70"/>
+      <c r="CA4" s="58" t="s">
+        <v>10</v>
+      </c>
+      <c r="CB4" s="58"/>
+      <c r="CC4" s="58"/>
+      <c r="CD4" s="58"/>
+      <c r="CE4" s="58"/>
+      <c r="CF4" s="58"/>
+      <c r="CG4" s="58"/>
+      <c r="CH4" s="58"/>
+      <c r="CI4" s="58"/>
+      <c r="CJ4" s="58"/>
+      <c r="CK4" s="62" t="s">
+        <v>320</v>
+      </c>
+      <c r="CL4" s="62"/>
+      <c r="CM4" s="62"/>
+      <c r="CN4" s="62"/>
+      <c r="CO4" s="62"/>
+      <c r="CP4" s="62"/>
+      <c r="CQ4" s="62"/>
+      <c r="CR4" s="62"/>
+      <c r="CS4" s="62"/>
+      <c r="CT4" s="62"/>
+      <c r="CU4" s="58" t="s">
         <v>321</v>
       </c>
-      <c r="Q4" s="69"/>
-      <c r="R4" s="69"/>
-      <c r="S4" s="69"/>
-      <c r="T4" s="69"/>
-      <c r="U4" s="70" t="s">
-        <v>5</v>
-      </c>
-      <c r="V4" s="70"/>
-      <c r="W4" s="70"/>
-      <c r="X4" s="70"/>
-      <c r="Y4" s="70"/>
-      <c r="Z4" s="70"/>
-      <c r="AA4" s="70"/>
-      <c r="AB4" s="71" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC4" s="71"/>
-      <c r="AD4" s="71"/>
-      <c r="AE4" s="62" t="s">
-        <v>7</v>
-      </c>
-      <c r="AF4" s="62"/>
-      <c r="AG4" s="73"/>
-      <c r="AH4" s="73"/>
-      <c r="AI4" s="73"/>
-      <c r="AJ4" s="73"/>
-      <c r="AK4" s="73"/>
-      <c r="AL4" s="74" t="s">
-        <v>8</v>
-      </c>
-      <c r="AM4" s="74"/>
-      <c r="AN4" s="74"/>
-      <c r="AO4" s="74"/>
-      <c r="AP4" s="74"/>
-      <c r="AQ4" s="74"/>
-      <c r="AR4" s="74"/>
-      <c r="AS4" s="74"/>
-      <c r="AT4" s="74"/>
-      <c r="AU4" s="74"/>
-      <c r="AV4" s="74"/>
-      <c r="AW4" s="74"/>
-      <c r="AX4" s="74"/>
-      <c r="AY4" s="74"/>
-      <c r="AZ4" s="74"/>
-      <c r="BA4" s="74"/>
-      <c r="BB4" s="74"/>
-      <c r="BC4" s="74"/>
-      <c r="BD4" s="74"/>
-      <c r="BE4" s="74"/>
-      <c r="BF4" s="74"/>
-      <c r="BG4" s="74"/>
-      <c r="BH4" s="74"/>
-      <c r="BI4" s="74"/>
-      <c r="BJ4" s="74"/>
-      <c r="BK4" s="74"/>
-      <c r="BL4" s="74"/>
-      <c r="BM4" s="74"/>
-      <c r="BN4" s="74"/>
-      <c r="BO4" s="74"/>
-      <c r="BP4" s="74"/>
-      <c r="BQ4" s="72" t="s">
-        <v>9</v>
-      </c>
-      <c r="BR4" s="72"/>
-      <c r="BS4" s="72"/>
-      <c r="BT4" s="72"/>
-      <c r="BU4" s="72"/>
-      <c r="BV4" s="72"/>
-      <c r="BW4" s="72"/>
-      <c r="BX4" s="72"/>
-      <c r="BY4" s="72"/>
-      <c r="BZ4" s="72"/>
-      <c r="CA4" s="88" t="s">
-        <v>10</v>
-      </c>
-      <c r="CB4" s="88"/>
-      <c r="CC4" s="88"/>
-      <c r="CD4" s="88"/>
-      <c r="CE4" s="88"/>
-      <c r="CF4" s="88"/>
-      <c r="CG4" s="88"/>
-      <c r="CH4" s="88"/>
-      <c r="CI4" s="88"/>
-      <c r="CJ4" s="88"/>
-      <c r="CK4" s="89" t="s">
+      <c r="CV4" s="58"/>
+      <c r="CW4" s="58"/>
+      <c r="CX4" s="58"/>
+      <c r="CY4" s="58"/>
+      <c r="CZ4" s="58"/>
+      <c r="DA4" s="58"/>
+      <c r="DB4" s="58"/>
+      <c r="DC4" s="58"/>
+      <c r="DD4" s="58"/>
+      <c r="DE4" s="62" t="s">
         <v>322</v>
       </c>
-      <c r="CL4" s="89"/>
-      <c r="CM4" s="89"/>
-      <c r="CN4" s="89"/>
-      <c r="CO4" s="89"/>
-      <c r="CP4" s="89"/>
-      <c r="CQ4" s="89"/>
-      <c r="CR4" s="89"/>
-      <c r="CS4" s="89"/>
-      <c r="CT4" s="89"/>
-      <c r="CU4" s="88" t="s">
+      <c r="DF4" s="62"/>
+      <c r="DG4" s="62"/>
+      <c r="DH4" s="62"/>
+      <c r="DI4" s="62"/>
+      <c r="DJ4" s="62"/>
+      <c r="DK4" s="62"/>
+      <c r="DL4" s="62"/>
+      <c r="DM4" s="62"/>
+      <c r="DN4" s="62"/>
+      <c r="DO4" s="58" t="s">
         <v>323</v>
       </c>
-      <c r="CV4" s="88"/>
-      <c r="CW4" s="88"/>
-      <c r="CX4" s="88"/>
-      <c r="CY4" s="88"/>
-      <c r="CZ4" s="88"/>
-      <c r="DA4" s="88"/>
-      <c r="DB4" s="88"/>
-      <c r="DC4" s="88"/>
-      <c r="DD4" s="88"/>
-      <c r="DE4" s="89" t="s">
-        <v>324</v>
-      </c>
-      <c r="DF4" s="89"/>
-      <c r="DG4" s="89"/>
-      <c r="DH4" s="89"/>
-      <c r="DI4" s="89"/>
-      <c r="DJ4" s="89"/>
-      <c r="DK4" s="89"/>
-      <c r="DL4" s="89"/>
-      <c r="DM4" s="89"/>
-      <c r="DN4" s="89"/>
-      <c r="DO4" s="88" t="s">
-        <v>325</v>
-      </c>
-      <c r="DP4" s="88"/>
-      <c r="DQ4" s="88"/>
-      <c r="DR4" s="88"/>
-      <c r="DS4" s="88"/>
-      <c r="DT4" s="88"/>
-      <c r="DU4" s="88"/>
-      <c r="DV4" s="88"/>
-      <c r="DW4" s="88"/>
-      <c r="DX4" s="88"/>
-      <c r="DY4" s="90" t="s">
-        <v>366</v>
-      </c>
-      <c r="DZ4" s="91"/>
-      <c r="EA4" s="91"/>
-      <c r="EB4" s="91"/>
-      <c r="EC4" s="91"/>
-      <c r="ED4" s="91"/>
-      <c r="EE4" s="91"/>
-      <c r="EF4" s="91"/>
-      <c r="EG4" s="91"/>
-      <c r="EH4" s="92"/>
-      <c r="EI4" s="88" t="s">
-        <v>377</v>
-      </c>
-      <c r="EJ4" s="88"/>
-      <c r="EK4" s="88"/>
-      <c r="EL4" s="88"/>
-      <c r="EM4" s="88"/>
-      <c r="EN4" s="88"/>
-      <c r="EO4" s="88"/>
-      <c r="EP4" s="88"/>
-      <c r="EQ4" s="88"/>
-      <c r="ER4" s="88"/>
-      <c r="ES4" s="90" t="s">
-        <v>388</v>
-      </c>
-      <c r="ET4" s="91"/>
-      <c r="EU4" s="91"/>
-      <c r="EV4" s="91"/>
-      <c r="EW4" s="91"/>
-      <c r="EX4" s="91"/>
-      <c r="EY4" s="91"/>
-      <c r="EZ4" s="91"/>
-      <c r="FA4" s="91"/>
-      <c r="FB4" s="92"/>
-      <c r="FC4" s="75" t="s">
+      <c r="DP4" s="58"/>
+      <c r="DQ4" s="58"/>
+      <c r="DR4" s="58"/>
+      <c r="DS4" s="58"/>
+      <c r="DT4" s="58"/>
+      <c r="DU4" s="58"/>
+      <c r="DV4" s="58"/>
+      <c r="DW4" s="58"/>
+      <c r="DX4" s="58"/>
+      <c r="DY4" s="59" t="s">
+        <v>364</v>
+      </c>
+      <c r="DZ4" s="60"/>
+      <c r="EA4" s="60"/>
+      <c r="EB4" s="60"/>
+      <c r="EC4" s="60"/>
+      <c r="ED4" s="60"/>
+      <c r="EE4" s="60"/>
+      <c r="EF4" s="60"/>
+      <c r="EG4" s="60"/>
+      <c r="EH4" s="61"/>
+      <c r="EI4" s="58" t="s">
+        <v>375</v>
+      </c>
+      <c r="EJ4" s="58"/>
+      <c r="EK4" s="58"/>
+      <c r="EL4" s="58"/>
+      <c r="EM4" s="58"/>
+      <c r="EN4" s="58"/>
+      <c r="EO4" s="58"/>
+      <c r="EP4" s="58"/>
+      <c r="EQ4" s="58"/>
+      <c r="ER4" s="58"/>
+      <c r="ES4" s="59" t="s">
+        <v>386</v>
+      </c>
+      <c r="ET4" s="60"/>
+      <c r="EU4" s="60"/>
+      <c r="EV4" s="60"/>
+      <c r="EW4" s="60"/>
+      <c r="EX4" s="60"/>
+      <c r="EY4" s="60"/>
+      <c r="EZ4" s="60"/>
+      <c r="FA4" s="60"/>
+      <c r="FB4" s="61"/>
+      <c r="FC4" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="FD4" s="75"/>
-      <c r="FE4" s="75"/>
-      <c r="FF4" s="75"/>
-      <c r="FG4" s="75"/>
-      <c r="FH4" s="75"/>
-      <c r="FI4" s="75"/>
-      <c r="FJ4" s="75"/>
-      <c r="FK4" s="75"/>
-      <c r="FL4" s="75"/>
-      <c r="FM4" s="76" t="s">
+      <c r="FD4" s="76"/>
+      <c r="FE4" s="76"/>
+      <c r="FF4" s="76"/>
+      <c r="FG4" s="76"/>
+      <c r="FH4" s="76"/>
+      <c r="FI4" s="76"/>
+      <c r="FJ4" s="76"/>
+      <c r="FK4" s="76"/>
+      <c r="FL4" s="76"/>
+      <c r="FM4" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="FN4" s="76"/>
-      <c r="FO4" s="76"/>
-      <c r="FP4" s="76"/>
-      <c r="FQ4" s="76"/>
-      <c r="FR4" s="76"/>
-      <c r="FS4" s="76"/>
-      <c r="FT4" s="76"/>
-      <c r="FU4" s="76"/>
-      <c r="FV4" s="76"/>
-      <c r="FW4" s="77" t="s">
+      <c r="FN4" s="77"/>
+      <c r="FO4" s="77"/>
+      <c r="FP4" s="77"/>
+      <c r="FQ4" s="77"/>
+      <c r="FR4" s="77"/>
+      <c r="FS4" s="77"/>
+      <c r="FT4" s="77"/>
+      <c r="FU4" s="77"/>
+      <c r="FV4" s="77"/>
+      <c r="FW4" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="FX4" s="77"/>
-      <c r="FY4" s="77"/>
-      <c r="FZ4" s="77"/>
-      <c r="GA4" s="77"/>
-      <c r="GB4" s="77"/>
-      <c r="GC4" s="77"/>
-      <c r="GD4" s="77"/>
-      <c r="GE4" s="77"/>
-      <c r="GF4" s="77"/>
-      <c r="GG4" s="78" t="s">
+      <c r="FX4" s="78"/>
+      <c r="FY4" s="78"/>
+      <c r="FZ4" s="78"/>
+      <c r="GA4" s="78"/>
+      <c r="GB4" s="78"/>
+      <c r="GC4" s="78"/>
+      <c r="GD4" s="78"/>
+      <c r="GE4" s="78"/>
+      <c r="GF4" s="78"/>
+      <c r="GG4" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="GH4" s="78"/>
-      <c r="GI4" s="78"/>
-      <c r="GJ4" s="78"/>
-      <c r="GK4" s="78"/>
-      <c r="GL4" s="78"/>
-      <c r="GM4" s="78"/>
-      <c r="GN4" s="78"/>
-      <c r="GO4" s="78"/>
-      <c r="GP4" s="78"/>
-      <c r="GQ4" s="79" t="s">
+      <c r="GH4" s="79"/>
+      <c r="GI4" s="79"/>
+      <c r="GJ4" s="79"/>
+      <c r="GK4" s="79"/>
+      <c r="GL4" s="79"/>
+      <c r="GM4" s="79"/>
+      <c r="GN4" s="79"/>
+      <c r="GO4" s="79"/>
+      <c r="GP4" s="79"/>
+      <c r="GQ4" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="GR4" s="79"/>
-      <c r="GS4" s="79"/>
-      <c r="GT4" s="79"/>
-      <c r="GU4" s="79"/>
-      <c r="GV4" s="79"/>
-      <c r="GW4" s="79"/>
-      <c r="GX4" s="79"/>
-      <c r="GY4" s="79"/>
-      <c r="GZ4" s="79"/>
-      <c r="HA4" s="80" t="s">
-        <v>416</v>
-      </c>
-      <c r="HB4" s="80"/>
-      <c r="HC4" s="80"/>
-      <c r="HD4" s="80"/>
-      <c r="HE4" s="80"/>
-      <c r="HF4" s="80"/>
-      <c r="HG4" s="80"/>
-      <c r="HH4" s="80"/>
-      <c r="HI4" s="80"/>
-      <c r="HJ4" s="80"/>
-      <c r="HK4" s="72" t="s">
-        <v>166</v>
-      </c>
-      <c r="HL4" s="72"/>
-      <c r="HM4" s="72"/>
-      <c r="HN4" s="72"/>
-      <c r="HO4" s="72"/>
-      <c r="HP4" s="72"/>
-      <c r="HQ4" s="72"/>
-      <c r="HR4" s="72"/>
-      <c r="HS4" s="72"/>
-      <c r="HT4" s="72"/>
-      <c r="HU4" s="72" t="s">
-        <v>177</v>
-      </c>
-      <c r="HV4" s="72"/>
-      <c r="HW4" s="72"/>
-      <c r="HX4" s="72"/>
-      <c r="HY4" s="72"/>
-      <c r="HZ4" s="72"/>
-      <c r="IA4" s="72"/>
-      <c r="IB4" s="72"/>
-      <c r="IC4" s="72"/>
-      <c r="ID4" s="72"/>
-      <c r="IE4" s="72" t="s">
-        <v>188</v>
-      </c>
-      <c r="IF4" s="72"/>
-      <c r="IG4" s="72"/>
-      <c r="IH4" s="72"/>
-      <c r="II4" s="72"/>
-      <c r="IJ4" s="72"/>
-      <c r="IK4" s="72"/>
-      <c r="IL4" s="72"/>
-      <c r="IM4" s="72"/>
-      <c r="IN4" s="72"/>
-      <c r="IO4" s="72" t="s">
-        <v>199</v>
-      </c>
-      <c r="IP4" s="72"/>
-      <c r="IQ4" s="72"/>
-      <c r="IR4" s="72"/>
-      <c r="IS4" s="72"/>
-      <c r="IT4" s="72"/>
-      <c r="IU4" s="72"/>
-      <c r="IV4" s="72"/>
-      <c r="IW4" s="72"/>
-      <c r="IX4" s="72"/>
-      <c r="IY4" s="83" t="s">
-        <v>210</v>
-      </c>
-      <c r="IZ4" s="84"/>
-      <c r="JA4" s="84"/>
-      <c r="JB4" s="84"/>
-      <c r="JC4" s="84"/>
-      <c r="JD4" s="84"/>
-      <c r="JE4" s="84"/>
-      <c r="JF4" s="84"/>
-      <c r="JG4" s="84"/>
-      <c r="JH4" s="85"/>
-      <c r="JI4" s="83" t="s">
-        <v>221</v>
-      </c>
-      <c r="JJ4" s="84"/>
-      <c r="JK4" s="84"/>
-      <c r="JL4" s="84"/>
-      <c r="JM4" s="84"/>
-      <c r="JN4" s="84"/>
-      <c r="JO4" s="84"/>
-      <c r="JP4" s="84"/>
-      <c r="JQ4" s="84"/>
-      <c r="JR4" s="85"/>
-      <c r="JS4" s="83" t="s">
-        <v>232</v>
-      </c>
-      <c r="JT4" s="84"/>
-      <c r="JU4" s="84"/>
-      <c r="JV4" s="84"/>
-      <c r="JW4" s="84"/>
-      <c r="JX4" s="84"/>
-      <c r="JY4" s="84"/>
-      <c r="JZ4" s="84"/>
-      <c r="KA4" s="84"/>
-      <c r="KB4" s="85"/>
-      <c r="KC4" s="83" t="s">
-        <v>232</v>
-      </c>
-      <c r="KD4" s="84"/>
-      <c r="KE4" s="84"/>
-      <c r="KF4" s="84"/>
-      <c r="KG4" s="84"/>
-      <c r="KH4" s="84"/>
-      <c r="KI4" s="84"/>
-      <c r="KJ4" s="84"/>
-      <c r="KK4" s="84"/>
-      <c r="KL4" s="85"/>
-      <c r="KM4" s="83" t="s">
-        <v>253</v>
-      </c>
-      <c r="KN4" s="84"/>
-      <c r="KO4" s="84"/>
-      <c r="KP4" s="84"/>
-      <c r="KQ4" s="84"/>
-      <c r="KR4" s="84"/>
-      <c r="KS4" s="84"/>
-      <c r="KT4" s="84"/>
-      <c r="KU4" s="84"/>
-      <c r="KV4" s="85"/>
-      <c r="KW4" s="86" t="s">
-        <v>264</v>
-      </c>
-      <c r="KX4" s="86"/>
-      <c r="KY4" s="86"/>
-      <c r="KZ4" s="86"/>
-      <c r="LA4" s="86"/>
-      <c r="LB4" s="86"/>
-      <c r="LC4" s="86"/>
-      <c r="LD4" s="86"/>
-      <c r="LE4" s="86"/>
-      <c r="LF4" s="86"/>
-      <c r="LG4" s="86" t="s">
-        <v>275</v>
-      </c>
-      <c r="LH4" s="86"/>
-      <c r="LI4" s="86"/>
-      <c r="LJ4" s="86"/>
-      <c r="LK4" s="86"/>
-      <c r="LL4" s="86"/>
-      <c r="LM4" s="86"/>
-      <c r="LN4" s="86"/>
-      <c r="LO4" s="86"/>
-      <c r="LP4" s="86"/>
-      <c r="LQ4" s="86" t="s">
-        <v>281</v>
-      </c>
-      <c r="LR4" s="86"/>
-      <c r="LS4" s="86"/>
-      <c r="LT4" s="86"/>
-      <c r="LU4" s="86"/>
-      <c r="LV4" s="86"/>
-      <c r="LW4" s="86"/>
-      <c r="LX4" s="86"/>
-      <c r="LY4" s="86"/>
-      <c r="LZ4" s="86"/>
-      <c r="MA4" s="86" t="s">
-        <v>292</v>
-      </c>
-      <c r="MB4" s="86"/>
-      <c r="MC4" s="86"/>
-      <c r="MD4" s="86"/>
-      <c r="ME4" s="86"/>
-      <c r="MF4" s="86"/>
-      <c r="MG4" s="86"/>
-      <c r="MH4" s="86"/>
-      <c r="MI4" s="86"/>
-      <c r="MJ4" s="86"/>
-      <c r="MK4" s="87" t="s">
+      <c r="GR4" s="80"/>
+      <c r="GS4" s="80"/>
+      <c r="GT4" s="80"/>
+      <c r="GU4" s="80"/>
+      <c r="GV4" s="80"/>
+      <c r="GW4" s="80"/>
+      <c r="GX4" s="80"/>
+      <c r="GY4" s="80"/>
+      <c r="GZ4" s="80"/>
+      <c r="HA4" s="63" t="s">
+        <v>414</v>
+      </c>
+      <c r="HB4" s="63"/>
+      <c r="HC4" s="63"/>
+      <c r="HD4" s="63"/>
+      <c r="HE4" s="63"/>
+      <c r="HF4" s="63"/>
+      <c r="HG4" s="63"/>
+      <c r="HH4" s="63"/>
+      <c r="HI4" s="63"/>
+      <c r="HJ4" s="63"/>
+      <c r="HK4" s="70" t="s">
+        <v>164</v>
+      </c>
+      <c r="HL4" s="70"/>
+      <c r="HM4" s="70"/>
+      <c r="HN4" s="70"/>
+      <c r="HO4" s="70"/>
+      <c r="HP4" s="70"/>
+      <c r="HQ4" s="70"/>
+      <c r="HR4" s="70"/>
+      <c r="HS4" s="70"/>
+      <c r="HT4" s="70"/>
+      <c r="HU4" s="70" t="s">
+        <v>175</v>
+      </c>
+      <c r="HV4" s="70"/>
+      <c r="HW4" s="70"/>
+      <c r="HX4" s="70"/>
+      <c r="HY4" s="70"/>
+      <c r="HZ4" s="70"/>
+      <c r="IA4" s="70"/>
+      <c r="IB4" s="70"/>
+      <c r="IC4" s="70"/>
+      <c r="ID4" s="70"/>
+      <c r="IE4" s="70" t="s">
+        <v>186</v>
+      </c>
+      <c r="IF4" s="70"/>
+      <c r="IG4" s="70"/>
+      <c r="IH4" s="70"/>
+      <c r="II4" s="70"/>
+      <c r="IJ4" s="70"/>
+      <c r="IK4" s="70"/>
+      <c r="IL4" s="70"/>
+      <c r="IM4" s="70"/>
+      <c r="IN4" s="70"/>
+      <c r="IO4" s="70" t="s">
+        <v>197</v>
+      </c>
+      <c r="IP4" s="70"/>
+      <c r="IQ4" s="70"/>
+      <c r="IR4" s="70"/>
+      <c r="IS4" s="70"/>
+      <c r="IT4" s="70"/>
+      <c r="IU4" s="70"/>
+      <c r="IV4" s="70"/>
+      <c r="IW4" s="70"/>
+      <c r="IX4" s="70"/>
+      <c r="IY4" s="71" t="s">
+        <v>208</v>
+      </c>
+      <c r="IZ4" s="72"/>
+      <c r="JA4" s="72"/>
+      <c r="JB4" s="72"/>
+      <c r="JC4" s="72"/>
+      <c r="JD4" s="72"/>
+      <c r="JE4" s="72"/>
+      <c r="JF4" s="72"/>
+      <c r="JG4" s="72"/>
+      <c r="JH4" s="73"/>
+      <c r="JI4" s="71" t="s">
+        <v>219</v>
+      </c>
+      <c r="JJ4" s="72"/>
+      <c r="JK4" s="72"/>
+      <c r="JL4" s="72"/>
+      <c r="JM4" s="72"/>
+      <c r="JN4" s="72"/>
+      <c r="JO4" s="72"/>
+      <c r="JP4" s="72"/>
+      <c r="JQ4" s="72"/>
+      <c r="JR4" s="73"/>
+      <c r="JS4" s="71" t="s">
+        <v>230</v>
+      </c>
+      <c r="JT4" s="72"/>
+      <c r="JU4" s="72"/>
+      <c r="JV4" s="72"/>
+      <c r="JW4" s="72"/>
+      <c r="JX4" s="72"/>
+      <c r="JY4" s="72"/>
+      <c r="JZ4" s="72"/>
+      <c r="KA4" s="72"/>
+      <c r="KB4" s="73"/>
+      <c r="KC4" s="71" t="s">
+        <v>230</v>
+      </c>
+      <c r="KD4" s="72"/>
+      <c r="KE4" s="72"/>
+      <c r="KF4" s="72"/>
+      <c r="KG4" s="72"/>
+      <c r="KH4" s="72"/>
+      <c r="KI4" s="72"/>
+      <c r="KJ4" s="72"/>
+      <c r="KK4" s="72"/>
+      <c r="KL4" s="73"/>
+      <c r="KM4" s="71" t="s">
+        <v>251</v>
+      </c>
+      <c r="KN4" s="72"/>
+      <c r="KO4" s="72"/>
+      <c r="KP4" s="72"/>
+      <c r="KQ4" s="72"/>
+      <c r="KR4" s="72"/>
+      <c r="KS4" s="72"/>
+      <c r="KT4" s="72"/>
+      <c r="KU4" s="72"/>
+      <c r="KV4" s="73"/>
+      <c r="KW4" s="74" t="s">
+        <v>262</v>
+      </c>
+      <c r="KX4" s="74"/>
+      <c r="KY4" s="74"/>
+      <c r="KZ4" s="74"/>
+      <c r="LA4" s="74"/>
+      <c r="LB4" s="74"/>
+      <c r="LC4" s="74"/>
+      <c r="LD4" s="74"/>
+      <c r="LE4" s="74"/>
+      <c r="LF4" s="74"/>
+      <c r="LG4" s="74" t="s">
+        <v>273</v>
+      </c>
+      <c r="LH4" s="74"/>
+      <c r="LI4" s="74"/>
+      <c r="LJ4" s="74"/>
+      <c r="LK4" s="74"/>
+      <c r="LL4" s="74"/>
+      <c r="LM4" s="74"/>
+      <c r="LN4" s="74"/>
+      <c r="LO4" s="74"/>
+      <c r="LP4" s="74"/>
+      <c r="LQ4" s="74" t="s">
+        <v>279</v>
+      </c>
+      <c r="LR4" s="74"/>
+      <c r="LS4" s="74"/>
+      <c r="LT4" s="74"/>
+      <c r="LU4" s="74"/>
+      <c r="LV4" s="74"/>
+      <c r="LW4" s="74"/>
+      <c r="LX4" s="74"/>
+      <c r="LY4" s="74"/>
+      <c r="LZ4" s="74"/>
+      <c r="MA4" s="74" t="s">
+        <v>290</v>
+      </c>
+      <c r="MB4" s="74"/>
+      <c r="MC4" s="74"/>
+      <c r="MD4" s="74"/>
+      <c r="ME4" s="74"/>
+      <c r="MF4" s="74"/>
+      <c r="MG4" s="74"/>
+      <c r="MH4" s="74"/>
+      <c r="MI4" s="74"/>
+      <c r="MJ4" s="74"/>
+      <c r="MK4" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="ML4" s="87"/>
-      <c r="MM4" s="87"/>
-      <c r="MN4" s="87"/>
-      <c r="MO4" s="87"/>
-      <c r="MP4" s="87"/>
-      <c r="MQ4" s="87"/>
-      <c r="MR4" s="87"/>
-      <c r="MS4" s="87"/>
-      <c r="MT4" s="87"/>
-      <c r="MU4" s="87"/>
-      <c r="MV4" s="87"/>
-      <c r="MW4" s="87"/>
-      <c r="MX4" s="58" t="s">
-        <v>110</v>
-      </c>
-      <c r="MY4" s="81"/>
-      <c r="MZ4" s="59"/>
+      <c r="ML4" s="75"/>
+      <c r="MM4" s="75"/>
+      <c r="MN4" s="75"/>
+      <c r="MO4" s="75"/>
+      <c r="MP4" s="75"/>
+      <c r="MQ4" s="75"/>
+      <c r="MR4" s="75"/>
+      <c r="MS4" s="75"/>
+      <c r="MT4" s="75"/>
+      <c r="MU4" s="75"/>
+      <c r="MV4" s="75"/>
+      <c r="MW4" s="75"/>
+      <c r="MX4" s="64" t="s">
+        <v>108</v>
+      </c>
+      <c r="MY4" s="65"/>
+      <c r="MZ4" s="66"/>
       <c r="NA4" s="38"/>
-      <c r="NB4" s="58" t="s">
-        <v>114</v>
-      </c>
-      <c r="NC4" s="59"/>
+      <c r="NB4" s="64" t="s">
+        <v>112</v>
+      </c>
+      <c r="NC4" s="66"/>
       <c r="ND4" s="56"/>
       <c r="NE4" s="54"/>
     </row>
     <row r="5" spans="1:369" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="65"/>
-      <c r="B5" s="65"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="67"/>
-      <c r="J5" s="67"/>
-      <c r="K5" s="67"/>
-      <c r="L5" s="67"/>
-      <c r="M5" s="68"/>
-      <c r="N5" s="68"/>
-      <c r="O5" s="68"/>
-      <c r="P5" s="69"/>
-      <c r="Q5" s="69"/>
-      <c r="R5" s="69"/>
-      <c r="S5" s="69"/>
-      <c r="T5" s="69"/>
-      <c r="U5" s="70"/>
-      <c r="V5" s="70"/>
-      <c r="W5" s="70"/>
-      <c r="X5" s="70"/>
-      <c r="Y5" s="70"/>
-      <c r="Z5" s="70"/>
-      <c r="AA5" s="70"/>
-      <c r="AB5" s="71"/>
-      <c r="AC5" s="71"/>
-      <c r="AD5" s="71"/>
-      <c r="AE5" s="62"/>
-      <c r="AF5" s="62"/>
-      <c r="AG5" s="73"/>
-      <c r="AH5" s="73"/>
-      <c r="AI5" s="73"/>
-      <c r="AJ5" s="73"/>
-      <c r="AK5" s="73"/>
-      <c r="AL5" s="74"/>
-      <c r="AM5" s="74"/>
-      <c r="AN5" s="74"/>
-      <c r="AO5" s="74"/>
-      <c r="AP5" s="74"/>
-      <c r="AQ5" s="74"/>
-      <c r="AR5" s="74"/>
-      <c r="AS5" s="74"/>
-      <c r="AT5" s="74"/>
-      <c r="AU5" s="74"/>
-      <c r="AV5" s="74"/>
-      <c r="AW5" s="74"/>
-      <c r="AX5" s="74"/>
-      <c r="AY5" s="74"/>
-      <c r="AZ5" s="74"/>
-      <c r="BA5" s="74"/>
-      <c r="BB5" s="74"/>
-      <c r="BC5" s="74"/>
-      <c r="BD5" s="74"/>
-      <c r="BE5" s="74"/>
-      <c r="BF5" s="74"/>
-      <c r="BG5" s="74"/>
-      <c r="BH5" s="74"/>
-      <c r="BI5" s="74"/>
-      <c r="BJ5" s="74"/>
-      <c r="BK5" s="74"/>
-      <c r="BL5" s="74"/>
-      <c r="BM5" s="74"/>
-      <c r="BN5" s="74"/>
-      <c r="BO5" s="74"/>
-      <c r="BP5" s="74"/>
+      <c r="A5" s="84"/>
+      <c r="B5" s="84"/>
+      <c r="C5" s="85"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="85"/>
+      <c r="H5" s="85"/>
+      <c r="I5" s="86"/>
+      <c r="J5" s="86"/>
+      <c r="K5" s="86"/>
+      <c r="L5" s="86"/>
+      <c r="M5" s="87"/>
+      <c r="N5" s="87"/>
+      <c r="O5" s="87"/>
+      <c r="P5" s="88"/>
+      <c r="Q5" s="88"/>
+      <c r="R5" s="88"/>
+      <c r="S5" s="88"/>
+      <c r="T5" s="88"/>
+      <c r="U5" s="89"/>
+      <c r="V5" s="89"/>
+      <c r="W5" s="89"/>
+      <c r="X5" s="89"/>
+      <c r="Y5" s="89"/>
+      <c r="Z5" s="89"/>
+      <c r="AA5" s="89"/>
+      <c r="AB5" s="90"/>
+      <c r="AC5" s="90"/>
+      <c r="AD5" s="90"/>
+      <c r="AE5" s="81"/>
+      <c r="AF5" s="81"/>
+      <c r="AG5" s="91"/>
+      <c r="AH5" s="91"/>
+      <c r="AI5" s="91"/>
+      <c r="AJ5" s="91"/>
+      <c r="AK5" s="91"/>
+      <c r="AL5" s="92"/>
+      <c r="AM5" s="92"/>
+      <c r="AN5" s="92"/>
+      <c r="AO5" s="92"/>
+      <c r="AP5" s="92"/>
+      <c r="AQ5" s="92"/>
+      <c r="AR5" s="92"/>
+      <c r="AS5" s="92"/>
+      <c r="AT5" s="92"/>
+      <c r="AU5" s="92"/>
+      <c r="AV5" s="92"/>
+      <c r="AW5" s="92"/>
+      <c r="AX5" s="92"/>
+      <c r="AY5" s="92"/>
+      <c r="AZ5" s="92"/>
+      <c r="BA5" s="92"/>
+      <c r="BB5" s="92"/>
+      <c r="BC5" s="92"/>
+      <c r="BD5" s="92"/>
+      <c r="BE5" s="92"/>
+      <c r="BF5" s="92"/>
+      <c r="BG5" s="92"/>
+      <c r="BH5" s="92"/>
+      <c r="BI5" s="92"/>
+      <c r="BJ5" s="92"/>
+      <c r="BK5" s="92"/>
+      <c r="BL5" s="92"/>
+      <c r="BM5" s="92"/>
+      <c r="BN5" s="92"/>
+      <c r="BO5" s="92"/>
+      <c r="BP5" s="92"/>
       <c r="BQ5" s="7" t="s">
         <v>19</v>
       </c>
@@ -4804,25 +4804,25 @@
       <c r="MJ5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="MK5" s="87"/>
-      <c r="ML5" s="87"/>
-      <c r="MM5" s="87"/>
-      <c r="MN5" s="87"/>
-      <c r="MO5" s="87"/>
-      <c r="MP5" s="87"/>
-      <c r="MQ5" s="87"/>
-      <c r="MR5" s="87"/>
-      <c r="MS5" s="87"/>
-      <c r="MT5" s="87"/>
-      <c r="MU5" s="87"/>
-      <c r="MV5" s="87"/>
-      <c r="MW5" s="87"/>
-      <c r="MX5" s="60"/>
-      <c r="MY5" s="82"/>
-      <c r="MZ5" s="61"/>
+      <c r="MK5" s="75"/>
+      <c r="ML5" s="75"/>
+      <c r="MM5" s="75"/>
+      <c r="MN5" s="75"/>
+      <c r="MO5" s="75"/>
+      <c r="MP5" s="75"/>
+      <c r="MQ5" s="75"/>
+      <c r="MR5" s="75"/>
+      <c r="MS5" s="75"/>
+      <c r="MT5" s="75"/>
+      <c r="MU5" s="75"/>
+      <c r="MV5" s="75"/>
+      <c r="MW5" s="75"/>
+      <c r="MX5" s="67"/>
+      <c r="MY5" s="68"/>
+      <c r="MZ5" s="69"/>
       <c r="NA5" s="38"/>
-      <c r="NB5" s="60"/>
-      <c r="NC5" s="61"/>
+      <c r="NB5" s="67"/>
+      <c r="NC5" s="69"/>
       <c r="ND5" s="57"/>
       <c r="NE5" s="55"/>
     </row>
@@ -4918,7 +4918,7 @@
         <v>52</v>
       </c>
       <c r="AE6" s="9" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="AF6" s="16" t="s">
         <v>53</v>
@@ -4927,7 +4927,7 @@
         <v>54</v>
       </c>
       <c r="AH6" s="17" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="AI6" s="17" t="s">
         <v>55</v>
@@ -4945,1001 +4945,1001 @@
         <v>59</v>
       </c>
       <c r="AN6" s="18" t="s">
+        <v>397</v>
+      </c>
+      <c r="AO6" s="18" t="s">
+        <v>398</v>
+      </c>
+      <c r="AP6" s="18" t="s">
         <v>399</v>
       </c>
-      <c r="AO6" s="18" t="s">
+      <c r="AQ6" s="18" t="s">
         <v>400</v>
       </c>
-      <c r="AP6" s="18" t="s">
+      <c r="AR6" s="18" t="s">
         <v>401</v>
       </c>
-      <c r="AQ6" s="18" t="s">
+      <c r="AS6" s="18" t="s">
         <v>402</v>
       </c>
-      <c r="AR6" s="18" t="s">
+      <c r="AT6" s="18" t="s">
         <v>403</v>
-      </c>
-      <c r="AS6" s="18" t="s">
-        <v>404</v>
-      </c>
-      <c r="AT6" s="18" t="s">
-        <v>405</v>
       </c>
       <c r="AU6" s="18" t="s">
         <v>60</v>
       </c>
       <c r="AV6" s="18" t="s">
+        <v>415</v>
+      </c>
+      <c r="AW6" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="AW6" s="18" t="s">
+      <c r="AX6" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="AX6" s="18" t="s">
+      <c r="AY6" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="AY6" s="18" t="s">
+      <c r="AZ6" s="18" t="s">
+        <v>416</v>
+      </c>
+      <c r="BA6" s="18" t="s">
+        <v>306</v>
+      </c>
+      <c r="BB6" s="18" t="s">
+        <v>307</v>
+      </c>
+      <c r="BC6" s="18" t="s">
+        <v>308</v>
+      </c>
+      <c r="BD6" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="BE6" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="BF6" s="18" t="s">
+        <v>311</v>
+      </c>
+      <c r="BG6" s="18" t="s">
+        <v>312</v>
+      </c>
+      <c r="BH6" s="18" t="s">
+        <v>313</v>
+      </c>
+      <c r="BI6" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="BJ6" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="BK6" s="18" t="s">
+        <v>316</v>
+      </c>
+      <c r="BL6" s="18" t="s">
+        <v>317</v>
+      </c>
+      <c r="BM6" s="18" t="s">
+        <v>318</v>
+      </c>
+      <c r="BN6" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="AZ6" s="18" t="s">
+      <c r="BO6" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="BA6" s="18" t="s">
-        <v>308</v>
-      </c>
-      <c r="BB6" s="18" t="s">
-        <v>309</v>
-      </c>
-      <c r="BC6" s="18" t="s">
-        <v>310</v>
-      </c>
-      <c r="BD6" s="18" t="s">
-        <v>311</v>
-      </c>
-      <c r="BE6" s="18" t="s">
-        <v>312</v>
-      </c>
-      <c r="BF6" s="18" t="s">
-        <v>313</v>
-      </c>
-      <c r="BG6" s="18" t="s">
-        <v>314</v>
-      </c>
-      <c r="BH6" s="18" t="s">
-        <v>315</v>
-      </c>
-      <c r="BI6" s="18" t="s">
-        <v>316</v>
-      </c>
-      <c r="BJ6" s="18" t="s">
-        <v>317</v>
-      </c>
-      <c r="BK6" s="18" t="s">
-        <v>318</v>
-      </c>
-      <c r="BL6" s="18" t="s">
-        <v>319</v>
-      </c>
-      <c r="BM6" s="18" t="s">
-        <v>320</v>
-      </c>
-      <c r="BN6" s="18" t="s">
+      <c r="BP6" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="BO6" s="18" t="s">
+      <c r="BQ6" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="BP6" s="18" t="s">
+      <c r="BR6" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="BQ6" s="18" t="s">
+      <c r="BS6" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="BR6" s="18" t="s">
+      <c r="BT6" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="BS6" s="18" t="s">
+      <c r="BU6" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="BV6" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="BW6" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="BX6" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="BY6" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="BZ6" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="CA6" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="BT6" s="18" t="s">
+      <c r="CB6" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="BU6" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="BV6" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="BW6" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="BX6" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="BY6" s="18" t="s">
+      <c r="CC6" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="CD6" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="CE6" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="BZ6" s="18" t="s">
+      <c r="CF6" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="CA6" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="CB6" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="CC6" s="18" t="s">
+      <c r="CG6" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="CH6" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="CI6" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="CJ6" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="CK6" s="18" t="s">
+        <v>324</v>
+      </c>
+      <c r="CL6" s="18" t="s">
+        <v>325</v>
+      </c>
+      <c r="CM6" s="18" t="s">
+        <v>326</v>
+      </c>
+      <c r="CN6" s="18" t="s">
+        <v>327</v>
+      </c>
+      <c r="CO6" s="18" t="s">
+        <v>328</v>
+      </c>
+      <c r="CP6" s="18" t="s">
+        <v>329</v>
+      </c>
+      <c r="CQ6" s="18" t="s">
+        <v>330</v>
+      </c>
+      <c r="CR6" s="18" t="s">
+        <v>331</v>
+      </c>
+      <c r="CS6" s="18" t="s">
+        <v>332</v>
+      </c>
+      <c r="CT6" s="18" t="s">
+        <v>333</v>
+      </c>
+      <c r="CU6" s="18" t="s">
+        <v>334</v>
+      </c>
+      <c r="CV6" s="18" t="s">
+        <v>335</v>
+      </c>
+      <c r="CW6" s="18" t="s">
+        <v>336</v>
+      </c>
+      <c r="CX6" s="18" t="s">
+        <v>337</v>
+      </c>
+      <c r="CY6" s="18" t="s">
+        <v>338</v>
+      </c>
+      <c r="CZ6" s="18" t="s">
+        <v>339</v>
+      </c>
+      <c r="DA6" s="18" t="s">
+        <v>340</v>
+      </c>
+      <c r="DB6" s="18" t="s">
+        <v>341</v>
+      </c>
+      <c r="DC6" s="18" t="s">
+        <v>342</v>
+      </c>
+      <c r="DD6" s="18" t="s">
+        <v>343</v>
+      </c>
+      <c r="DE6" s="18" t="s">
+        <v>344</v>
+      </c>
+      <c r="DF6" s="18" t="s">
+        <v>345</v>
+      </c>
+      <c r="DG6" s="18" t="s">
+        <v>346</v>
+      </c>
+      <c r="DH6" s="18" t="s">
+        <v>347</v>
+      </c>
+      <c r="DI6" s="18" t="s">
+        <v>348</v>
+      </c>
+      <c r="DJ6" s="18" t="s">
+        <v>349</v>
+      </c>
+      <c r="DK6" s="18" t="s">
+        <v>350</v>
+      </c>
+      <c r="DL6" s="18" t="s">
+        <v>351</v>
+      </c>
+      <c r="DM6" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="DN6" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="DO6" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="DP6" s="18" t="s">
+        <v>355</v>
+      </c>
+      <c r="DQ6" s="18" t="s">
+        <v>356</v>
+      </c>
+      <c r="DR6" s="18" t="s">
+        <v>357</v>
+      </c>
+      <c r="DS6" s="18" t="s">
+        <v>358</v>
+      </c>
+      <c r="DT6" s="18" t="s">
+        <v>359</v>
+      </c>
+      <c r="DU6" s="18" t="s">
+        <v>360</v>
+      </c>
+      <c r="DV6" s="18" t="s">
+        <v>361</v>
+      </c>
+      <c r="DW6" s="18" t="s">
+        <v>362</v>
+      </c>
+      <c r="DX6" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="DY6" s="18" t="s">
+        <v>365</v>
+      </c>
+      <c r="DZ6" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="EA6" s="18" t="s">
+        <v>367</v>
+      </c>
+      <c r="EB6" s="18" t="s">
+        <v>368</v>
+      </c>
+      <c r="EC6" s="18" t="s">
+        <v>369</v>
+      </c>
+      <c r="ED6" s="18" t="s">
+        <v>370</v>
+      </c>
+      <c r="EE6" s="18" t="s">
+        <v>371</v>
+      </c>
+      <c r="EF6" s="18" t="s">
+        <v>372</v>
+      </c>
+      <c r="EG6" s="18" t="s">
+        <v>373</v>
+      </c>
+      <c r="EH6" s="18" t="s">
+        <v>374</v>
+      </c>
+      <c r="EI6" s="18" t="s">
+        <v>376</v>
+      </c>
+      <c r="EJ6" s="18" t="s">
+        <v>377</v>
+      </c>
+      <c r="EK6" s="18" t="s">
+        <v>378</v>
+      </c>
+      <c r="EL6" s="18" t="s">
+        <v>379</v>
+      </c>
+      <c r="EM6" s="18" t="s">
+        <v>380</v>
+      </c>
+      <c r="EN6" s="18" t="s">
+        <v>381</v>
+      </c>
+      <c r="EO6" s="18" t="s">
+        <v>382</v>
+      </c>
+      <c r="EP6" s="18" t="s">
+        <v>383</v>
+      </c>
+      <c r="EQ6" s="18" t="s">
+        <v>384</v>
+      </c>
+      <c r="ER6" s="18" t="s">
+        <v>385</v>
+      </c>
+      <c r="ES6" s="18" t="s">
+        <v>387</v>
+      </c>
+      <c r="ET6" s="18" t="s">
+        <v>388</v>
+      </c>
+      <c r="EU6" s="18" t="s">
+        <v>389</v>
+      </c>
+      <c r="EV6" s="18" t="s">
+        <v>390</v>
+      </c>
+      <c r="EW6" s="18" t="s">
+        <v>391</v>
+      </c>
+      <c r="EX6" s="18" t="s">
+        <v>392</v>
+      </c>
+      <c r="EY6" s="18" t="s">
+        <v>393</v>
+      </c>
+      <c r="EZ6" s="18" t="s">
+        <v>394</v>
+      </c>
+      <c r="FA6" s="18" t="s">
+        <v>395</v>
+      </c>
+      <c r="FB6" s="18" t="s">
+        <v>396</v>
+      </c>
+      <c r="FC6" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="CD6" s="18" t="s">
+      <c r="FD6" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="CE6" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="CF6" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="CG6" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="CH6" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="CI6" s="18" t="s">
+      <c r="FE6" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="FF6" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="FG6" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="CJ6" s="18" t="s">
+      <c r="FH6" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="CK6" s="18" t="s">
-        <v>326</v>
-      </c>
-      <c r="CL6" s="18" t="s">
-        <v>327</v>
-      </c>
-      <c r="CM6" s="18" t="s">
-        <v>328</v>
-      </c>
-      <c r="CN6" s="18" t="s">
-        <v>329</v>
-      </c>
-      <c r="CO6" s="18" t="s">
-        <v>330</v>
-      </c>
-      <c r="CP6" s="18" t="s">
-        <v>331</v>
-      </c>
-      <c r="CQ6" s="18" t="s">
-        <v>332</v>
-      </c>
-      <c r="CR6" s="18" t="s">
-        <v>333</v>
-      </c>
-      <c r="CS6" s="18" t="s">
-        <v>334</v>
-      </c>
-      <c r="CT6" s="18" t="s">
-        <v>335</v>
-      </c>
-      <c r="CU6" s="18" t="s">
-        <v>336</v>
-      </c>
-      <c r="CV6" s="18" t="s">
-        <v>337</v>
-      </c>
-      <c r="CW6" s="18" t="s">
-        <v>338</v>
-      </c>
-      <c r="CX6" s="18" t="s">
-        <v>339</v>
-      </c>
-      <c r="CY6" s="18" t="s">
-        <v>340</v>
-      </c>
-      <c r="CZ6" s="18" t="s">
-        <v>341</v>
-      </c>
-      <c r="DA6" s="18" t="s">
-        <v>342</v>
-      </c>
-      <c r="DB6" s="18" t="s">
-        <v>343</v>
-      </c>
-      <c r="DC6" s="18" t="s">
-        <v>344</v>
-      </c>
-      <c r="DD6" s="18" t="s">
-        <v>345</v>
-      </c>
-      <c r="DE6" s="18" t="s">
-        <v>346</v>
-      </c>
-      <c r="DF6" s="18" t="s">
-        <v>347</v>
-      </c>
-      <c r="DG6" s="18" t="s">
-        <v>348</v>
-      </c>
-      <c r="DH6" s="18" t="s">
-        <v>349</v>
-      </c>
-      <c r="DI6" s="18" t="s">
-        <v>350</v>
-      </c>
-      <c r="DJ6" s="18" t="s">
-        <v>351</v>
-      </c>
-      <c r="DK6" s="18" t="s">
-        <v>352</v>
-      </c>
-      <c r="DL6" s="18" t="s">
-        <v>353</v>
-      </c>
-      <c r="DM6" s="18" t="s">
-        <v>354</v>
-      </c>
-      <c r="DN6" s="18" t="s">
-        <v>355</v>
-      </c>
-      <c r="DO6" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="DP6" s="18" t="s">
-        <v>357</v>
-      </c>
-      <c r="DQ6" s="18" t="s">
-        <v>358</v>
-      </c>
-      <c r="DR6" s="18" t="s">
-        <v>359</v>
-      </c>
-      <c r="DS6" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="DT6" s="18" t="s">
-        <v>361</v>
-      </c>
-      <c r="DU6" s="18" t="s">
-        <v>362</v>
-      </c>
-      <c r="DV6" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="DW6" s="18" t="s">
-        <v>364</v>
-      </c>
-      <c r="DX6" s="18" t="s">
-        <v>365</v>
-      </c>
-      <c r="DY6" s="18" t="s">
-        <v>367</v>
-      </c>
-      <c r="DZ6" s="18" t="s">
-        <v>368</v>
-      </c>
-      <c r="EA6" s="18" t="s">
-        <v>369</v>
-      </c>
-      <c r="EB6" s="18" t="s">
-        <v>370</v>
-      </c>
-      <c r="EC6" s="18" t="s">
-        <v>371</v>
-      </c>
-      <c r="ED6" s="18" t="s">
-        <v>372</v>
-      </c>
-      <c r="EE6" s="18" t="s">
-        <v>373</v>
-      </c>
-      <c r="EF6" s="18" t="s">
-        <v>374</v>
-      </c>
-      <c r="EG6" s="18" t="s">
-        <v>375</v>
-      </c>
-      <c r="EH6" s="18" t="s">
-        <v>376</v>
-      </c>
-      <c r="EI6" s="18" t="s">
-        <v>378</v>
-      </c>
-      <c r="EJ6" s="18" t="s">
-        <v>379</v>
-      </c>
-      <c r="EK6" s="18" t="s">
-        <v>380</v>
-      </c>
-      <c r="EL6" s="18" t="s">
-        <v>381</v>
-      </c>
-      <c r="EM6" s="18" t="s">
-        <v>382</v>
-      </c>
-      <c r="EN6" s="18" t="s">
-        <v>383</v>
-      </c>
-      <c r="EO6" s="18" t="s">
-        <v>384</v>
-      </c>
-      <c r="EP6" s="18" t="s">
-        <v>385</v>
-      </c>
-      <c r="EQ6" s="18" t="s">
-        <v>386</v>
-      </c>
-      <c r="ER6" s="18" t="s">
-        <v>387</v>
-      </c>
-      <c r="ES6" s="18" t="s">
-        <v>389</v>
-      </c>
-      <c r="ET6" s="18" t="s">
-        <v>390</v>
-      </c>
-      <c r="EU6" s="18" t="s">
-        <v>391</v>
-      </c>
-      <c r="EV6" s="18" t="s">
-        <v>392</v>
-      </c>
-      <c r="EW6" s="18" t="s">
-        <v>393</v>
-      </c>
-      <c r="EX6" s="18" t="s">
-        <v>394</v>
-      </c>
-      <c r="EY6" s="18" t="s">
-        <v>395</v>
-      </c>
-      <c r="EZ6" s="18" t="s">
-        <v>396</v>
-      </c>
-      <c r="FA6" s="18" t="s">
-        <v>397</v>
-      </c>
-      <c r="FB6" s="18" t="s">
-        <v>398</v>
-      </c>
-      <c r="FC6" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="FD6" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="FE6" s="18" t="s">
+      <c r="FI6" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="FJ6" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="FK6" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="FL6" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="FM6" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="FF6" s="18" t="s">
+      <c r="FN6" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="FG6" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="FH6" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="FI6" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="FJ6" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="FK6" s="18" t="s">
+      <c r="FO6" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="FP6" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="FQ6" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="FL6" s="18" t="s">
+      <c r="FR6" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="FM6" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="FN6" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="FO6" s="18" t="s">
+      <c r="FS6" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="FT6" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="FU6" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="FV6" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="FW6" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="FP6" s="18" t="s">
+      <c r="FX6" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="FQ6" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="FR6" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="FS6" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="FT6" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="FU6" s="18" t="s">
+      <c r="FY6" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="FZ6" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="GA6" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="FV6" s="18" t="s">
+      <c r="GB6" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="FW6" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="FX6" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="FY6" s="9" t="s">
+      <c r="GC6" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="GD6" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="GE6" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="GF6" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="GG6" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="FZ6" s="9" t="s">
+      <c r="GH6" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="GA6" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="GB6" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="GC6" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="GD6" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="GE6" s="9" t="s">
+      <c r="GI6" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="GJ6" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="GK6" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="GF6" s="9" t="s">
+      <c r="GL6" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="GG6" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="GH6" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="GI6" s="9" t="s">
+      <c r="GM6" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="GN6" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="GO6" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="GP6" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="GQ6" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="GJ6" s="9" t="s">
+      <c r="GR6" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="GK6" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="GL6" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="GM6" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="GN6" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="GO6" s="9" t="s">
+      <c r="GS6" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="GT6" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="GU6" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="GP6" s="9" t="s">
+      <c r="GV6" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="GQ6" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="GR6" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="GS6" s="9" t="s">
+      <c r="GW6" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="GX6" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="GY6" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="GZ6" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="HA6" s="18" t="s">
+        <v>404</v>
+      </c>
+      <c r="HB6" s="18" t="s">
+        <v>405</v>
+      </c>
+      <c r="HC6" s="18" t="s">
+        <v>406</v>
+      </c>
+      <c r="HD6" s="18" t="s">
+        <v>407</v>
+      </c>
+      <c r="HE6" s="18" t="s">
+        <v>408</v>
+      </c>
+      <c r="HF6" s="18" t="s">
+        <v>409</v>
+      </c>
+      <c r="HG6" s="18" t="s">
+        <v>410</v>
+      </c>
+      <c r="HH6" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="HI6" s="18" t="s">
+        <v>412</v>
+      </c>
+      <c r="HJ6" s="18" t="s">
+        <v>413</v>
+      </c>
+      <c r="HK6" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="HL6" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="HM6" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="HN6" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="HO6" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="HP6" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="HQ6" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="HR6" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="HS6" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="HT6" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="HU6" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="HV6" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="HW6" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="HX6" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="HY6" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="HZ6" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="IA6" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="IB6" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="IC6" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="ID6" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="IE6" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="IF6" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="IG6" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="IH6" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="II6" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="IJ6" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="IK6" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="IL6" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="IM6" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="IN6" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="IO6" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="IP6" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="IQ6" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="IR6" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="IS6" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="IT6" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="IU6" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="IV6" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="IW6" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="IX6" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="IY6" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="IZ6" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="JA6" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="JB6" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="JC6" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="JD6" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="JE6" s="18" t="s">
+        <v>215</v>
+      </c>
+      <c r="JF6" s="18" t="s">
+        <v>216</v>
+      </c>
+      <c r="JG6" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="JH6" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="JI6" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="JJ6" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="JK6" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="JL6" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="JM6" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="JN6" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="JO6" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="JP6" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="JQ6" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="JR6" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="JS6" s="18" t="s">
+        <v>232</v>
+      </c>
+      <c r="JT6" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="JU6" s="18" t="s">
+        <v>233</v>
+      </c>
+      <c r="JV6" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="JW6" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="JX6" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="JY6" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="JZ6" s="18" t="s">
+        <v>238</v>
+      </c>
+      <c r="KA6" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="KB6" s="18" t="s">
+        <v>240</v>
+      </c>
+      <c r="KC6" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="KD6" s="18" t="s">
+        <v>242</v>
+      </c>
+      <c r="KE6" s="18" t="s">
+        <v>243</v>
+      </c>
+      <c r="KF6" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="KG6" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="KH6" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="KI6" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="KJ6" s="18" t="s">
+        <v>248</v>
+      </c>
+      <c r="KK6" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="KL6" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="KM6" s="18" t="s">
+        <v>252</v>
+      </c>
+      <c r="KN6" s="18" t="s">
+        <v>253</v>
+      </c>
+      <c r="KO6" s="18" t="s">
+        <v>254</v>
+      </c>
+      <c r="KP6" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="KQ6" s="18" t="s">
+        <v>256</v>
+      </c>
+      <c r="KR6" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="KS6" s="18" t="s">
+        <v>258</v>
+      </c>
+      <c r="KT6" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="KU6" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="KV6" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="KW6" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="KX6" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="KY6" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="KZ6" s="18" t="s">
+        <v>266</v>
+      </c>
+      <c r="LA6" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="LB6" s="18" t="s">
+        <v>268</v>
+      </c>
+      <c r="LC6" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="LD6" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="LE6" s="18" t="s">
+        <v>271</v>
+      </c>
+      <c r="LF6" s="18" t="s">
+        <v>272</v>
+      </c>
+      <c r="LG6" s="18" t="s">
+        <v>274</v>
+      </c>
+      <c r="LH6" s="18" t="s">
+        <v>275</v>
+      </c>
+      <c r="LI6" s="18" t="s">
+        <v>276</v>
+      </c>
+      <c r="LJ6" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="LK6" s="18" t="s">
+        <v>278</v>
+      </c>
+      <c r="LL6" s="18" t="s">
+        <v>301</v>
+      </c>
+      <c r="LM6" s="18" t="s">
+        <v>302</v>
+      </c>
+      <c r="LN6" s="18" t="s">
+        <v>303</v>
+      </c>
+      <c r="LO6" s="18" t="s">
+        <v>304</v>
+      </c>
+      <c r="LP6" s="18" t="s">
+        <v>305</v>
+      </c>
+      <c r="LQ6" s="18" t="s">
+        <v>280</v>
+      </c>
+      <c r="LR6" s="18" t="s">
+        <v>281</v>
+      </c>
+      <c r="LS6" s="18" t="s">
+        <v>282</v>
+      </c>
+      <c r="LT6" s="18" t="s">
+        <v>283</v>
+      </c>
+      <c r="LU6" s="18" t="s">
+        <v>284</v>
+      </c>
+      <c r="LV6" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="LW6" s="18" t="s">
+        <v>286</v>
+      </c>
+      <c r="LX6" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="LY6" s="18" t="s">
+        <v>288</v>
+      </c>
+      <c r="LZ6" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="MA6" s="18" t="s">
+        <v>291</v>
+      </c>
+      <c r="MB6" s="18" t="s">
+        <v>292</v>
+      </c>
+      <c r="MC6" s="18" t="s">
+        <v>293</v>
+      </c>
+      <c r="MD6" s="18" t="s">
+        <v>294</v>
+      </c>
+      <c r="ME6" s="18" t="s">
+        <v>295</v>
+      </c>
+      <c r="MF6" s="18" t="s">
+        <v>296</v>
+      </c>
+      <c r="MG6" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="MH6" s="18" t="s">
+        <v>298</v>
+      </c>
+      <c r="MI6" s="18" t="s">
+        <v>299</v>
+      </c>
+      <c r="MJ6" s="18" t="s">
+        <v>300</v>
+      </c>
+      <c r="MK6" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="GT6" s="9" t="s">
+      <c r="ML6" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="GU6" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="GV6" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="GW6" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="GX6" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="GY6" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="GZ6" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="HA6" s="18" t="s">
-        <v>406</v>
-      </c>
-      <c r="HB6" s="18" t="s">
-        <v>407</v>
-      </c>
-      <c r="HC6" s="18" t="s">
-        <v>408</v>
-      </c>
-      <c r="HD6" s="18" t="s">
-        <v>409</v>
-      </c>
-      <c r="HE6" s="18" t="s">
-        <v>410</v>
-      </c>
-      <c r="HF6" s="18" t="s">
-        <v>411</v>
-      </c>
-      <c r="HG6" s="18" t="s">
-        <v>412</v>
-      </c>
-      <c r="HH6" s="18" t="s">
-        <v>413</v>
-      </c>
-      <c r="HI6" s="18" t="s">
-        <v>414</v>
-      </c>
-      <c r="HJ6" s="18" t="s">
-        <v>415</v>
-      </c>
-      <c r="HK6" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="HL6" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="HM6" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="HN6" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="HO6" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="HP6" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="HQ6" s="18" t="s">
-        <v>173</v>
-      </c>
-      <c r="HR6" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="HS6" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="HT6" s="18" t="s">
-        <v>176</v>
-      </c>
-      <c r="HU6" s="18" t="s">
-        <v>178</v>
-      </c>
-      <c r="HV6" s="18" t="s">
-        <v>179</v>
-      </c>
-      <c r="HW6" s="18" t="s">
-        <v>180</v>
-      </c>
-      <c r="HX6" s="18" t="s">
-        <v>181</v>
-      </c>
-      <c r="HY6" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="HZ6" s="18" t="s">
-        <v>183</v>
-      </c>
-      <c r="IA6" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="IB6" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="IC6" s="18" t="s">
-        <v>186</v>
-      </c>
-      <c r="ID6" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="IE6" s="18" t="s">
-        <v>189</v>
-      </c>
-      <c r="IF6" s="18" t="s">
-        <v>190</v>
-      </c>
-      <c r="IG6" s="18" t="s">
-        <v>191</v>
-      </c>
-      <c r="IH6" s="18" t="s">
-        <v>192</v>
-      </c>
-      <c r="II6" s="18" t="s">
-        <v>193</v>
-      </c>
-      <c r="IJ6" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="IK6" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="IL6" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="IM6" s="18" t="s">
-        <v>197</v>
-      </c>
-      <c r="IN6" s="18" t="s">
-        <v>198</v>
-      </c>
-      <c r="IO6" s="18" t="s">
-        <v>200</v>
-      </c>
-      <c r="IP6" s="18" t="s">
-        <v>201</v>
-      </c>
-      <c r="IQ6" s="18" t="s">
-        <v>202</v>
-      </c>
-      <c r="IR6" s="18" t="s">
-        <v>203</v>
-      </c>
-      <c r="IS6" s="18" t="s">
-        <v>204</v>
-      </c>
-      <c r="IT6" s="18" t="s">
-        <v>205</v>
-      </c>
-      <c r="IU6" s="18" t="s">
-        <v>206</v>
-      </c>
-      <c r="IV6" s="18" t="s">
-        <v>207</v>
-      </c>
-      <c r="IW6" s="18" t="s">
-        <v>208</v>
-      </c>
-      <c r="IX6" s="18" t="s">
-        <v>209</v>
-      </c>
-      <c r="IY6" s="18" t="s">
-        <v>211</v>
-      </c>
-      <c r="IZ6" s="18" t="s">
-        <v>212</v>
-      </c>
-      <c r="JA6" s="18" t="s">
-        <v>213</v>
-      </c>
-      <c r="JB6" s="18" t="s">
-        <v>214</v>
-      </c>
-      <c r="JC6" s="18" t="s">
-        <v>215</v>
-      </c>
-      <c r="JD6" s="18" t="s">
-        <v>216</v>
-      </c>
-      <c r="JE6" s="18" t="s">
-        <v>217</v>
-      </c>
-      <c r="JF6" s="18" t="s">
-        <v>218</v>
-      </c>
-      <c r="JG6" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="JH6" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="JI6" s="18" t="s">
-        <v>222</v>
-      </c>
-      <c r="JJ6" s="18" t="s">
-        <v>223</v>
-      </c>
-      <c r="JK6" s="18" t="s">
-        <v>224</v>
-      </c>
-      <c r="JL6" s="18" t="s">
-        <v>225</v>
-      </c>
-      <c r="JM6" s="18" t="s">
-        <v>226</v>
-      </c>
-      <c r="JN6" s="18" t="s">
-        <v>227</v>
-      </c>
-      <c r="JO6" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="JP6" s="18" t="s">
-        <v>229</v>
-      </c>
-      <c r="JQ6" s="18" t="s">
-        <v>230</v>
-      </c>
-      <c r="JR6" s="18" t="s">
-        <v>231</v>
-      </c>
-      <c r="JS6" s="18" t="s">
-        <v>234</v>
-      </c>
-      <c r="JT6" s="18" t="s">
-        <v>233</v>
-      </c>
-      <c r="JU6" s="18" t="s">
-        <v>235</v>
-      </c>
-      <c r="JV6" s="18" t="s">
-        <v>236</v>
-      </c>
-      <c r="JW6" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="JX6" s="18" t="s">
-        <v>238</v>
-      </c>
-      <c r="JY6" s="18" t="s">
-        <v>239</v>
-      </c>
-      <c r="JZ6" s="18" t="s">
-        <v>240</v>
-      </c>
-      <c r="KA6" s="18" t="s">
-        <v>241</v>
-      </c>
-      <c r="KB6" s="18" t="s">
-        <v>242</v>
-      </c>
-      <c r="KC6" s="18" t="s">
-        <v>243</v>
-      </c>
-      <c r="KD6" s="18" t="s">
-        <v>244</v>
-      </c>
-      <c r="KE6" s="18" t="s">
-        <v>245</v>
-      </c>
-      <c r="KF6" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="KG6" s="18" t="s">
-        <v>247</v>
-      </c>
-      <c r="KH6" s="18" t="s">
-        <v>248</v>
-      </c>
-      <c r="KI6" s="18" t="s">
-        <v>249</v>
-      </c>
-      <c r="KJ6" s="18" t="s">
-        <v>250</v>
-      </c>
-      <c r="KK6" s="18" t="s">
-        <v>251</v>
-      </c>
-      <c r="KL6" s="18" t="s">
-        <v>252</v>
-      </c>
-      <c r="KM6" s="18" t="s">
-        <v>254</v>
-      </c>
-      <c r="KN6" s="18" t="s">
-        <v>255</v>
-      </c>
-      <c r="KO6" s="18" t="s">
-        <v>256</v>
-      </c>
-      <c r="KP6" s="18" t="s">
-        <v>257</v>
-      </c>
-      <c r="KQ6" s="18" t="s">
-        <v>258</v>
-      </c>
-      <c r="KR6" s="18" t="s">
-        <v>259</v>
-      </c>
-      <c r="KS6" s="18" t="s">
-        <v>260</v>
-      </c>
-      <c r="KT6" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="KU6" s="18" t="s">
-        <v>262</v>
-      </c>
-      <c r="KV6" s="18" t="s">
-        <v>263</v>
-      </c>
-      <c r="KW6" s="18" t="s">
-        <v>265</v>
-      </c>
-      <c r="KX6" s="18" t="s">
-        <v>266</v>
-      </c>
-      <c r="KY6" s="18" t="s">
-        <v>267</v>
-      </c>
-      <c r="KZ6" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="LA6" s="18" t="s">
-        <v>269</v>
-      </c>
-      <c r="LB6" s="18" t="s">
-        <v>270</v>
-      </c>
-      <c r="LC6" s="18" t="s">
-        <v>271</v>
-      </c>
-      <c r="LD6" s="18" t="s">
-        <v>272</v>
-      </c>
-      <c r="LE6" s="18" t="s">
-        <v>273</v>
-      </c>
-      <c r="LF6" s="18" t="s">
-        <v>274</v>
-      </c>
-      <c r="LG6" s="18" t="s">
-        <v>276</v>
-      </c>
-      <c r="LH6" s="18" t="s">
-        <v>277</v>
-      </c>
-      <c r="LI6" s="18" t="s">
-        <v>278</v>
-      </c>
-      <c r="LJ6" s="18" t="s">
-        <v>279</v>
-      </c>
-      <c r="LK6" s="18" t="s">
-        <v>280</v>
-      </c>
-      <c r="LL6" s="18" t="s">
-        <v>303</v>
-      </c>
-      <c r="LM6" s="18" t="s">
-        <v>304</v>
-      </c>
-      <c r="LN6" s="18" t="s">
-        <v>305</v>
-      </c>
-      <c r="LO6" s="18" t="s">
-        <v>306</v>
-      </c>
-      <c r="LP6" s="18" t="s">
-        <v>307</v>
-      </c>
-      <c r="LQ6" s="18" t="s">
-        <v>282</v>
-      </c>
-      <c r="LR6" s="18" t="s">
-        <v>283</v>
-      </c>
-      <c r="LS6" s="18" t="s">
-        <v>284</v>
-      </c>
-      <c r="LT6" s="18" t="s">
-        <v>285</v>
-      </c>
-      <c r="LU6" s="18" t="s">
-        <v>286</v>
-      </c>
-      <c r="LV6" s="18" t="s">
-        <v>287</v>
-      </c>
-      <c r="LW6" s="18" t="s">
-        <v>288</v>
-      </c>
-      <c r="LX6" s="18" t="s">
-        <v>289</v>
-      </c>
-      <c r="LY6" s="18" t="s">
-        <v>290</v>
-      </c>
-      <c r="LZ6" s="18" t="s">
-        <v>291</v>
-      </c>
-      <c r="MA6" s="18" t="s">
-        <v>293</v>
-      </c>
-      <c r="MB6" s="18" t="s">
-        <v>294</v>
-      </c>
-      <c r="MC6" s="18" t="s">
-        <v>295</v>
-      </c>
-      <c r="MD6" s="18" t="s">
-        <v>296</v>
-      </c>
-      <c r="ME6" s="18" t="s">
-        <v>297</v>
-      </c>
-      <c r="MF6" s="18" t="s">
-        <v>298</v>
-      </c>
-      <c r="MG6" s="18" t="s">
-        <v>299</v>
-      </c>
-      <c r="MH6" s="18" t="s">
-        <v>300</v>
-      </c>
-      <c r="MI6" s="18" t="s">
-        <v>301</v>
-      </c>
-      <c r="MJ6" s="18" t="s">
-        <v>302</v>
-      </c>
-      <c r="MK6" s="18" t="s">
+      <c r="MM6" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="ML6" s="18" t="s">
+      <c r="MN6" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="MM6" s="18" t="s">
+      <c r="MO6" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="MN6" s="18" t="s">
+      <c r="MP6" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="MO6" s="18" t="s">
+      <c r="MQ6" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="MP6" s="18" t="s">
+      <c r="MR6" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="MQ6" s="18" t="s">
+      <c r="MS6" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="MR6" s="18" t="s">
+      <c r="MT6" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="MS6" s="18" t="s">
+      <c r="MU6" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="MT6" s="18" t="s">
+      <c r="MV6" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="MU6" s="18" t="s">
+      <c r="MW6" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="MV6" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="MW6" s="18" t="s">
+      <c r="MX6" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="MY6" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="MZ6" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="NA6" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="MX6" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="MY6" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="MZ6" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="NA6" s="18" t="s">
-        <v>111</v>
-      </c>
       <c r="NB6" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="NC6" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="ND6" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="NC6" s="18" t="s">
+      <c r="NE6" s="18" t="s">
         <v>116</v>
-      </c>
-      <c r="ND6" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="NE6" s="18" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:369" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="40"/>
       <c r="B7" s="40"/>
       <c r="C7" s="40" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D7" s="40"/>
       <c r="E7" s="40"/>
@@ -5952,17 +5952,17 @@
       <c r="L7" s="42"/>
       <c r="M7" s="42"/>
       <c r="N7" s="42" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="O7" s="42" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="P7" s="42"/>
       <c r="Q7" s="43" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="R7" s="43" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="S7" s="42"/>
       <c r="T7" s="42"/>
@@ -5974,13 +5974,13 @@
       <c r="Z7" s="47"/>
       <c r="AA7" s="46"/>
       <c r="AB7" s="41" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="AC7" s="41" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="AD7" s="41" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="AE7" s="42"/>
       <c r="AF7" s="48"/>
@@ -6114,43 +6114,43 @@
         <v>0</v>
       </c>
       <c r="BQ7" s="51">
-        <f>CA7+CK7+CU7+DE7+DO7+DY7+EI7+ES7+FC7+FM7+FW7+GG7+GQ7+HA7</f>
+        <f t="shared" ref="BQ7:BZ7" si="1">CA7+CK7+CU7+DE7+DO7+DY7+EI7+ES7+FC7+FM7+FW7+GG7+GQ7+HA7</f>
         <v>0</v>
       </c>
       <c r="BR7" s="51">
-        <f>CB7+CL7+CV7+DF7+DP7+DZ7+EJ7+ET7+FD7+FN7+FX7+GH7+GR7+HB7</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BS7" s="51">
-        <f>CC7+CM7+CW7+DG7+DQ7+EA7+EK7+EU7+FE7+FO7+FY7+GI7+GS7+HC7</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BT7" s="51">
-        <f>CD7+CN7+CX7+DH7+DR7+EB7+EL7+EV7+FF7+FP7+FZ7+GJ7+GT7+HD7</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BU7" s="51">
-        <f>CE7+CO7+CY7+DI7+DS7+EC7+EM7+EW7+FG7+FQ7+GA7+GK7+GU7+HE7</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BV7" s="51">
-        <f>CF7+CP7+CZ7+DJ7+DT7+ED7+EN7+EX7+FH7+FR7+GB7+GL7+GV7+HF7</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BW7" s="51">
-        <f>CG7+CQ7+DA7+DK7+DU7+EE7+EO7+EY7+FI7+FS7+GC7+GM7+GW7+HG7</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BX7" s="51">
-        <f>CH7+CR7+DB7+DL7+DV7+EF7+EP7+EZ7+FJ7+FT7+GD7+GN7+GX7+HH7</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BY7" s="51">
-        <f>CI7+CS7+DC7+DM7+DW7+EG7+EQ7+FA7+FK7+FU7+GE7+GO7+GY7+HI7</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BZ7" s="51">
-        <f>CJ7+CT7+DD7+DN7+DX7+EH7+ER7+FB7+FL7+FV7+GF7+GP7+GZ7+HJ7</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="CA7" s="46"/>
@@ -6448,33 +6448,6 @@
   </sheetData>
   <autoFilter ref="A6:NA6" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="43">
-    <mergeCell ref="EI4:ER4"/>
-    <mergeCell ref="ES4:FB4"/>
-    <mergeCell ref="CA4:CJ4"/>
-    <mergeCell ref="CU4:DD4"/>
-    <mergeCell ref="DE4:DN4"/>
-    <mergeCell ref="DO4:DX4"/>
-    <mergeCell ref="DY4:EH4"/>
-    <mergeCell ref="HA4:HJ4"/>
-    <mergeCell ref="MX4:MZ5"/>
-    <mergeCell ref="HU4:ID4"/>
-    <mergeCell ref="KM4:KV4"/>
-    <mergeCell ref="KW4:LF4"/>
-    <mergeCell ref="LG4:LP4"/>
-    <mergeCell ref="MA4:MJ4"/>
-    <mergeCell ref="MK4:MW5"/>
-    <mergeCell ref="IE4:IN4"/>
-    <mergeCell ref="IO4:IX4"/>
-    <mergeCell ref="IY4:JH4"/>
-    <mergeCell ref="JI4:JR4"/>
-    <mergeCell ref="JS4:KB4"/>
-    <mergeCell ref="KC4:KL4"/>
-    <mergeCell ref="LQ4:LZ4"/>
-    <mergeCell ref="FC4:FL4"/>
-    <mergeCell ref="FM4:FV4"/>
-    <mergeCell ref="FW4:GF4"/>
-    <mergeCell ref="GG4:GP4"/>
-    <mergeCell ref="GQ4:GZ4"/>
     <mergeCell ref="NB4:NC5"/>
     <mergeCell ref="AE4:AF5"/>
     <mergeCell ref="A1:B1"/>
@@ -6491,6 +6464,33 @@
     <mergeCell ref="AL4:BP5"/>
     <mergeCell ref="BQ4:BZ4"/>
     <mergeCell ref="CK4:CT4"/>
+    <mergeCell ref="FC4:FL4"/>
+    <mergeCell ref="FM4:FV4"/>
+    <mergeCell ref="FW4:GF4"/>
+    <mergeCell ref="GG4:GP4"/>
+    <mergeCell ref="GQ4:GZ4"/>
+    <mergeCell ref="HA4:HJ4"/>
+    <mergeCell ref="MX4:MZ5"/>
+    <mergeCell ref="HU4:ID4"/>
+    <mergeCell ref="KM4:KV4"/>
+    <mergeCell ref="KW4:LF4"/>
+    <mergeCell ref="LG4:LP4"/>
+    <mergeCell ref="MA4:MJ4"/>
+    <mergeCell ref="MK4:MW5"/>
+    <mergeCell ref="IE4:IN4"/>
+    <mergeCell ref="IO4:IX4"/>
+    <mergeCell ref="IY4:JH4"/>
+    <mergeCell ref="JI4:JR4"/>
+    <mergeCell ref="JS4:KB4"/>
+    <mergeCell ref="KC4:KL4"/>
+    <mergeCell ref="LQ4:LZ4"/>
+    <mergeCell ref="EI4:ER4"/>
+    <mergeCell ref="ES4:FB4"/>
+    <mergeCell ref="CA4:CJ4"/>
+    <mergeCell ref="CU4:DD4"/>
+    <mergeCell ref="DE4:DN4"/>
+    <mergeCell ref="DO4:DX4"/>
+    <mergeCell ref="DY4:EH4"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A6">
     <cfRule type="duplicateValues" dxfId="0" priority="92"/>

</xml_diff>

<commit_message>
[RUBY-2585] Adjust FCRM1 report - natural measures yes/no option
</commit_message>
<xml_diff>
--- a/lib/fcerm1_template.xlsx
+++ b/lib/fcerm1_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lb000070\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E994A4C9-33C1-4204-B14E-19CC60276746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F477D19-A2BE-468F-A183-C8870840E886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -344,9 +344,6 @@
     <t>OM4c Total</t>
   </si>
   <si>
-    <t>Main natural flood management measure</t>
-  </si>
-  <si>
     <t>Cost of associated Natural Flood Risk Measures (£)</t>
   </si>
   <si>
@@ -1317,6 +1314,9 @@
   </si>
   <si>
     <t>Does this project contain any Natural Flood Risk Management Measures?</t>
+  </si>
+  <si>
+    <t>Main natural flood management measure (s)</t>
   </si>
 </sst>
 </file>
@@ -1886,18 +1886,75 @@
     <xf numFmtId="0" fontId="12" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="21" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1928,68 +1985,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="5" fillId="11" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -2298,11 +2298,11 @@
   <dimension ref="A1:NF7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="BM7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="MN7" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
       <selection pane="topRight" activeCell="C7" sqref="C7"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="BO6" sqref="BO6"/>
+      <selection pane="bottomRight" activeCell="MO7" sqref="MO7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2331,10 +2331,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:370" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="63"/>
+      <c r="B1" s="82"/>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
       <c r="E1" s="20"/>
@@ -2705,10 +2705,10 @@
       <c r="NF1" s="39"/>
     </row>
     <row r="2" spans="1:370" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="64" t="s">
-        <v>159</v>
-      </c>
-      <c r="B2" s="64"/>
+      <c r="A2" s="83" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="83"/>
       <c r="C2" s="19"/>
       <c r="D2" s="29"/>
       <c r="E2" s="20"/>
@@ -3451,201 +3451,201 @@
       <c r="NF3" s="39"/>
     </row>
     <row r="4" spans="1:370" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="66" t="s">
+      <c r="B4" s="84"/>
+      <c r="C4" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="67" t="s">
+      <c r="D4" s="85"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="85"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
+      <c r="I4" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="67"/>
-      <c r="K4" s="67"/>
-      <c r="L4" s="67"/>
-      <c r="M4" s="67"/>
-      <c r="N4" s="68" t="s">
+      <c r="J4" s="86"/>
+      <c r="K4" s="86"/>
+      <c r="L4" s="86"/>
+      <c r="M4" s="86"/>
+      <c r="N4" s="87" t="s">
         <v>4</v>
       </c>
-      <c r="O4" s="68"/>
-      <c r="P4" s="68"/>
-      <c r="Q4" s="69" t="s">
+      <c r="O4" s="87"/>
+      <c r="P4" s="87"/>
+      <c r="Q4" s="88" t="s">
+        <v>316</v>
+      </c>
+      <c r="R4" s="88"/>
+      <c r="S4" s="88"/>
+      <c r="T4" s="88"/>
+      <c r="U4" s="88"/>
+      <c r="V4" s="89" t="s">
+        <v>5</v>
+      </c>
+      <c r="W4" s="89"/>
+      <c r="X4" s="89"/>
+      <c r="Y4" s="89"/>
+      <c r="Z4" s="89"/>
+      <c r="AA4" s="89"/>
+      <c r="AB4" s="89"/>
+      <c r="AC4" s="90" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD4" s="90"/>
+      <c r="AE4" s="90"/>
+      <c r="AF4" s="81" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG4" s="81"/>
+      <c r="AH4" s="91"/>
+      <c r="AI4" s="91"/>
+      <c r="AJ4" s="91"/>
+      <c r="AK4" s="91"/>
+      <c r="AL4" s="91"/>
+      <c r="AM4" s="92" t="s">
+        <v>8</v>
+      </c>
+      <c r="AN4" s="92"/>
+      <c r="AO4" s="92"/>
+      <c r="AP4" s="92"/>
+      <c r="AQ4" s="92"/>
+      <c r="AR4" s="92"/>
+      <c r="AS4" s="92"/>
+      <c r="AT4" s="92"/>
+      <c r="AU4" s="92"/>
+      <c r="AV4" s="92"/>
+      <c r="AW4" s="92"/>
+      <c r="AX4" s="92"/>
+      <c r="AY4" s="92"/>
+      <c r="AZ4" s="92"/>
+      <c r="BA4" s="92"/>
+      <c r="BB4" s="92"/>
+      <c r="BC4" s="92"/>
+      <c r="BD4" s="92"/>
+      <c r="BE4" s="92"/>
+      <c r="BF4" s="92"/>
+      <c r="BG4" s="92"/>
+      <c r="BH4" s="92"/>
+      <c r="BI4" s="92"/>
+      <c r="BJ4" s="92"/>
+      <c r="BK4" s="92"/>
+      <c r="BL4" s="92"/>
+      <c r="BM4" s="92"/>
+      <c r="BN4" s="92"/>
+      <c r="BO4" s="92"/>
+      <c r="BP4" s="92"/>
+      <c r="BQ4" s="92"/>
+      <c r="BR4" s="70" t="s">
+        <v>9</v>
+      </c>
+      <c r="BS4" s="70"/>
+      <c r="BT4" s="70"/>
+      <c r="BU4" s="70"/>
+      <c r="BV4" s="70"/>
+      <c r="BW4" s="70"/>
+      <c r="BX4" s="70"/>
+      <c r="BY4" s="70"/>
+      <c r="BZ4" s="70"/>
+      <c r="CA4" s="70"/>
+      <c r="CB4" s="58" t="s">
+        <v>10</v>
+      </c>
+      <c r="CC4" s="58"/>
+      <c r="CD4" s="58"/>
+      <c r="CE4" s="58"/>
+      <c r="CF4" s="58"/>
+      <c r="CG4" s="58"/>
+      <c r="CH4" s="58"/>
+      <c r="CI4" s="58"/>
+      <c r="CJ4" s="58"/>
+      <c r="CK4" s="58"/>
+      <c r="CL4" s="62" t="s">
         <v>317</v>
       </c>
-      <c r="R4" s="69"/>
-      <c r="S4" s="69"/>
-      <c r="T4" s="69"/>
-      <c r="U4" s="69"/>
-      <c r="V4" s="70" t="s">
-        <v>5</v>
-      </c>
-      <c r="W4" s="70"/>
-      <c r="X4" s="70"/>
-      <c r="Y4" s="70"/>
-      <c r="Z4" s="70"/>
-      <c r="AA4" s="70"/>
-      <c r="AB4" s="70"/>
-      <c r="AC4" s="71" t="s">
-        <v>6</v>
-      </c>
-      <c r="AD4" s="71"/>
-      <c r="AE4" s="71"/>
-      <c r="AF4" s="62" t="s">
-        <v>7</v>
-      </c>
-      <c r="AG4" s="62"/>
-      <c r="AH4" s="73"/>
-      <c r="AI4" s="73"/>
-      <c r="AJ4" s="73"/>
-      <c r="AK4" s="73"/>
-      <c r="AL4" s="73"/>
-      <c r="AM4" s="74" t="s">
-        <v>8</v>
-      </c>
-      <c r="AN4" s="74"/>
-      <c r="AO4" s="74"/>
-      <c r="AP4" s="74"/>
-      <c r="AQ4" s="74"/>
-      <c r="AR4" s="74"/>
-      <c r="AS4" s="74"/>
-      <c r="AT4" s="74"/>
-      <c r="AU4" s="74"/>
-      <c r="AV4" s="74"/>
-      <c r="AW4" s="74"/>
-      <c r="AX4" s="74"/>
-      <c r="AY4" s="74"/>
-      <c r="AZ4" s="74"/>
-      <c r="BA4" s="74"/>
-      <c r="BB4" s="74"/>
-      <c r="BC4" s="74"/>
-      <c r="BD4" s="74"/>
-      <c r="BE4" s="74"/>
-      <c r="BF4" s="74"/>
-      <c r="BG4" s="74"/>
-      <c r="BH4" s="74"/>
-      <c r="BI4" s="74"/>
-      <c r="BJ4" s="74"/>
-      <c r="BK4" s="74"/>
-      <c r="BL4" s="74"/>
-      <c r="BM4" s="74"/>
-      <c r="BN4" s="74"/>
-      <c r="BO4" s="74"/>
-      <c r="BP4" s="74"/>
-      <c r="BQ4" s="74"/>
-      <c r="BR4" s="72" t="s">
-        <v>9</v>
-      </c>
-      <c r="BS4" s="72"/>
-      <c r="BT4" s="72"/>
-      <c r="BU4" s="72"/>
-      <c r="BV4" s="72"/>
-      <c r="BW4" s="72"/>
-      <c r="BX4" s="72"/>
-      <c r="BY4" s="72"/>
-      <c r="BZ4" s="72"/>
-      <c r="CA4" s="72"/>
-      <c r="CB4" s="89" t="s">
-        <v>10</v>
-      </c>
-      <c r="CC4" s="89"/>
-      <c r="CD4" s="89"/>
-      <c r="CE4" s="89"/>
-      <c r="CF4" s="89"/>
-      <c r="CG4" s="89"/>
-      <c r="CH4" s="89"/>
-      <c r="CI4" s="89"/>
-      <c r="CJ4" s="89"/>
-      <c r="CK4" s="89"/>
-      <c r="CL4" s="75" t="s">
+      <c r="CM4" s="62"/>
+      <c r="CN4" s="62"/>
+      <c r="CO4" s="62"/>
+      <c r="CP4" s="62"/>
+      <c r="CQ4" s="62"/>
+      <c r="CR4" s="62"/>
+      <c r="CS4" s="62"/>
+      <c r="CT4" s="62"/>
+      <c r="CU4" s="62"/>
+      <c r="CV4" s="58" t="s">
         <v>318</v>
       </c>
-      <c r="CM4" s="75"/>
-      <c r="CN4" s="75"/>
-      <c r="CO4" s="75"/>
-      <c r="CP4" s="75"/>
-      <c r="CQ4" s="75"/>
-      <c r="CR4" s="75"/>
-      <c r="CS4" s="75"/>
-      <c r="CT4" s="75"/>
-      <c r="CU4" s="75"/>
-      <c r="CV4" s="89" t="s">
+      <c r="CW4" s="58"/>
+      <c r="CX4" s="58"/>
+      <c r="CY4" s="58"/>
+      <c r="CZ4" s="58"/>
+      <c r="DA4" s="58"/>
+      <c r="DB4" s="58"/>
+      <c r="DC4" s="58"/>
+      <c r="DD4" s="58"/>
+      <c r="DE4" s="58"/>
+      <c r="DF4" s="62" t="s">
         <v>319</v>
       </c>
-      <c r="CW4" s="89"/>
-      <c r="CX4" s="89"/>
-      <c r="CY4" s="89"/>
-      <c r="CZ4" s="89"/>
-      <c r="DA4" s="89"/>
-      <c r="DB4" s="89"/>
-      <c r="DC4" s="89"/>
-      <c r="DD4" s="89"/>
-      <c r="DE4" s="89"/>
-      <c r="DF4" s="75" t="s">
+      <c r="DG4" s="62"/>
+      <c r="DH4" s="62"/>
+      <c r="DI4" s="62"/>
+      <c r="DJ4" s="62"/>
+      <c r="DK4" s="62"/>
+      <c r="DL4" s="62"/>
+      <c r="DM4" s="62"/>
+      <c r="DN4" s="62"/>
+      <c r="DO4" s="62"/>
+      <c r="DP4" s="58" t="s">
         <v>320</v>
       </c>
-      <c r="DG4" s="75"/>
-      <c r="DH4" s="75"/>
-      <c r="DI4" s="75"/>
-      <c r="DJ4" s="75"/>
-      <c r="DK4" s="75"/>
-      <c r="DL4" s="75"/>
-      <c r="DM4" s="75"/>
-      <c r="DN4" s="75"/>
-      <c r="DO4" s="75"/>
-      <c r="DP4" s="89" t="s">
-        <v>321</v>
-      </c>
-      <c r="DQ4" s="89"/>
-      <c r="DR4" s="89"/>
-      <c r="DS4" s="89"/>
-      <c r="DT4" s="89"/>
-      <c r="DU4" s="89"/>
-      <c r="DV4" s="89"/>
-      <c r="DW4" s="89"/>
-      <c r="DX4" s="89"/>
-      <c r="DY4" s="89"/>
-      <c r="DZ4" s="90" t="s">
-        <v>362</v>
-      </c>
-      <c r="EA4" s="91"/>
-      <c r="EB4" s="91"/>
-      <c r="EC4" s="91"/>
-      <c r="ED4" s="91"/>
-      <c r="EE4" s="91"/>
-      <c r="EF4" s="91"/>
-      <c r="EG4" s="91"/>
-      <c r="EH4" s="91"/>
-      <c r="EI4" s="92"/>
-      <c r="EJ4" s="89" t="s">
-        <v>373</v>
-      </c>
-      <c r="EK4" s="89"/>
-      <c r="EL4" s="89"/>
-      <c r="EM4" s="89"/>
-      <c r="EN4" s="89"/>
-      <c r="EO4" s="89"/>
-      <c r="EP4" s="89"/>
-      <c r="EQ4" s="89"/>
-      <c r="ER4" s="89"/>
-      <c r="ES4" s="89"/>
-      <c r="ET4" s="90" t="s">
-        <v>384</v>
-      </c>
-      <c r="EU4" s="91"/>
-      <c r="EV4" s="91"/>
-      <c r="EW4" s="91"/>
-      <c r="EX4" s="91"/>
-      <c r="EY4" s="91"/>
-      <c r="EZ4" s="91"/>
-      <c r="FA4" s="91"/>
-      <c r="FB4" s="91"/>
-      <c r="FC4" s="92"/>
+      <c r="DQ4" s="58"/>
+      <c r="DR4" s="58"/>
+      <c r="DS4" s="58"/>
+      <c r="DT4" s="58"/>
+      <c r="DU4" s="58"/>
+      <c r="DV4" s="58"/>
+      <c r="DW4" s="58"/>
+      <c r="DX4" s="58"/>
+      <c r="DY4" s="58"/>
+      <c r="DZ4" s="59" t="s">
+        <v>361</v>
+      </c>
+      <c r="EA4" s="60"/>
+      <c r="EB4" s="60"/>
+      <c r="EC4" s="60"/>
+      <c r="ED4" s="60"/>
+      <c r="EE4" s="60"/>
+      <c r="EF4" s="60"/>
+      <c r="EG4" s="60"/>
+      <c r="EH4" s="60"/>
+      <c r="EI4" s="61"/>
+      <c r="EJ4" s="58" t="s">
+        <v>372</v>
+      </c>
+      <c r="EK4" s="58"/>
+      <c r="EL4" s="58"/>
+      <c r="EM4" s="58"/>
+      <c r="EN4" s="58"/>
+      <c r="EO4" s="58"/>
+      <c r="EP4" s="58"/>
+      <c r="EQ4" s="58"/>
+      <c r="ER4" s="58"/>
+      <c r="ES4" s="58"/>
+      <c r="ET4" s="59" t="s">
+        <v>383</v>
+      </c>
+      <c r="EU4" s="60"/>
+      <c r="EV4" s="60"/>
+      <c r="EW4" s="60"/>
+      <c r="EX4" s="60"/>
+      <c r="EY4" s="60"/>
+      <c r="EZ4" s="60"/>
+      <c r="FA4" s="60"/>
+      <c r="FB4" s="60"/>
+      <c r="FC4" s="61"/>
       <c r="FD4" s="76" t="s">
         <v>11</v>
       </c>
@@ -3706,272 +3706,272 @@
       <c r="GY4" s="80"/>
       <c r="GZ4" s="80"/>
       <c r="HA4" s="80"/>
-      <c r="HB4" s="81" t="s">
-        <v>412</v>
-      </c>
-      <c r="HC4" s="81"/>
-      <c r="HD4" s="81"/>
-      <c r="HE4" s="81"/>
-      <c r="HF4" s="81"/>
-      <c r="HG4" s="81"/>
-      <c r="HH4" s="81"/>
-      <c r="HI4" s="81"/>
-      <c r="HJ4" s="81"/>
-      <c r="HK4" s="81"/>
-      <c r="HL4" s="72" t="s">
-        <v>162</v>
-      </c>
-      <c r="HM4" s="72"/>
-      <c r="HN4" s="72"/>
-      <c r="HO4" s="72"/>
-      <c r="HP4" s="72"/>
-      <c r="HQ4" s="72"/>
-      <c r="HR4" s="72"/>
-      <c r="HS4" s="72"/>
-      <c r="HT4" s="72"/>
-      <c r="HU4" s="72"/>
-      <c r="HV4" s="72" t="s">
-        <v>173</v>
-      </c>
-      <c r="HW4" s="72"/>
-      <c r="HX4" s="72"/>
-      <c r="HY4" s="72"/>
-      <c r="HZ4" s="72"/>
-      <c r="IA4" s="72"/>
-      <c r="IB4" s="72"/>
-      <c r="IC4" s="72"/>
-      <c r="ID4" s="72"/>
-      <c r="IE4" s="72"/>
-      <c r="IF4" s="72" t="s">
-        <v>184</v>
-      </c>
-      <c r="IG4" s="72"/>
-      <c r="IH4" s="72"/>
-      <c r="II4" s="72"/>
-      <c r="IJ4" s="72"/>
-      <c r="IK4" s="72"/>
-      <c r="IL4" s="72"/>
-      <c r="IM4" s="72"/>
-      <c r="IN4" s="72"/>
-      <c r="IO4" s="72"/>
-      <c r="IP4" s="72" t="s">
-        <v>195</v>
-      </c>
-      <c r="IQ4" s="72"/>
-      <c r="IR4" s="72"/>
-      <c r="IS4" s="72"/>
-      <c r="IT4" s="72"/>
-      <c r="IU4" s="72"/>
-      <c r="IV4" s="72"/>
-      <c r="IW4" s="72"/>
-      <c r="IX4" s="72"/>
-      <c r="IY4" s="72"/>
-      <c r="IZ4" s="84" t="s">
-        <v>206</v>
-      </c>
-      <c r="JA4" s="85"/>
-      <c r="JB4" s="85"/>
-      <c r="JC4" s="85"/>
-      <c r="JD4" s="85"/>
-      <c r="JE4" s="85"/>
-      <c r="JF4" s="85"/>
-      <c r="JG4" s="85"/>
-      <c r="JH4" s="85"/>
-      <c r="JI4" s="86"/>
-      <c r="JJ4" s="84" t="s">
-        <v>217</v>
-      </c>
-      <c r="JK4" s="85"/>
-      <c r="JL4" s="85"/>
-      <c r="JM4" s="85"/>
-      <c r="JN4" s="85"/>
-      <c r="JO4" s="85"/>
-      <c r="JP4" s="85"/>
-      <c r="JQ4" s="85"/>
-      <c r="JR4" s="85"/>
-      <c r="JS4" s="86"/>
-      <c r="JT4" s="84" t="s">
-        <v>228</v>
-      </c>
-      <c r="JU4" s="85"/>
-      <c r="JV4" s="85"/>
-      <c r="JW4" s="85"/>
-      <c r="JX4" s="85"/>
-      <c r="JY4" s="85"/>
-      <c r="JZ4" s="85"/>
-      <c r="KA4" s="85"/>
-      <c r="KB4" s="85"/>
-      <c r="KC4" s="86"/>
-      <c r="KD4" s="84" t="s">
-        <v>228</v>
-      </c>
-      <c r="KE4" s="85"/>
-      <c r="KF4" s="85"/>
-      <c r="KG4" s="85"/>
-      <c r="KH4" s="85"/>
-      <c r="KI4" s="85"/>
-      <c r="KJ4" s="85"/>
-      <c r="KK4" s="85"/>
-      <c r="KL4" s="85"/>
-      <c r="KM4" s="86"/>
-      <c r="KN4" s="84" t="s">
-        <v>249</v>
-      </c>
-      <c r="KO4" s="85"/>
-      <c r="KP4" s="85"/>
-      <c r="KQ4" s="85"/>
-      <c r="KR4" s="85"/>
-      <c r="KS4" s="85"/>
-      <c r="KT4" s="85"/>
-      <c r="KU4" s="85"/>
-      <c r="KV4" s="85"/>
-      <c r="KW4" s="86"/>
-      <c r="KX4" s="87" t="s">
-        <v>260</v>
-      </c>
-      <c r="KY4" s="87"/>
-      <c r="KZ4" s="87"/>
-      <c r="LA4" s="87"/>
-      <c r="LB4" s="87"/>
-      <c r="LC4" s="87"/>
-      <c r="LD4" s="87"/>
-      <c r="LE4" s="87"/>
-      <c r="LF4" s="87"/>
-      <c r="LG4" s="87"/>
-      <c r="LH4" s="87" t="s">
-        <v>271</v>
-      </c>
-      <c r="LI4" s="87"/>
-      <c r="LJ4" s="87"/>
-      <c r="LK4" s="87"/>
-      <c r="LL4" s="87"/>
-      <c r="LM4" s="87"/>
-      <c r="LN4" s="87"/>
-      <c r="LO4" s="87"/>
-      <c r="LP4" s="87"/>
-      <c r="LQ4" s="87"/>
-      <c r="LR4" s="87" t="s">
-        <v>277</v>
-      </c>
-      <c r="LS4" s="87"/>
-      <c r="LT4" s="87"/>
-      <c r="LU4" s="87"/>
-      <c r="LV4" s="87"/>
-      <c r="LW4" s="87"/>
-      <c r="LX4" s="87"/>
-      <c r="LY4" s="87"/>
-      <c r="LZ4" s="87"/>
-      <c r="MA4" s="87"/>
-      <c r="MB4" s="87" t="s">
-        <v>288</v>
-      </c>
-      <c r="MC4" s="87"/>
-      <c r="MD4" s="87"/>
-      <c r="ME4" s="87"/>
-      <c r="MF4" s="87"/>
-      <c r="MG4" s="87"/>
-      <c r="MH4" s="87"/>
-      <c r="MI4" s="87"/>
-      <c r="MJ4" s="87"/>
-      <c r="MK4" s="87"/>
-      <c r="ML4" s="88" t="s">
+      <c r="HB4" s="63" t="s">
+        <v>411</v>
+      </c>
+      <c r="HC4" s="63"/>
+      <c r="HD4" s="63"/>
+      <c r="HE4" s="63"/>
+      <c r="HF4" s="63"/>
+      <c r="HG4" s="63"/>
+      <c r="HH4" s="63"/>
+      <c r="HI4" s="63"/>
+      <c r="HJ4" s="63"/>
+      <c r="HK4" s="63"/>
+      <c r="HL4" s="70" t="s">
+        <v>161</v>
+      </c>
+      <c r="HM4" s="70"/>
+      <c r="HN4" s="70"/>
+      <c r="HO4" s="70"/>
+      <c r="HP4" s="70"/>
+      <c r="HQ4" s="70"/>
+      <c r="HR4" s="70"/>
+      <c r="HS4" s="70"/>
+      <c r="HT4" s="70"/>
+      <c r="HU4" s="70"/>
+      <c r="HV4" s="70" t="s">
+        <v>172</v>
+      </c>
+      <c r="HW4" s="70"/>
+      <c r="HX4" s="70"/>
+      <c r="HY4" s="70"/>
+      <c r="HZ4" s="70"/>
+      <c r="IA4" s="70"/>
+      <c r="IB4" s="70"/>
+      <c r="IC4" s="70"/>
+      <c r="ID4" s="70"/>
+      <c r="IE4" s="70"/>
+      <c r="IF4" s="70" t="s">
+        <v>183</v>
+      </c>
+      <c r="IG4" s="70"/>
+      <c r="IH4" s="70"/>
+      <c r="II4" s="70"/>
+      <c r="IJ4" s="70"/>
+      <c r="IK4" s="70"/>
+      <c r="IL4" s="70"/>
+      <c r="IM4" s="70"/>
+      <c r="IN4" s="70"/>
+      <c r="IO4" s="70"/>
+      <c r="IP4" s="70" t="s">
+        <v>194</v>
+      </c>
+      <c r="IQ4" s="70"/>
+      <c r="IR4" s="70"/>
+      <c r="IS4" s="70"/>
+      <c r="IT4" s="70"/>
+      <c r="IU4" s="70"/>
+      <c r="IV4" s="70"/>
+      <c r="IW4" s="70"/>
+      <c r="IX4" s="70"/>
+      <c r="IY4" s="70"/>
+      <c r="IZ4" s="71" t="s">
+        <v>205</v>
+      </c>
+      <c r="JA4" s="72"/>
+      <c r="JB4" s="72"/>
+      <c r="JC4" s="72"/>
+      <c r="JD4" s="72"/>
+      <c r="JE4" s="72"/>
+      <c r="JF4" s="72"/>
+      <c r="JG4" s="72"/>
+      <c r="JH4" s="72"/>
+      <c r="JI4" s="73"/>
+      <c r="JJ4" s="71" t="s">
+        <v>216</v>
+      </c>
+      <c r="JK4" s="72"/>
+      <c r="JL4" s="72"/>
+      <c r="JM4" s="72"/>
+      <c r="JN4" s="72"/>
+      <c r="JO4" s="72"/>
+      <c r="JP4" s="72"/>
+      <c r="JQ4" s="72"/>
+      <c r="JR4" s="72"/>
+      <c r="JS4" s="73"/>
+      <c r="JT4" s="71" t="s">
+        <v>227</v>
+      </c>
+      <c r="JU4" s="72"/>
+      <c r="JV4" s="72"/>
+      <c r="JW4" s="72"/>
+      <c r="JX4" s="72"/>
+      <c r="JY4" s="72"/>
+      <c r="JZ4" s="72"/>
+      <c r="KA4" s="72"/>
+      <c r="KB4" s="72"/>
+      <c r="KC4" s="73"/>
+      <c r="KD4" s="71" t="s">
+        <v>227</v>
+      </c>
+      <c r="KE4" s="72"/>
+      <c r="KF4" s="72"/>
+      <c r="KG4" s="72"/>
+      <c r="KH4" s="72"/>
+      <c r="KI4" s="72"/>
+      <c r="KJ4" s="72"/>
+      <c r="KK4" s="72"/>
+      <c r="KL4" s="72"/>
+      <c r="KM4" s="73"/>
+      <c r="KN4" s="71" t="s">
+        <v>248</v>
+      </c>
+      <c r="KO4" s="72"/>
+      <c r="KP4" s="72"/>
+      <c r="KQ4" s="72"/>
+      <c r="KR4" s="72"/>
+      <c r="KS4" s="72"/>
+      <c r="KT4" s="72"/>
+      <c r="KU4" s="72"/>
+      <c r="KV4" s="72"/>
+      <c r="KW4" s="73"/>
+      <c r="KX4" s="74" t="s">
+        <v>259</v>
+      </c>
+      <c r="KY4" s="74"/>
+      <c r="KZ4" s="74"/>
+      <c r="LA4" s="74"/>
+      <c r="LB4" s="74"/>
+      <c r="LC4" s="74"/>
+      <c r="LD4" s="74"/>
+      <c r="LE4" s="74"/>
+      <c r="LF4" s="74"/>
+      <c r="LG4" s="74"/>
+      <c r="LH4" s="74" t="s">
+        <v>270</v>
+      </c>
+      <c r="LI4" s="74"/>
+      <c r="LJ4" s="74"/>
+      <c r="LK4" s="74"/>
+      <c r="LL4" s="74"/>
+      <c r="LM4" s="74"/>
+      <c r="LN4" s="74"/>
+      <c r="LO4" s="74"/>
+      <c r="LP4" s="74"/>
+      <c r="LQ4" s="74"/>
+      <c r="LR4" s="74" t="s">
+        <v>276</v>
+      </c>
+      <c r="LS4" s="74"/>
+      <c r="LT4" s="74"/>
+      <c r="LU4" s="74"/>
+      <c r="LV4" s="74"/>
+      <c r="LW4" s="74"/>
+      <c r="LX4" s="74"/>
+      <c r="LY4" s="74"/>
+      <c r="LZ4" s="74"/>
+      <c r="MA4" s="74"/>
+      <c r="MB4" s="74" t="s">
+        <v>287</v>
+      </c>
+      <c r="MC4" s="74"/>
+      <c r="MD4" s="74"/>
+      <c r="ME4" s="74"/>
+      <c r="MF4" s="74"/>
+      <c r="MG4" s="74"/>
+      <c r="MH4" s="74"/>
+      <c r="MI4" s="74"/>
+      <c r="MJ4" s="74"/>
+      <c r="MK4" s="74"/>
+      <c r="ML4" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="MM4" s="88"/>
-      <c r="MN4" s="88"/>
-      <c r="MO4" s="88"/>
-      <c r="MP4" s="88"/>
-      <c r="MQ4" s="88"/>
-      <c r="MR4" s="88"/>
-      <c r="MS4" s="88"/>
-      <c r="MT4" s="88"/>
-      <c r="MU4" s="88"/>
-      <c r="MV4" s="88"/>
-      <c r="MW4" s="88"/>
-      <c r="MX4" s="88"/>
-      <c r="MY4" s="58" t="s">
-        <v>106</v>
-      </c>
-      <c r="MZ4" s="82"/>
-      <c r="NA4" s="59"/>
+      <c r="MM4" s="75"/>
+      <c r="MN4" s="75"/>
+      <c r="MO4" s="75"/>
+      <c r="MP4" s="75"/>
+      <c r="MQ4" s="75"/>
+      <c r="MR4" s="75"/>
+      <c r="MS4" s="75"/>
+      <c r="MT4" s="75"/>
+      <c r="MU4" s="75"/>
+      <c r="MV4" s="75"/>
+      <c r="MW4" s="75"/>
+      <c r="MX4" s="75"/>
+      <c r="MY4" s="64" t="s">
+        <v>105</v>
+      </c>
+      <c r="MZ4" s="65"/>
+      <c r="NA4" s="66"/>
       <c r="NB4" s="38"/>
-      <c r="NC4" s="58" t="s">
-        <v>110</v>
-      </c>
-      <c r="ND4" s="59"/>
+      <c r="NC4" s="64" t="s">
+        <v>109</v>
+      </c>
+      <c r="ND4" s="66"/>
       <c r="NE4" s="56"/>
       <c r="NF4" s="54"/>
     </row>
     <row r="5" spans="1:370" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="65"/>
-      <c r="B5" s="65"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="67"/>
-      <c r="J5" s="67"/>
-      <c r="K5" s="67"/>
-      <c r="L5" s="67"/>
-      <c r="M5" s="67"/>
-      <c r="N5" s="68"/>
-      <c r="O5" s="68"/>
-      <c r="P5" s="68"/>
-      <c r="Q5" s="69"/>
-      <c r="R5" s="69"/>
-      <c r="S5" s="69"/>
-      <c r="T5" s="69"/>
-      <c r="U5" s="69"/>
-      <c r="V5" s="70"/>
-      <c r="W5" s="70"/>
-      <c r="X5" s="70"/>
-      <c r="Y5" s="70"/>
-      <c r="Z5" s="70"/>
-      <c r="AA5" s="70"/>
-      <c r="AB5" s="70"/>
-      <c r="AC5" s="71"/>
-      <c r="AD5" s="71"/>
-      <c r="AE5" s="71"/>
-      <c r="AF5" s="62"/>
-      <c r="AG5" s="62"/>
-      <c r="AH5" s="73"/>
-      <c r="AI5" s="73"/>
-      <c r="AJ5" s="73"/>
-      <c r="AK5" s="73"/>
-      <c r="AL5" s="73"/>
-      <c r="AM5" s="74"/>
-      <c r="AN5" s="74"/>
-      <c r="AO5" s="74"/>
-      <c r="AP5" s="74"/>
-      <c r="AQ5" s="74"/>
-      <c r="AR5" s="74"/>
-      <c r="AS5" s="74"/>
-      <c r="AT5" s="74"/>
-      <c r="AU5" s="74"/>
-      <c r="AV5" s="74"/>
-      <c r="AW5" s="74"/>
-      <c r="AX5" s="74"/>
-      <c r="AY5" s="74"/>
-      <c r="AZ5" s="74"/>
-      <c r="BA5" s="74"/>
-      <c r="BB5" s="74"/>
-      <c r="BC5" s="74"/>
-      <c r="BD5" s="74"/>
-      <c r="BE5" s="74"/>
-      <c r="BF5" s="74"/>
-      <c r="BG5" s="74"/>
-      <c r="BH5" s="74"/>
-      <c r="BI5" s="74"/>
-      <c r="BJ5" s="74"/>
-      <c r="BK5" s="74"/>
-      <c r="BL5" s="74"/>
-      <c r="BM5" s="74"/>
-      <c r="BN5" s="74"/>
-      <c r="BO5" s="74"/>
-      <c r="BP5" s="74"/>
-      <c r="BQ5" s="74"/>
+      <c r="A5" s="84"/>
+      <c r="B5" s="84"/>
+      <c r="C5" s="85"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="85"/>
+      <c r="H5" s="85"/>
+      <c r="I5" s="86"/>
+      <c r="J5" s="86"/>
+      <c r="K5" s="86"/>
+      <c r="L5" s="86"/>
+      <c r="M5" s="86"/>
+      <c r="N5" s="87"/>
+      <c r="O5" s="87"/>
+      <c r="P5" s="87"/>
+      <c r="Q5" s="88"/>
+      <c r="R5" s="88"/>
+      <c r="S5" s="88"/>
+      <c r="T5" s="88"/>
+      <c r="U5" s="88"/>
+      <c r="V5" s="89"/>
+      <c r="W5" s="89"/>
+      <c r="X5" s="89"/>
+      <c r="Y5" s="89"/>
+      <c r="Z5" s="89"/>
+      <c r="AA5" s="89"/>
+      <c r="AB5" s="89"/>
+      <c r="AC5" s="90"/>
+      <c r="AD5" s="90"/>
+      <c r="AE5" s="90"/>
+      <c r="AF5" s="81"/>
+      <c r="AG5" s="81"/>
+      <c r="AH5" s="91"/>
+      <c r="AI5" s="91"/>
+      <c r="AJ5" s="91"/>
+      <c r="AK5" s="91"/>
+      <c r="AL5" s="91"/>
+      <c r="AM5" s="92"/>
+      <c r="AN5" s="92"/>
+      <c r="AO5" s="92"/>
+      <c r="AP5" s="92"/>
+      <c r="AQ5" s="92"/>
+      <c r="AR5" s="92"/>
+      <c r="AS5" s="92"/>
+      <c r="AT5" s="92"/>
+      <c r="AU5" s="92"/>
+      <c r="AV5" s="92"/>
+      <c r="AW5" s="92"/>
+      <c r="AX5" s="92"/>
+      <c r="AY5" s="92"/>
+      <c r="AZ5" s="92"/>
+      <c r="BA5" s="92"/>
+      <c r="BB5" s="92"/>
+      <c r="BC5" s="92"/>
+      <c r="BD5" s="92"/>
+      <c r="BE5" s="92"/>
+      <c r="BF5" s="92"/>
+      <c r="BG5" s="92"/>
+      <c r="BH5" s="92"/>
+      <c r="BI5" s="92"/>
+      <c r="BJ5" s="92"/>
+      <c r="BK5" s="92"/>
+      <c r="BL5" s="92"/>
+      <c r="BM5" s="92"/>
+      <c r="BN5" s="92"/>
+      <c r="BO5" s="92"/>
+      <c r="BP5" s="92"/>
+      <c r="BQ5" s="92"/>
       <c r="BR5" s="7" t="s">
         <v>19</v>
       </c>
@@ -4812,25 +4812,25 @@
       <c r="MK5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="ML5" s="88"/>
-      <c r="MM5" s="88"/>
-      <c r="MN5" s="88"/>
-      <c r="MO5" s="88"/>
-      <c r="MP5" s="88"/>
-      <c r="MQ5" s="88"/>
-      <c r="MR5" s="88"/>
-      <c r="MS5" s="88"/>
-      <c r="MT5" s="88"/>
-      <c r="MU5" s="88"/>
-      <c r="MV5" s="88"/>
-      <c r="MW5" s="88"/>
-      <c r="MX5" s="88"/>
-      <c r="MY5" s="60"/>
-      <c r="MZ5" s="83"/>
-      <c r="NA5" s="61"/>
+      <c r="ML5" s="75"/>
+      <c r="MM5" s="75"/>
+      <c r="MN5" s="75"/>
+      <c r="MO5" s="75"/>
+      <c r="MP5" s="75"/>
+      <c r="MQ5" s="75"/>
+      <c r="MR5" s="75"/>
+      <c r="MS5" s="75"/>
+      <c r="MT5" s="75"/>
+      <c r="MU5" s="75"/>
+      <c r="MV5" s="75"/>
+      <c r="MW5" s="75"/>
+      <c r="MX5" s="75"/>
+      <c r="MY5" s="67"/>
+      <c r="MZ5" s="68"/>
+      <c r="NA5" s="69"/>
       <c r="NB5" s="38"/>
-      <c r="NC5" s="60"/>
-      <c r="ND5" s="61"/>
+      <c r="NC5" s="67"/>
+      <c r="ND5" s="69"/>
       <c r="NE5" s="57"/>
       <c r="NF5" s="55"/>
     </row>
@@ -4863,10 +4863,10 @@
         <v>31</v>
       </c>
       <c r="J6" s="9" t="s">
+        <v>414</v>
+      </c>
+      <c r="K6" s="9" t="s">
         <v>415</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>416</v>
       </c>
       <c r="L6" s="9" t="s">
         <v>32</v>
@@ -4929,7 +4929,7 @@
         <v>51</v>
       </c>
       <c r="AF6" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AG6" s="16" t="s">
         <v>52</v>
@@ -4938,7 +4938,7 @@
         <v>53</v>
       </c>
       <c r="AI6" s="17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AJ6" s="17" t="s">
         <v>54</v>
@@ -4956,31 +4956,31 @@
         <v>58</v>
       </c>
       <c r="AO6" s="18" t="s">
+        <v>394</v>
+      </c>
+      <c r="AP6" s="18" t="s">
         <v>395</v>
       </c>
-      <c r="AP6" s="18" t="s">
+      <c r="AQ6" s="18" t="s">
         <v>396</v>
       </c>
-      <c r="AQ6" s="18" t="s">
+      <c r="AR6" s="18" t="s">
         <v>397</v>
       </c>
-      <c r="AR6" s="18" t="s">
+      <c r="AS6" s="18" t="s">
         <v>398</v>
       </c>
-      <c r="AS6" s="18" t="s">
+      <c r="AT6" s="18" t="s">
         <v>399</v>
       </c>
-      <c r="AT6" s="18" t="s">
+      <c r="AU6" s="18" t="s">
         <v>400</v>
-      </c>
-      <c r="AU6" s="18" t="s">
-        <v>401</v>
       </c>
       <c r="AV6" s="18" t="s">
         <v>59</v>
       </c>
       <c r="AW6" s="18" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="AX6" s="18" t="s">
         <v>60</v>
@@ -4992,46 +4992,46 @@
         <v>62</v>
       </c>
       <c r="BA6" s="18" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="BB6" s="18" t="s">
+        <v>303</v>
+      </c>
+      <c r="BC6" s="18" t="s">
         <v>304</v>
       </c>
-      <c r="BC6" s="18" t="s">
+      <c r="BD6" s="18" t="s">
         <v>305</v>
       </c>
-      <c r="BD6" s="18" t="s">
+      <c r="BE6" s="18" t="s">
         <v>306</v>
       </c>
-      <c r="BE6" s="18" t="s">
+      <c r="BF6" s="18" t="s">
         <v>307</v>
       </c>
-      <c r="BF6" s="18" t="s">
+      <c r="BG6" s="18" t="s">
         <v>308</v>
       </c>
-      <c r="BG6" s="18" t="s">
+      <c r="BH6" s="18" t="s">
         <v>309</v>
       </c>
-      <c r="BH6" s="18" t="s">
+      <c r="BI6" s="18" t="s">
         <v>310</v>
       </c>
-      <c r="BI6" s="18" t="s">
+      <c r="BJ6" s="18" t="s">
         <v>311</v>
       </c>
-      <c r="BJ6" s="18" t="s">
+      <c r="BK6" s="18" t="s">
         <v>312</v>
       </c>
-      <c r="BK6" s="18" t="s">
+      <c r="BL6" s="18" t="s">
         <v>313</v>
       </c>
-      <c r="BL6" s="18" t="s">
+      <c r="BM6" s="18" t="s">
         <v>314</v>
       </c>
-      <c r="BM6" s="18" t="s">
+      <c r="BN6" s="18" t="s">
         <v>315</v>
-      </c>
-      <c r="BN6" s="18" t="s">
-        <v>316</v>
       </c>
       <c r="BO6" s="18" t="s">
         <v>63</v>
@@ -5055,22 +5055,22 @@
         <v>69</v>
       </c>
       <c r="BV6" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="BW6" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="BW6" s="18" t="s">
+      <c r="BX6" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="BX6" s="18" t="s">
+      <c r="BY6" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="BY6" s="18" t="s">
+      <c r="BZ6" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="BZ6" s="18" t="s">
+      <c r="CA6" s="18" t="s">
         <v>121</v>
-      </c>
-      <c r="CA6" s="18" t="s">
-        <v>122</v>
       </c>
       <c r="CB6" s="18" t="s">
         <v>70</v>
@@ -5085,232 +5085,232 @@
         <v>73</v>
       </c>
       <c r="CF6" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="CG6" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="CG6" s="18" t="s">
+      <c r="CH6" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="CH6" s="18" t="s">
+      <c r="CI6" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="CI6" s="18" t="s">
+      <c r="CJ6" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="CJ6" s="18" t="s">
+      <c r="CK6" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="CK6" s="18" t="s">
-        <v>128</v>
-      </c>
       <c r="CL6" s="18" t="s">
+        <v>321</v>
+      </c>
+      <c r="CM6" s="18" t="s">
         <v>322</v>
       </c>
-      <c r="CM6" s="18" t="s">
+      <c r="CN6" s="18" t="s">
         <v>323</v>
       </c>
-      <c r="CN6" s="18" t="s">
+      <c r="CO6" s="18" t="s">
         <v>324</v>
       </c>
-      <c r="CO6" s="18" t="s">
+      <c r="CP6" s="18" t="s">
         <v>325</v>
       </c>
-      <c r="CP6" s="18" t="s">
+      <c r="CQ6" s="18" t="s">
         <v>326</v>
       </c>
-      <c r="CQ6" s="18" t="s">
+      <c r="CR6" s="18" t="s">
         <v>327</v>
       </c>
-      <c r="CR6" s="18" t="s">
+      <c r="CS6" s="18" t="s">
         <v>328</v>
       </c>
-      <c r="CS6" s="18" t="s">
+      <c r="CT6" s="18" t="s">
         <v>329</v>
       </c>
-      <c r="CT6" s="18" t="s">
+      <c r="CU6" s="18" t="s">
         <v>330</v>
       </c>
-      <c r="CU6" s="18" t="s">
+      <c r="CV6" s="18" t="s">
         <v>331</v>
       </c>
-      <c r="CV6" s="18" t="s">
+      <c r="CW6" s="18" t="s">
         <v>332</v>
       </c>
-      <c r="CW6" s="18" t="s">
+      <c r="CX6" s="18" t="s">
         <v>333</v>
       </c>
-      <c r="CX6" s="18" t="s">
+      <c r="CY6" s="18" t="s">
         <v>334</v>
       </c>
-      <c r="CY6" s="18" t="s">
+      <c r="CZ6" s="18" t="s">
         <v>335</v>
       </c>
-      <c r="CZ6" s="18" t="s">
+      <c r="DA6" s="18" t="s">
         <v>336</v>
       </c>
-      <c r="DA6" s="18" t="s">
+      <c r="DB6" s="18" t="s">
         <v>337</v>
       </c>
-      <c r="DB6" s="18" t="s">
+      <c r="DC6" s="18" t="s">
         <v>338</v>
       </c>
-      <c r="DC6" s="18" t="s">
+      <c r="DD6" s="18" t="s">
         <v>339</v>
       </c>
-      <c r="DD6" s="18" t="s">
+      <c r="DE6" s="18" t="s">
         <v>340</v>
       </c>
-      <c r="DE6" s="18" t="s">
+      <c r="DF6" s="18" t="s">
         <v>341</v>
       </c>
-      <c r="DF6" s="18" t="s">
+      <c r="DG6" s="18" t="s">
         <v>342</v>
       </c>
-      <c r="DG6" s="18" t="s">
+      <c r="DH6" s="18" t="s">
         <v>343</v>
       </c>
-      <c r="DH6" s="18" t="s">
+      <c r="DI6" s="18" t="s">
         <v>344</v>
       </c>
-      <c r="DI6" s="18" t="s">
+      <c r="DJ6" s="18" t="s">
         <v>345</v>
       </c>
-      <c r="DJ6" s="18" t="s">
+      <c r="DK6" s="18" t="s">
         <v>346</v>
       </c>
-      <c r="DK6" s="18" t="s">
+      <c r="DL6" s="18" t="s">
         <v>347</v>
       </c>
-      <c r="DL6" s="18" t="s">
+      <c r="DM6" s="18" t="s">
         <v>348</v>
       </c>
-      <c r="DM6" s="18" t="s">
+      <c r="DN6" s="18" t="s">
         <v>349</v>
       </c>
-      <c r="DN6" s="18" t="s">
+      <c r="DO6" s="18" t="s">
         <v>350</v>
       </c>
-      <c r="DO6" s="18" t="s">
+      <c r="DP6" s="18" t="s">
         <v>351</v>
       </c>
-      <c r="DP6" s="18" t="s">
+      <c r="DQ6" s="18" t="s">
         <v>352</v>
       </c>
-      <c r="DQ6" s="18" t="s">
+      <c r="DR6" s="18" t="s">
         <v>353</v>
       </c>
-      <c r="DR6" s="18" t="s">
+      <c r="DS6" s="18" t="s">
         <v>354</v>
       </c>
-      <c r="DS6" s="18" t="s">
+      <c r="DT6" s="18" t="s">
         <v>355</v>
       </c>
-      <c r="DT6" s="18" t="s">
+      <c r="DU6" s="18" t="s">
         <v>356</v>
       </c>
-      <c r="DU6" s="18" t="s">
+      <c r="DV6" s="18" t="s">
         <v>357</v>
       </c>
-      <c r="DV6" s="18" t="s">
+      <c r="DW6" s="18" t="s">
         <v>358</v>
       </c>
-      <c r="DW6" s="18" t="s">
+      <c r="DX6" s="18" t="s">
         <v>359</v>
       </c>
-      <c r="DX6" s="18" t="s">
+      <c r="DY6" s="18" t="s">
         <v>360</v>
       </c>
-      <c r="DY6" s="18" t="s">
-        <v>361</v>
-      </c>
       <c r="DZ6" s="18" t="s">
+        <v>362</v>
+      </c>
+      <c r="EA6" s="18" t="s">
         <v>363</v>
       </c>
-      <c r="EA6" s="18" t="s">
+      <c r="EB6" s="18" t="s">
         <v>364</v>
       </c>
-      <c r="EB6" s="18" t="s">
+      <c r="EC6" s="18" t="s">
         <v>365</v>
       </c>
-      <c r="EC6" s="18" t="s">
+      <c r="ED6" s="18" t="s">
         <v>366</v>
       </c>
-      <c r="ED6" s="18" t="s">
+      <c r="EE6" s="18" t="s">
         <v>367</v>
       </c>
-      <c r="EE6" s="18" t="s">
+      <c r="EF6" s="18" t="s">
         <v>368</v>
       </c>
-      <c r="EF6" s="18" t="s">
+      <c r="EG6" s="18" t="s">
         <v>369</v>
       </c>
-      <c r="EG6" s="18" t="s">
+      <c r="EH6" s="18" t="s">
         <v>370</v>
       </c>
-      <c r="EH6" s="18" t="s">
+      <c r="EI6" s="18" t="s">
         <v>371</v>
       </c>
-      <c r="EI6" s="18" t="s">
-        <v>372</v>
-      </c>
       <c r="EJ6" s="18" t="s">
+        <v>373</v>
+      </c>
+      <c r="EK6" s="18" t="s">
         <v>374</v>
       </c>
-      <c r="EK6" s="18" t="s">
+      <c r="EL6" s="18" t="s">
         <v>375</v>
       </c>
-      <c r="EL6" s="18" t="s">
+      <c r="EM6" s="18" t="s">
         <v>376</v>
       </c>
-      <c r="EM6" s="18" t="s">
+      <c r="EN6" s="18" t="s">
         <v>377</v>
       </c>
-      <c r="EN6" s="18" t="s">
+      <c r="EO6" s="18" t="s">
         <v>378</v>
       </c>
-      <c r="EO6" s="18" t="s">
+      <c r="EP6" s="18" t="s">
         <v>379</v>
       </c>
-      <c r="EP6" s="18" t="s">
+      <c r="EQ6" s="18" t="s">
         <v>380</v>
       </c>
-      <c r="EQ6" s="18" t="s">
+      <c r="ER6" s="18" t="s">
         <v>381</v>
       </c>
-      <c r="ER6" s="18" t="s">
+      <c r="ES6" s="18" t="s">
         <v>382</v>
       </c>
-      <c r="ES6" s="18" t="s">
-        <v>383</v>
-      </c>
       <c r="ET6" s="18" t="s">
+        <v>384</v>
+      </c>
+      <c r="EU6" s="18" t="s">
         <v>385</v>
       </c>
-      <c r="EU6" s="18" t="s">
+      <c r="EV6" s="18" t="s">
         <v>386</v>
       </c>
-      <c r="EV6" s="18" t="s">
+      <c r="EW6" s="18" t="s">
         <v>387</v>
       </c>
-      <c r="EW6" s="18" t="s">
+      <c r="EX6" s="18" t="s">
         <v>388</v>
       </c>
-      <c r="EX6" s="18" t="s">
+      <c r="EY6" s="18" t="s">
         <v>389</v>
       </c>
-      <c r="EY6" s="18" t="s">
+      <c r="EZ6" s="18" t="s">
         <v>390</v>
       </c>
-      <c r="EZ6" s="18" t="s">
+      <c r="FA6" s="18" t="s">
         <v>391</v>
       </c>
-      <c r="FA6" s="18" t="s">
+      <c r="FB6" s="18" t="s">
         <v>392</v>
       </c>
-      <c r="FB6" s="18" t="s">
+      <c r="FC6" s="18" t="s">
         <v>393</v>
-      </c>
-      <c r="FC6" s="18" t="s">
-        <v>394</v>
       </c>
       <c r="FD6" s="18" t="s">
         <v>74</v>
@@ -5325,22 +5325,22 @@
         <v>77</v>
       </c>
       <c r="FH6" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="FI6" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="FI6" s="18" t="s">
+      <c r="FJ6" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="FJ6" s="18" t="s">
+      <c r="FK6" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="FK6" s="18" t="s">
+      <c r="FL6" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="FL6" s="18" t="s">
+      <c r="FM6" s="18" t="s">
         <v>133</v>
-      </c>
-      <c r="FM6" s="18" t="s">
-        <v>134</v>
       </c>
       <c r="FN6" s="18" t="s">
         <v>78</v>
@@ -5355,22 +5355,22 @@
         <v>81</v>
       </c>
       <c r="FR6" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="FS6" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="FS6" s="18" t="s">
+      <c r="FT6" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="FT6" s="18" t="s">
+      <c r="FU6" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="FU6" s="18" t="s">
+      <c r="FV6" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="FV6" s="18" t="s">
+      <c r="FW6" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="FW6" s="18" t="s">
-        <v>140</v>
       </c>
       <c r="FX6" s="9" t="s">
         <v>82</v>
@@ -5385,22 +5385,22 @@
         <v>85</v>
       </c>
       <c r="GB6" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="GC6" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="GC6" s="9" t="s">
+      <c r="GD6" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="GD6" s="9" t="s">
+      <c r="GE6" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="GE6" s="9" t="s">
+      <c r="GF6" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="GF6" s="9" t="s">
+      <c r="GG6" s="9" t="s">
         <v>145</v>
-      </c>
-      <c r="GG6" s="9" t="s">
-        <v>146</v>
       </c>
       <c r="GH6" s="9" t="s">
         <v>86</v>
@@ -5415,22 +5415,22 @@
         <v>89</v>
       </c>
       <c r="GL6" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="GM6" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="GM6" s="9" t="s">
+      <c r="GN6" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="GN6" s="9" t="s">
+      <c r="GO6" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="GO6" s="9" t="s">
+      <c r="GP6" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="GP6" s="9" t="s">
+      <c r="GQ6" s="9" t="s">
         <v>151</v>
-      </c>
-      <c r="GQ6" s="9" t="s">
-        <v>152</v>
       </c>
       <c r="GR6" s="9" t="s">
         <v>90</v>
@@ -5445,442 +5445,442 @@
         <v>93</v>
       </c>
       <c r="GV6" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="GW6" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="GW6" s="9" t="s">
+      <c r="GX6" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="GX6" s="9" t="s">
+      <c r="GY6" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="GY6" s="9" t="s">
+      <c r="GZ6" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="GZ6" s="9" t="s">
+      <c r="HA6" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="HA6" s="9" t="s">
-        <v>158</v>
-      </c>
       <c r="HB6" s="18" t="s">
+        <v>401</v>
+      </c>
+      <c r="HC6" s="18" t="s">
         <v>402</v>
       </c>
-      <c r="HC6" s="18" t="s">
+      <c r="HD6" s="18" t="s">
         <v>403</v>
       </c>
-      <c r="HD6" s="18" t="s">
+      <c r="HE6" s="18" t="s">
         <v>404</v>
       </c>
-      <c r="HE6" s="18" t="s">
+      <c r="HF6" s="18" t="s">
         <v>405</v>
       </c>
-      <c r="HF6" s="18" t="s">
+      <c r="HG6" s="18" t="s">
         <v>406</v>
       </c>
-      <c r="HG6" s="18" t="s">
+      <c r="HH6" s="18" t="s">
         <v>407</v>
       </c>
-      <c r="HH6" s="18" t="s">
+      <c r="HI6" s="18" t="s">
         <v>408</v>
       </c>
-      <c r="HI6" s="18" t="s">
+      <c r="HJ6" s="18" t="s">
         <v>409</v>
       </c>
-      <c r="HJ6" s="18" t="s">
+      <c r="HK6" s="18" t="s">
         <v>410</v>
       </c>
-      <c r="HK6" s="18" t="s">
-        <v>411</v>
-      </c>
       <c r="HL6" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="HM6" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="HM6" s="18" t="s">
+      <c r="HN6" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="HN6" s="18" t="s">
+      <c r="HO6" s="18" t="s">
         <v>165</v>
       </c>
-      <c r="HO6" s="18" t="s">
+      <c r="HP6" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="HP6" s="18" t="s">
+      <c r="HQ6" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="HQ6" s="18" t="s">
+      <c r="HR6" s="18" t="s">
         <v>168</v>
       </c>
-      <c r="HR6" s="18" t="s">
+      <c r="HS6" s="18" t="s">
         <v>169</v>
       </c>
-      <c r="HS6" s="18" t="s">
+      <c r="HT6" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="HT6" s="18" t="s">
+      <c r="HU6" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="HU6" s="18" t="s">
-        <v>172</v>
-      </c>
       <c r="HV6" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="HW6" s="18" t="s">
         <v>174</v>
       </c>
-      <c r="HW6" s="18" t="s">
+      <c r="HX6" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="HX6" s="18" t="s">
+      <c r="HY6" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="HY6" s="18" t="s">
+      <c r="HZ6" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="HZ6" s="18" t="s">
+      <c r="IA6" s="18" t="s">
         <v>178</v>
       </c>
-      <c r="IA6" s="18" t="s">
+      <c r="IB6" s="18" t="s">
         <v>179</v>
       </c>
-      <c r="IB6" s="18" t="s">
+      <c r="IC6" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="IC6" s="18" t="s">
+      <c r="ID6" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="ID6" s="18" t="s">
+      <c r="IE6" s="18" t="s">
         <v>182</v>
       </c>
-      <c r="IE6" s="18" t="s">
-        <v>183</v>
-      </c>
       <c r="IF6" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="IG6" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="IG6" s="18" t="s">
+      <c r="IH6" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="IH6" s="18" t="s">
+      <c r="II6" s="18" t="s">
         <v>187</v>
       </c>
-      <c r="II6" s="18" t="s">
+      <c r="IJ6" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="IJ6" s="18" t="s">
+      <c r="IK6" s="18" t="s">
         <v>189</v>
       </c>
-      <c r="IK6" s="18" t="s">
+      <c r="IL6" s="18" t="s">
         <v>190</v>
       </c>
-      <c r="IL6" s="18" t="s">
+      <c r="IM6" s="18" t="s">
         <v>191</v>
       </c>
-      <c r="IM6" s="18" t="s">
+      <c r="IN6" s="18" t="s">
         <v>192</v>
       </c>
-      <c r="IN6" s="18" t="s">
+      <c r="IO6" s="18" t="s">
         <v>193</v>
       </c>
-      <c r="IO6" s="18" t="s">
-        <v>194</v>
-      </c>
       <c r="IP6" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="IQ6" s="18" t="s">
         <v>196</v>
       </c>
-      <c r="IQ6" s="18" t="s">
+      <c r="IR6" s="18" t="s">
         <v>197</v>
       </c>
-      <c r="IR6" s="18" t="s">
+      <c r="IS6" s="18" t="s">
         <v>198</v>
       </c>
-      <c r="IS6" s="18" t="s">
+      <c r="IT6" s="18" t="s">
         <v>199</v>
       </c>
-      <c r="IT6" s="18" t="s">
+      <c r="IU6" s="18" t="s">
         <v>200</v>
       </c>
-      <c r="IU6" s="18" t="s">
+      <c r="IV6" s="18" t="s">
         <v>201</v>
       </c>
-      <c r="IV6" s="18" t="s">
+      <c r="IW6" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="IW6" s="18" t="s">
+      <c r="IX6" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="IX6" s="18" t="s">
+      <c r="IY6" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="IY6" s="18" t="s">
-        <v>205</v>
-      </c>
       <c r="IZ6" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="JA6" s="18" t="s">
         <v>207</v>
       </c>
-      <c r="JA6" s="18" t="s">
+      <c r="JB6" s="18" t="s">
         <v>208</v>
       </c>
-      <c r="JB6" s="18" t="s">
+      <c r="JC6" s="18" t="s">
         <v>209</v>
       </c>
-      <c r="JC6" s="18" t="s">
+      <c r="JD6" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="JD6" s="18" t="s">
+      <c r="JE6" s="18" t="s">
         <v>211</v>
       </c>
-      <c r="JE6" s="18" t="s">
+      <c r="JF6" s="18" t="s">
         <v>212</v>
       </c>
-      <c r="JF6" s="18" t="s">
+      <c r="JG6" s="18" t="s">
         <v>213</v>
       </c>
-      <c r="JG6" s="18" t="s">
+      <c r="JH6" s="18" t="s">
         <v>214</v>
       </c>
-      <c r="JH6" s="18" t="s">
+      <c r="JI6" s="18" t="s">
         <v>215</v>
       </c>
-      <c r="JI6" s="18" t="s">
-        <v>216</v>
-      </c>
       <c r="JJ6" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="JK6" s="18" t="s">
         <v>218</v>
       </c>
-      <c r="JK6" s="18" t="s">
+      <c r="JL6" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="JL6" s="18" t="s">
+      <c r="JM6" s="18" t="s">
         <v>220</v>
       </c>
-      <c r="JM6" s="18" t="s">
+      <c r="JN6" s="18" t="s">
         <v>221</v>
       </c>
-      <c r="JN6" s="18" t="s">
+      <c r="JO6" s="18" t="s">
         <v>222</v>
       </c>
-      <c r="JO6" s="18" t="s">
+      <c r="JP6" s="18" t="s">
         <v>223</v>
       </c>
-      <c r="JP6" s="18" t="s">
+      <c r="JQ6" s="18" t="s">
         <v>224</v>
       </c>
-      <c r="JQ6" s="18" t="s">
+      <c r="JR6" s="18" t="s">
         <v>225</v>
       </c>
-      <c r="JR6" s="18" t="s">
+      <c r="JS6" s="18" t="s">
         <v>226</v>
       </c>
-      <c r="JS6" s="18" t="s">
-        <v>227</v>
-      </c>
       <c r="JT6" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="JU6" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="JV6" s="18" t="s">
         <v>230</v>
       </c>
-      <c r="JU6" s="18" t="s">
-        <v>229</v>
-      </c>
-      <c r="JV6" s="18" t="s">
+      <c r="JW6" s="18" t="s">
         <v>231</v>
       </c>
-      <c r="JW6" s="18" t="s">
+      <c r="JX6" s="18" t="s">
         <v>232</v>
       </c>
-      <c r="JX6" s="18" t="s">
+      <c r="JY6" s="18" t="s">
         <v>233</v>
       </c>
-      <c r="JY6" s="18" t="s">
+      <c r="JZ6" s="18" t="s">
         <v>234</v>
       </c>
-      <c r="JZ6" s="18" t="s">
+      <c r="KA6" s="18" t="s">
         <v>235</v>
       </c>
-      <c r="KA6" s="18" t="s">
+      <c r="KB6" s="18" t="s">
         <v>236</v>
       </c>
-      <c r="KB6" s="18" t="s">
+      <c r="KC6" s="18" t="s">
         <v>237</v>
       </c>
-      <c r="KC6" s="18" t="s">
+      <c r="KD6" s="18" t="s">
         <v>238</v>
       </c>
-      <c r="KD6" s="18" t="s">
+      <c r="KE6" s="18" t="s">
         <v>239</v>
       </c>
-      <c r="KE6" s="18" t="s">
+      <c r="KF6" s="18" t="s">
         <v>240</v>
       </c>
-      <c r="KF6" s="18" t="s">
+      <c r="KG6" s="18" t="s">
         <v>241</v>
       </c>
-      <c r="KG6" s="18" t="s">
+      <c r="KH6" s="18" t="s">
         <v>242</v>
       </c>
-      <c r="KH6" s="18" t="s">
+      <c r="KI6" s="18" t="s">
         <v>243</v>
       </c>
-      <c r="KI6" s="18" t="s">
+      <c r="KJ6" s="18" t="s">
         <v>244</v>
       </c>
-      <c r="KJ6" s="18" t="s">
+      <c r="KK6" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="KK6" s="18" t="s">
+      <c r="KL6" s="18" t="s">
         <v>246</v>
       </c>
-      <c r="KL6" s="18" t="s">
+      <c r="KM6" s="18" t="s">
         <v>247</v>
       </c>
-      <c r="KM6" s="18" t="s">
-        <v>248</v>
-      </c>
       <c r="KN6" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="KO6" s="18" t="s">
         <v>250</v>
       </c>
-      <c r="KO6" s="18" t="s">
+      <c r="KP6" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="KP6" s="18" t="s">
+      <c r="KQ6" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="KQ6" s="18" t="s">
+      <c r="KR6" s="18" t="s">
         <v>253</v>
       </c>
-      <c r="KR6" s="18" t="s">
+      <c r="KS6" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="KS6" s="18" t="s">
+      <c r="KT6" s="18" t="s">
         <v>255</v>
       </c>
-      <c r="KT6" s="18" t="s">
+      <c r="KU6" s="18" t="s">
         <v>256</v>
       </c>
-      <c r="KU6" s="18" t="s">
+      <c r="KV6" s="18" t="s">
         <v>257</v>
       </c>
-      <c r="KV6" s="18" t="s">
+      <c r="KW6" s="18" t="s">
         <v>258</v>
       </c>
-      <c r="KW6" s="18" t="s">
-        <v>259</v>
-      </c>
       <c r="KX6" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="KY6" s="18" t="s">
         <v>261</v>
       </c>
-      <c r="KY6" s="18" t="s">
+      <c r="KZ6" s="18" t="s">
         <v>262</v>
       </c>
-      <c r="KZ6" s="18" t="s">
+      <c r="LA6" s="18" t="s">
         <v>263</v>
       </c>
-      <c r="LA6" s="18" t="s">
+      <c r="LB6" s="18" t="s">
         <v>264</v>
       </c>
-      <c r="LB6" s="18" t="s">
+      <c r="LC6" s="18" t="s">
         <v>265</v>
       </c>
-      <c r="LC6" s="18" t="s">
+      <c r="LD6" s="18" t="s">
         <v>266</v>
       </c>
-      <c r="LD6" s="18" t="s">
+      <c r="LE6" s="18" t="s">
         <v>267</v>
       </c>
-      <c r="LE6" s="18" t="s">
+      <c r="LF6" s="18" t="s">
         <v>268</v>
       </c>
-      <c r="LF6" s="18" t="s">
+      <c r="LG6" s="18" t="s">
         <v>269</v>
       </c>
-      <c r="LG6" s="18" t="s">
-        <v>270</v>
-      </c>
       <c r="LH6" s="18" t="s">
+        <v>271</v>
+      </c>
+      <c r="LI6" s="18" t="s">
         <v>272</v>
       </c>
-      <c r="LI6" s="18" t="s">
+      <c r="LJ6" s="18" t="s">
         <v>273</v>
       </c>
-      <c r="LJ6" s="18" t="s">
+      <c r="LK6" s="18" t="s">
         <v>274</v>
       </c>
-      <c r="LK6" s="18" t="s">
+      <c r="LL6" s="18" t="s">
         <v>275</v>
       </c>
-      <c r="LL6" s="18" t="s">
-        <v>276</v>
-      </c>
       <c r="LM6" s="18" t="s">
+        <v>298</v>
+      </c>
+      <c r="LN6" s="18" t="s">
         <v>299</v>
       </c>
-      <c r="LN6" s="18" t="s">
+      <c r="LO6" s="18" t="s">
         <v>300</v>
       </c>
-      <c r="LO6" s="18" t="s">
+      <c r="LP6" s="18" t="s">
         <v>301</v>
       </c>
-      <c r="LP6" s="18" t="s">
+      <c r="LQ6" s="18" t="s">
         <v>302</v>
       </c>
-      <c r="LQ6" s="18" t="s">
-        <v>303</v>
-      </c>
       <c r="LR6" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="LS6" s="18" t="s">
         <v>278</v>
       </c>
-      <c r="LS6" s="18" t="s">
+      <c r="LT6" s="18" t="s">
         <v>279</v>
       </c>
-      <c r="LT6" s="18" t="s">
+      <c r="LU6" s="18" t="s">
         <v>280</v>
       </c>
-      <c r="LU6" s="18" t="s">
+      <c r="LV6" s="18" t="s">
         <v>281</v>
       </c>
-      <c r="LV6" s="18" t="s">
+      <c r="LW6" s="18" t="s">
         <v>282</v>
       </c>
-      <c r="LW6" s="18" t="s">
+      <c r="LX6" s="18" t="s">
         <v>283</v>
       </c>
-      <c r="LX6" s="18" t="s">
+      <c r="LY6" s="18" t="s">
         <v>284</v>
       </c>
-      <c r="LY6" s="18" t="s">
+      <c r="LZ6" s="18" t="s">
         <v>285</v>
       </c>
-      <c r="LZ6" s="18" t="s">
+      <c r="MA6" s="18" t="s">
         <v>286</v>
       </c>
-      <c r="MA6" s="18" t="s">
-        <v>287</v>
-      </c>
       <c r="MB6" s="18" t="s">
+        <v>288</v>
+      </c>
+      <c r="MC6" s="18" t="s">
         <v>289</v>
       </c>
-      <c r="MC6" s="18" t="s">
+      <c r="MD6" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="MD6" s="18" t="s">
+      <c r="ME6" s="18" t="s">
         <v>291</v>
       </c>
-      <c r="ME6" s="18" t="s">
+      <c r="MF6" s="18" t="s">
         <v>292</v>
       </c>
-      <c r="MF6" s="18" t="s">
+      <c r="MG6" s="18" t="s">
         <v>293</v>
       </c>
-      <c r="MG6" s="18" t="s">
+      <c r="MH6" s="18" t="s">
         <v>294</v>
       </c>
-      <c r="MH6" s="18" t="s">
+      <c r="MI6" s="18" t="s">
         <v>295</v>
       </c>
-      <c r="MI6" s="18" t="s">
+      <c r="MJ6" s="18" t="s">
         <v>296</v>
       </c>
-      <c r="MJ6" s="18" t="s">
+      <c r="MK6" s="18" t="s">
         <v>297</v>
-      </c>
-      <c r="MK6" s="18" t="s">
-        <v>298</v>
       </c>
       <c r="ML6" s="18" t="s">
         <v>94</v>
@@ -5892,65 +5892,65 @@
         <v>96</v>
       </c>
       <c r="MO6" s="18" t="s">
+        <v>416</v>
+      </c>
+      <c r="MP6" s="18" t="s">
         <v>417</v>
       </c>
-      <c r="MP6" s="18" t="s">
+      <c r="MQ6" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="MQ6" s="18" t="s">
+      <c r="MR6" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="MR6" s="18" t="s">
+      <c r="MS6" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="MS6" s="18" t="s">
+      <c r="MT6" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="MT6" s="18" t="s">
+      <c r="MU6" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="MU6" s="18" t="s">
+      <c r="MV6" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="MV6" s="18" t="s">
+      <c r="MW6" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="MW6" s="18" t="s">
+      <c r="MX6" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="MX6" s="18" t="s">
-        <v>105</v>
-      </c>
       <c r="MY6" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="MZ6" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="MZ6" s="18" t="s">
-        <v>116</v>
-      </c>
       <c r="NA6" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="NB6" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="NC6" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="ND6" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="ND6" s="18" t="s">
+      <c r="NE6" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="NE6" s="18" t="s">
+      <c r="NF6" s="18" t="s">
         <v>113</v>
-      </c>
-      <c r="NF6" s="18" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:370" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="40"/>
       <c r="B7" s="40"/>
       <c r="C7" s="40" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D7" s="40"/>
       <c r="E7" s="40"/>
@@ -5964,17 +5964,17 @@
       <c r="M7" s="42"/>
       <c r="N7" s="42"/>
       <c r="O7" s="42" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="P7" s="42" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Q7" s="42"/>
       <c r="R7" s="43" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="S7" s="43" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="T7" s="42"/>
       <c r="U7" s="42"/>
@@ -5986,13 +5986,13 @@
       <c r="AA7" s="47"/>
       <c r="AB7" s="46"/>
       <c r="AC7" s="41" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AD7" s="41" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AE7" s="41" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AF7" s="42"/>
       <c r="AG7" s="48"/>
@@ -6460,33 +6460,6 @@
   </sheetData>
   <autoFilter ref="A6:NB6" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="43">
-    <mergeCell ref="EJ4:ES4"/>
-    <mergeCell ref="ET4:FC4"/>
-    <mergeCell ref="CB4:CK4"/>
-    <mergeCell ref="CV4:DE4"/>
-    <mergeCell ref="DF4:DO4"/>
-    <mergeCell ref="DP4:DY4"/>
-    <mergeCell ref="DZ4:EI4"/>
-    <mergeCell ref="HB4:HK4"/>
-    <mergeCell ref="MY4:NA5"/>
-    <mergeCell ref="HV4:IE4"/>
-    <mergeCell ref="KN4:KW4"/>
-    <mergeCell ref="KX4:LG4"/>
-    <mergeCell ref="LH4:LQ4"/>
-    <mergeCell ref="MB4:MK4"/>
-    <mergeCell ref="ML4:MX5"/>
-    <mergeCell ref="IF4:IO4"/>
-    <mergeCell ref="IP4:IY4"/>
-    <mergeCell ref="IZ4:JI4"/>
-    <mergeCell ref="JJ4:JS4"/>
-    <mergeCell ref="JT4:KC4"/>
-    <mergeCell ref="KD4:KM4"/>
-    <mergeCell ref="LR4:MA4"/>
-    <mergeCell ref="FD4:FM4"/>
-    <mergeCell ref="FN4:FW4"/>
-    <mergeCell ref="FX4:GG4"/>
-    <mergeCell ref="GH4:GQ4"/>
-    <mergeCell ref="GR4:HA4"/>
     <mergeCell ref="NC4:ND5"/>
     <mergeCell ref="AF4:AG5"/>
     <mergeCell ref="A1:B1"/>
@@ -6503,6 +6476,33 @@
     <mergeCell ref="AM4:BQ5"/>
     <mergeCell ref="BR4:CA4"/>
     <mergeCell ref="CL4:CU4"/>
+    <mergeCell ref="FD4:FM4"/>
+    <mergeCell ref="FN4:FW4"/>
+    <mergeCell ref="FX4:GG4"/>
+    <mergeCell ref="GH4:GQ4"/>
+    <mergeCell ref="GR4:HA4"/>
+    <mergeCell ref="HB4:HK4"/>
+    <mergeCell ref="MY4:NA5"/>
+    <mergeCell ref="HV4:IE4"/>
+    <mergeCell ref="KN4:KW4"/>
+    <mergeCell ref="KX4:LG4"/>
+    <mergeCell ref="LH4:LQ4"/>
+    <mergeCell ref="MB4:MK4"/>
+    <mergeCell ref="ML4:MX5"/>
+    <mergeCell ref="IF4:IO4"/>
+    <mergeCell ref="IP4:IY4"/>
+    <mergeCell ref="IZ4:JI4"/>
+    <mergeCell ref="JJ4:JS4"/>
+    <mergeCell ref="JT4:KC4"/>
+    <mergeCell ref="KD4:KM4"/>
+    <mergeCell ref="LR4:MA4"/>
+    <mergeCell ref="EJ4:ES4"/>
+    <mergeCell ref="ET4:FC4"/>
+    <mergeCell ref="CB4:CK4"/>
+    <mergeCell ref="CV4:DE4"/>
+    <mergeCell ref="DF4:DO4"/>
+    <mergeCell ref="DP4:DY4"/>
+    <mergeCell ref="DZ4:EI4"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A6">
     <cfRule type="duplicateValues" dxfId="0" priority="92"/>

</xml_diff>

<commit_message>
[RUBY-3008] fixing typo in spreadsheet column title
</commit_message>
<xml_diff>
--- a/lib/fcerm1_template.xlsx
+++ b/lib/fcerm1_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lb000070\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F576E1FF-EC2A-49F1-A3BF-2AAB10D77015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8BFC6A-507F-4F53-BC7F-E5AA370D9630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="417">
   <si>
     <t>FCRM1 - National Capital Programme</t>
   </si>
@@ -1311,6 +1311,10 @@
   </si>
   <si>
     <t>rOM4B Major improvement</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Outcome Measures
+ rOM2B.c Delivery</t>
   </si>
 </sst>
 </file>
@@ -1863,6 +1867,99 @@
     <xf numFmtId="0" fontId="11" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="11" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="23" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1874,99 +1971,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="22" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="11" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -2275,11 +2279,11 @@
   <dimension ref="A1:ND7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="BM7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="KD7" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
       <selection pane="topRight" activeCell="C7" sqref="C7"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="BM15" sqref="BM15"/>
+      <selection pane="bottomRight" activeCell="KA5" sqref="KA5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2307,10 +2311,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:368" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="80"/>
+      <c r="B1" s="61"/>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
       <c r="E1" s="20"/>
@@ -2679,10 +2683,10 @@
       <c r="ND1" s="38"/>
     </row>
     <row r="2" spans="1:368" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="62" t="s">
         <v>145</v>
       </c>
-      <c r="B2" s="81"/>
+      <c r="B2" s="62"/>
       <c r="C2" s="19"/>
       <c r="D2" s="28"/>
       <c r="E2" s="20"/>
@@ -3421,198 +3425,198 @@
       <c r="ND3" s="38"/>
     </row>
     <row r="4" spans="1:368" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="82" t="s">
+      <c r="A4" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="82"/>
-      <c r="C4" s="83" t="s">
+      <c r="B4" s="63"/>
+      <c r="C4" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="83"/>
-      <c r="E4" s="83"/>
-      <c r="F4" s="83"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="84" t="s">
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="84"/>
-      <c r="K4" s="84"/>
-      <c r="L4" s="84"/>
-      <c r="M4" s="84"/>
-      <c r="N4" s="85" t="s">
+      <c r="J4" s="65"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="65"/>
+      <c r="M4" s="65"/>
+      <c r="N4" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="O4" s="85"/>
-      <c r="P4" s="85"/>
-      <c r="Q4" s="86" t="s">
+      <c r="O4" s="66"/>
+      <c r="P4" s="66"/>
+      <c r="Q4" s="67" t="s">
         <v>303</v>
       </c>
-      <c r="R4" s="86"/>
-      <c r="S4" s="86"/>
-      <c r="T4" s="86"/>
-      <c r="U4" s="86"/>
-      <c r="V4" s="87" t="s">
+      <c r="R4" s="67"/>
+      <c r="S4" s="67"/>
+      <c r="T4" s="67"/>
+      <c r="U4" s="67"/>
+      <c r="V4" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="W4" s="87"/>
-      <c r="X4" s="87"/>
-      <c r="Y4" s="87"/>
-      <c r="Z4" s="87"/>
-      <c r="AA4" s="87"/>
-      <c r="AB4" s="87"/>
-      <c r="AC4" s="88" t="s">
+      <c r="W4" s="68"/>
+      <c r="X4" s="68"/>
+      <c r="Y4" s="68"/>
+      <c r="Z4" s="68"/>
+      <c r="AA4" s="68"/>
+      <c r="AB4" s="68"/>
+      <c r="AC4" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="AD4" s="88"/>
-      <c r="AE4" s="88"/>
-      <c r="AF4" s="79" t="s">
+      <c r="AD4" s="69"/>
+      <c r="AE4" s="69"/>
+      <c r="AF4" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="AG4" s="79"/>
-      <c r="AH4" s="89"/>
-      <c r="AI4" s="89"/>
-      <c r="AJ4" s="89"/>
-      <c r="AK4" s="89"/>
-      <c r="AL4" s="89"/>
-      <c r="AM4" s="90" t="s">
+      <c r="AG4" s="60"/>
+      <c r="AH4" s="71"/>
+      <c r="AI4" s="71"/>
+      <c r="AJ4" s="71"/>
+      <c r="AK4" s="71"/>
+      <c r="AL4" s="71"/>
+      <c r="AM4" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="AN4" s="90"/>
-      <c r="AO4" s="90"/>
-      <c r="AP4" s="90"/>
-      <c r="AQ4" s="90"/>
-      <c r="AR4" s="90"/>
-      <c r="AS4" s="90"/>
-      <c r="AT4" s="90"/>
-      <c r="AU4" s="90"/>
-      <c r="AV4" s="90"/>
-      <c r="AW4" s="90"/>
-      <c r="AX4" s="90"/>
-      <c r="AY4" s="90"/>
-      <c r="AZ4" s="90"/>
-      <c r="BA4" s="90"/>
-      <c r="BB4" s="90"/>
-      <c r="BC4" s="90"/>
-      <c r="BD4" s="90"/>
-      <c r="BE4" s="90"/>
-      <c r="BF4" s="90"/>
-      <c r="BG4" s="90"/>
-      <c r="BH4" s="90"/>
-      <c r="BI4" s="90"/>
-      <c r="BJ4" s="90"/>
-      <c r="BK4" s="90"/>
-      <c r="BL4" s="90"/>
-      <c r="BM4" s="90"/>
-      <c r="BN4" s="90"/>
-      <c r="BO4" s="68" t="s">
+      <c r="AN4" s="72"/>
+      <c r="AO4" s="72"/>
+      <c r="AP4" s="72"/>
+      <c r="AQ4" s="72"/>
+      <c r="AR4" s="72"/>
+      <c r="AS4" s="72"/>
+      <c r="AT4" s="72"/>
+      <c r="AU4" s="72"/>
+      <c r="AV4" s="72"/>
+      <c r="AW4" s="72"/>
+      <c r="AX4" s="72"/>
+      <c r="AY4" s="72"/>
+      <c r="AZ4" s="72"/>
+      <c r="BA4" s="72"/>
+      <c r="BB4" s="72"/>
+      <c r="BC4" s="72"/>
+      <c r="BD4" s="72"/>
+      <c r="BE4" s="72"/>
+      <c r="BF4" s="72"/>
+      <c r="BG4" s="72"/>
+      <c r="BH4" s="72"/>
+      <c r="BI4" s="72"/>
+      <c r="BJ4" s="72"/>
+      <c r="BK4" s="72"/>
+      <c r="BL4" s="72"/>
+      <c r="BM4" s="72"/>
+      <c r="BN4" s="72"/>
+      <c r="BO4" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="BP4" s="68"/>
-      <c r="BQ4" s="68"/>
-      <c r="BR4" s="68"/>
-      <c r="BS4" s="68"/>
-      <c r="BT4" s="68"/>
-      <c r="BU4" s="68"/>
-      <c r="BV4" s="68"/>
-      <c r="BW4" s="68"/>
-      <c r="BX4" s="68"/>
-      <c r="BY4" s="56" t="s">
+      <c r="BP4" s="70"/>
+      <c r="BQ4" s="70"/>
+      <c r="BR4" s="70"/>
+      <c r="BS4" s="70"/>
+      <c r="BT4" s="70"/>
+      <c r="BU4" s="70"/>
+      <c r="BV4" s="70"/>
+      <c r="BW4" s="70"/>
+      <c r="BX4" s="70"/>
+      <c r="BY4" s="87" t="s">
         <v>10</v>
       </c>
-      <c r="BZ4" s="56"/>
-      <c r="CA4" s="56"/>
-      <c r="CB4" s="56"/>
-      <c r="CC4" s="56"/>
-      <c r="CD4" s="56"/>
-      <c r="CE4" s="56"/>
-      <c r="CF4" s="56"/>
-      <c r="CG4" s="56"/>
-      <c r="CH4" s="56"/>
-      <c r="CI4" s="60" t="s">
+      <c r="BZ4" s="87"/>
+      <c r="CA4" s="87"/>
+      <c r="CB4" s="87"/>
+      <c r="CC4" s="87"/>
+      <c r="CD4" s="87"/>
+      <c r="CE4" s="87"/>
+      <c r="CF4" s="87"/>
+      <c r="CG4" s="87"/>
+      <c r="CH4" s="87"/>
+      <c r="CI4" s="73" t="s">
         <v>404</v>
       </c>
-      <c r="CJ4" s="60"/>
-      <c r="CK4" s="60"/>
-      <c r="CL4" s="60"/>
-      <c r="CM4" s="60"/>
-      <c r="CN4" s="60"/>
-      <c r="CO4" s="60"/>
-      <c r="CP4" s="60"/>
-      <c r="CQ4" s="60"/>
-      <c r="CR4" s="60"/>
-      <c r="CS4" s="56" t="s">
+      <c r="CJ4" s="73"/>
+      <c r="CK4" s="73"/>
+      <c r="CL4" s="73"/>
+      <c r="CM4" s="73"/>
+      <c r="CN4" s="73"/>
+      <c r="CO4" s="73"/>
+      <c r="CP4" s="73"/>
+      <c r="CQ4" s="73"/>
+      <c r="CR4" s="73"/>
+      <c r="CS4" s="87" t="s">
         <v>403</v>
       </c>
-      <c r="CT4" s="56"/>
-      <c r="CU4" s="56"/>
-      <c r="CV4" s="56"/>
-      <c r="CW4" s="56"/>
-      <c r="CX4" s="56"/>
-      <c r="CY4" s="56"/>
-      <c r="CZ4" s="56"/>
-      <c r="DA4" s="56"/>
-      <c r="DB4" s="56"/>
-      <c r="DC4" s="60" t="s">
+      <c r="CT4" s="87"/>
+      <c r="CU4" s="87"/>
+      <c r="CV4" s="87"/>
+      <c r="CW4" s="87"/>
+      <c r="CX4" s="87"/>
+      <c r="CY4" s="87"/>
+      <c r="CZ4" s="87"/>
+      <c r="DA4" s="87"/>
+      <c r="DB4" s="87"/>
+      <c r="DC4" s="73" t="s">
         <v>402</v>
       </c>
-      <c r="DD4" s="60"/>
-      <c r="DE4" s="60"/>
-      <c r="DF4" s="60"/>
-      <c r="DG4" s="60"/>
-      <c r="DH4" s="60"/>
-      <c r="DI4" s="60"/>
-      <c r="DJ4" s="60"/>
-      <c r="DK4" s="60"/>
-      <c r="DL4" s="60"/>
-      <c r="DM4" s="56" t="s">
+      <c r="DD4" s="73"/>
+      <c r="DE4" s="73"/>
+      <c r="DF4" s="73"/>
+      <c r="DG4" s="73"/>
+      <c r="DH4" s="73"/>
+      <c r="DI4" s="73"/>
+      <c r="DJ4" s="73"/>
+      <c r="DK4" s="73"/>
+      <c r="DL4" s="73"/>
+      <c r="DM4" s="87" t="s">
         <v>304</v>
       </c>
-      <c r="DN4" s="56"/>
-      <c r="DO4" s="56"/>
-      <c r="DP4" s="56"/>
-      <c r="DQ4" s="56"/>
-      <c r="DR4" s="56"/>
-      <c r="DS4" s="56"/>
-      <c r="DT4" s="56"/>
-      <c r="DU4" s="56"/>
-      <c r="DV4" s="56"/>
-      <c r="DW4" s="57" t="s">
+      <c r="DN4" s="87"/>
+      <c r="DO4" s="87"/>
+      <c r="DP4" s="87"/>
+      <c r="DQ4" s="87"/>
+      <c r="DR4" s="87"/>
+      <c r="DS4" s="87"/>
+      <c r="DT4" s="87"/>
+      <c r="DU4" s="87"/>
+      <c r="DV4" s="87"/>
+      <c r="DW4" s="88" t="s">
         <v>401</v>
       </c>
-      <c r="DX4" s="58"/>
-      <c r="DY4" s="58"/>
-      <c r="DZ4" s="58"/>
-      <c r="EA4" s="58"/>
-      <c r="EB4" s="58"/>
-      <c r="EC4" s="58"/>
-      <c r="ED4" s="58"/>
-      <c r="EE4" s="58"/>
-      <c r="EF4" s="59"/>
-      <c r="EG4" s="56" t="s">
+      <c r="DX4" s="89"/>
+      <c r="DY4" s="89"/>
+      <c r="DZ4" s="89"/>
+      <c r="EA4" s="89"/>
+      <c r="EB4" s="89"/>
+      <c r="EC4" s="89"/>
+      <c r="ED4" s="89"/>
+      <c r="EE4" s="89"/>
+      <c r="EF4" s="90"/>
+      <c r="EG4" s="87" t="s">
         <v>400</v>
       </c>
-      <c r="EH4" s="56"/>
-      <c r="EI4" s="56"/>
-      <c r="EJ4" s="56"/>
-      <c r="EK4" s="56"/>
-      <c r="EL4" s="56"/>
-      <c r="EM4" s="56"/>
-      <c r="EN4" s="56"/>
-      <c r="EO4" s="56"/>
-      <c r="EP4" s="56"/>
-      <c r="EQ4" s="57" t="s">
+      <c r="EH4" s="87"/>
+      <c r="EI4" s="87"/>
+      <c r="EJ4" s="87"/>
+      <c r="EK4" s="87"/>
+      <c r="EL4" s="87"/>
+      <c r="EM4" s="87"/>
+      <c r="EN4" s="87"/>
+      <c r="EO4" s="87"/>
+      <c r="EP4" s="87"/>
+      <c r="EQ4" s="88" t="s">
         <v>399</v>
       </c>
-      <c r="ER4" s="58"/>
-      <c r="ES4" s="58"/>
-      <c r="ET4" s="58"/>
-      <c r="EU4" s="58"/>
-      <c r="EV4" s="58"/>
-      <c r="EW4" s="58"/>
-      <c r="EX4" s="58"/>
-      <c r="EY4" s="58"/>
-      <c r="EZ4" s="59"/>
+      <c r="ER4" s="89"/>
+      <c r="ES4" s="89"/>
+      <c r="ET4" s="89"/>
+      <c r="EU4" s="89"/>
+      <c r="EV4" s="89"/>
+      <c r="EW4" s="89"/>
+      <c r="EX4" s="89"/>
+      <c r="EY4" s="89"/>
+      <c r="EZ4" s="90"/>
       <c r="FA4" s="74" t="s">
         <v>11</v>
       </c>
@@ -3673,270 +3677,270 @@
       <c r="GV4" s="78"/>
       <c r="GW4" s="78"/>
       <c r="GX4" s="78"/>
-      <c r="GY4" s="61" t="s">
+      <c r="GY4" s="79" t="s">
         <v>392</v>
       </c>
-      <c r="GZ4" s="61"/>
-      <c r="HA4" s="61"/>
-      <c r="HB4" s="61"/>
-      <c r="HC4" s="61"/>
-      <c r="HD4" s="61"/>
-      <c r="HE4" s="61"/>
-      <c r="HF4" s="61"/>
-      <c r="HG4" s="61"/>
-      <c r="HH4" s="61"/>
-      <c r="HI4" s="68" t="s">
+      <c r="GZ4" s="79"/>
+      <c r="HA4" s="79"/>
+      <c r="HB4" s="79"/>
+      <c r="HC4" s="79"/>
+      <c r="HD4" s="79"/>
+      <c r="HE4" s="79"/>
+      <c r="HF4" s="79"/>
+      <c r="HG4" s="79"/>
+      <c r="HH4" s="79"/>
+      <c r="HI4" s="70" t="s">
         <v>148</v>
       </c>
-      <c r="HJ4" s="68"/>
-      <c r="HK4" s="68"/>
-      <c r="HL4" s="68"/>
-      <c r="HM4" s="68"/>
-      <c r="HN4" s="68"/>
-      <c r="HO4" s="68"/>
-      <c r="HP4" s="68"/>
-      <c r="HQ4" s="68"/>
-      <c r="HR4" s="68"/>
-      <c r="HS4" s="68" t="s">
+      <c r="HJ4" s="70"/>
+      <c r="HK4" s="70"/>
+      <c r="HL4" s="70"/>
+      <c r="HM4" s="70"/>
+      <c r="HN4" s="70"/>
+      <c r="HO4" s="70"/>
+      <c r="HP4" s="70"/>
+      <c r="HQ4" s="70"/>
+      <c r="HR4" s="70"/>
+      <c r="HS4" s="70" t="s">
         <v>159</v>
       </c>
-      <c r="HT4" s="68"/>
-      <c r="HU4" s="68"/>
-      <c r="HV4" s="68"/>
-      <c r="HW4" s="68"/>
-      <c r="HX4" s="68"/>
-      <c r="HY4" s="68"/>
-      <c r="HZ4" s="68"/>
-      <c r="IA4" s="68"/>
-      <c r="IB4" s="68"/>
-      <c r="IC4" s="68" t="s">
+      <c r="HT4" s="70"/>
+      <c r="HU4" s="70"/>
+      <c r="HV4" s="70"/>
+      <c r="HW4" s="70"/>
+      <c r="HX4" s="70"/>
+      <c r="HY4" s="70"/>
+      <c r="HZ4" s="70"/>
+      <c r="IA4" s="70"/>
+      <c r="IB4" s="70"/>
+      <c r="IC4" s="70" t="s">
         <v>170</v>
       </c>
-      <c r="ID4" s="68"/>
-      <c r="IE4" s="68"/>
-      <c r="IF4" s="68"/>
-      <c r="IG4" s="68"/>
-      <c r="IH4" s="68"/>
-      <c r="II4" s="68"/>
-      <c r="IJ4" s="68"/>
-      <c r="IK4" s="68"/>
-      <c r="IL4" s="68"/>
-      <c r="IM4" s="68" t="s">
+      <c r="ID4" s="70"/>
+      <c r="IE4" s="70"/>
+      <c r="IF4" s="70"/>
+      <c r="IG4" s="70"/>
+      <c r="IH4" s="70"/>
+      <c r="II4" s="70"/>
+      <c r="IJ4" s="70"/>
+      <c r="IK4" s="70"/>
+      <c r="IL4" s="70"/>
+      <c r="IM4" s="70" t="s">
         <v>181</v>
       </c>
-      <c r="IN4" s="68"/>
-      <c r="IO4" s="68"/>
-      <c r="IP4" s="68"/>
-      <c r="IQ4" s="68"/>
-      <c r="IR4" s="68"/>
-      <c r="IS4" s="68"/>
-      <c r="IT4" s="68"/>
-      <c r="IU4" s="68"/>
-      <c r="IV4" s="68"/>
-      <c r="IW4" s="69" t="s">
+      <c r="IN4" s="70"/>
+      <c r="IO4" s="70"/>
+      <c r="IP4" s="70"/>
+      <c r="IQ4" s="70"/>
+      <c r="IR4" s="70"/>
+      <c r="IS4" s="70"/>
+      <c r="IT4" s="70"/>
+      <c r="IU4" s="70"/>
+      <c r="IV4" s="70"/>
+      <c r="IW4" s="82" t="s">
         <v>192</v>
       </c>
-      <c r="IX4" s="70"/>
-      <c r="IY4" s="70"/>
-      <c r="IZ4" s="70"/>
-      <c r="JA4" s="70"/>
-      <c r="JB4" s="70"/>
-      <c r="JC4" s="70"/>
-      <c r="JD4" s="70"/>
-      <c r="JE4" s="70"/>
-      <c r="JF4" s="71"/>
-      <c r="JG4" s="69" t="s">
+      <c r="IX4" s="83"/>
+      <c r="IY4" s="83"/>
+      <c r="IZ4" s="83"/>
+      <c r="JA4" s="83"/>
+      <c r="JB4" s="83"/>
+      <c r="JC4" s="83"/>
+      <c r="JD4" s="83"/>
+      <c r="JE4" s="83"/>
+      <c r="JF4" s="84"/>
+      <c r="JG4" s="82" t="s">
         <v>203</v>
       </c>
-      <c r="JH4" s="70"/>
-      <c r="JI4" s="70"/>
-      <c r="JJ4" s="70"/>
-      <c r="JK4" s="70"/>
-      <c r="JL4" s="70"/>
-      <c r="JM4" s="70"/>
-      <c r="JN4" s="70"/>
-      <c r="JO4" s="70"/>
-      <c r="JP4" s="71"/>
-      <c r="JQ4" s="69" t="s">
+      <c r="JH4" s="83"/>
+      <c r="JI4" s="83"/>
+      <c r="JJ4" s="83"/>
+      <c r="JK4" s="83"/>
+      <c r="JL4" s="83"/>
+      <c r="JM4" s="83"/>
+      <c r="JN4" s="83"/>
+      <c r="JO4" s="83"/>
+      <c r="JP4" s="84"/>
+      <c r="JQ4" s="82" t="s">
         <v>214</v>
       </c>
-      <c r="JR4" s="70"/>
-      <c r="JS4" s="70"/>
-      <c r="JT4" s="70"/>
-      <c r="JU4" s="70"/>
-      <c r="JV4" s="70"/>
-      <c r="JW4" s="70"/>
-      <c r="JX4" s="70"/>
-      <c r="JY4" s="70"/>
-      <c r="JZ4" s="71"/>
-      <c r="KA4" s="69" t="s">
-        <v>214</v>
-      </c>
-      <c r="KB4" s="70"/>
-      <c r="KC4" s="70"/>
-      <c r="KD4" s="70"/>
-      <c r="KE4" s="70"/>
-      <c r="KF4" s="70"/>
-      <c r="KG4" s="70"/>
-      <c r="KH4" s="70"/>
-      <c r="KI4" s="70"/>
-      <c r="KJ4" s="71"/>
-      <c r="KK4" s="69" t="s">
+      <c r="JR4" s="83"/>
+      <c r="JS4" s="83"/>
+      <c r="JT4" s="83"/>
+      <c r="JU4" s="83"/>
+      <c r="JV4" s="83"/>
+      <c r="JW4" s="83"/>
+      <c r="JX4" s="83"/>
+      <c r="JY4" s="83"/>
+      <c r="JZ4" s="84"/>
+      <c r="KA4" s="82" t="s">
+        <v>416</v>
+      </c>
+      <c r="KB4" s="83"/>
+      <c r="KC4" s="83"/>
+      <c r="KD4" s="83"/>
+      <c r="KE4" s="83"/>
+      <c r="KF4" s="83"/>
+      <c r="KG4" s="83"/>
+      <c r="KH4" s="83"/>
+      <c r="KI4" s="83"/>
+      <c r="KJ4" s="84"/>
+      <c r="KK4" s="82" t="s">
         <v>235</v>
       </c>
-      <c r="KL4" s="70"/>
-      <c r="KM4" s="70"/>
-      <c r="KN4" s="70"/>
-      <c r="KO4" s="70"/>
-      <c r="KP4" s="70"/>
-      <c r="KQ4" s="70"/>
-      <c r="KR4" s="70"/>
-      <c r="KS4" s="70"/>
-      <c r="KT4" s="71"/>
-      <c r="KU4" s="72" t="s">
+      <c r="KL4" s="83"/>
+      <c r="KM4" s="83"/>
+      <c r="KN4" s="83"/>
+      <c r="KO4" s="83"/>
+      <c r="KP4" s="83"/>
+      <c r="KQ4" s="83"/>
+      <c r="KR4" s="83"/>
+      <c r="KS4" s="83"/>
+      <c r="KT4" s="84"/>
+      <c r="KU4" s="85" t="s">
         <v>246</v>
       </c>
-      <c r="KV4" s="72"/>
-      <c r="KW4" s="72"/>
-      <c r="KX4" s="72"/>
-      <c r="KY4" s="72"/>
-      <c r="KZ4" s="72"/>
-      <c r="LA4" s="72"/>
-      <c r="LB4" s="72"/>
-      <c r="LC4" s="72"/>
-      <c r="LD4" s="72"/>
-      <c r="LE4" s="72" t="s">
+      <c r="KV4" s="85"/>
+      <c r="KW4" s="85"/>
+      <c r="KX4" s="85"/>
+      <c r="KY4" s="85"/>
+      <c r="KZ4" s="85"/>
+      <c r="LA4" s="85"/>
+      <c r="LB4" s="85"/>
+      <c r="LC4" s="85"/>
+      <c r="LD4" s="85"/>
+      <c r="LE4" s="85" t="s">
         <v>257</v>
       </c>
-      <c r="LF4" s="72"/>
-      <c r="LG4" s="72"/>
-      <c r="LH4" s="72"/>
-      <c r="LI4" s="72"/>
-      <c r="LJ4" s="72"/>
-      <c r="LK4" s="72"/>
-      <c r="LL4" s="72"/>
-      <c r="LM4" s="72"/>
-      <c r="LN4" s="72"/>
-      <c r="LO4" s="72" t="s">
+      <c r="LF4" s="85"/>
+      <c r="LG4" s="85"/>
+      <c r="LH4" s="85"/>
+      <c r="LI4" s="85"/>
+      <c r="LJ4" s="85"/>
+      <c r="LK4" s="85"/>
+      <c r="LL4" s="85"/>
+      <c r="LM4" s="85"/>
+      <c r="LN4" s="85"/>
+      <c r="LO4" s="85" t="s">
         <v>263</v>
       </c>
-      <c r="LP4" s="72"/>
-      <c r="LQ4" s="72"/>
-      <c r="LR4" s="72"/>
-      <c r="LS4" s="72"/>
-      <c r="LT4" s="72"/>
-      <c r="LU4" s="72"/>
-      <c r="LV4" s="72"/>
-      <c r="LW4" s="72"/>
-      <c r="LX4" s="72"/>
-      <c r="LY4" s="72" t="s">
+      <c r="LP4" s="85"/>
+      <c r="LQ4" s="85"/>
+      <c r="LR4" s="85"/>
+      <c r="LS4" s="85"/>
+      <c r="LT4" s="85"/>
+      <c r="LU4" s="85"/>
+      <c r="LV4" s="85"/>
+      <c r="LW4" s="85"/>
+      <c r="LX4" s="85"/>
+      <c r="LY4" s="85" t="s">
         <v>274</v>
       </c>
-      <c r="LZ4" s="72"/>
-      <c r="MA4" s="72"/>
-      <c r="MB4" s="72"/>
-      <c r="MC4" s="72"/>
-      <c r="MD4" s="72"/>
-      <c r="ME4" s="72"/>
-      <c r="MF4" s="72"/>
-      <c r="MG4" s="72"/>
-      <c r="MH4" s="72"/>
-      <c r="MI4" s="73" t="s">
+      <c r="LZ4" s="85"/>
+      <c r="MA4" s="85"/>
+      <c r="MB4" s="85"/>
+      <c r="MC4" s="85"/>
+      <c r="MD4" s="85"/>
+      <c r="ME4" s="85"/>
+      <c r="MF4" s="85"/>
+      <c r="MG4" s="85"/>
+      <c r="MH4" s="85"/>
+      <c r="MI4" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="MJ4" s="73"/>
-      <c r="MK4" s="73"/>
-      <c r="ML4" s="73"/>
-      <c r="MM4" s="73"/>
-      <c r="MN4" s="73"/>
-      <c r="MO4" s="73"/>
-      <c r="MP4" s="73"/>
-      <c r="MQ4" s="73"/>
-      <c r="MR4" s="73"/>
-      <c r="MS4" s="73"/>
-      <c r="MT4" s="73"/>
-      <c r="MU4" s="73"/>
-      <c r="MV4" s="73"/>
-      <c r="MW4" s="62" t="s">
+      <c r="MJ4" s="86"/>
+      <c r="MK4" s="86"/>
+      <c r="ML4" s="86"/>
+      <c r="MM4" s="86"/>
+      <c r="MN4" s="86"/>
+      <c r="MO4" s="86"/>
+      <c r="MP4" s="86"/>
+      <c r="MQ4" s="86"/>
+      <c r="MR4" s="86"/>
+      <c r="MS4" s="86"/>
+      <c r="MT4" s="86"/>
+      <c r="MU4" s="86"/>
+      <c r="MV4" s="86"/>
+      <c r="MW4" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="MX4" s="63"/>
-      <c r="MY4" s="64"/>
+      <c r="MX4" s="80"/>
+      <c r="MY4" s="57"/>
       <c r="MZ4" s="37"/>
-      <c r="NA4" s="62" t="s">
+      <c r="NA4" s="56" t="s">
         <v>96</v>
       </c>
-      <c r="NB4" s="64"/>
+      <c r="NB4" s="57"/>
       <c r="NC4" s="54"/>
       <c r="ND4" s="52"/>
     </row>
     <row r="5" spans="1:368" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="82"/>
-      <c r="B5" s="82"/>
-      <c r="C5" s="83"/>
-      <c r="D5" s="83"/>
-      <c r="E5" s="83"/>
-      <c r="F5" s="83"/>
-      <c r="G5" s="83"/>
-      <c r="H5" s="83"/>
-      <c r="I5" s="84"/>
-      <c r="J5" s="84"/>
-      <c r="K5" s="84"/>
-      <c r="L5" s="84"/>
-      <c r="M5" s="84"/>
-      <c r="N5" s="85"/>
-      <c r="O5" s="85"/>
-      <c r="P5" s="85"/>
-      <c r="Q5" s="86"/>
-      <c r="R5" s="86"/>
-      <c r="S5" s="86"/>
-      <c r="T5" s="86"/>
-      <c r="U5" s="86"/>
-      <c r="V5" s="87"/>
-      <c r="W5" s="87"/>
-      <c r="X5" s="87"/>
-      <c r="Y5" s="87"/>
-      <c r="Z5" s="87"/>
-      <c r="AA5" s="87"/>
-      <c r="AB5" s="87"/>
-      <c r="AC5" s="88"/>
-      <c r="AD5" s="88"/>
-      <c r="AE5" s="88"/>
-      <c r="AF5" s="79"/>
-      <c r="AG5" s="79"/>
-      <c r="AH5" s="89"/>
-      <c r="AI5" s="89"/>
-      <c r="AJ5" s="89"/>
-      <c r="AK5" s="89"/>
-      <c r="AL5" s="89"/>
-      <c r="AM5" s="90"/>
-      <c r="AN5" s="90"/>
-      <c r="AO5" s="90"/>
-      <c r="AP5" s="90"/>
-      <c r="AQ5" s="90"/>
-      <c r="AR5" s="90"/>
-      <c r="AS5" s="90"/>
-      <c r="AT5" s="90"/>
-      <c r="AU5" s="90"/>
-      <c r="AV5" s="90"/>
-      <c r="AW5" s="90"/>
-      <c r="AX5" s="90"/>
-      <c r="AY5" s="90"/>
-      <c r="AZ5" s="90"/>
-      <c r="BA5" s="90"/>
-      <c r="BB5" s="90"/>
-      <c r="BC5" s="90"/>
-      <c r="BD5" s="90"/>
-      <c r="BE5" s="90"/>
-      <c r="BF5" s="90"/>
-      <c r="BG5" s="90"/>
-      <c r="BH5" s="90"/>
-      <c r="BI5" s="90"/>
-      <c r="BJ5" s="90"/>
-      <c r="BK5" s="90"/>
-      <c r="BL5" s="90"/>
-      <c r="BM5" s="90"/>
-      <c r="BN5" s="90"/>
+      <c r="A5" s="63"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="65"/>
+      <c r="K5" s="65"/>
+      <c r="L5" s="65"/>
+      <c r="M5" s="65"/>
+      <c r="N5" s="66"/>
+      <c r="O5" s="66"/>
+      <c r="P5" s="66"/>
+      <c r="Q5" s="67"/>
+      <c r="R5" s="67"/>
+      <c r="S5" s="67"/>
+      <c r="T5" s="67"/>
+      <c r="U5" s="67"/>
+      <c r="V5" s="68"/>
+      <c r="W5" s="68"/>
+      <c r="X5" s="68"/>
+      <c r="Y5" s="68"/>
+      <c r="Z5" s="68"/>
+      <c r="AA5" s="68"/>
+      <c r="AB5" s="68"/>
+      <c r="AC5" s="69"/>
+      <c r="AD5" s="69"/>
+      <c r="AE5" s="69"/>
+      <c r="AF5" s="60"/>
+      <c r="AG5" s="60"/>
+      <c r="AH5" s="71"/>
+      <c r="AI5" s="71"/>
+      <c r="AJ5" s="71"/>
+      <c r="AK5" s="71"/>
+      <c r="AL5" s="71"/>
+      <c r="AM5" s="72"/>
+      <c r="AN5" s="72"/>
+      <c r="AO5" s="72"/>
+      <c r="AP5" s="72"/>
+      <c r="AQ5" s="72"/>
+      <c r="AR5" s="72"/>
+      <c r="AS5" s="72"/>
+      <c r="AT5" s="72"/>
+      <c r="AU5" s="72"/>
+      <c r="AV5" s="72"/>
+      <c r="AW5" s="72"/>
+      <c r="AX5" s="72"/>
+      <c r="AY5" s="72"/>
+      <c r="AZ5" s="72"/>
+      <c r="BA5" s="72"/>
+      <c r="BB5" s="72"/>
+      <c r="BC5" s="72"/>
+      <c r="BD5" s="72"/>
+      <c r="BE5" s="72"/>
+      <c r="BF5" s="72"/>
+      <c r="BG5" s="72"/>
+      <c r="BH5" s="72"/>
+      <c r="BI5" s="72"/>
+      <c r="BJ5" s="72"/>
+      <c r="BK5" s="72"/>
+      <c r="BL5" s="72"/>
+      <c r="BM5" s="72"/>
+      <c r="BN5" s="72"/>
       <c r="BO5" s="7" t="s">
         <v>19</v>
       </c>
@@ -4777,26 +4781,26 @@
       <c r="MH5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="MI5" s="73"/>
-      <c r="MJ5" s="73"/>
-      <c r="MK5" s="73"/>
-      <c r="ML5" s="73"/>
-      <c r="MM5" s="73"/>
-      <c r="MN5" s="73"/>
-      <c r="MO5" s="73"/>
-      <c r="MP5" s="73"/>
-      <c r="MQ5" s="73"/>
-      <c r="MR5" s="73"/>
-      <c r="MS5" s="73"/>
-      <c r="MT5" s="73"/>
-      <c r="MU5" s="73"/>
-      <c r="MV5" s="73"/>
-      <c r="MW5" s="65"/>
-      <c r="MX5" s="66"/>
-      <c r="MY5" s="67"/>
+      <c r="MI5" s="86"/>
+      <c r="MJ5" s="86"/>
+      <c r="MK5" s="86"/>
+      <c r="ML5" s="86"/>
+      <c r="MM5" s="86"/>
+      <c r="MN5" s="86"/>
+      <c r="MO5" s="86"/>
+      <c r="MP5" s="86"/>
+      <c r="MQ5" s="86"/>
+      <c r="MR5" s="86"/>
+      <c r="MS5" s="86"/>
+      <c r="MT5" s="86"/>
+      <c r="MU5" s="86"/>
+      <c r="MV5" s="86"/>
+      <c r="MW5" s="58"/>
+      <c r="MX5" s="81"/>
+      <c r="MY5" s="59"/>
       <c r="MZ5" s="37"/>
-      <c r="NA5" s="65"/>
-      <c r="NB5" s="67"/>
+      <c r="NA5" s="58"/>
+      <c r="NB5" s="59"/>
       <c r="NC5" s="55"/>
       <c r="ND5" s="53"/>
     </row>
@@ -6409,6 +6413,33 @@
   </sheetData>
   <autoFilter ref="A6:MZ6" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="43">
+    <mergeCell ref="EG4:EP4"/>
+    <mergeCell ref="EQ4:EZ4"/>
+    <mergeCell ref="BY4:CH4"/>
+    <mergeCell ref="CS4:DB4"/>
+    <mergeCell ref="DC4:DL4"/>
+    <mergeCell ref="DM4:DV4"/>
+    <mergeCell ref="DW4:EF4"/>
+    <mergeCell ref="GY4:HH4"/>
+    <mergeCell ref="MW4:MY5"/>
+    <mergeCell ref="HS4:IB4"/>
+    <mergeCell ref="KK4:KT4"/>
+    <mergeCell ref="KU4:LD4"/>
+    <mergeCell ref="LE4:LN4"/>
+    <mergeCell ref="LY4:MH4"/>
+    <mergeCell ref="MI4:MV5"/>
+    <mergeCell ref="IC4:IL4"/>
+    <mergeCell ref="IM4:IV4"/>
+    <mergeCell ref="IW4:JF4"/>
+    <mergeCell ref="JG4:JP4"/>
+    <mergeCell ref="JQ4:JZ4"/>
+    <mergeCell ref="KA4:KJ4"/>
+    <mergeCell ref="LO4:LX4"/>
+    <mergeCell ref="FA4:FJ4"/>
+    <mergeCell ref="FK4:FT4"/>
+    <mergeCell ref="FU4:GD4"/>
+    <mergeCell ref="GE4:GN4"/>
+    <mergeCell ref="GO4:GX4"/>
     <mergeCell ref="NA4:NB5"/>
     <mergeCell ref="AF4:AG5"/>
     <mergeCell ref="A1:B1"/>
@@ -6425,33 +6456,6 @@
     <mergeCell ref="AM4:BN5"/>
     <mergeCell ref="BO4:BX4"/>
     <mergeCell ref="CI4:CR4"/>
-    <mergeCell ref="FA4:FJ4"/>
-    <mergeCell ref="FK4:FT4"/>
-    <mergeCell ref="FU4:GD4"/>
-    <mergeCell ref="GE4:GN4"/>
-    <mergeCell ref="GO4:GX4"/>
-    <mergeCell ref="GY4:HH4"/>
-    <mergeCell ref="MW4:MY5"/>
-    <mergeCell ref="HS4:IB4"/>
-    <mergeCell ref="KK4:KT4"/>
-    <mergeCell ref="KU4:LD4"/>
-    <mergeCell ref="LE4:LN4"/>
-    <mergeCell ref="LY4:MH4"/>
-    <mergeCell ref="MI4:MV5"/>
-    <mergeCell ref="IC4:IL4"/>
-    <mergeCell ref="IM4:IV4"/>
-    <mergeCell ref="IW4:JF4"/>
-    <mergeCell ref="JG4:JP4"/>
-    <mergeCell ref="JQ4:JZ4"/>
-    <mergeCell ref="KA4:KJ4"/>
-    <mergeCell ref="LO4:LX4"/>
-    <mergeCell ref="EG4:EP4"/>
-    <mergeCell ref="EQ4:EZ4"/>
-    <mergeCell ref="BY4:CH4"/>
-    <mergeCell ref="CS4:DB4"/>
-    <mergeCell ref="DC4:DL4"/>
-    <mergeCell ref="DM4:DV4"/>
-    <mergeCell ref="DW4:EF4"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A6">
     <cfRule type="duplicateValues" dxfId="0" priority="92"/>

</xml_diff>

<commit_message>
[RUBY-2881] Adding Last Updated By column to FCRM report
</commit_message>
<xml_diff>
--- a/lib/fcerm1_template.xlsx
+++ b/lib/fcerm1_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lb000070\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8BFC6A-507F-4F53-BC7F-E5AA370D9630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{740BBFC3-527A-4FB7-B0B3-C9B33B67F0F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="419">
   <si>
     <t>FCRM1 - National Capital Programme</t>
   </si>
@@ -1315,6 +1315,12 @@
   <si>
     <t xml:space="preserve"> Outcome Measures
  rOM2B.c Delivery</t>
+  </si>
+  <si>
+    <t>Updated at</t>
+  </si>
+  <si>
+    <t>Updated by</t>
   </si>
 </sst>
 </file>
@@ -1546,7 +1552,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1646,19 +1652,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color auto="1"/>
       </left>
       <right/>
@@ -1707,7 +1700,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1861,24 +1854,75 @@
     <xf numFmtId="0" fontId="11" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="9" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="21" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="9" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1909,68 +1953,23 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="5" fillId="11" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -2276,14 +2275,14 @@
     <tabColor rgb="FF92D050"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:ND7"/>
+  <dimension ref="A1:NE7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="KD7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="NB7" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
       <selection pane="topRight" activeCell="C7" sqref="C7"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="KA5" sqref="KA5"/>
+      <selection pane="bottomRight" activeCell="ND6" sqref="ND6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2305,16 +2304,16 @@
     <col min="364" max="364" width="17.109375" style="6" bestFit="1" customWidth="1"/>
     <col min="365" max="365" width="19.6640625" style="6" customWidth="1"/>
     <col min="366" max="366" width="21.5546875" style="6" customWidth="1"/>
-    <col min="367" max="367" width="19.6640625" style="6" customWidth="1"/>
-    <col min="368" max="368" width="21.5546875" style="6" customWidth="1"/>
-    <col min="369" max="16384" width="8.6640625" style="6"/>
+    <col min="367" max="368" width="19.6640625" style="6" customWidth="1"/>
+    <col min="369" max="369" width="21.5546875" style="6" customWidth="1"/>
+    <col min="370" max="16384" width="8.6640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:368" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="61" t="s">
+    <row r="1" spans="1:369" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="61"/>
+      <c r="B1" s="78"/>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
       <c r="E1" s="20"/>
@@ -2681,12 +2680,13 @@
       <c r="NB1" s="38"/>
       <c r="NC1" s="38"/>
       <c r="ND1" s="38"/>
+      <c r="NE1" s="38"/>
     </row>
-    <row r="2" spans="1:368" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="62" t="s">
+    <row r="2" spans="1:369" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="79" t="s">
         <v>145</v>
       </c>
-      <c r="B2" s="62"/>
+      <c r="B2" s="79"/>
       <c r="C2" s="19"/>
       <c r="D2" s="28"/>
       <c r="E2" s="20"/>
@@ -3053,8 +3053,9 @@
       <c r="NB2" s="38"/>
       <c r="NC2" s="38"/>
       <c r="ND2" s="38"/>
+      <c r="NE2" s="38"/>
     </row>
-    <row r="3" spans="1:368" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:369" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="30"/>
       <c r="B3" s="31"/>
       <c r="C3" s="31"/>
@@ -3423,524 +3424,528 @@
       <c r="NB3" s="38"/>
       <c r="NC3" s="38"/>
       <c r="ND3" s="38"/>
+      <c r="NE3" s="38"/>
     </row>
-    <row r="4" spans="1:368" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="63" t="s">
+    <row r="4" spans="1:369" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="63"/>
-      <c r="C4" s="64" t="s">
+      <c r="B4" s="80"/>
+      <c r="C4" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
-      <c r="H4" s="64"/>
-      <c r="I4" s="65" t="s">
+      <c r="D4" s="81"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="65"/>
-      <c r="K4" s="65"/>
-      <c r="L4" s="65"/>
-      <c r="M4" s="65"/>
-      <c r="N4" s="66" t="s">
+      <c r="J4" s="82"/>
+      <c r="K4" s="82"/>
+      <c r="L4" s="82"/>
+      <c r="M4" s="82"/>
+      <c r="N4" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="O4" s="66"/>
-      <c r="P4" s="66"/>
-      <c r="Q4" s="67" t="s">
+      <c r="O4" s="83"/>
+      <c r="P4" s="83"/>
+      <c r="Q4" s="84" t="s">
         <v>303</v>
       </c>
-      <c r="R4" s="67"/>
-      <c r="S4" s="67"/>
-      <c r="T4" s="67"/>
-      <c r="U4" s="67"/>
-      <c r="V4" s="68" t="s">
+      <c r="R4" s="84"/>
+      <c r="S4" s="84"/>
+      <c r="T4" s="84"/>
+      <c r="U4" s="84"/>
+      <c r="V4" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="W4" s="68"/>
-      <c r="X4" s="68"/>
-      <c r="Y4" s="68"/>
-      <c r="Z4" s="68"/>
-      <c r="AA4" s="68"/>
-      <c r="AB4" s="68"/>
-      <c r="AC4" s="69" t="s">
+      <c r="W4" s="85"/>
+      <c r="X4" s="85"/>
+      <c r="Y4" s="85"/>
+      <c r="Z4" s="85"/>
+      <c r="AA4" s="85"/>
+      <c r="AB4" s="85"/>
+      <c r="AC4" s="86" t="s">
         <v>6</v>
       </c>
-      <c r="AD4" s="69"/>
-      <c r="AE4" s="69"/>
-      <c r="AF4" s="60" t="s">
+      <c r="AD4" s="86"/>
+      <c r="AE4" s="86"/>
+      <c r="AF4" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="AG4" s="60"/>
-      <c r="AH4" s="71"/>
-      <c r="AI4" s="71"/>
-      <c r="AJ4" s="71"/>
-      <c r="AK4" s="71"/>
-      <c r="AL4" s="71"/>
-      <c r="AM4" s="72" t="s">
+      <c r="AG4" s="77"/>
+      <c r="AH4" s="87"/>
+      <c r="AI4" s="87"/>
+      <c r="AJ4" s="87"/>
+      <c r="AK4" s="87"/>
+      <c r="AL4" s="87"/>
+      <c r="AM4" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="AN4" s="72"/>
-      <c r="AO4" s="72"/>
-      <c r="AP4" s="72"/>
-      <c r="AQ4" s="72"/>
-      <c r="AR4" s="72"/>
-      <c r="AS4" s="72"/>
-      <c r="AT4" s="72"/>
-      <c r="AU4" s="72"/>
-      <c r="AV4" s="72"/>
-      <c r="AW4" s="72"/>
-      <c r="AX4" s="72"/>
-      <c r="AY4" s="72"/>
-      <c r="AZ4" s="72"/>
-      <c r="BA4" s="72"/>
-      <c r="BB4" s="72"/>
-      <c r="BC4" s="72"/>
-      <c r="BD4" s="72"/>
-      <c r="BE4" s="72"/>
-      <c r="BF4" s="72"/>
-      <c r="BG4" s="72"/>
-      <c r="BH4" s="72"/>
-      <c r="BI4" s="72"/>
-      <c r="BJ4" s="72"/>
-      <c r="BK4" s="72"/>
-      <c r="BL4" s="72"/>
-      <c r="BM4" s="72"/>
-      <c r="BN4" s="72"/>
-      <c r="BO4" s="70" t="s">
+      <c r="AN4" s="88"/>
+      <c r="AO4" s="88"/>
+      <c r="AP4" s="88"/>
+      <c r="AQ4" s="88"/>
+      <c r="AR4" s="88"/>
+      <c r="AS4" s="88"/>
+      <c r="AT4" s="88"/>
+      <c r="AU4" s="88"/>
+      <c r="AV4" s="88"/>
+      <c r="AW4" s="88"/>
+      <c r="AX4" s="88"/>
+      <c r="AY4" s="88"/>
+      <c r="AZ4" s="88"/>
+      <c r="BA4" s="88"/>
+      <c r="BB4" s="88"/>
+      <c r="BC4" s="88"/>
+      <c r="BD4" s="88"/>
+      <c r="BE4" s="88"/>
+      <c r="BF4" s="88"/>
+      <c r="BG4" s="88"/>
+      <c r="BH4" s="88"/>
+      <c r="BI4" s="88"/>
+      <c r="BJ4" s="88"/>
+      <c r="BK4" s="88"/>
+      <c r="BL4" s="88"/>
+      <c r="BM4" s="88"/>
+      <c r="BN4" s="88"/>
+      <c r="BO4" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="BP4" s="70"/>
-      <c r="BQ4" s="70"/>
-      <c r="BR4" s="70"/>
-      <c r="BS4" s="70"/>
-      <c r="BT4" s="70"/>
-      <c r="BU4" s="70"/>
-      <c r="BV4" s="70"/>
-      <c r="BW4" s="70"/>
-      <c r="BX4" s="70"/>
-      <c r="BY4" s="87" t="s">
+      <c r="BP4" s="66"/>
+      <c r="BQ4" s="66"/>
+      <c r="BR4" s="66"/>
+      <c r="BS4" s="66"/>
+      <c r="BT4" s="66"/>
+      <c r="BU4" s="66"/>
+      <c r="BV4" s="66"/>
+      <c r="BW4" s="66"/>
+      <c r="BX4" s="66"/>
+      <c r="BY4" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="BZ4" s="87"/>
-      <c r="CA4" s="87"/>
-      <c r="CB4" s="87"/>
-      <c r="CC4" s="87"/>
-      <c r="CD4" s="87"/>
-      <c r="CE4" s="87"/>
-      <c r="CF4" s="87"/>
-      <c r="CG4" s="87"/>
-      <c r="CH4" s="87"/>
-      <c r="CI4" s="73" t="s">
+      <c r="BZ4" s="54"/>
+      <c r="CA4" s="54"/>
+      <c r="CB4" s="54"/>
+      <c r="CC4" s="54"/>
+      <c r="CD4" s="54"/>
+      <c r="CE4" s="54"/>
+      <c r="CF4" s="54"/>
+      <c r="CG4" s="54"/>
+      <c r="CH4" s="54"/>
+      <c r="CI4" s="58" t="s">
         <v>404</v>
       </c>
-      <c r="CJ4" s="73"/>
-      <c r="CK4" s="73"/>
-      <c r="CL4" s="73"/>
-      <c r="CM4" s="73"/>
-      <c r="CN4" s="73"/>
-      <c r="CO4" s="73"/>
-      <c r="CP4" s="73"/>
-      <c r="CQ4" s="73"/>
-      <c r="CR4" s="73"/>
-      <c r="CS4" s="87" t="s">
+      <c r="CJ4" s="58"/>
+      <c r="CK4" s="58"/>
+      <c r="CL4" s="58"/>
+      <c r="CM4" s="58"/>
+      <c r="CN4" s="58"/>
+      <c r="CO4" s="58"/>
+      <c r="CP4" s="58"/>
+      <c r="CQ4" s="58"/>
+      <c r="CR4" s="58"/>
+      <c r="CS4" s="54" t="s">
         <v>403</v>
       </c>
-      <c r="CT4" s="87"/>
-      <c r="CU4" s="87"/>
-      <c r="CV4" s="87"/>
-      <c r="CW4" s="87"/>
-      <c r="CX4" s="87"/>
-      <c r="CY4" s="87"/>
-      <c r="CZ4" s="87"/>
-      <c r="DA4" s="87"/>
-      <c r="DB4" s="87"/>
-      <c r="DC4" s="73" t="s">
+      <c r="CT4" s="54"/>
+      <c r="CU4" s="54"/>
+      <c r="CV4" s="54"/>
+      <c r="CW4" s="54"/>
+      <c r="CX4" s="54"/>
+      <c r="CY4" s="54"/>
+      <c r="CZ4" s="54"/>
+      <c r="DA4" s="54"/>
+      <c r="DB4" s="54"/>
+      <c r="DC4" s="58" t="s">
         <v>402</v>
       </c>
-      <c r="DD4" s="73"/>
-      <c r="DE4" s="73"/>
-      <c r="DF4" s="73"/>
-      <c r="DG4" s="73"/>
-      <c r="DH4" s="73"/>
-      <c r="DI4" s="73"/>
-      <c r="DJ4" s="73"/>
-      <c r="DK4" s="73"/>
-      <c r="DL4" s="73"/>
-      <c r="DM4" s="87" t="s">
+      <c r="DD4" s="58"/>
+      <c r="DE4" s="58"/>
+      <c r="DF4" s="58"/>
+      <c r="DG4" s="58"/>
+      <c r="DH4" s="58"/>
+      <c r="DI4" s="58"/>
+      <c r="DJ4" s="58"/>
+      <c r="DK4" s="58"/>
+      <c r="DL4" s="58"/>
+      <c r="DM4" s="54" t="s">
         <v>304</v>
       </c>
-      <c r="DN4" s="87"/>
-      <c r="DO4" s="87"/>
-      <c r="DP4" s="87"/>
-      <c r="DQ4" s="87"/>
-      <c r="DR4" s="87"/>
-      <c r="DS4" s="87"/>
-      <c r="DT4" s="87"/>
-      <c r="DU4" s="87"/>
-      <c r="DV4" s="87"/>
-      <c r="DW4" s="88" t="s">
+      <c r="DN4" s="54"/>
+      <c r="DO4" s="54"/>
+      <c r="DP4" s="54"/>
+      <c r="DQ4" s="54"/>
+      <c r="DR4" s="54"/>
+      <c r="DS4" s="54"/>
+      <c r="DT4" s="54"/>
+      <c r="DU4" s="54"/>
+      <c r="DV4" s="54"/>
+      <c r="DW4" s="55" t="s">
         <v>401</v>
       </c>
-      <c r="DX4" s="89"/>
-      <c r="DY4" s="89"/>
-      <c r="DZ4" s="89"/>
-      <c r="EA4" s="89"/>
-      <c r="EB4" s="89"/>
-      <c r="EC4" s="89"/>
-      <c r="ED4" s="89"/>
-      <c r="EE4" s="89"/>
-      <c r="EF4" s="90"/>
-      <c r="EG4" s="87" t="s">
+      <c r="DX4" s="56"/>
+      <c r="DY4" s="56"/>
+      <c r="DZ4" s="56"/>
+      <c r="EA4" s="56"/>
+      <c r="EB4" s="56"/>
+      <c r="EC4" s="56"/>
+      <c r="ED4" s="56"/>
+      <c r="EE4" s="56"/>
+      <c r="EF4" s="57"/>
+      <c r="EG4" s="54" t="s">
         <v>400</v>
       </c>
-      <c r="EH4" s="87"/>
-      <c r="EI4" s="87"/>
-      <c r="EJ4" s="87"/>
-      <c r="EK4" s="87"/>
-      <c r="EL4" s="87"/>
-      <c r="EM4" s="87"/>
-      <c r="EN4" s="87"/>
-      <c r="EO4" s="87"/>
-      <c r="EP4" s="87"/>
-      <c r="EQ4" s="88" t="s">
+      <c r="EH4" s="54"/>
+      <c r="EI4" s="54"/>
+      <c r="EJ4" s="54"/>
+      <c r="EK4" s="54"/>
+      <c r="EL4" s="54"/>
+      <c r="EM4" s="54"/>
+      <c r="EN4" s="54"/>
+      <c r="EO4" s="54"/>
+      <c r="EP4" s="54"/>
+      <c r="EQ4" s="55" t="s">
         <v>399</v>
       </c>
-      <c r="ER4" s="89"/>
-      <c r="ES4" s="89"/>
-      <c r="ET4" s="89"/>
-      <c r="EU4" s="89"/>
-      <c r="EV4" s="89"/>
-      <c r="EW4" s="89"/>
-      <c r="EX4" s="89"/>
-      <c r="EY4" s="89"/>
-      <c r="EZ4" s="90"/>
-      <c r="FA4" s="74" t="s">
+      <c r="ER4" s="56"/>
+      <c r="ES4" s="56"/>
+      <c r="ET4" s="56"/>
+      <c r="EU4" s="56"/>
+      <c r="EV4" s="56"/>
+      <c r="EW4" s="56"/>
+      <c r="EX4" s="56"/>
+      <c r="EY4" s="56"/>
+      <c r="EZ4" s="57"/>
+      <c r="FA4" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="FB4" s="74"/>
-      <c r="FC4" s="74"/>
-      <c r="FD4" s="74"/>
-      <c r="FE4" s="74"/>
-      <c r="FF4" s="74"/>
-      <c r="FG4" s="74"/>
-      <c r="FH4" s="74"/>
-      <c r="FI4" s="74"/>
-      <c r="FJ4" s="74"/>
-      <c r="FK4" s="75" t="s">
+      <c r="FB4" s="72"/>
+      <c r="FC4" s="72"/>
+      <c r="FD4" s="72"/>
+      <c r="FE4" s="72"/>
+      <c r="FF4" s="72"/>
+      <c r="FG4" s="72"/>
+      <c r="FH4" s="72"/>
+      <c r="FI4" s="72"/>
+      <c r="FJ4" s="72"/>
+      <c r="FK4" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="FL4" s="75"/>
-      <c r="FM4" s="75"/>
-      <c r="FN4" s="75"/>
-      <c r="FO4" s="75"/>
-      <c r="FP4" s="75"/>
-      <c r="FQ4" s="75"/>
-      <c r="FR4" s="75"/>
-      <c r="FS4" s="75"/>
-      <c r="FT4" s="75"/>
-      <c r="FU4" s="76" t="s">
+      <c r="FL4" s="73"/>
+      <c r="FM4" s="73"/>
+      <c r="FN4" s="73"/>
+      <c r="FO4" s="73"/>
+      <c r="FP4" s="73"/>
+      <c r="FQ4" s="73"/>
+      <c r="FR4" s="73"/>
+      <c r="FS4" s="73"/>
+      <c r="FT4" s="73"/>
+      <c r="FU4" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="FV4" s="76"/>
-      <c r="FW4" s="76"/>
-      <c r="FX4" s="76"/>
-      <c r="FY4" s="76"/>
-      <c r="FZ4" s="76"/>
-      <c r="GA4" s="76"/>
-      <c r="GB4" s="76"/>
-      <c r="GC4" s="76"/>
-      <c r="GD4" s="76"/>
-      <c r="GE4" s="77" t="s">
+      <c r="FV4" s="74"/>
+      <c r="FW4" s="74"/>
+      <c r="FX4" s="74"/>
+      <c r="FY4" s="74"/>
+      <c r="FZ4" s="74"/>
+      <c r="GA4" s="74"/>
+      <c r="GB4" s="74"/>
+      <c r="GC4" s="74"/>
+      <c r="GD4" s="74"/>
+      <c r="GE4" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="GF4" s="77"/>
-      <c r="GG4" s="77"/>
-      <c r="GH4" s="77"/>
-      <c r="GI4" s="77"/>
-      <c r="GJ4" s="77"/>
-      <c r="GK4" s="77"/>
-      <c r="GL4" s="77"/>
-      <c r="GM4" s="77"/>
-      <c r="GN4" s="77"/>
-      <c r="GO4" s="78" t="s">
+      <c r="GF4" s="75"/>
+      <c r="GG4" s="75"/>
+      <c r="GH4" s="75"/>
+      <c r="GI4" s="75"/>
+      <c r="GJ4" s="75"/>
+      <c r="GK4" s="75"/>
+      <c r="GL4" s="75"/>
+      <c r="GM4" s="75"/>
+      <c r="GN4" s="75"/>
+      <c r="GO4" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="GP4" s="78"/>
-      <c r="GQ4" s="78"/>
-      <c r="GR4" s="78"/>
-      <c r="GS4" s="78"/>
-      <c r="GT4" s="78"/>
-      <c r="GU4" s="78"/>
-      <c r="GV4" s="78"/>
-      <c r="GW4" s="78"/>
-      <c r="GX4" s="78"/>
-      <c r="GY4" s="79" t="s">
+      <c r="GP4" s="76"/>
+      <c r="GQ4" s="76"/>
+      <c r="GR4" s="76"/>
+      <c r="GS4" s="76"/>
+      <c r="GT4" s="76"/>
+      <c r="GU4" s="76"/>
+      <c r="GV4" s="76"/>
+      <c r="GW4" s="76"/>
+      <c r="GX4" s="76"/>
+      <c r="GY4" s="59" t="s">
         <v>392</v>
       </c>
-      <c r="GZ4" s="79"/>
-      <c r="HA4" s="79"/>
-      <c r="HB4" s="79"/>
-      <c r="HC4" s="79"/>
-      <c r="HD4" s="79"/>
-      <c r="HE4" s="79"/>
-      <c r="HF4" s="79"/>
-      <c r="HG4" s="79"/>
-      <c r="HH4" s="79"/>
-      <c r="HI4" s="70" t="s">
+      <c r="GZ4" s="59"/>
+      <c r="HA4" s="59"/>
+      <c r="HB4" s="59"/>
+      <c r="HC4" s="59"/>
+      <c r="HD4" s="59"/>
+      <c r="HE4" s="59"/>
+      <c r="HF4" s="59"/>
+      <c r="HG4" s="59"/>
+      <c r="HH4" s="59"/>
+      <c r="HI4" s="66" t="s">
         <v>148</v>
       </c>
-      <c r="HJ4" s="70"/>
-      <c r="HK4" s="70"/>
-      <c r="HL4" s="70"/>
-      <c r="HM4" s="70"/>
-      <c r="HN4" s="70"/>
-      <c r="HO4" s="70"/>
-      <c r="HP4" s="70"/>
-      <c r="HQ4" s="70"/>
-      <c r="HR4" s="70"/>
-      <c r="HS4" s="70" t="s">
+      <c r="HJ4" s="66"/>
+      <c r="HK4" s="66"/>
+      <c r="HL4" s="66"/>
+      <c r="HM4" s="66"/>
+      <c r="HN4" s="66"/>
+      <c r="HO4" s="66"/>
+      <c r="HP4" s="66"/>
+      <c r="HQ4" s="66"/>
+      <c r="HR4" s="66"/>
+      <c r="HS4" s="66" t="s">
         <v>159</v>
       </c>
-      <c r="HT4" s="70"/>
-      <c r="HU4" s="70"/>
-      <c r="HV4" s="70"/>
-      <c r="HW4" s="70"/>
-      <c r="HX4" s="70"/>
-      <c r="HY4" s="70"/>
-      <c r="HZ4" s="70"/>
-      <c r="IA4" s="70"/>
-      <c r="IB4" s="70"/>
-      <c r="IC4" s="70" t="s">
+      <c r="HT4" s="66"/>
+      <c r="HU4" s="66"/>
+      <c r="HV4" s="66"/>
+      <c r="HW4" s="66"/>
+      <c r="HX4" s="66"/>
+      <c r="HY4" s="66"/>
+      <c r="HZ4" s="66"/>
+      <c r="IA4" s="66"/>
+      <c r="IB4" s="66"/>
+      <c r="IC4" s="66" t="s">
         <v>170</v>
       </c>
-      <c r="ID4" s="70"/>
-      <c r="IE4" s="70"/>
-      <c r="IF4" s="70"/>
-      <c r="IG4" s="70"/>
-      <c r="IH4" s="70"/>
-      <c r="II4" s="70"/>
-      <c r="IJ4" s="70"/>
-      <c r="IK4" s="70"/>
-      <c r="IL4" s="70"/>
-      <c r="IM4" s="70" t="s">
+      <c r="ID4" s="66"/>
+      <c r="IE4" s="66"/>
+      <c r="IF4" s="66"/>
+      <c r="IG4" s="66"/>
+      <c r="IH4" s="66"/>
+      <c r="II4" s="66"/>
+      <c r="IJ4" s="66"/>
+      <c r="IK4" s="66"/>
+      <c r="IL4" s="66"/>
+      <c r="IM4" s="66" t="s">
         <v>181</v>
       </c>
-      <c r="IN4" s="70"/>
-      <c r="IO4" s="70"/>
-      <c r="IP4" s="70"/>
-      <c r="IQ4" s="70"/>
-      <c r="IR4" s="70"/>
-      <c r="IS4" s="70"/>
-      <c r="IT4" s="70"/>
-      <c r="IU4" s="70"/>
-      <c r="IV4" s="70"/>
-      <c r="IW4" s="82" t="s">
+      <c r="IN4" s="66"/>
+      <c r="IO4" s="66"/>
+      <c r="IP4" s="66"/>
+      <c r="IQ4" s="66"/>
+      <c r="IR4" s="66"/>
+      <c r="IS4" s="66"/>
+      <c r="IT4" s="66"/>
+      <c r="IU4" s="66"/>
+      <c r="IV4" s="66"/>
+      <c r="IW4" s="67" t="s">
         <v>192</v>
       </c>
-      <c r="IX4" s="83"/>
-      <c r="IY4" s="83"/>
-      <c r="IZ4" s="83"/>
-      <c r="JA4" s="83"/>
-      <c r="JB4" s="83"/>
-      <c r="JC4" s="83"/>
-      <c r="JD4" s="83"/>
-      <c r="JE4" s="83"/>
-      <c r="JF4" s="84"/>
-      <c r="JG4" s="82" t="s">
+      <c r="IX4" s="68"/>
+      <c r="IY4" s="68"/>
+      <c r="IZ4" s="68"/>
+      <c r="JA4" s="68"/>
+      <c r="JB4" s="68"/>
+      <c r="JC4" s="68"/>
+      <c r="JD4" s="68"/>
+      <c r="JE4" s="68"/>
+      <c r="JF4" s="69"/>
+      <c r="JG4" s="67" t="s">
         <v>203</v>
       </c>
-      <c r="JH4" s="83"/>
-      <c r="JI4" s="83"/>
-      <c r="JJ4" s="83"/>
-      <c r="JK4" s="83"/>
-      <c r="JL4" s="83"/>
-      <c r="JM4" s="83"/>
-      <c r="JN4" s="83"/>
-      <c r="JO4" s="83"/>
-      <c r="JP4" s="84"/>
-      <c r="JQ4" s="82" t="s">
+      <c r="JH4" s="68"/>
+      <c r="JI4" s="68"/>
+      <c r="JJ4" s="68"/>
+      <c r="JK4" s="68"/>
+      <c r="JL4" s="68"/>
+      <c r="JM4" s="68"/>
+      <c r="JN4" s="68"/>
+      <c r="JO4" s="68"/>
+      <c r="JP4" s="69"/>
+      <c r="JQ4" s="67" t="s">
         <v>214</v>
       </c>
-      <c r="JR4" s="83"/>
-      <c r="JS4" s="83"/>
-      <c r="JT4" s="83"/>
-      <c r="JU4" s="83"/>
-      <c r="JV4" s="83"/>
-      <c r="JW4" s="83"/>
-      <c r="JX4" s="83"/>
-      <c r="JY4" s="83"/>
-      <c r="JZ4" s="84"/>
-      <c r="KA4" s="82" t="s">
+      <c r="JR4" s="68"/>
+      <c r="JS4" s="68"/>
+      <c r="JT4" s="68"/>
+      <c r="JU4" s="68"/>
+      <c r="JV4" s="68"/>
+      <c r="JW4" s="68"/>
+      <c r="JX4" s="68"/>
+      <c r="JY4" s="68"/>
+      <c r="JZ4" s="69"/>
+      <c r="KA4" s="67" t="s">
         <v>416</v>
       </c>
-      <c r="KB4" s="83"/>
-      <c r="KC4" s="83"/>
-      <c r="KD4" s="83"/>
-      <c r="KE4" s="83"/>
-      <c r="KF4" s="83"/>
-      <c r="KG4" s="83"/>
-      <c r="KH4" s="83"/>
-      <c r="KI4" s="83"/>
-      <c r="KJ4" s="84"/>
-      <c r="KK4" s="82" t="s">
+      <c r="KB4" s="68"/>
+      <c r="KC4" s="68"/>
+      <c r="KD4" s="68"/>
+      <c r="KE4" s="68"/>
+      <c r="KF4" s="68"/>
+      <c r="KG4" s="68"/>
+      <c r="KH4" s="68"/>
+      <c r="KI4" s="68"/>
+      <c r="KJ4" s="69"/>
+      <c r="KK4" s="67" t="s">
         <v>235</v>
       </c>
-      <c r="KL4" s="83"/>
-      <c r="KM4" s="83"/>
-      <c r="KN4" s="83"/>
-      <c r="KO4" s="83"/>
-      <c r="KP4" s="83"/>
-      <c r="KQ4" s="83"/>
-      <c r="KR4" s="83"/>
-      <c r="KS4" s="83"/>
-      <c r="KT4" s="84"/>
-      <c r="KU4" s="85" t="s">
+      <c r="KL4" s="68"/>
+      <c r="KM4" s="68"/>
+      <c r="KN4" s="68"/>
+      <c r="KO4" s="68"/>
+      <c r="KP4" s="68"/>
+      <c r="KQ4" s="68"/>
+      <c r="KR4" s="68"/>
+      <c r="KS4" s="68"/>
+      <c r="KT4" s="69"/>
+      <c r="KU4" s="70" t="s">
         <v>246</v>
       </c>
-      <c r="KV4" s="85"/>
-      <c r="KW4" s="85"/>
-      <c r="KX4" s="85"/>
-      <c r="KY4" s="85"/>
-      <c r="KZ4" s="85"/>
-      <c r="LA4" s="85"/>
-      <c r="LB4" s="85"/>
-      <c r="LC4" s="85"/>
-      <c r="LD4" s="85"/>
-      <c r="LE4" s="85" t="s">
+      <c r="KV4" s="70"/>
+      <c r="KW4" s="70"/>
+      <c r="KX4" s="70"/>
+      <c r="KY4" s="70"/>
+      <c r="KZ4" s="70"/>
+      <c r="LA4" s="70"/>
+      <c r="LB4" s="70"/>
+      <c r="LC4" s="70"/>
+      <c r="LD4" s="70"/>
+      <c r="LE4" s="70" t="s">
         <v>257</v>
       </c>
-      <c r="LF4" s="85"/>
-      <c r="LG4" s="85"/>
-      <c r="LH4" s="85"/>
-      <c r="LI4" s="85"/>
-      <c r="LJ4" s="85"/>
-      <c r="LK4" s="85"/>
-      <c r="LL4" s="85"/>
-      <c r="LM4" s="85"/>
-      <c r="LN4" s="85"/>
-      <c r="LO4" s="85" t="s">
+      <c r="LF4" s="70"/>
+      <c r="LG4" s="70"/>
+      <c r="LH4" s="70"/>
+      <c r="LI4" s="70"/>
+      <c r="LJ4" s="70"/>
+      <c r="LK4" s="70"/>
+      <c r="LL4" s="70"/>
+      <c r="LM4" s="70"/>
+      <c r="LN4" s="70"/>
+      <c r="LO4" s="70" t="s">
         <v>263</v>
       </c>
-      <c r="LP4" s="85"/>
-      <c r="LQ4" s="85"/>
-      <c r="LR4" s="85"/>
-      <c r="LS4" s="85"/>
-      <c r="LT4" s="85"/>
-      <c r="LU4" s="85"/>
-      <c r="LV4" s="85"/>
-      <c r="LW4" s="85"/>
-      <c r="LX4" s="85"/>
-      <c r="LY4" s="85" t="s">
+      <c r="LP4" s="70"/>
+      <c r="LQ4" s="70"/>
+      <c r="LR4" s="70"/>
+      <c r="LS4" s="70"/>
+      <c r="LT4" s="70"/>
+      <c r="LU4" s="70"/>
+      <c r="LV4" s="70"/>
+      <c r="LW4" s="70"/>
+      <c r="LX4" s="70"/>
+      <c r="LY4" s="70" t="s">
         <v>274</v>
       </c>
-      <c r="LZ4" s="85"/>
-      <c r="MA4" s="85"/>
-      <c r="MB4" s="85"/>
-      <c r="MC4" s="85"/>
-      <c r="MD4" s="85"/>
-      <c r="ME4" s="85"/>
-      <c r="MF4" s="85"/>
-      <c r="MG4" s="85"/>
-      <c r="MH4" s="85"/>
-      <c r="MI4" s="86" t="s">
+      <c r="LZ4" s="70"/>
+      <c r="MA4" s="70"/>
+      <c r="MB4" s="70"/>
+      <c r="MC4" s="70"/>
+      <c r="MD4" s="70"/>
+      <c r="ME4" s="70"/>
+      <c r="MF4" s="70"/>
+      <c r="MG4" s="70"/>
+      <c r="MH4" s="70"/>
+      <c r="MI4" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="MJ4" s="86"/>
-      <c r="MK4" s="86"/>
-      <c r="ML4" s="86"/>
-      <c r="MM4" s="86"/>
-      <c r="MN4" s="86"/>
-      <c r="MO4" s="86"/>
-      <c r="MP4" s="86"/>
-      <c r="MQ4" s="86"/>
-      <c r="MR4" s="86"/>
-      <c r="MS4" s="86"/>
-      <c r="MT4" s="86"/>
-      <c r="MU4" s="86"/>
-      <c r="MV4" s="86"/>
-      <c r="MW4" s="56" t="s">
+      <c r="MJ4" s="71"/>
+      <c r="MK4" s="71"/>
+      <c r="ML4" s="71"/>
+      <c r="MM4" s="71"/>
+      <c r="MN4" s="71"/>
+      <c r="MO4" s="71"/>
+      <c r="MP4" s="71"/>
+      <c r="MQ4" s="71"/>
+      <c r="MR4" s="71"/>
+      <c r="MS4" s="71"/>
+      <c r="MT4" s="71"/>
+      <c r="MU4" s="71"/>
+      <c r="MV4" s="71"/>
+      <c r="MW4" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="MX4" s="80"/>
-      <c r="MY4" s="57"/>
+      <c r="MX4" s="61"/>
+      <c r="MY4" s="62"/>
       <c r="MZ4" s="37"/>
-      <c r="NA4" s="56" t="s">
+      <c r="NA4" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="NB4" s="57"/>
-      <c r="NC4" s="54"/>
-      <c r="ND4" s="52"/>
+      <c r="NB4" s="62"/>
+      <c r="NC4" s="89" t="s">
+        <v>99</v>
+      </c>
+      <c r="ND4" s="90"/>
+      <c r="NE4" s="52"/>
     </row>
-    <row r="5" spans="1:368" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="63"/>
-      <c r="B5" s="63"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64"/>
-      <c r="G5" s="64"/>
-      <c r="H5" s="64"/>
-      <c r="I5" s="65"/>
-      <c r="J5" s="65"/>
-      <c r="K5" s="65"/>
-      <c r="L5" s="65"/>
-      <c r="M5" s="65"/>
-      <c r="N5" s="66"/>
-      <c r="O5" s="66"/>
-      <c r="P5" s="66"/>
-      <c r="Q5" s="67"/>
-      <c r="R5" s="67"/>
-      <c r="S5" s="67"/>
-      <c r="T5" s="67"/>
-      <c r="U5" s="67"/>
-      <c r="V5" s="68"/>
-      <c r="W5" s="68"/>
-      <c r="X5" s="68"/>
-      <c r="Y5" s="68"/>
-      <c r="Z5" s="68"/>
-      <c r="AA5" s="68"/>
-      <c r="AB5" s="68"/>
-      <c r="AC5" s="69"/>
-      <c r="AD5" s="69"/>
-      <c r="AE5" s="69"/>
-      <c r="AF5" s="60"/>
-      <c r="AG5" s="60"/>
-      <c r="AH5" s="71"/>
-      <c r="AI5" s="71"/>
-      <c r="AJ5" s="71"/>
-      <c r="AK5" s="71"/>
-      <c r="AL5" s="71"/>
-      <c r="AM5" s="72"/>
-      <c r="AN5" s="72"/>
-      <c r="AO5" s="72"/>
-      <c r="AP5" s="72"/>
-      <c r="AQ5" s="72"/>
-      <c r="AR5" s="72"/>
-      <c r="AS5" s="72"/>
-      <c r="AT5" s="72"/>
-      <c r="AU5" s="72"/>
-      <c r="AV5" s="72"/>
-      <c r="AW5" s="72"/>
-      <c r="AX5" s="72"/>
-      <c r="AY5" s="72"/>
-      <c r="AZ5" s="72"/>
-      <c r="BA5" s="72"/>
-      <c r="BB5" s="72"/>
-      <c r="BC5" s="72"/>
-      <c r="BD5" s="72"/>
-      <c r="BE5" s="72"/>
-      <c r="BF5" s="72"/>
-      <c r="BG5" s="72"/>
-      <c r="BH5" s="72"/>
-      <c r="BI5" s="72"/>
-      <c r="BJ5" s="72"/>
-      <c r="BK5" s="72"/>
-      <c r="BL5" s="72"/>
-      <c r="BM5" s="72"/>
-      <c r="BN5" s="72"/>
+    <row r="5" spans="1:369" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="80"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="81"/>
+      <c r="H5" s="81"/>
+      <c r="I5" s="82"/>
+      <c r="J5" s="82"/>
+      <c r="K5" s="82"/>
+      <c r="L5" s="82"/>
+      <c r="M5" s="82"/>
+      <c r="N5" s="83"/>
+      <c r="O5" s="83"/>
+      <c r="P5" s="83"/>
+      <c r="Q5" s="84"/>
+      <c r="R5" s="84"/>
+      <c r="S5" s="84"/>
+      <c r="T5" s="84"/>
+      <c r="U5" s="84"/>
+      <c r="V5" s="85"/>
+      <c r="W5" s="85"/>
+      <c r="X5" s="85"/>
+      <c r="Y5" s="85"/>
+      <c r="Z5" s="85"/>
+      <c r="AA5" s="85"/>
+      <c r="AB5" s="85"/>
+      <c r="AC5" s="86"/>
+      <c r="AD5" s="86"/>
+      <c r="AE5" s="86"/>
+      <c r="AF5" s="77"/>
+      <c r="AG5" s="77"/>
+      <c r="AH5" s="87"/>
+      <c r="AI5" s="87"/>
+      <c r="AJ5" s="87"/>
+      <c r="AK5" s="87"/>
+      <c r="AL5" s="87"/>
+      <c r="AM5" s="88"/>
+      <c r="AN5" s="88"/>
+      <c r="AO5" s="88"/>
+      <c r="AP5" s="88"/>
+      <c r="AQ5" s="88"/>
+      <c r="AR5" s="88"/>
+      <c r="AS5" s="88"/>
+      <c r="AT5" s="88"/>
+      <c r="AU5" s="88"/>
+      <c r="AV5" s="88"/>
+      <c r="AW5" s="88"/>
+      <c r="AX5" s="88"/>
+      <c r="AY5" s="88"/>
+      <c r="AZ5" s="88"/>
+      <c r="BA5" s="88"/>
+      <c r="BB5" s="88"/>
+      <c r="BC5" s="88"/>
+      <c r="BD5" s="88"/>
+      <c r="BE5" s="88"/>
+      <c r="BF5" s="88"/>
+      <c r="BG5" s="88"/>
+      <c r="BH5" s="88"/>
+      <c r="BI5" s="88"/>
+      <c r="BJ5" s="88"/>
+      <c r="BK5" s="88"/>
+      <c r="BL5" s="88"/>
+      <c r="BM5" s="88"/>
+      <c r="BN5" s="88"/>
       <c r="BO5" s="7" t="s">
         <v>19</v>
       </c>
@@ -4781,30 +4786,31 @@
       <c r="MH5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="MI5" s="86"/>
-      <c r="MJ5" s="86"/>
-      <c r="MK5" s="86"/>
-      <c r="ML5" s="86"/>
-      <c r="MM5" s="86"/>
-      <c r="MN5" s="86"/>
-      <c r="MO5" s="86"/>
-      <c r="MP5" s="86"/>
-      <c r="MQ5" s="86"/>
-      <c r="MR5" s="86"/>
-      <c r="MS5" s="86"/>
-      <c r="MT5" s="86"/>
-      <c r="MU5" s="86"/>
-      <c r="MV5" s="86"/>
-      <c r="MW5" s="58"/>
-      <c r="MX5" s="81"/>
-      <c r="MY5" s="59"/>
+      <c r="MI5" s="71"/>
+      <c r="MJ5" s="71"/>
+      <c r="MK5" s="71"/>
+      <c r="ML5" s="71"/>
+      <c r="MM5" s="71"/>
+      <c r="MN5" s="71"/>
+      <c r="MO5" s="71"/>
+      <c r="MP5" s="71"/>
+      <c r="MQ5" s="71"/>
+      <c r="MR5" s="71"/>
+      <c r="MS5" s="71"/>
+      <c r="MT5" s="71"/>
+      <c r="MU5" s="71"/>
+      <c r="MV5" s="71"/>
+      <c r="MW5" s="63"/>
+      <c r="MX5" s="64"/>
+      <c r="MY5" s="65"/>
       <c r="MZ5" s="37"/>
-      <c r="NA5" s="58"/>
-      <c r="NB5" s="59"/>
-      <c r="NC5" s="55"/>
-      <c r="ND5" s="53"/>
+      <c r="NA5" s="63"/>
+      <c r="NB5" s="65"/>
+      <c r="NC5" s="91"/>
+      <c r="ND5" s="92"/>
+      <c r="NE5" s="53"/>
     </row>
-    <row r="6" spans="1:368" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:369" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>23</v>
       </c>
@@ -5904,13 +5910,16 @@
         <v>98</v>
       </c>
       <c r="NC6" s="18" t="s">
-        <v>99</v>
+        <v>417</v>
       </c>
       <c r="ND6" s="18" t="s">
+        <v>418</v>
+      </c>
+      <c r="NE6" s="18" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:368" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:369" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="39"/>
       <c r="B7" s="39"/>
       <c r="C7" s="39" t="s">
@@ -6409,37 +6418,12 @@
       <c r="NB7" s="51"/>
       <c r="NC7" s="51"/>
       <c r="ND7" s="51"/>
+      <c r="NE7" s="51"/>
     </row>
   </sheetData>
   <autoFilter ref="A6:MZ6" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <mergeCells count="43">
-    <mergeCell ref="EG4:EP4"/>
-    <mergeCell ref="EQ4:EZ4"/>
-    <mergeCell ref="BY4:CH4"/>
-    <mergeCell ref="CS4:DB4"/>
-    <mergeCell ref="DC4:DL4"/>
-    <mergeCell ref="DM4:DV4"/>
-    <mergeCell ref="DW4:EF4"/>
-    <mergeCell ref="GY4:HH4"/>
-    <mergeCell ref="MW4:MY5"/>
-    <mergeCell ref="HS4:IB4"/>
-    <mergeCell ref="KK4:KT4"/>
-    <mergeCell ref="KU4:LD4"/>
-    <mergeCell ref="LE4:LN4"/>
-    <mergeCell ref="LY4:MH4"/>
-    <mergeCell ref="MI4:MV5"/>
-    <mergeCell ref="IC4:IL4"/>
-    <mergeCell ref="IM4:IV4"/>
-    <mergeCell ref="IW4:JF4"/>
-    <mergeCell ref="JG4:JP4"/>
-    <mergeCell ref="JQ4:JZ4"/>
-    <mergeCell ref="KA4:KJ4"/>
-    <mergeCell ref="LO4:LX4"/>
-    <mergeCell ref="FA4:FJ4"/>
-    <mergeCell ref="FK4:FT4"/>
-    <mergeCell ref="FU4:GD4"/>
-    <mergeCell ref="GE4:GN4"/>
-    <mergeCell ref="GO4:GX4"/>
+  <mergeCells count="44">
+    <mergeCell ref="NC4:ND5"/>
     <mergeCell ref="NA4:NB5"/>
     <mergeCell ref="AF4:AG5"/>
     <mergeCell ref="A1:B1"/>
@@ -6456,6 +6440,33 @@
     <mergeCell ref="AM4:BN5"/>
     <mergeCell ref="BO4:BX4"/>
     <mergeCell ref="CI4:CR4"/>
+    <mergeCell ref="FA4:FJ4"/>
+    <mergeCell ref="FK4:FT4"/>
+    <mergeCell ref="FU4:GD4"/>
+    <mergeCell ref="GE4:GN4"/>
+    <mergeCell ref="GO4:GX4"/>
+    <mergeCell ref="GY4:HH4"/>
+    <mergeCell ref="MW4:MY5"/>
+    <mergeCell ref="HS4:IB4"/>
+    <mergeCell ref="KK4:KT4"/>
+    <mergeCell ref="KU4:LD4"/>
+    <mergeCell ref="LE4:LN4"/>
+    <mergeCell ref="LY4:MH4"/>
+    <mergeCell ref="MI4:MV5"/>
+    <mergeCell ref="IC4:IL4"/>
+    <mergeCell ref="IM4:IV4"/>
+    <mergeCell ref="IW4:JF4"/>
+    <mergeCell ref="JG4:JP4"/>
+    <mergeCell ref="JQ4:JZ4"/>
+    <mergeCell ref="KA4:KJ4"/>
+    <mergeCell ref="LO4:LX4"/>
+    <mergeCell ref="EG4:EP4"/>
+    <mergeCell ref="EQ4:EZ4"/>
+    <mergeCell ref="BY4:CH4"/>
+    <mergeCell ref="CS4:DB4"/>
+    <mergeCell ref="DC4:DL4"/>
+    <mergeCell ref="DM4:DV4"/>
+    <mergeCell ref="DW4:EF4"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A6">
     <cfRule type="duplicateValues" dxfId="0" priority="92"/>

</xml_diff>

<commit_message>
[RUBY-3853] Change "Operational Maintenance Cost" column to "Operation and Maintenance Cost" in xlsx file
</commit_message>
<xml_diff>
--- a/lib/fcerm1_template.xlsx
+++ b/lib/fcerm1_template.xlsx
@@ -1307,7 +1307,7 @@
     <t xml:space="preserve">Net Carbon Economic Benefit</t>
   </si>
   <si>
-    <t xml:space="preserve">Operational Maintenance Cost</t>
+    <t xml:space="preserve">Operation and Maintenance Cost</t>
   </si>
   <si>
     <t xml:space="preserve">Updated at</t>
@@ -1665,15 +1665,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1681,31 +1681,31 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1713,11 +1713,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1725,31 +1725,31 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1757,151 +1757,151 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="11" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="11" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="6" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="7" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="8" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="8" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="9" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="9" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="11" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="10" fillId="11" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="12" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="12" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="13" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="13" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="14" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="14" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="15" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="15" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="16" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="16" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="17" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="17" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="18" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="18" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="19" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="19" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="6" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="7" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="20" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="20" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="21" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="21" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="22" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="22" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="15" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="15" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="22" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="22" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="16" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="16" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="22" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="22" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="10" fillId="0" borderId="1" xfId="25" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="171" fontId="10" fillId="0" borderId="1" xfId="25" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="25" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="25" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="10" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="171" fontId="10" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="172" fontId="10" fillId="0" borderId="1" xfId="25" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="172" fontId="10" fillId="0" borderId="1" xfId="25" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1913,11 +1913,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1925,15 +1925,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1941,7 +1941,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1949,19 +1949,19 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="173" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="173" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="174" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="174" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1969,11 +1969,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="173" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="173" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2260,11 +2260,11 @@
   <dimension ref="A1:NI7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="NB7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="NC7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="NB1" activeCellId="0" sqref="NB1"/>
+      <selection pane="topRight" activeCell="NC1" activeCellId="0" sqref="NC1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="ND6" activeCellId="0" sqref="ND6"/>
+      <selection pane="bottomRight" activeCell="NF6" activeCellId="0" sqref="NF6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
[RUBY-3853] Change "Operational Maintenance Cost" column to "Operation and (#1162)
Maintenance Cost" in xlsx file
</commit_message>
<xml_diff>
--- a/lib/fcerm1_template.xlsx
+++ b/lib/fcerm1_template.xlsx
@@ -1307,7 +1307,7 @@
     <t xml:space="preserve">Net Carbon Economic Benefit</t>
   </si>
   <si>
-    <t xml:space="preserve">Operational Maintenance Cost</t>
+    <t xml:space="preserve">Operation and Maintenance Cost</t>
   </si>
   <si>
     <t xml:space="preserve">Updated at</t>
@@ -1665,15 +1665,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1681,31 +1681,31 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1713,11 +1713,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1725,31 +1725,31 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1757,151 +1757,151 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="11" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="11" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="6" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="7" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="8" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="8" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="9" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="9" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="11" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="10" fillId="11" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="12" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="12" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="13" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="13" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="14" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="14" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="15" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="15" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="16" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="16" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="17" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="17" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="18" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="18" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="19" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="19" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="6" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="7" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="20" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="20" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="21" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="21" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="22" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="22" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="15" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="15" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="22" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="22" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="16" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="16" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="22" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="22" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="10" fillId="0" borderId="1" xfId="25" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="171" fontId="10" fillId="0" borderId="1" xfId="25" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="25" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="25" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="10" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="171" fontId="10" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="172" fontId="10" fillId="0" borderId="1" xfId="25" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="172" fontId="10" fillId="0" borderId="1" xfId="25" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1913,11 +1913,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1925,15 +1925,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1941,7 +1941,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1949,19 +1949,19 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="173" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="173" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="174" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="174" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1969,11 +1969,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="173" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="173" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2260,11 +2260,11 @@
   <dimension ref="A1:NI7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="NB7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="NC7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="NB1" activeCellId="0" sqref="NB1"/>
+      <selection pane="topRight" activeCell="NC1" activeCellId="0" sqref="NC1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="ND6" activeCellId="0" sqref="ND6"/>
+      <selection pane="bottomRight" activeCell="NF6" activeCellId="0" sqref="NF6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>